<commit_message>
Replace PMPM terminology with PMPY
Do this because that is how things are actually priced.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t>Annual PMPM Add-on Data Fees (with implicit forces):</t>
   </si>
   <si>
-    <t>PRM Increase on PMPM Add-on fees:</t>
-  </si>
-  <si>
     <t>Annual PMPM Add-on Product Fees (Marginal over data fees)</t>
   </si>
   <si>
@@ -322,9 +319,6 @@
   </si>
   <si>
     <t>Existing Collaborative Discount</t>
-  </si>
-  <si>
-    <t>PMPM Add-Ons</t>
   </si>
   <si>
     <t>25k-50k</t>
@@ -457,6 +451,12 @@
   </si>
   <si>
     <t>Frequency Multiplier</t>
+  </si>
+  <si>
+    <t>PMPY Add-Ons</t>
+  </si>
+  <si>
+    <t>PRM Increase on PMPY Add-on fees:</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1211,7 +1211,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="91" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="70">
         <v>43101</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="71">
         <v>36</v>
@@ -1227,29 +1227,29 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="67" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="68"/>
       <c r="C4" s="72"/>
       <c r="D4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
     </row>
     <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="55" t="s">
         <v>29</v>
@@ -1314,12 +1314,12 @@
       <c r="G8" s="55"/>
       <c r="H8" s="56"/>
       <c r="L8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="55">
         <v>1</v>
@@ -1331,12 +1331,12 @@
       <c r="G9" s="55"/>
       <c r="H9" s="56"/>
       <c r="L9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="69" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D10" s="55" t="s">
         <v>29</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>29</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D24" s="55" t="s">
         <v>3</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="92" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="93"/>
       <c r="D25" s="94" t="s">
@@ -1581,7 +1581,7 @@
   <dimension ref="B2:U45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
@@ -1602,19 +1602,19 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>110</v>
-      </c>
-      <c r="G2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D44, Calcs!D56)</f>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D66, Calcs!D75)</f>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1">
         <f>SUM(Calcs!D67, Calcs!D76)</f>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1">
         <f>SUM(Calcs!D68, Calcs!D77)</f>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D29" s="1">
         <f>Calcs!D106</f>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="1">
         <f>Calcs!D108</f>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="7">
         <f>(D32/12*Inputs!$C$2+D4)*$C$35</f>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
@@ -2548,10 +2548,10 @@
   <dimension ref="B1:N70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2573,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="50"/>
       <c r="H1" s="50"/>
@@ -2590,10 +2590,10 @@
         <v>42</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9" t="s">
@@ -2603,10 +2603,10 @@
         <v>42</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -2616,7 +2616,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$5:$H$5, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1">
         <f>SUMIF(Inputs!$D$5:$H$5, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D20:H20)</f>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G19" s="48" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="H19" s="10">
         <v>0.1</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="18">
         <f>SUM(Calcs!D32:H32)</f>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C38" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D38" s="20">
         <f>SUM(Calcs!D84:H84)</f>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C39" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D39" s="20">
         <f>SUM(Calcs!D85:H85)</f>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C40" s="81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" s="84">
         <f>SUM(Calcs!D86:H86)</f>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C47" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D47" s="20">
         <f>SUM(Calcs!D93:H93)</f>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C48" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D48" s="20">
         <f>SUM(Calcs!D94:H94)</f>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C49" s="81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="84">
         <f>SUM(Calcs!D95:H95)</f>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D53" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D54" s="1">
         <f>Outputs_External!D30</f>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C57" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D57" s="23">
         <f>SUM(K56:N56)</f>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
@@ -4557,7 +4557,7 @@
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="27"/>
       <c r="C68" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D68" s="23">
         <f>SUM(Calcs!D66:H66)+SUM(Calcs!D75:H75)</f>
@@ -4601,7 +4601,7 @@
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="27"/>
       <c r="C69" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D69" s="23">
         <f>SUM(Calcs!D67:H67)+SUM(Calcs!D76:H76)</f>
@@ -4645,7 +4645,7 @@
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="27"/>
       <c r="C70" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D70" s="23">
         <f>SUM(Calcs!D68:H68)+SUM(Calcs!D77:H77)</f>
@@ -4728,20 +4728,20 @@
         <v>36</v>
       </c>
       <c r="H1" s="61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="61"/>
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
       <c r="M1" s="61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N1" s="61"/>
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
       <c r="Q1" s="61"/>
       <c r="S1" s="61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T1" s="61"/>
       <c r="U1" s="61"/>
@@ -4749,60 +4749,60 @@
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="62" t="s">
         <v>65</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>66</v>
       </c>
       <c r="J2" s="62" t="s">
         <v>42</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M2" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="62" t="s">
         <v>65</v>
-      </c>
-      <c r="N2" s="62" t="s">
-        <v>66</v>
       </c>
       <c r="O2" s="62" t="s">
         <v>42</v>
       </c>
       <c r="P2" s="62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S2" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="62" t="s">
         <v>65</v>
-      </c>
-      <c r="T2" s="62" t="s">
-        <v>66</v>
       </c>
       <c r="U2" s="62" t="s">
         <v>42</v>
       </c>
       <c r="V2" s="62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W2" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
@@ -11608,19 +11608,19 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>110</v>
-      </c>
-      <c r="G2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" t="s">
-        <v>112</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>31</v>
@@ -11675,18 +11675,18 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="K5" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L5" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6" s="5">
         <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K6,0),$L6-$K6),0)</f>
@@ -11720,7 +11720,7 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="5">
         <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K7,0),$L7-$K7),0)</f>
@@ -11755,7 +11755,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="5">
         <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K8,0),$L8-$K8),0)</f>
@@ -11790,7 +11790,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="5">
         <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K9,0),$L9-$K9),0)</f>
@@ -11825,7 +11825,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="78" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="79">
         <f>IFERROR(SUMPRODUCT(D6:D9,$M$6:$M$9)/SUM(D6:D9),0)</f>
@@ -11850,7 +11850,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="78" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="80">
         <f>SUM(D6:D9)</f>
@@ -12037,7 +12037,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$21="Y"), Prices!$C15, 0)</f>
@@ -12292,7 +12292,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="18">
         <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
@@ -12549,7 +12549,7 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" s="18">
         <f>IF(AND(Inputs!D16="Y",Inputs!D$21="N"),Prices!$C15,0)</f>
@@ -12804,7 +12804,7 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D56" s="18">
         <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))</f>
@@ -13004,7 +13004,7 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C66" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D66" s="20">
         <f>IF(Inputs!D24="Y", Prices!$C24 * IF(Inputs!D23="Y",1-Prices!$L$20,1), 0)</f>
@@ -13029,7 +13029,7 @@
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C67" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D67" s="20">
         <f>IF(Inputs!D25="Y", Prices!$C25, 0)</f>
@@ -13054,7 +13054,7 @@
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C68" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D68" s="84">
         <f>IF(Inputs!D10="Y", Prices!$C26, 0)</f>
@@ -13082,7 +13082,7 @@
         <v>46</v>
       </c>
       <c r="J70" s="89" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
@@ -13277,7 +13277,7 @@
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D75" s="20">
         <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D24 = "Y", D$11*Prices!$E24 * IF(Inputs!D23="Y",1-Prices!$L$20,1), 0)))*D$10</f>
@@ -13326,7 +13326,7 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C76" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D76" s="20">
         <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D25 = "Y", D$11*Prices!$E25, 0)))*D$10</f>
@@ -13375,7 +13375,7 @@
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C77" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D77" s="84">
         <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D10 = "Y", D$11*Prices!$E26, 0)))*D$10</f>
@@ -13616,7 +13616,7 @@
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C84" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D84" s="20">
         <f t="shared" ref="D84:H84" si="15">D66</f>
@@ -13661,7 +13661,7 @@
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C85" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D85" s="20">
         <f t="shared" ref="D85:H85" si="17">D67</f>
@@ -13706,7 +13706,7 @@
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C86" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D86" s="84">
         <f t="shared" ref="D86:H86" si="19">D68</f>
@@ -13851,7 +13851,7 @@
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C93" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D93" s="20">
         <f t="shared" ref="D93:H93" si="21">D75</f>
@@ -13876,7 +13876,7 @@
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C94" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D94" s="20">
         <f t="shared" ref="D94:H94" si="22">D76</f>
@@ -13901,7 +13901,7 @@
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C95" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D95" s="84">
         <f t="shared" ref="D95:H95" si="23">D77</f>
@@ -13990,7 +13990,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D100" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A100, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A100, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -14018,7 +14018,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D101" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A101, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A101, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -14046,7 +14046,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D102" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A102, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A102, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -14071,7 +14071,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D104" s="7">
         <f>SUM(D38:D47, D50:D59, D62:D68, D71:D77, D98:D102)</f>
@@ -14131,7 +14131,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D108" s="1">
         <f>IF(Inputs!$D$6 = "Y", Prices!$L$18, 0)*-1</f>
@@ -14152,7 +14152,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D110" s="7">
         <f>SUM(D104, D106)</f>
@@ -14178,7 +14178,7 @@
     <row r="113" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="27"/>
       <c r="C113" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D113" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D104,$D$104:$H$104),5)</f>
@@ -14271,13 +14271,13 @@
     <row r="118" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="27"/>
       <c r="C118" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="27"/>
       <c r="D119" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E119" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(2, $D$116:$H$116, 0))*Prices!$L$10*-1</f>
@@ -14287,7 +14287,7 @@
     <row r="120" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="27"/>
       <c r="D120" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E120" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(3, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14297,7 +14297,7 @@
     <row r="121" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="27"/>
       <c r="D121" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E121" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(4, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14307,7 +14307,7 @@
     <row r="122" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="27"/>
       <c r="D122" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E122" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(5, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14327,7 +14327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14352,7 +14354,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1">
         <v>5000</v>
@@ -14379,7 +14381,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="F4" s="76">
         <v>0.6</v>
@@ -14399,16 +14401,16 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E5" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>88</v>
-      </c>
       <c r="H5" s="48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K5" t="s">
         <v>26</v>
@@ -14456,7 +14458,7 @@
       <c r="C8" s="43"/>
       <c r="D8" s="39"/>
       <c r="K8" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -14468,7 +14470,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
       <c r="K9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -14499,7 +14501,7 @@
         <v>9.6000000000000009E-3</v>
       </c>
       <c r="K10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L10" s="3">
         <v>0.45</v>
@@ -14530,7 +14532,7 @@
         <v>1.4000000000000002E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L11" s="3">
         <v>0.5</v>
@@ -14612,7 +14614,7 @@
         <v>1.4000000000000002E-2</v>
       </c>
       <c r="K14" s="58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L14" s="57">
         <v>1.2500000000000001E-2</v>
@@ -14620,7 +14622,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="44">
         <f>$L$25*4000</f>
@@ -14643,7 +14645,7 @@
         <v>1.4000000000000002E-2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L15" s="54">
         <v>43466</v>
@@ -14726,7 +14728,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L18" s="1">
         <v>3525</v>
@@ -14764,7 +14766,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L20" s="3">
         <v>0.3</v>
@@ -14845,7 +14847,7 @@
         <v>0.05</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L23" s="96">
         <f>18000/15000</f>
@@ -14854,7 +14856,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24" s="45">
         <v>33600</v>
@@ -14877,7 +14879,7 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="45">
         <f>$L$25*20000</f>
@@ -14900,7 +14902,7 @@
         <v>3.3600000000000005E-2</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L25" s="97">
         <f>IF(Inputs!$C$3="Monthly",Prices!$L$23,1)</f>
@@ -14909,7 +14911,7 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26" s="82">
         <f>$L$25*6750</f>

</xml_diff>

<commit_message>
Refine the CaregiverChecklist pricing.
Do this because some of the interactions with CCR weren't quite correct.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1203,7 +1203,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
@@ -1517,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
@@ -1605,7 +1605,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="E21" s="1">
         <f>SUM(Calcs!E64, Calcs!E74)</f>
-        <v>0</v>
+        <v>80220</v>
       </c>
       <c r="F21" s="1">
         <f>SUM(Calcs!F64, Calcs!F74)</f>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="E29" s="1">
         <f>SUM(Calcs!E102:E106)</f>
-        <v>0</v>
+        <v>-24066</v>
       </c>
       <c r="F29" s="1">
         <f>SUM(Calcs!F102:F106)</f>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="E33" s="7">
         <f>SUM(E7:E16, E19:E26, E29:E30)</f>
-        <v>149620</v>
+        <v>205774</v>
       </c>
       <c r="F33" s="7">
         <f>SUM(F7:F16, F19:F26, F29:F30)</f>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="E38" s="7">
         <f>(E33/12*Inputs!$C$2+E4)*$C$36</f>
-        <v>508860</v>
+        <v>677322</v>
       </c>
       <c r="F38" s="7">
         <f>(F33/12*Inputs!$C$2+F4)*$C$36</f>
@@ -2565,13 +2565,13 @@
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C42" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>617860</v>
+        <v>786322</v>
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C43" s="52">
         <f>SUM(D38:H38)</f>
-        <v>617860</v>
+        <v>786322</v>
       </c>
       <c r="D43" s="1"/>
       <c r="G43" s="1"/>
@@ -2607,7 +2607,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D23:H23)</f>
-        <v>12000</v>
+        <v>6000</v>
       </c>
       <c r="F17" s="33">
         <v>0.1</v>
@@ -3135,11 +3135,11 @@
       </c>
       <c r="K17" s="20">
         <f t="shared" si="3"/>
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="L17" s="20">
         <f>G17*$D17</f>
-        <v>10800</v>
+        <v>5400</v>
       </c>
       <c r="M17" s="20">
         <f t="shared" si="2"/>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="D29" s="20">
         <f>SUM(Calcs!D33:H33)</f>
-        <v>0</v>
+        <v>22750</v>
       </c>
       <c r="F29" s="37">
         <f t="shared" si="11"/>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="L29" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>22750</v>
       </c>
       <c r="M29" s="20">
         <f t="shared" si="10"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="D30" s="20">
         <f>SUM(Calcs!D34:H34)</f>
-        <v>0</v>
+        <v>9100</v>
       </c>
       <c r="F30" s="37">
         <f t="shared" si="11"/>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="L30" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>9100</v>
       </c>
       <c r="M30" s="20">
         <f t="shared" si="10"/>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="D36" s="20">
         <f>SUM(Calcs!D84:H84)</f>
-        <v>18000</v>
+        <v>42000</v>
       </c>
       <c r="F36" s="33">
         <v>0.1</v>
@@ -3725,11 +3725,11 @@
       </c>
       <c r="K36" s="20">
         <f t="shared" si="12"/>
-        <v>1800</v>
+        <v>4200</v>
       </c>
       <c r="L36" s="20">
         <f t="shared" si="12"/>
-        <v>16200</v>
+        <v>37800</v>
       </c>
       <c r="M36" s="20">
         <f t="shared" si="12"/>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="D37" s="20">
         <f>SUM(Calcs!D85:H85)</f>
-        <v>18000</v>
+        <v>42000</v>
       </c>
       <c r="F37" s="33">
         <v>0.1</v>
@@ -3762,11 +3762,11 @@
       </c>
       <c r="K37" s="20">
         <f t="shared" ref="K37" si="14">F37*$D37</f>
-        <v>1800</v>
+        <v>4200</v>
       </c>
       <c r="L37" s="20">
         <f t="shared" ref="L37" si="15">G37*$D37</f>
-        <v>16200</v>
+        <v>37800</v>
       </c>
       <c r="M37" s="20">
         <f t="shared" ref="M37" si="16">H37*$D37</f>
@@ -3955,15 +3955,15 @@
         <v>0</v>
       </c>
       <c r="F44" s="49">
-        <f>IFERROR((1-G44)*F34/SUM(F34,H34),0)</f>
+        <f t="shared" ref="F44:F50" si="28">IFERROR((1-G44)*F34/SUM(F34,H34),0)</f>
         <v>0.8</v>
       </c>
       <c r="G44" s="49">
-        <f>MIN(1,G34+$H$19)</f>
+        <f t="shared" ref="G44:G50" si="29">MIN(1,G34+$H$19)</f>
         <v>0.2</v>
       </c>
       <c r="H44" s="49">
-        <f>IFERROR((1-G44)*H34/SUM(F34,H34),0)</f>
+        <f t="shared" ref="H44:H50" si="30">IFERROR((1-G44)*H34/SUM(F34,H34),0)</f>
         <v>0</v>
       </c>
       <c r="I44" s="49">
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="29">
-        <f t="shared" ref="L44:L48" si="28">G44*$D44</f>
+        <f t="shared" ref="L44:L48" si="31">G44*$D44</f>
         <v>0</v>
       </c>
       <c r="M44" s="29">
@@ -3995,15 +3995,15 @@
         <v>0</v>
       </c>
       <c r="F45" s="30">
-        <f>IFERROR((1-G45)*F35/SUM(F35,H35),0)</f>
+        <f t="shared" si="28"/>
         <v>0.8</v>
       </c>
       <c r="G45" s="30">
-        <f>MIN(1,G35+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="H45" s="30">
-        <f>IFERROR((1-G45)*H35/SUM(F35,H35),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I45" s="30">
@@ -4014,15 +4014,15 @@
         <v>0</v>
       </c>
       <c r="L45" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M45" s="18">
-        <f t="shared" ref="M45:N48" si="29">H45*$D45</f>
+        <f t="shared" ref="M45:N48" si="32">H45*$D45</f>
         <v>0</v>
       </c>
       <c r="N45" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -4032,37 +4032,37 @@
       </c>
       <c r="D46" s="20">
         <f>SUM(Calcs!D94:H94)</f>
-        <v>0</v>
+        <v>6370</v>
       </c>
       <c r="F46" s="31">
-        <f>IFERROR((1-G46)*F36/SUM(F36,H36),0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G46" s="31">
-        <f>MIN(1,G36+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="H46" s="31">
-        <f>IFERROR((1-G46)*H36/SUM(F36,H36),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I46" s="31">
         <v>0</v>
       </c>
       <c r="K46" s="20">
-        <f t="shared" ref="K46:K48" si="30">F46*$D46</f>
+        <f t="shared" ref="K46:K48" si="33">F46*$D46</f>
         <v>0</v>
       </c>
       <c r="L46" s="20">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>6370</v>
       </c>
       <c r="M46" s="20">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N46" s="20">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -4075,34 +4075,34 @@
         <v>38220</v>
       </c>
       <c r="F47" s="31">
-        <f>IFERROR((1-G47)*F37/SUM(F37,H37),0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G47" s="31">
-        <f>MIN(1,G37+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="H47" s="31">
-        <f>IFERROR((1-G47)*H37/SUM(F37,H37),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I47" s="31">
         <v>0</v>
       </c>
       <c r="K47" s="20">
-        <f t="shared" ref="K47" si="31">F47*$D47</f>
+        <f t="shared" ref="K47" si="34">F47*$D47</f>
         <v>0</v>
       </c>
       <c r="L47" s="20">
-        <f t="shared" ref="L47" si="32">G47*$D47</f>
+        <f t="shared" ref="L47" si="35">G47*$D47</f>
         <v>38220</v>
       </c>
       <c r="M47" s="20">
-        <f t="shared" ref="M47" si="33">H47*$D47</f>
+        <f t="shared" ref="M47" si="36">H47*$D47</f>
         <v>0</v>
       </c>
       <c r="N47" s="20">
-        <f t="shared" ref="N47" si="34">I47*$D47</f>
+        <f t="shared" ref="N47" si="37">I47*$D47</f>
         <v>0</v>
       </c>
     </row>
@@ -4115,34 +4115,34 @@
         <v>0</v>
       </c>
       <c r="F48" s="31">
-        <f>IFERROR((1-G48)*F38/SUM(F38,H38),0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G48" s="31">
-        <f>MIN(1,G38+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="H48" s="31">
-        <f>IFERROR((1-G48)*H38/SUM(F38,H38),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I48" s="31">
         <v>0</v>
       </c>
       <c r="K48" s="20">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L48" s="20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M48" s="20">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N48" s="20">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -4155,34 +4155,34 @@
         <v>0</v>
       </c>
       <c r="F49" s="31">
-        <f>IFERROR((1-G49)*F39/SUM(F39,H39),0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G49" s="31">
-        <f>MIN(1,G39+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="H49" s="31">
-        <f>IFERROR((1-G49)*H39/SUM(F39,H39),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I49" s="31">
         <v>0</v>
       </c>
       <c r="K49" s="20">
-        <f t="shared" ref="K49:K50" si="35">F49*$D49</f>
+        <f t="shared" ref="K49:K50" si="38">F49*$D49</f>
         <v>0</v>
       </c>
       <c r="L49" s="20">
-        <f t="shared" ref="L49:L50" si="36">G49*$D49</f>
+        <f t="shared" ref="L49:L50" si="39">G49*$D49</f>
         <v>0</v>
       </c>
       <c r="M49" s="20">
-        <f t="shared" ref="M49:M50" si="37">H49*$D49</f>
+        <f t="shared" ref="M49:M50" si="40">H49*$D49</f>
         <v>0</v>
       </c>
       <c r="N49" s="20">
-        <f t="shared" ref="N49:N50" si="38">I49*$D49</f>
+        <f t="shared" ref="N49:N50" si="41">I49*$D49</f>
         <v>0</v>
       </c>
     </row>
@@ -4195,34 +4195,34 @@
         <v>0</v>
       </c>
       <c r="F50" s="31">
-        <f>IFERROR((1-G50)*F40/SUM(F40,H40),0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G50" s="31">
-        <f>MIN(1,G40+$H$19)</f>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="H50" s="31">
-        <f>IFERROR((1-G50)*H40/SUM(F40,H40),0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I50" s="31">
         <v>0</v>
       </c>
       <c r="K50" s="20">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L50" s="20">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="M50" s="20">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="N50" s="20">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
@@ -4235,34 +4235,34 @@
         <v>0</v>
       </c>
       <c r="F51" s="87">
-        <f t="shared" ref="F51" si="39">IFERROR((1-G51)*F41/SUM(F41,H41),0)</f>
+        <f t="shared" ref="F51" si="42">IFERROR((1-G51)*F41/SUM(F41,H41),0)</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="G51" s="87">
-        <f t="shared" ref="G51" si="40">MIN(1,G41+$H$19)</f>
+        <f t="shared" ref="G51" si="43">MIN(1,G41+$H$19)</f>
         <v>0.9</v>
       </c>
       <c r="H51" s="87">
-        <f t="shared" ref="H51" si="41">IFERROR((1-G51)*H41/SUM(F41,H41),0)</f>
+        <f t="shared" ref="H51" si="44">IFERROR((1-G51)*H41/SUM(F41,H41),0)</f>
         <v>0</v>
       </c>
       <c r="I51" s="87">
         <v>0</v>
       </c>
       <c r="K51" s="84">
-        <f t="shared" ref="K51" si="42">F51*$D51</f>
+        <f t="shared" ref="K51" si="45">F51*$D51</f>
         <v>0</v>
       </c>
       <c r="L51" s="84">
-        <f t="shared" ref="L51" si="43">G51*$D51</f>
+        <f t="shared" ref="L51" si="46">G51*$D51</f>
         <v>0</v>
       </c>
       <c r="M51" s="84">
-        <f t="shared" ref="M51" si="44">H51*$D51</f>
+        <f t="shared" ref="M51" si="47">H51*$D51</f>
         <v>0</v>
       </c>
       <c r="N51" s="84">
-        <f t="shared" ref="N51" si="45">I51*$D51</f>
+        <f t="shared" ref="N51" si="48">I51*$D51</f>
         <v>0</v>
       </c>
     </row>
@@ -4285,31 +4285,31 @@
       </c>
       <c r="D54" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
-        <v>0</v>
+        <v>-24066</v>
       </c>
       <c r="F54" s="8">
         <f>IFERROR(SUM(K66:K72)/SUM($K$66:$N$72), 0)</f>
-        <v>0.1</v>
+        <v>6.8728522336769765E-2</v>
       </c>
       <c r="G54" s="8">
-        <f t="shared" ref="G54:I54" si="46">IFERROR(SUM(L66:L72)/SUM($K$66:$N$72), 0)</f>
-        <v>0.9</v>
+        <f t="shared" ref="G54:I54" si="49">IFERROR(SUM(L66:L72)/SUM($K$66:$N$72), 0)</f>
+        <v>0.93127147766323026</v>
       </c>
       <c r="H54" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="I54" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="K54" s="12">
         <f>F54*$D$54</f>
-        <v>0</v>
+        <v>-1654.0206185567013</v>
       </c>
       <c r="L54" s="12">
         <f>G54*$D$54</f>
-        <v>0</v>
+        <v>-22411.9793814433</v>
       </c>
       <c r="M54" s="12">
         <f>H54*$D$54</f>
@@ -4330,11 +4330,11 @@
       </c>
       <c r="F55" s="3">
         <f>IFERROR(SUM(K8:K54)/SUM($K8:$N54), 0)</f>
-        <v>0.18948573609388417</v>
+        <v>0.15902977485172853</v>
       </c>
       <c r="G55" s="3">
         <f>IFERROR(SUM(L8:L54)/SUM($K8:$N54), 0)</f>
-        <v>0.81051426390611581</v>
+        <v>0.84097022514827147</v>
       </c>
       <c r="H55" s="3">
         <f>IFERROR(SUM(M8:M54)/SUM($K8:$N54), 0)</f>
@@ -4346,11 +4346,11 @@
       </c>
       <c r="K55" s="12">
         <f>F55*$D$55</f>
-        <v>-5116.1148745348728</v>
+        <v>-4293.8039209966701</v>
       </c>
       <c r="L55" s="12">
         <f>G55*$D$55</f>
-        <v>-21883.885125465127</v>
+        <v>-22706.19607900333</v>
       </c>
       <c r="M55" s="12">
         <f>H55*$D$55</f>
@@ -4387,15 +4387,15 @@
         <v>0</v>
       </c>
       <c r="L56" s="12">
-        <f t="shared" ref="L56:N56" si="47">$D$56*G56</f>
+        <f t="shared" ref="L56:N56" si="50">$D$56*G56</f>
         <v>0</v>
       </c>
       <c r="M56" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="N56" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
     </row>
@@ -4410,15 +4410,15 @@
       </c>
       <c r="D58" s="1">
         <f>SUM(Outputs_External!D33:'Outputs_External'!H33)</f>
-        <v>182620</v>
+        <v>238774</v>
       </c>
       <c r="K58" s="12">
         <f>SUM(K54:K56, K34:K41, K8:K17,K22:K31,K44:K51)</f>
-        <v>34603.885125465131</v>
+        <v>37972.175460446633</v>
       </c>
       <c r="L58" s="12">
         <f>SUM(L54:L56, L34:L41, L8:L17,L22:L31,L44:L51)</f>
-        <v>148016.11487453489</v>
+        <v>200801.82453955337</v>
       </c>
       <c r="M58" s="12">
         <f>SUM(M54:M56, M34:M41, M8:M17,M22:M31,M44:M51)</f>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="D59" s="23">
         <f>SUM(K58:N58)</f>
-        <v>182620.00000000003</v>
+        <v>238774</v>
       </c>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
@@ -4452,15 +4452,15 @@
       </c>
       <c r="D61" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>617860</v>
+        <v>786322</v>
       </c>
       <c r="K61" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>114811.65537639537</v>
+        <v>124916.52638133988</v>
       </c>
       <c r="L61" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>503048.34462360456</v>
+        <v>661405.47361866012</v>
       </c>
       <c r="M61" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
@@ -4475,11 +4475,11 @@
       <c r="D62" s="1"/>
       <c r="K62" s="53">
         <f>IFERROR(K61/$D$61, 0)</f>
-        <v>0.18582147311105326</v>
+        <v>0.1588617975604649</v>
       </c>
       <c r="L62" s="53">
         <f>IFERROR(L61/$D$61, 0)</f>
-        <v>0.81417852688894665</v>
+        <v>0.84113820243953508</v>
       </c>
       <c r="M62" s="53">
         <f>IFERROR(M61/$D$61, 0)</f>
@@ -4539,19 +4539,19 @@
       </c>
       <c r="J66" s="21"/>
       <c r="K66" s="25">
-        <f t="shared" ref="K66:N68" si="48">F66*$D66</f>
+        <f t="shared" ref="K66:N68" si="51">F66*$D66</f>
         <v>0</v>
       </c>
       <c r="L66" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M66" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="N66" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
@@ -4583,19 +4583,19 @@
       </c>
       <c r="J67" s="21"/>
       <c r="K67" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="L67" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M67" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="N67" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
@@ -4606,16 +4606,16 @@
       </c>
       <c r="D68" s="23">
         <f>SUM(Calcs!D64:H64)+SUM(Calcs!D74:H74)</f>
-        <v>42000</v>
+        <v>122220</v>
       </c>
       <c r="E68" s="21"/>
       <c r="F68" s="24">
         <f>IFERROR(SUM(K36,K15:K17,K46,K29:K31)/SUM($K$36:$N$36,$K$15:$M$17,$K$46:$N$46,$K$29:$N$31),0)</f>
-        <v>0.1</v>
+        <v>6.8728522336769765E-2</v>
       </c>
       <c r="G68" s="24">
         <f>IFERROR(SUM(L36,L15:L17,L46,L29:L31)/SUM($K$36:$N$36,$K$15:$M$17,$K$46:$N$46,$K$29:$N$31),0)</f>
-        <v>0.9</v>
+        <v>0.93127147766323026</v>
       </c>
       <c r="H68" s="24">
         <f>IFERROR(SUM(M36,M15:M17,M46,M29:M31)/SUM($K$36:$N$36,$K$15:$M$17,$K$46:$N$46,$K$29:$N$31),0)</f>
@@ -4627,19 +4627,19 @@
       </c>
       <c r="J68" s="21"/>
       <c r="K68" s="25">
-        <f t="shared" si="48"/>
-        <v>4200</v>
+        <f t="shared" si="51"/>
+        <v>8400</v>
       </c>
       <c r="L68" s="25">
-        <f t="shared" si="48"/>
-        <v>37800</v>
+        <f t="shared" si="51"/>
+        <v>113820</v>
       </c>
       <c r="M68" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="N68" s="25">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
@@ -4654,36 +4654,36 @@
       </c>
       <c r="E69" s="21"/>
       <c r="F69" s="24">
-        <f>IFERROR(SUM(K38,K48)/SUM($K38:$N38,$K48:$N48),0)</f>
+        <f t="shared" ref="F69:I71" si="52">IFERROR(SUM(K38,K48)/SUM($K38:$N38,$K48:$N48),0)</f>
         <v>0</v>
       </c>
       <c r="G69" s="24">
-        <f>IFERROR(SUM(L38,L48)/SUM($K38:$N38,$K48:$N48),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="H69" s="24">
-        <f>IFERROR(SUM(M38,M48)/SUM($K38:$N38,$K48:$N48),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="I69" s="24">
-        <f>IFERROR(SUM(N38,N48)/SUM($K38:$N38,$K48:$N48),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J69" s="21"/>
       <c r="K69" s="25">
-        <f t="shared" ref="K69:K72" si="49">F69*$D69</f>
+        <f t="shared" ref="K69:K72" si="53">F69*$D69</f>
         <v>0</v>
       </c>
       <c r="L69" s="25">
-        <f t="shared" ref="L69:L72" si="50">G69*$D69</f>
+        <f t="shared" ref="L69:L72" si="54">G69*$D69</f>
         <v>0</v>
       </c>
       <c r="M69" s="25">
-        <f t="shared" ref="M69:M72" si="51">H69*$D69</f>
+        <f t="shared" ref="M69:M72" si="55">H69*$D69</f>
         <v>0</v>
       </c>
       <c r="N69" s="25">
-        <f t="shared" ref="N69:N72" si="52">I69*$D69</f>
+        <f t="shared" ref="N69:N72" si="56">I69*$D69</f>
         <v>0</v>
       </c>
     </row>
@@ -4698,36 +4698,36 @@
       </c>
       <c r="E70" s="21"/>
       <c r="F70" s="24">
-        <f>IFERROR(SUM(K39,K49)/SUM($K39:$N39,$K49:$N49),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="G70" s="24">
-        <f>IFERROR(SUM(L39,L49)/SUM($K39:$N39,$K49:$N49),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="H70" s="24">
-        <f>IFERROR(SUM(M39,M49)/SUM($K39:$N39,$K49:$N49),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="I70" s="24">
-        <f>IFERROR(SUM(N39,N49)/SUM($K39:$N39,$K49:$N49),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J70" s="21"/>
       <c r="K70" s="25">
-        <f t="shared" ref="K70:K71" si="53">F70*$D70</f>
+        <f t="shared" ref="K70:K71" si="57">F70*$D70</f>
         <v>0</v>
       </c>
       <c r="L70" s="25">
-        <f t="shared" ref="L70:L71" si="54">G70*$D70</f>
+        <f t="shared" ref="L70:L71" si="58">G70*$D70</f>
         <v>0</v>
       </c>
       <c r="M70" s="25">
-        <f t="shared" ref="M70:M71" si="55">H70*$D70</f>
+        <f t="shared" ref="M70:M71" si="59">H70*$D70</f>
         <v>0</v>
       </c>
       <c r="N70" s="25">
-        <f t="shared" ref="N70:N71" si="56">I70*$D70</f>
+        <f t="shared" ref="N70:N71" si="60">I70*$D70</f>
         <v>0</v>
       </c>
     </row>
@@ -4742,36 +4742,36 @@
       </c>
       <c r="E71" s="21"/>
       <c r="F71" s="24">
-        <f>IFERROR(SUM(K40,K50)/SUM($K40:$N40,$K50:$N50),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="G71" s="24">
-        <f>IFERROR(SUM(L40,L50)/SUM($K40:$N40,$K50:$N50),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="H71" s="24">
-        <f>IFERROR(SUM(M40,M50)/SUM($K40:$N40,$K50:$N50),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="I71" s="24">
-        <f>IFERROR(SUM(N40,N50)/SUM($K40:$N40,$K50:$N50),0)</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J71" s="21"/>
       <c r="K71" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="L71" s="25">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="M71" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="N71" s="25">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -4786,36 +4786,36 @@
       </c>
       <c r="E72" s="21"/>
       <c r="F72" s="24">
-        <f t="shared" ref="F72" si="57">IFERROR(SUM(K41,K51)/SUM($K41:$N41,$K51:$N51),0)</f>
+        <f t="shared" ref="F72" si="61">IFERROR(SUM(K41,K51)/SUM($K41:$N41,$K51:$N51),0)</f>
         <v>0</v>
       </c>
       <c r="G72" s="24">
-        <f t="shared" ref="G72" si="58">IFERROR(SUM(L41,L51)/SUM($K41:$N41,$K51:$N51),0)</f>
+        <f t="shared" ref="G72" si="62">IFERROR(SUM(L41,L51)/SUM($K41:$N41,$K51:$N51),0)</f>
         <v>0</v>
       </c>
       <c r="H72" s="24">
-        <f t="shared" ref="H72" si="59">IFERROR(SUM(M41,M51)/SUM($K41:$N41,$K51:$N51),0)</f>
+        <f t="shared" ref="H72" si="63">IFERROR(SUM(M41,M51)/SUM($K41:$N41,$K51:$N51),0)</f>
         <v>0</v>
       </c>
       <c r="I72" s="24">
-        <f t="shared" ref="I72" si="60">IFERROR(SUM(N41,N51)/SUM($K41:$N41,$K51:$N51),0)</f>
+        <f t="shared" ref="I72" si="64">IFERROR(SUM(N41,N51)/SUM($K41:$N41,$K51:$N51),0)</f>
         <v>0</v>
       </c>
       <c r="J72" s="21"/>
       <c r="K72" s="25">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L72" s="25">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="M72" s="25">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="N72" s="25">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
     </row>
@@ -4833,7 +4833,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5380,15 +5380,15 @@
       </c>
       <c r="M9" s="63">
         <f>$F9*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N9" s="63">
         <f>$F9*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O9" s="63">
         <f>$F9*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P9" s="63">
         <f>$F9*Outputs_Internal!M$58/12</f>
@@ -5454,15 +5454,15 @@
       </c>
       <c r="M10" s="63">
         <f>$F10*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N10" s="63">
         <f>$F10*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O10" s="63">
         <f>$F10*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P10" s="63">
         <f>$F10*Outputs_Internal!M$58/12</f>
@@ -5528,15 +5528,15 @@
       </c>
       <c r="M11" s="63">
         <f>$F11*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N11" s="63">
         <f>$F11*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O11" s="63">
         <f>$F11*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P11" s="63">
         <f>$F11*Outputs_Internal!M$58/12</f>
@@ -5548,15 +5548,15 @@
       </c>
       <c r="S11" s="63">
         <f t="shared" si="1"/>
-        <v>115654.99999999999</v>
+        <v>129693.49999999999</v>
       </c>
       <c r="T11" s="63">
         <f t="shared" si="2"/>
-        <v>19650.971281366285</v>
+        <v>20493.043865111656</v>
       </c>
       <c r="U11" s="63">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>96004.028718633708</v>
+        <v>109200.45613488834</v>
       </c>
       <c r="V11" s="63">
         <f t="shared" si="4"/>
@@ -5602,15 +5602,15 @@
       </c>
       <c r="M12" s="63">
         <f>$F12*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N12" s="63">
         <f>$F12*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O12" s="63">
         <f>$F12*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P12" s="63">
         <f>$F12*Outputs_Internal!M$58/12</f>
@@ -5676,15 +5676,15 @@
       </c>
       <c r="M13" s="63">
         <f>$F13*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N13" s="63">
         <f>$F13*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O13" s="63">
         <f>$F13*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P13" s="63">
         <f>$F13*Outputs_Internal!M$58/12</f>
@@ -5750,15 +5750,15 @@
       </c>
       <c r="M14" s="63">
         <f>$F14*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N14" s="63">
         <f>$F14*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O14" s="63">
         <f>$F14*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P14" s="63">
         <f>$F14*Outputs_Internal!M$58/12</f>
@@ -5770,15 +5770,15 @@
       </c>
       <c r="S14" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T14" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U14" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V14" s="63">
         <f t="shared" si="4"/>
@@ -5824,15 +5824,15 @@
       </c>
       <c r="M15" s="63">
         <f>$F15*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N15" s="63">
         <f>$F15*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O15" s="63">
         <f>$F15*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P15" s="63">
         <f>$F15*Outputs_Internal!M$58/12</f>
@@ -5898,15 +5898,15 @@
       </c>
       <c r="M16" s="63">
         <f>$F16*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N16" s="63">
         <f>$F16*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O16" s="63">
         <f>$F16*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P16" s="63">
         <f>$F16*Outputs_Internal!M$58/12</f>
@@ -5972,15 +5972,15 @@
       </c>
       <c r="M17" s="63">
         <f>$F17*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N17" s="63">
         <f>$F17*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O17" s="63">
         <f>$F17*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P17" s="63">
         <f>$F17*Outputs_Internal!M$58/12</f>
@@ -5992,15 +5992,15 @@
       </c>
       <c r="S17" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T17" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U17" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V17" s="63">
         <f t="shared" si="4"/>
@@ -6046,15 +6046,15 @@
       </c>
       <c r="M18" s="63">
         <f>$F18*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N18" s="63">
         <f>$F18*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O18" s="63">
         <f>$F18*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P18" s="63">
         <f>$F18*Outputs_Internal!M$58/12</f>
@@ -6120,15 +6120,15 @@
       </c>
       <c r="M19" s="63">
         <f>$F19*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N19" s="63">
         <f>$F19*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O19" s="63">
         <f>$F19*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P19" s="63">
         <f>$F19*Outputs_Internal!M$58/12</f>
@@ -6194,15 +6194,15 @@
       </c>
       <c r="M20" s="63">
         <f>$F20*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N20" s="63">
         <f>$F20*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O20" s="63">
         <f>$F20*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P20" s="63">
         <f>$F20*Outputs_Internal!M$58/12</f>
@@ -6214,15 +6214,15 @@
       </c>
       <c r="S20" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T20" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U20" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V20" s="63">
         <f t="shared" si="4"/>
@@ -6268,15 +6268,15 @@
       </c>
       <c r="M21" s="63">
         <f>$F21*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N21" s="63">
         <f>$F21*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O21" s="63">
         <f>$F21*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P21" s="63">
         <f>$F21*Outputs_Internal!M$58/12</f>
@@ -6342,15 +6342,15 @@
       </c>
       <c r="M22" s="63">
         <f>$F22*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N22" s="63">
         <f>$F22*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O22" s="63">
         <f>$F22*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P22" s="63">
         <f>$F22*Outputs_Internal!M$58/12</f>
@@ -6416,15 +6416,15 @@
       </c>
       <c r="M23" s="63">
         <f>$F23*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N23" s="63">
         <f>$F23*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O23" s="63">
         <f>$F23*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P23" s="63">
         <f>$F23*Outputs_Internal!M$58/12</f>
@@ -6436,15 +6436,15 @@
       </c>
       <c r="S23" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T23" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U23" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V23" s="63">
         <f t="shared" si="4"/>
@@ -6490,15 +6490,15 @@
       </c>
       <c r="M24" s="63">
         <f>$F24*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N24" s="63">
         <f>$F24*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O24" s="63">
         <f>$F24*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P24" s="63">
         <f>$F24*Outputs_Internal!M$58/12</f>
@@ -6564,15 +6564,15 @@
       </c>
       <c r="M25" s="63">
         <f>$F25*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N25" s="63">
         <f>$F25*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O25" s="63">
         <f>$F25*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P25" s="63">
         <f>$F25*Outputs_Internal!M$58/12</f>
@@ -6638,15 +6638,15 @@
       </c>
       <c r="M26" s="63">
         <f>$F26*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N26" s="63">
         <f>$F26*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O26" s="63">
         <f>$F26*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P26" s="63">
         <f>$F26*Outputs_Internal!M$58/12</f>
@@ -6658,15 +6658,15 @@
       </c>
       <c r="S26" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T26" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U26" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V26" s="63">
         <f t="shared" si="4"/>
@@ -6712,15 +6712,15 @@
       </c>
       <c r="M27" s="63">
         <f>$F27*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N27" s="63">
         <f>$F27*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O27" s="63">
         <f>$F27*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!M$58/12</f>
@@ -6786,15 +6786,15 @@
       </c>
       <c r="M28" s="63">
         <f>$F28*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N28" s="63">
         <f>$F28*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O28" s="63">
         <f>$F28*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!M$58/12</f>
@@ -6860,15 +6860,15 @@
       </c>
       <c r="M29" s="63">
         <f>$F29*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N29" s="63">
         <f>$F29*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O29" s="63">
         <f>$F29*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!M$58/12</f>
@@ -6880,15 +6880,15 @@
       </c>
       <c r="S29" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T29" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U29" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V29" s="63">
         <f t="shared" si="4"/>
@@ -6934,15 +6934,15 @@
       </c>
       <c r="M30" s="63">
         <f>$F30*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N30" s="63">
         <f>$F30*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O30" s="63">
         <f>$F30*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!M$58/12</f>
@@ -7008,15 +7008,15 @@
       </c>
       <c r="M31" s="63">
         <f>$F31*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N31" s="63">
         <f>$F31*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O31" s="63">
         <f>$F31*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!M$58/12</f>
@@ -7082,15 +7082,15 @@
       </c>
       <c r="M32" s="63">
         <f>$F32*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N32" s="63">
         <f>$F32*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O32" s="63">
         <f>$F32*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!M$58/12</f>
@@ -7102,15 +7102,15 @@
       </c>
       <c r="S32" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T32" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U32" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V32" s="63">
         <f t="shared" si="4"/>
@@ -7156,15 +7156,15 @@
       </c>
       <c r="M33" s="63">
         <f>$F33*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N33" s="63">
         <f>$F33*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O33" s="63">
         <f>$F33*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!M$58/12</f>
@@ -7230,15 +7230,15 @@
       </c>
       <c r="M34" s="63">
         <f>$F34*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N34" s="63">
         <f>$F34*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O34" s="63">
         <f>$F34*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!M$58/12</f>
@@ -7304,15 +7304,15 @@
       </c>
       <c r="M35" s="63">
         <f>$F35*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N35" s="63">
         <f>$F35*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O35" s="63">
         <f>$F35*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!M$58/12</f>
@@ -7324,15 +7324,15 @@
       </c>
       <c r="S35" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T35" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U35" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V35" s="63">
         <f t="shared" si="4"/>
@@ -7378,15 +7378,15 @@
       </c>
       <c r="M36" s="63">
         <f>$F36*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N36" s="63">
         <f>$F36*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O36" s="63">
         <f>$F36*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!M$58/12</f>
@@ -7452,15 +7452,15 @@
       </c>
       <c r="M37" s="63">
         <f>$F37*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N37" s="63">
         <f>$F37*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O37" s="63">
         <f>$F37*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!M$58/12</f>
@@ -7526,15 +7526,15 @@
       </c>
       <c r="M38" s="63">
         <f>$F38*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N38" s="63">
         <f>$F38*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O38" s="63">
         <f>$F38*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!M$58/12</f>
@@ -7546,15 +7546,15 @@
       </c>
       <c r="S38" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T38" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U38" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V38" s="63">
         <f t="shared" si="4"/>
@@ -7600,15 +7600,15 @@
       </c>
       <c r="M39" s="63">
         <f>$F39*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N39" s="63">
         <f>$F39*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O39" s="63">
         <f>$F39*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!M$58/12</f>
@@ -7674,15 +7674,15 @@
       </c>
       <c r="M40" s="63">
         <f>$F40*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N40" s="63">
         <f>$F40*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O40" s="63">
         <f>$F40*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!M$58/12</f>
@@ -7748,15 +7748,15 @@
       </c>
       <c r="M41" s="63">
         <f>$F41*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N41" s="63">
         <f>$F41*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O41" s="63">
         <f>$F41*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!M$58/12</f>
@@ -7768,15 +7768,15 @@
       </c>
       <c r="S41" s="63">
         <f t="shared" si="1"/>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T41" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U41" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V41" s="63">
         <f t="shared" si="4"/>
@@ -7822,15 +7822,15 @@
       </c>
       <c r="M42" s="63">
         <f>$F42*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N42" s="63">
         <f>$F42*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O42" s="63">
         <f>$F42*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!M$58/12</f>
@@ -7896,15 +7896,15 @@
       </c>
       <c r="M43" s="63">
         <f>$F43*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N43" s="63">
         <f>$F43*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O43" s="63">
         <f>$F43*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!M$58/12</f>
@@ -7970,15 +7970,15 @@
       </c>
       <c r="M44" s="63">
         <f>$F44*Outputs_Internal!$D$58/12</f>
-        <v>15218.333333333334</v>
+        <v>19897.833333333332</v>
       </c>
       <c r="N44" s="63">
         <f>$F44*Outputs_Internal!K$58/12</f>
-        <v>2883.6570937887609</v>
+        <v>3164.3479550372194</v>
       </c>
       <c r="O44" s="63">
         <f>$F44*Outputs_Internal!L$58/12</f>
-        <v>12334.676239544575</v>
+        <v>16733.485378296115</v>
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!M$58/12</f>
@@ -7990,15 +7990,15 @@
       </c>
       <c r="S44" s="63">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>45655</v>
+        <v>59693.5</v>
       </c>
       <c r="T44" s="63">
         <f t="shared" si="2"/>
-        <v>8650.9712813662827</v>
+        <v>9493.0438651116583</v>
       </c>
       <c r="U44" s="63">
         <f t="shared" si="3"/>
-        <v>37004.028718633723</v>
+        <v>50200.456134888344</v>
       </c>
       <c r="V44" s="63">
         <f t="shared" si="4"/>
@@ -11727,7 +11727,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12198,7 +12198,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$22="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$22="Y",Inputs!D$23="Y"), Prices!$C16, 0)</f>
         <v>12000</v>
       </c>
       <c r="E21" s="20">
@@ -12206,15 +12206,15 @@
         <v>12000</v>
       </c>
       <c r="F21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$22="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$22="Y",Inputs!F$23="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="G21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$22="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$22="Y",Inputs!G$23="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$22="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$22="Y",Inputs!H$23="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12223,23 +12223,23 @@
         <v>12</v>
       </c>
       <c r="D22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D18="Y",Inputs!D$22="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D18="Y",Inputs!D$22="Y",Inputs!D$23="Y"), Prices!$C17, 0)</f>
         <v>6000</v>
       </c>
       <c r="E22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E18="Y",Inputs!E$22="Y",Inputs!$E23="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E18="Y",Inputs!E$22="Y",Inputs!E$23="Y"), Prices!$C17, 0)</f>
         <v>6000</v>
       </c>
       <c r="F22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F18="Y",Inputs!F$22="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F18="Y",Inputs!F$22="Y",Inputs!F$23="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G18="Y",Inputs!G$22="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G18="Y",Inputs!G$22="Y",Inputs!G$23="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="H22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H18="Y",Inputs!H$22="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H18="Y",Inputs!H$22="Y",Inputs!H$23="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12248,23 +12248,23 @@
         <v>23</v>
       </c>
       <c r="D23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D19="Y",Inputs!D$22="Y"), Prices!$C18, 0)</f>
+        <f>IF(Inputs!D$5="N",0, IF(OR(Inputs!D19="Y",Inputs!D$22="Y",Inputs!D$23="Y"), Prices!$C18, 0))</f>
         <v>6000</v>
       </c>
       <c r="E23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E19="Y",Inputs!E$22="Y",Inputs!E23="Y"), Prices!$C18, 0)</f>
-        <v>6000</v>
+        <f>IF(Inputs!E$5="N",0, IF(OR(Inputs!E19="Y",Inputs!E$22="Y",Inputs!E$23="Y"), Prices!$C18, 0))</f>
+        <v>0</v>
       </c>
       <c r="F23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F19="Y",Inputs!F$22="Y"), Prices!$C18, 0)</f>
+        <f>IF(Inputs!F$5="N",0, IF(OR(Inputs!F19="Y",Inputs!F$22="Y",Inputs!F$23="Y"), Prices!$C18, 0))</f>
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G19="Y",Inputs!G$22="Y"), Prices!$C18, 0)</f>
+        <f>IF(Inputs!G$5="N",0, IF(OR(Inputs!G19="Y",Inputs!G$22="Y",Inputs!G$23="Y"), Prices!$C18, 0))</f>
         <v>0</v>
       </c>
       <c r="H23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H19="Y",Inputs!H$22="Y"), Prices!$C18, 0)</f>
+        <f>IF(Inputs!H$5="N",0, IF(OR(Inputs!H19="Y",Inputs!H$22="Y",Inputs!H$23="Y"), Prices!$C18, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12453,23 +12453,23 @@
         <v>11</v>
       </c>
       <c r="D33" s="20">
-        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D17="Y",Inputs!D$22="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D17="Y",Inputs!D$22="Y",Inputs!D$23="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E33" s="20">
-        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E17="Y",Inputs!E$22="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
-        <v>0</v>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E17="Y",Inputs!E$22="Y",Inputs!E$23="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
+        <v>22750</v>
       </c>
       <c r="F33" s="20">
-        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F17="Y",Inputs!F$22="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F17="Y",Inputs!F$22="Y",Inputs!F$23="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G33" s="20">
-        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G17="Y",Inputs!G$22="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G17="Y",Inputs!G$22="Y",Inputs!G$23="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H33" s="20">
-        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$22="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$22="Y",Inputs!H$23="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12478,23 +12478,23 @@
         <v>12</v>
       </c>
       <c r="D34" s="20">
-        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D18="Y",Inputs!D$22="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D18="Y",Inputs!D$22="Y",Inputs!D$23="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E34" s="20">
-        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E18="Y",Inputs!E$22="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
-        <v>0</v>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E18="Y",Inputs!E$22="Y",Inputs!E$23="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
+        <v>9100</v>
       </c>
       <c r="F34" s="20">
-        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F18="Y",Inputs!F$22="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F18="Y",Inputs!F$22="Y",Inputs!F$23="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G34" s="20">
-        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G18="Y",Inputs!G$22="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G18="Y",Inputs!G$22="Y",Inputs!G$23="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H34" s="20">
-        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H18="Y",Inputs!H$22="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H18="Y",Inputs!H$22="Y",Inputs!H$23="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12710,23 +12710,23 @@
         <v>11</v>
       </c>
       <c r="D45" s="20">
-        <f>IF(AND(Inputs!D17="Y",Inputs!D$22="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!D17="Y",Inputs!D$22="N",Inputs!D$23="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="E45" s="20">
-        <f>IF(AND(Inputs!E17="Y",Inputs!E$22="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!E17="Y",Inputs!E$22="N",Inputs!E$23="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="F45" s="20">
-        <f>IF(AND(Inputs!F17="Y",Inputs!F$22="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!F17="Y",Inputs!F$22="N",Inputs!F$23="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="G45" s="20">
-        <f>IF(AND(Inputs!G17="Y",Inputs!G$22="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!G17="Y",Inputs!G$22="N",Inputs!G$23="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="H45" s="20">
-        <f>IF(AND(Inputs!H17="Y",Inputs!H$22="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!H17="Y",Inputs!H$22="N",Inputs!H$23="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12735,23 +12735,23 @@
         <v>12</v>
       </c>
       <c r="D46" s="20">
-        <f>IF(AND(Inputs!D18="Y",Inputs!D$22="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!D18="Y",Inputs!D$22="N",Inputs!D$23="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="E46" s="20">
-        <f>IF(AND(Inputs!E18="Y",Inputs!E$22="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!E18="Y",Inputs!E$22="N",Inputs!E$23="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="F46" s="20">
-        <f>IF(AND(Inputs!F18="Y",Inputs!F$22="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!F18="Y",Inputs!F$22="N",Inputs!F$23="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="G46" s="20">
-        <f>IF(AND(Inputs!G18="Y",Inputs!G$22="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!G18="Y",Inputs!G$22="N",Inputs!G$23="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="H46" s="20">
-        <f>IF(AND(Inputs!H18="Y",Inputs!H$22="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!H18="Y",Inputs!H$22="N",Inputs!H$23="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12760,23 +12760,23 @@
         <v>23</v>
       </c>
       <c r="D47" s="20">
-        <f>IF(AND(Inputs!D19="Y",Inputs!D$22="N"),Prices!$C18,0)</f>
+        <f>IF(Inputs!D$5="N",0,IF(AND(Inputs!D19="Y",Inputs!D$22="N",Inputs!D$23="N"),Prices!$C18,0))</f>
         <v>0</v>
       </c>
       <c r="E47" s="20">
-        <f>IF(AND(Inputs!E19="Y",Inputs!E$22="N"),Prices!$C18,0)</f>
+        <f>IF(Inputs!E$5="N",0,IF(AND(Inputs!E19="Y",Inputs!E$22="N",Inputs!E$23="N"),Prices!$C18,0))</f>
         <v>0</v>
       </c>
       <c r="F47" s="20">
-        <f>IF(AND(Inputs!F19="Y",Inputs!F$22="N"),Prices!$C18,0)</f>
+        <f>IF(Inputs!F$5="N",0,IF(AND(Inputs!F19="Y",Inputs!F$22="N",Inputs!F$23="N"),Prices!$C18,0))</f>
         <v>0</v>
       </c>
       <c r="G47" s="20">
-        <f>IF(AND(Inputs!G19="Y",Inputs!G$22="N"),Prices!$C18,0)</f>
+        <f>IF(Inputs!G$5="N",0,IF(AND(Inputs!G19="Y",Inputs!G$22="N",Inputs!G$23="N"),Prices!$C18,0))</f>
         <v>0</v>
       </c>
       <c r="H47" s="20">
-        <f>IF(AND(Inputs!H19="Y",Inputs!H$22="N"),Prices!$C18,0)</f>
+        <f>IF(Inputs!H$5="N",0,IF(AND(Inputs!H19="Y",Inputs!H$22="N",Inputs!H$23="N"),Prices!$C18,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12965,23 +12965,23 @@
         <v>11</v>
       </c>
       <c r="D57" s="20">
-        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D17="Y",Inputs!D$22="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D17="Y",Inputs!D$22="N",Inputs!D$23="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E57" s="20">
-        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E17="Y",Inputs!E$22="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E17="Y",Inputs!E$22="N",Inputs!E$23="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F57" s="20">
-        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F17="Y",Inputs!F$22="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F17="Y",Inputs!F$22="N",Inputs!F$23="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G57" s="20">
-        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G17="Y",Inputs!G$22="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G17="Y",Inputs!G$22="N",Inputs!G$23="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H57" s="20">
-        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$22="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$22="N",Inputs!H$23="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12990,23 +12990,23 @@
         <v>12</v>
       </c>
       <c r="D58" s="20">
-        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D18="Y",Inputs!D$22="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D18="Y",Inputs!D$22="N",Inputs!D$23="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E58" s="20">
-        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E18="Y",Inputs!E$22="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E18="Y",Inputs!E$22="N",Inputs!E$23="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F58" s="20">
-        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F18="Y",Inputs!F$22="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F18="Y",Inputs!F$22="N",Inputs!F$23="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G58" s="20">
-        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G18="Y",Inputs!G$22="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G18="Y",Inputs!G$22="N",Inputs!G$23="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H58" s="20">
-        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H18="Y",Inputs!H$22="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H18="Y",Inputs!H$22="N",Inputs!H$23="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -13095,7 +13095,7 @@
       </c>
       <c r="E64" s="20">
         <f>IF(Inputs!E22="Y", Prices!$C22, 0)</f>
-        <v>0</v>
+        <v>42000</v>
       </c>
       <c r="F64" s="20">
         <f>IF(Inputs!F22="Y", Prices!$C22, 0)</f>
@@ -13345,7 +13345,7 @@
       </c>
       <c r="E74" s="20">
         <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E22, 0)))*E$10</f>
-        <v>0</v>
+        <v>38220</v>
       </c>
       <c r="F74" s="20">
         <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E22, 0)))*F$10</f>
@@ -13369,7 +13369,7 @@
       </c>
       <c r="L74" s="23">
         <f t="shared" si="5"/>
-        <v>1.2000000000000001E-3</v>
+        <v>80220.001199999999</v>
       </c>
       <c r="M74" s="23">
         <f t="shared" si="5"/>
@@ -13741,7 +13741,7 @@
       </c>
       <c r="E84" s="20">
         <f>IF(E64=0,0,E64-SUM(E21:E23))</f>
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="F84" s="20">
         <f>IF(F64=0,0,F64-SUM(F21:F23))</f>
@@ -13761,7 +13761,7 @@
       </c>
       <c r="L84" s="21">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M84" s="21">
         <f t="shared" si="14"/>
@@ -13781,23 +13781,23 @@
         <v>130</v>
       </c>
       <c r="D85" s="20">
-        <f>IF(D65=0,0,D65-IF(Inputs!E22="Y", 0,SUM(D21:D23)))</f>
+        <f>IF(D65=0,0,D65-IF(Inputs!D22="Y", 0, SUM(D21:D23)))</f>
         <v>0</v>
       </c>
       <c r="E85" s="20">
         <f>IF(E65=0,0,E65-IF(Inputs!E22="Y", 0, SUM(E21:E23)))</f>
-        <v>18000</v>
+        <v>42000</v>
       </c>
       <c r="F85" s="20">
-        <f>IF(F65=0,0,F65-IF(Inputs!E22="Y", 0,SUM(F21:F23)))</f>
+        <f>IF(F65=0,0,F65-IF(Inputs!F22="Y", 0, SUM(F21:F23)))</f>
         <v>0</v>
       </c>
       <c r="G85" s="20">
-        <f>IF(G65=0,0,G65-IF(Inputs!E22="Y", 0,SUM(G21:G23)))</f>
+        <f>IF(G65=0,0,G65-IF(Inputs!G22="Y", 0, SUM(G21:G23)))</f>
         <v>0</v>
       </c>
       <c r="H85" s="20">
-        <f>IF(H65=0,0,H65-IF(Inputs!E22="Y", 0,SUM(H21:H23)))</f>
+        <f>IF(H65=0,0,H65-IF(Inputs!H22="Y", 0, SUM(H21:H23)))</f>
         <v>0</v>
       </c>
       <c r="K85" s="21">
@@ -13851,7 +13851,7 @@
       </c>
       <c r="L86" s="21">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M86" s="21">
         <f t="shared" si="16"/>
@@ -13896,7 +13896,7 @@
       </c>
       <c r="L87" s="21">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M87" s="21">
         <f t="shared" si="18"/>
@@ -13941,7 +13941,7 @@
       </c>
       <c r="L88" s="21">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M88" s="21">
         <f t="shared" si="20"/>
@@ -13986,7 +13986,7 @@
       </c>
       <c r="L89" s="21">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M89" s="21">
         <f t="shared" si="22"/>
@@ -14061,7 +14061,7 @@
       </c>
       <c r="E94" s="20">
         <f>IF(E74=0,0,E74-SUM(E33:E34))</f>
-        <v>0</v>
+        <v>6370</v>
       </c>
       <c r="F94" s="20">
         <f>IF(F74=0,0,F74-SUM(F33:F34))</f>
@@ -14081,7 +14081,7 @@
         <v>130</v>
       </c>
       <c r="D95" s="20">
-        <f>IF(D75=0,0,D75-IF(Inputs!E22="Y", 0,SUM(D33:D34)))</f>
+        <f>IF(D75=0,0,D75-IF(Inputs!D22="Y", 0,SUM(D33:D34)))</f>
         <v>0</v>
       </c>
       <c r="E95" s="20">
@@ -14089,15 +14089,15 @@
         <v>38220</v>
       </c>
       <c r="F95" s="20">
-        <f>IF(F75=0,0,F75-IF(Inputs!E22="Y", 0,SUM(F33:F34)))</f>
+        <f>IF(F75=0,0,F75-IF(Inputs!F22="Y", 0,SUM(F33:F34)))</f>
         <v>0</v>
       </c>
       <c r="G95" s="20">
-        <f>IF(G75=0,0,G75-IF(Inputs!E22="Y", 0,SUM(G33:G34)))</f>
+        <f>IF(G75=0,0,G75-IF(Inputs!G22="Y", 0,SUM(G33:G34)))</f>
         <v>0</v>
       </c>
       <c r="H95" s="20">
-        <f>IF(H75=0,0,H75-IF(Inputs!E22="Y", 0,SUM(H33:H34)))</f>
+        <f>IF(H75=0,0,H75-IF(Inputs!H22="Y", 0,SUM(H33:H34)))</f>
         <v>0</v>
       </c>
     </row>
@@ -14219,7 +14219,7 @@
       </c>
       <c r="E102" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$62:E$69, MATCH($A102, L$82:L$89, 0)), INDEX(E$72:E$79, MATCH($A102, L$82:L$89, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>0</v>
+        <v>-24066</v>
       </c>
       <c r="F102" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(F$62:F$69, MATCH($A102, M$82:M$89, 0)), INDEX(F$72:F$79, MATCH($A102, M$82:M$89, 0)))*Prices!$L$5*-1, 0)</f>
@@ -14384,7 +14384,7 @@
       </c>
       <c r="E109" s="7">
         <f t="shared" ref="E109:H109" si="26">SUM(E38:E47, E50:E59, E62:E69, E72:E79, E102:E106)</f>
-        <v>149620</v>
+        <v>205774</v>
       </c>
       <c r="F109" s="7">
         <f t="shared" si="26"/>
@@ -14465,7 +14465,7 @@
       </c>
       <c r="E115" s="7">
         <f>SUM(E109, E111)</f>
-        <v>149620</v>
+        <v>205774</v>
       </c>
       <c r="F115" s="7">
         <f>SUM(F109, F111)</f>

</xml_diff>

<commit_message>
Fix total formula on Calcs.
Do this so it includes the existing collaborative discount.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="5"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -14460,23 +14460,23 @@
         <v>114</v>
       </c>
       <c r="D115" s="7">
-        <f>SUM(D109, D111)</f>
+        <f>SUM(D109, D111,D113)</f>
         <v>33000</v>
       </c>
       <c r="E115" s="7">
-        <f>SUM(E109, E111)</f>
+        <f t="shared" ref="E115:H115" si="28">SUM(E109, E111,E113)</f>
         <v>205774</v>
       </c>
       <c r="F115" s="7">
-        <f>SUM(F109, F111)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G115" s="7">
-        <f>SUM(G109, G111)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H115" s="7">
-        <f>SUM(H109, H111)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -14490,19 +14490,19 @@
         <v>2</v>
       </c>
       <c r="E118" s="21">
-        <f t="shared" ref="E118:H118" si="28">IFERROR(_xlfn.RANK.EQ(E109,$D$109:$H$109),5)</f>
+        <f t="shared" ref="E118:H118" si="29">IFERROR(_xlfn.RANK.EQ(E109,$D$109:$H$109),5)</f>
         <v>1</v>
       </c>
       <c r="F118" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="G118" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="H118" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
     </row>
@@ -14531,19 +14531,19 @@
         <v>2.1</v>
       </c>
       <c r="E120" s="21">
-        <f t="shared" ref="E120:H120" si="29">SUM(E118:E119)</f>
+        <f t="shared" ref="E120:H120" si="30">SUM(E118:E119)</f>
         <v>1.2</v>
       </c>
       <c r="F120" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3.3</v>
       </c>
       <c r="G120" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3.4</v>
       </c>
       <c r="H120" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3.5</v>
       </c>
     </row>
@@ -14554,19 +14554,19 @@
         <v>2</v>
       </c>
       <c r="E121" s="21">
-        <f t="shared" ref="E121:H121" si="30">_xlfn.RANK.EQ(E120, $D$120:$H$120, 5)</f>
+        <f t="shared" ref="E121:H121" si="31">_xlfn.RANK.EQ(E120, $D$120:$H$120, 5)</f>
         <v>1</v>
       </c>
       <c r="F121" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="G121" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="H121" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -14632,9 +14632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Make monthly overrides work on global monthly.
Do this because it was double applying before.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="135">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -470,6 +470,9 @@
   <si>
     <t>Base processing fee shift:</t>
   </si>
+  <si>
+    <t>Monthly Override Multiplier</t>
+  </si>
 </sst>
 </file>
 
@@ -486,8 +489,8 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -743,7 +746,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -912,8 +915,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1214,7 +1218,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2651,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3335,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="18">
-        <f t="shared" ref="L24:L33" si="9">G25*$D25</f>
+        <f t="shared" ref="L25:L33" si="9">G25*$D25</f>
         <v>0</v>
       </c>
       <c r="M25" s="18">
@@ -4901,7 +4905,7 @@
   <dimension ref="B1:W94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
@@ -11795,10 +11799,10 @@
   <dimension ref="A2:O131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J68" sqref="J68"/>
+      <selection pane="bottomRight" activeCell="D79" sqref="D79:H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12040,7 +12044,7 @@
         <v>0.40444444444444444</v>
       </c>
       <c r="F10" s="79">
-        <f t="shared" ref="E10:H10" si="0">IFERROR(SUMPRODUCT(F6:F9,$M$6:$M$9)/SUM(F6:F9),0)</f>
+        <f t="shared" ref="F10:H10" si="0">IFERROR(SUMPRODUCT(F6:F9,$M$6:$M$9)/SUM(F6:F9),0)</f>
         <v>0</v>
       </c>
       <c r="G10" s="79">
@@ -13236,23 +13240,23 @@
         <v>100</v>
       </c>
       <c r="D67" s="20">
-        <f>IF(Inputs!D26="Y", Prices!$C25 * IF(Inputs!D25="Y",1-Prices!$L$20,1), IF(Inputs!D26="Monthly", Prices!$C25 * Prices!$L$24 * IF(Inputs!D25="Y",1-Prices!$L$20,1), 0))</f>
+        <f>IF(Inputs!D26="Y", Prices!$C25 * IF(Inputs!D25="Y",1-Prices!$L$20,1), IF(Inputs!D26="Monthly", Prices!$C25 * Prices!$L$28 * IF(Inputs!D25="Y",1-Prices!$L$20,1), 0))</f>
         <v>0</v>
       </c>
       <c r="E67" s="20">
-        <f>IF(Inputs!E26="Y", Prices!$C25 * IF(Inputs!E25="Y",1-Prices!$L$20,1), IF(Inputs!E26="Monthly", Prices!$C25 * Prices!$L$24 * IF(Inputs!E25="Y",1-Prices!$L$20,1), 0))</f>
+        <f>IF(Inputs!E26="Y", Prices!$C25 * IF(Inputs!E25="Y",1-Prices!$L$20,1), IF(Inputs!E26="Monthly", Prices!$C25 * Prices!$L$28 * IF(Inputs!E25="Y",1-Prices!$L$20,1), 0))</f>
         <v>0</v>
       </c>
       <c r="F67" s="20">
-        <f>IF(Inputs!F26="Y", Prices!$C25 * IF(Inputs!F25="Y",1-Prices!$L$20,1), IF(Inputs!F26="Monthly", Prices!$C25 * Prices!$L$24 * IF(Inputs!F25="Y",1-Prices!$L$20,1), 0))</f>
+        <f>IF(Inputs!F26="Y", Prices!$C25 * IF(Inputs!F25="Y",1-Prices!$L$20,1), IF(Inputs!F26="Monthly", Prices!$C25 * Prices!$L$28 * IF(Inputs!F25="Y",1-Prices!$L$20,1), 0))</f>
         <v>0</v>
       </c>
       <c r="G67" s="20">
-        <f>IF(Inputs!G26="Y", Prices!$C25 * IF(Inputs!G25="Y",1-Prices!$L$20,1), IF(Inputs!G26="Monthly", Prices!$C25 * Prices!$L$24 * IF(Inputs!G25="Y",1-Prices!$L$20,1), 0))</f>
+        <f>IF(Inputs!G26="Y", Prices!$C25 * IF(Inputs!G25="Y",1-Prices!$L$20,1), IF(Inputs!G26="Monthly", Prices!$C25 * Prices!$L$28 * IF(Inputs!G25="Y",1-Prices!$L$20,1), 0))</f>
         <v>0</v>
       </c>
       <c r="H67" s="20">
-        <f>IF(Inputs!H26="Y", Prices!$C25 * IF(Inputs!H25="Y",1-Prices!$L$20,1), IF(Inputs!H26="Monthly", Prices!$C25 * Prices!$L$24 * IF(Inputs!H25="Y",1-Prices!$L$20,1), 0))</f>
+        <f>IF(Inputs!H26="Y", Prices!$C25 * IF(Inputs!H25="Y",1-Prices!$L$20,1), IF(Inputs!H26="Monthly", Prices!$C25 * Prices!$L$28 * IF(Inputs!H25="Y",1-Prices!$L$20,1), 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -13286,23 +13290,23 @@
         <v>97</v>
       </c>
       <c r="D69" s="84">
-        <f>IF(Inputs!D11="Y", Prices!$C27, IF(Inputs!D11="Monthly", Prices!C27 * Prices!$L$24, 0))</f>
+        <f>IF(Inputs!D11="Y", Prices!$C27, IF(Inputs!D11="Monthly", Prices!C27 * Prices!$L$28, 0))</f>
         <v>0</v>
       </c>
       <c r="E69" s="84">
-        <f>IF(Inputs!E11="Y", Prices!$C27, IF(Inputs!E11="Monthly", Prices!D27 * Prices!$L$24, 0))</f>
+        <f>IF(Inputs!E11="Y", Prices!$C27, IF(Inputs!E11="Monthly", Prices!D27 * Prices!$L$28, 0))</f>
         <v>0</v>
       </c>
       <c r="F69" s="84">
-        <f>IF(Inputs!F11="Y", Prices!$C27, IF(Inputs!F11="Monthly", Prices!E27 * Prices!$L$24, 0))</f>
+        <f>IF(Inputs!F11="Y", Prices!$C27, IF(Inputs!F11="Monthly", Prices!E27 * Prices!$L$28, 0))</f>
         <v>0</v>
       </c>
       <c r="G69" s="84">
-        <f>IF(Inputs!G11="Y", Prices!$C27, IF(Inputs!G11="Monthly", Prices!F27 * Prices!$L$24, 0))</f>
+        <f>IF(Inputs!G11="Y", Prices!$C27, IF(Inputs!G11="Monthly", Prices!F27 * Prices!$L$28, 0))</f>
         <v>0</v>
       </c>
       <c r="H69" s="84">
-        <f>IF(Inputs!H11="Y", Prices!$C27, IF(Inputs!H11="Monthly", Prices!G27 * Prices!$L$24, 0))</f>
+        <f>IF(Inputs!H11="Y", Prices!$C27, IF(Inputs!H11="Monthly", Prices!G27 * Prices!$L$28, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -13558,23 +13562,23 @@
         <v>100</v>
       </c>
       <c r="D77" s="20">
-        <f>IF(Inputs!D$6="Y", 0, IF(D$11 = "", 0, IF(Inputs!D26 = "Y", D$11*Prices!$E25 * IF(Inputs!D25="Y",1-Prices!$L$20,1),IF(Inputs!D26="Monthly", D$11*Prices!$E25 * Prices!$L$24 * IF(Inputs!D25="Y",1-Prices!$L$20,1), 0))))*D$10</f>
+        <f>IF(Inputs!D$6="Y", 0, IF(D$11 = "", 0, IF(Inputs!D26 = "Y", D$11*Prices!$E25 * IF(Inputs!D25="Y",1-Prices!$L$20,1),IF(Inputs!D26="Monthly", D$11*Prices!$E25 * Prices!$L$28 * IF(Inputs!D25="Y",1-Prices!$L$20,1), 0))))*D$10</f>
         <v>0</v>
       </c>
       <c r="E77" s="20">
-        <f>IF(Inputs!E$6="Y", 0, IF(E$11 = "", 0, IF(Inputs!E26 = "Y", E$11*Prices!$E25 * IF(Inputs!E25="Y",1-Prices!$L$20,1),IF(Inputs!E26="Monthly", E$11*Prices!$E25 * Prices!$L$24 * IF(Inputs!E25="Y",1-Prices!$L$20,1), 0))))*E$10</f>
+        <f>IF(Inputs!E$6="Y", 0, IF(E$11 = "", 0, IF(Inputs!E26 = "Y", E$11*Prices!$E25 * IF(Inputs!E25="Y",1-Prices!$L$20,1),IF(Inputs!E26="Monthly", E$11*Prices!$E25 * Prices!$L$28 * IF(Inputs!E25="Y",1-Prices!$L$20,1), 0))))*E$10</f>
         <v>0</v>
       </c>
       <c r="F77" s="20">
-        <f>IF(Inputs!F$6="Y", 0, IF(F$11 = "", 0, IF(Inputs!F26 = "Y", F$11*Prices!$E25 * IF(Inputs!F25="Y",1-Prices!$L$20,1),IF(Inputs!F26="Monthly", F$11*Prices!$E25 * Prices!$L$24 * IF(Inputs!F25="Y",1-Prices!$L$20,1), 0))))*F$10</f>
+        <f>IF(Inputs!F$6="Y", 0, IF(F$11 = "", 0, IF(Inputs!F26 = "Y", F$11*Prices!$E25 * IF(Inputs!F25="Y",1-Prices!$L$20,1),IF(Inputs!F26="Monthly", F$11*Prices!$E25 * Prices!$L$28 * IF(Inputs!F25="Y",1-Prices!$L$20,1), 0))))*F$10</f>
         <v>0</v>
       </c>
       <c r="G77" s="20">
-        <f>IF(Inputs!G$6="Y", 0, IF(G$11 = "", 0, IF(Inputs!G26 = "Y", G$11*Prices!$E25 * IF(Inputs!G25="Y",1-Prices!$L$20,1),IF(Inputs!G26="Monthly", G$11*Prices!$E25 * Prices!$L$24 * IF(Inputs!G25="Y",1-Prices!$L$20,1), 0))))*G$10</f>
+        <f>IF(Inputs!G$6="Y", 0, IF(G$11 = "", 0, IF(Inputs!G26 = "Y", G$11*Prices!$E25 * IF(Inputs!G25="Y",1-Prices!$L$20,1),IF(Inputs!G26="Monthly", G$11*Prices!$E25 * Prices!$L$28 * IF(Inputs!G25="Y",1-Prices!$L$20,1), 0))))*G$10</f>
         <v>0</v>
       </c>
       <c r="H77" s="20">
-        <f>IF(Inputs!H$6="Y", 0, IF(H$11 = "", 0, IF(Inputs!H26 = "Y", H$11*Prices!$E25 * IF(Inputs!H25="Y",1-Prices!$L$20,1),IF(Inputs!H26="Monthly", H$11*Prices!$E25 * Prices!$L$24 * IF(Inputs!H25="Y",1-Prices!$L$20,1), 0))))*H$10</f>
+        <f>IF(Inputs!H$6="Y", 0, IF(H$11 = "", 0, IF(Inputs!H26 = "Y", H$11*Prices!$E25 * IF(Inputs!H25="Y",1-Prices!$L$20,1),IF(Inputs!H26="Monthly", H$11*Prices!$E25 * Prices!$L$28 * IF(Inputs!H25="Y",1-Prices!$L$20,1), 0))))*H$10</f>
         <v>0</v>
       </c>
       <c r="J77" s="90">
@@ -13656,23 +13660,23 @@
         <v>97</v>
       </c>
       <c r="D79" s="84">
-        <f>IF(Inputs!D$6="Y", 0, IF(D$11 = "", 0, IF(Inputs!D11 = "Y", D$11*Prices!$E27, IF(Inputs!D11="Monthly", D$11*Prices!$E27*Prices!$L$24,0))))*D$10</f>
+        <f>IF(Inputs!D$6="Y", 0, IF(D$11 = "", 0, IF(Inputs!D11 = "Y", D$11*Prices!$E27, IF(Inputs!D11="Monthly", D$11*Prices!$E27*Prices!$L$28,0))))*D$10</f>
         <v>0</v>
       </c>
       <c r="E79" s="84">
-        <f>IF(Inputs!E$6="Y", 0, IF(E$11 = "", 0, IF(Inputs!E11 = "Y", E$11*Prices!$E27, IF(Inputs!E11="Monthly", E$11*Prices!$E27*Prices!$L$24,0))))*E$10</f>
+        <f>IF(Inputs!E$6="Y", 0, IF(E$11 = "", 0, IF(Inputs!E11 = "Y", E$11*Prices!$E27, IF(Inputs!E11="Monthly", E$11*Prices!$E27*Prices!$L$28,0))))*E$10</f>
         <v>0</v>
       </c>
       <c r="F79" s="84">
-        <f>IF(Inputs!F$6="Y", 0, IF(F$11 = "", 0, IF(Inputs!F11 = "Y", F$11*Prices!$E27, IF(Inputs!F11="Monthly", F$11*Prices!$E27*Prices!$L$24,0))))*F$10</f>
+        <f>IF(Inputs!F$6="Y", 0, IF(F$11 = "", 0, IF(Inputs!F11 = "Y", F$11*Prices!$E27, IF(Inputs!F11="Monthly", F$11*Prices!$E27*Prices!$L$28,0))))*F$10</f>
         <v>0</v>
       </c>
       <c r="G79" s="84">
-        <f>IF(Inputs!G$6="Y", 0, IF(G$11 = "", 0, IF(Inputs!G11 = "Y", G$11*Prices!$E27, IF(Inputs!G11="Monthly", G$11*Prices!$E27*Prices!$L$24,0))))*G$10</f>
+        <f>IF(Inputs!G$6="Y", 0, IF(G$11 = "", 0, IF(Inputs!G11 = "Y", G$11*Prices!$E27, IF(Inputs!G11="Monthly", G$11*Prices!$E27*Prices!$L$28,0))))*G$10</f>
         <v>0</v>
       </c>
       <c r="H79" s="84">
-        <f>IF(Inputs!H$6="Y", 0, IF(H$11 = "", 0, IF(Inputs!H11 = "Y", H$11*Prices!$E27, IF(Inputs!H11="Monthly", H$11*Prices!$E27*Prices!$L$24,0))))*H$10</f>
+        <f>IF(Inputs!H$6="Y", 0, IF(H$11 = "", 0, IF(Inputs!H11 = "Y", H$11*Prices!$E27, IF(Inputs!H11="Monthly", H$11*Prices!$E27*Prices!$L$28,0))))*H$10</f>
         <v>0</v>
       </c>
       <c r="J79" s="90">
@@ -13946,7 +13950,7 @@
         <v>0</v>
       </c>
       <c r="E87" s="20">
-        <f t="shared" ref="D87:H87" si="17">E67</f>
+        <f t="shared" ref="E87:H87" si="17">E67</f>
         <v>0</v>
       </c>
       <c r="F87" s="20">
@@ -14701,11 +14705,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L27"/>
+  <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15335,6 +15337,15 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L28" s="102">
+        <f>IF(Inputs!$C$3="Quarterly",$L$24,1)</f>
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add initial MARA info
Do this for something to work off of
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Outputs_Timeline" sheetId="8" r:id="rId4"/>
     <sheet name="Calcs" sheetId="1" r:id="rId5"/>
     <sheet name="Prices" sheetId="3" r:id="rId6"/>
+    <sheet name="MARA Prices" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="ACOInsight1">Inputs!$D$21:$D$22</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="140">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -473,12 +474,27 @@
   <si>
     <t>Monthly Override Multiplier</t>
   </si>
+  <si>
+    <t>Lower Bound</t>
+  </si>
+  <si>
+    <t>Upper Bound</t>
+  </si>
+  <si>
+    <t>PMPY</t>
+  </si>
+  <si>
+    <t>First Increase</t>
+  </si>
+  <si>
+    <t>Our Pricing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -491,6 +507,7 @@
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0.00000_);[Red]\(&quot;$&quot;#,##0.00000\)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -746,7 +763,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -918,6 +935,7 @@
     <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1214,24 +1232,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
     <col min="3" max="3" width="18" style="66" customWidth="1"/>
-    <col min="4" max="8" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="8" width="18.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" s="91" t="s">
         <v>59</v>
       </c>
@@ -1239,7 +1257,7 @@
         <v>43101</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="67" t="s">
         <v>73</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="67" t="s">
         <v>123</v>
       </c>
@@ -1255,7 +1273,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="67" t="s">
         <v>132</v>
       </c>
@@ -1263,7 +1281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="68"/>
       <c r="C5" s="72"/>
       <c r="D5" s="13" t="s">
@@ -1282,7 +1300,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="69" t="s">
         <v>5</v>
       </c>
@@ -1299,7 +1317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="69" t="s">
         <v>81</v>
       </c>
@@ -1316,7 +1334,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="69" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1348,7 @@
       <c r="G8" s="55"/>
       <c r="H8" s="56"/>
     </row>
-    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="69" t="s">
         <v>4</v>
       </c>
@@ -1347,7 +1365,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="69" t="s">
         <v>111</v>
       </c>
@@ -1364,7 +1382,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="69" t="s">
         <v>98</v>
       </c>
@@ -1378,7 +1396,7 @@
       <c r="G11" s="55"/>
       <c r="H11" s="56"/>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="69" t="s">
         <v>7</v>
       </c>
@@ -1395,7 +1413,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="69" t="s">
         <v>8</v>
       </c>
@@ -1412,7 +1430,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="69" t="s">
         <v>22</v>
       </c>
@@ -1426,7 +1444,7 @@
       <c r="G14" s="55"/>
       <c r="H14" s="56"/>
     </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="69" t="s">
         <v>9</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="69" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="69" t="s">
         <v>78</v>
       </c>
@@ -1477,7 +1495,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="69" t="s">
         <v>11</v>
       </c>
@@ -1491,7 +1509,7 @@
       <c r="G18" s="55"/>
       <c r="H18" s="56"/>
     </row>
-    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="69" t="s">
         <v>12</v>
       </c>
@@ -1505,7 +1523,7 @@
       <c r="G19" s="55"/>
       <c r="H19" s="56"/>
     </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="69" t="s">
         <v>13</v>
       </c>
@@ -1519,7 +1537,7 @@
       <c r="G20" s="55"/>
       <c r="H20" s="56"/>
     </row>
-    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="69" t="s">
         <v>14</v>
       </c>
@@ -1533,7 +1551,7 @@
       <c r="G21" s="55"/>
       <c r="H21" s="56"/>
     </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="69" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1565,7 @@
       <c r="G22" s="55"/>
       <c r="H22" s="56"/>
     </row>
-    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="69" t="s">
         <v>16</v>
       </c>
@@ -1561,7 +1579,7 @@
       <c r="G23" s="55"/>
       <c r="H23" s="56"/>
     </row>
-    <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="69" t="s">
         <v>130</v>
       </c>
@@ -1575,7 +1593,7 @@
       <c r="G24" s="55"/>
       <c r="H24" s="56"/>
     </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="69" t="s">
         <v>17</v>
       </c>
@@ -1589,7 +1607,7 @@
       <c r="G25" s="55"/>
       <c r="H25" s="56"/>
     </row>
-    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="69" t="s">
         <v>100</v>
       </c>
@@ -1603,7 +1621,7 @@
       <c r="G26" s="55"/>
       <c r="H26" s="56"/>
     </row>
-    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="92" t="s">
         <v>99</v>
       </c>
@@ -1652,20 +1670,20 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.26953125" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>106</v>
       </c>
@@ -1682,12 +1700,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1723,7 +1741,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1733,12 +1751,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -1774,7 +1792,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C8" s="17" t="s">
         <v>21</v>
       </c>
@@ -1810,7 +1828,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
@@ -1846,7 +1864,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
         <v>22</v>
       </c>
@@ -1881,7 +1899,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>9</v>
       </c>
@@ -1916,7 +1934,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
@@ -1951,7 +1969,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>78</v>
       </c>
@@ -1986,7 +2004,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C14" s="19" t="s">
         <v>11</v>
       </c>
@@ -2021,7 +2039,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
         <v>12</v>
       </c>
@@ -2056,7 +2074,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C16" s="19" t="s">
         <v>23</v>
       </c>
@@ -2091,12 +2109,12 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>14</v>
       </c>
@@ -2131,7 +2149,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>15</v>
       </c>
@@ -2166,7 +2184,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>16</v>
       </c>
@@ -2201,7 +2219,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>130</v>
       </c>
@@ -2236,7 +2254,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>17</v>
       </c>
@@ -2271,7 +2289,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>100</v>
       </c>
@@ -2306,7 +2324,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>99</v>
       </c>
@@ -2341,7 +2359,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>98</v>
       </c>
@@ -2376,12 +2394,12 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>39</v>
       </c>
@@ -2416,7 +2434,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>116</v>
       </c>
@@ -2451,7 +2469,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>83</v>
       </c>
@@ -2482,7 +2500,7 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
         <v>40</v>
       </c>
@@ -2514,7 +2532,7 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2528,7 +2546,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
         <v>75</v>
       </c>
@@ -2548,13 +2566,13 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C36" s="64">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
         <v>74</v>
       </c>
@@ -2586,7 +2604,7 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2601,18 +2619,18 @@
       <c r="T40" s="8"/>
       <c r="U40" s="8"/>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B41" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C42" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
         <v>629299</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C43" s="52">
         <f>SUM(D38:H38)</f>
         <v>629299</v>
@@ -2620,17 +2638,17 @@
       <c r="D43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2654,25 +2672,25 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.81640625" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
       <c r="F1" s="50" t="s">
         <v>58</v>
       </c>
@@ -2680,7 +2698,7 @@
       <c r="H1" s="50"/>
       <c r="I1" s="50"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D2" s="9" t="s">
         <v>44</v>
       </c>
@@ -2710,12 +2728,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>76</v>
       </c>
@@ -2754,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>77</v>
       </c>
@@ -2793,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
@@ -2805,7 +2823,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D7" s="7" t="s">
         <v>133</v>
       </c>
@@ -2821,7 +2839,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="26"/>
@@ -2830,7 +2848,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>54</v>
       </c>
@@ -2842,7 +2860,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C10" s="15" t="s">
         <v>2</v>
       </c>
@@ -2883,7 +2901,7 @@
       <c r="P10" s="101"/>
       <c r="Q10" s="101"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>21</v>
       </c>
@@ -2922,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>8</v>
       </c>
@@ -2960,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>22</v>
       </c>
@@ -2998,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
@@ -3036,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C15" s="17" t="s">
         <v>10</v>
       </c>
@@ -3073,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C16" s="17" t="s">
         <v>78</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
@@ -3149,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C18" s="19" t="s">
         <v>12</v>
       </c>
@@ -3187,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C19" s="19" t="s">
         <v>23</v>
       </c>
@@ -3225,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -3234,7 +3252,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="G21" s="48" t="s">
         <v>129</v>
       </c>
@@ -3246,7 +3264,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -3255,7 +3273,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>55</v>
       </c>
@@ -3267,7 +3285,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C24" s="15" t="s">
         <v>2</v>
       </c>
@@ -3309,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C25" s="17" t="s">
         <v>21</v>
       </c>
@@ -3351,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C26" s="17" t="s">
         <v>8</v>
       </c>
@@ -3393,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
         <v>22</v>
       </c>
@@ -3434,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>9</v>
       </c>
@@ -3475,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
         <v>10</v>
       </c>
@@ -3516,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C30" s="17" t="s">
         <v>78</v>
       </c>
@@ -3557,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C31" s="19" t="s">
         <v>11</v>
       </c>
@@ -3598,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C32" s="19" t="s">
         <v>12</v>
       </c>
@@ -3639,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C33" s="28" t="s">
         <v>23</v>
       </c>
@@ -3680,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -3689,7 +3707,7 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
         <v>47</v>
       </c>
@@ -3701,7 +3719,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C36" s="17" t="s">
         <v>14</v>
       </c>
@@ -3739,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C37" s="17" t="s">
         <v>15</v>
       </c>
@@ -3777,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C38" s="19" t="s">
         <v>16</v>
       </c>
@@ -3815,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C39" s="19" t="s">
         <v>130</v>
       </c>
@@ -3852,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C40" s="19" t="s">
         <v>17</v>
       </c>
@@ -3890,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C41" s="19" t="s">
         <v>100</v>
       </c>
@@ -3928,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C42" s="19" t="s">
         <v>99</v>
       </c>
@@ -3966,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C43" s="81" t="s">
         <v>98</v>
       </c>
@@ -4004,12 +4022,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
         <v>56</v>
       </c>
@@ -4021,7 +4039,7 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C46" s="28" t="s">
         <v>14</v>
       </c>
@@ -4061,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C47" s="17" t="s">
         <v>15</v>
       </c>
@@ -4101,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C48" s="19" t="s">
         <v>16</v>
       </c>
@@ -4141,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C49" s="19" t="s">
         <v>130</v>
       </c>
@@ -4181,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C50" s="19" t="s">
         <v>17</v>
       </c>
@@ -4221,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C51" s="19" t="s">
         <v>100</v>
       </c>
@@ -4261,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C52" s="19" t="s">
         <v>99</v>
       </c>
@@ -4301,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C53" s="81" t="s">
         <v>98</v>
       </c>
@@ -4341,12 +4359,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B55" s="6" t="s">
         <v>38</v>
       </c>
@@ -4354,7 +4372,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C56" t="s">
         <v>39</v>
       </c>
@@ -4395,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
         <v>116</v>
       </c>
@@ -4436,7 +4454,7 @@
         <v>-2.4980018054066022E-12</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>83</v>
       </c>
@@ -4474,12 +4492,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B60" s="6" t="s">
         <v>40</v>
       </c>
@@ -4504,7 +4522,7 @@
         <v>-2.4980018054066022E-12</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C61" s="21" t="s">
         <v>57</v>
       </c>
@@ -4516,12 +4534,12 @@
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B63" s="6" t="s">
         <v>71</v>
       </c>
@@ -4546,7 +4564,7 @@
         <v>-7.4940054162198066E-12</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D64" s="1"/>
       <c r="K64" s="53">
         <f>IFERROR(K63/$D$63, 0)</f>
@@ -4565,12 +4583,12 @@
         <v>-1.1908497258409446E-17</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B67" s="27" t="s">
         <v>53</v>
       </c>
@@ -4586,7 +4604,7 @@
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B68" s="27"/>
       <c r="C68" s="21" t="s">
         <v>14</v>
@@ -4630,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B69" s="27"/>
       <c r="C69" s="21" t="s">
         <v>15</v>
@@ -4674,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B70" s="27"/>
       <c r="C70" s="21" t="s">
         <v>16</v>
@@ -4718,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B71" s="27"/>
       <c r="C71" s="21" t="s">
         <v>17</v>
@@ -4762,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B72" s="27"/>
       <c r="C72" s="21" t="s">
         <v>100</v>
@@ -4806,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B73" s="27"/>
       <c r="C73" s="21" t="s">
         <v>99</v>
@@ -4850,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B74" s="27"/>
       <c r="C74" s="21" t="s">
         <v>98</v>
@@ -4911,26 +4929,26 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="60" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="60" customWidth="1"/>
-    <col min="8" max="11" width="8.7109375" style="63"/>
-    <col min="12" max="12" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.7109375" style="63"/>
-    <col min="16" max="16" width="11.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.5703125" customWidth="1"/>
-    <col min="22" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.453125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="60" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.54296875" style="60" customWidth="1"/>
+    <col min="8" max="11" width="8.7265625" style="63"/>
+    <col min="12" max="12" width="5.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="63" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.7265625" style="63"/>
+    <col min="16" max="16" width="11.81640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.81640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.54296875" customWidth="1"/>
+    <col min="22" max="23" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.35">
       <c r="F1" s="65">
         <f>COUNTIF(F3:F94,"&gt;0")</f>
         <v>36</v>
@@ -4955,7 +4973,7 @@
       <c r="U1" s="61"/>
       <c r="V1" s="61"/>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B2" s="59" t="s">
         <v>62</v>
       </c>
@@ -5013,7 +5031,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="60">
         <v>42917</v>
       </c>
@@ -5070,7 +5088,7 @@
       <c r="U3" s="63"/>
       <c r="V3" s="63"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B4" s="60">
         <f>EDATE(B3,1)</f>
         <v>42948</v>
@@ -5124,7 +5142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" s="60">
         <f t="shared" ref="B5:B68" si="0">EDATE(B4,1)</f>
         <v>42979</v>
@@ -5198,7 +5216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B6" s="60">
         <f t="shared" si="0"/>
         <v>43009</v>
@@ -5272,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B7" s="60">
         <f t="shared" si="0"/>
         <v>43040</v>
@@ -5346,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B8" s="60">
         <f t="shared" si="0"/>
         <v>43070</v>
@@ -5420,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B9" s="60">
         <f t="shared" si="0"/>
         <v>43101</v>
@@ -5494,7 +5512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B10" s="60">
         <f t="shared" si="0"/>
         <v>43132</v>
@@ -5568,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="60">
         <f t="shared" si="0"/>
         <v>43160</v>
@@ -5642,7 +5660,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B12" s="60">
         <f t="shared" si="0"/>
         <v>43191</v>
@@ -5716,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B13" s="60">
         <f t="shared" si="0"/>
         <v>43221</v>
@@ -5790,7 +5808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B14" s="60">
         <f t="shared" si="0"/>
         <v>43252</v>
@@ -5864,7 +5882,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B15" s="60">
         <f t="shared" si="0"/>
         <v>43282</v>
@@ -5938,7 +5956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B16" s="60">
         <f t="shared" si="0"/>
         <v>43313</v>
@@ -6012,7 +6030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B17" s="60">
         <f t="shared" si="0"/>
         <v>43344</v>
@@ -6086,7 +6104,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B18" s="60">
         <f t="shared" si="0"/>
         <v>43374</v>
@@ -6160,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B19" s="60">
         <f t="shared" si="0"/>
         <v>43405</v>
@@ -6234,7 +6252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B20" s="60">
         <f t="shared" si="0"/>
         <v>43435</v>
@@ -6308,7 +6326,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B21" s="60">
         <f t="shared" si="0"/>
         <v>43466</v>
@@ -6382,7 +6400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B22" s="60">
         <f t="shared" si="0"/>
         <v>43497</v>
@@ -6456,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B23" s="60">
         <f t="shared" si="0"/>
         <v>43525</v>
@@ -6530,7 +6548,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B24" s="60">
         <f t="shared" si="0"/>
         <v>43556</v>
@@ -6604,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B25" s="60">
         <f t="shared" si="0"/>
         <v>43586</v>
@@ -6678,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B26" s="60">
         <f t="shared" si="0"/>
         <v>43617</v>
@@ -6752,7 +6770,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B27" s="60">
         <f t="shared" si="0"/>
         <v>43647</v>
@@ -6826,7 +6844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B28" s="60">
         <f t="shared" si="0"/>
         <v>43678</v>
@@ -6900,7 +6918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B29" s="60">
         <f t="shared" si="0"/>
         <v>43709</v>
@@ -6974,7 +6992,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B30" s="60">
         <f t="shared" si="0"/>
         <v>43739</v>
@@ -7048,7 +7066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B31" s="60">
         <f t="shared" si="0"/>
         <v>43770</v>
@@ -7122,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B32" s="60">
         <f t="shared" si="0"/>
         <v>43800</v>
@@ -7196,7 +7214,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B33" s="60">
         <f t="shared" si="0"/>
         <v>43831</v>
@@ -7270,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B34" s="60">
         <f t="shared" si="0"/>
         <v>43862</v>
@@ -7344,7 +7362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B35" s="60">
         <f t="shared" si="0"/>
         <v>43891</v>
@@ -7418,7 +7436,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B36" s="60">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -7492,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B37" s="60">
         <f t="shared" si="0"/>
         <v>43952</v>
@@ -7566,7 +7584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B38" s="60">
         <f t="shared" si="0"/>
         <v>43983</v>
@@ -7640,7 +7658,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B39" s="60">
         <f t="shared" si="0"/>
         <v>44013</v>
@@ -7714,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B40" s="60">
         <f t="shared" si="0"/>
         <v>44044</v>
@@ -7788,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B41" s="60">
         <f t="shared" si="0"/>
         <v>44075</v>
@@ -7862,7 +7880,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B42" s="60">
         <f t="shared" si="0"/>
         <v>44105</v>
@@ -7936,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B43" s="60">
         <f t="shared" si="0"/>
         <v>44136</v>
@@ -8010,7 +8028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B44" s="60">
         <f t="shared" si="0"/>
         <v>44166</v>
@@ -8084,7 +8102,7 @@
         <v>-6.2450045135165055E-13</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B45" s="60">
         <f t="shared" si="0"/>
         <v>44197</v>
@@ -8158,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B46" s="60">
         <f t="shared" si="0"/>
         <v>44228</v>
@@ -8232,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B47" s="60">
         <f t="shared" si="0"/>
         <v>44256</v>
@@ -8306,7 +8324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B48" s="60">
         <f t="shared" si="0"/>
         <v>44287</v>
@@ -8380,7 +8398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B49" s="60">
         <f t="shared" si="0"/>
         <v>44317</v>
@@ -8454,7 +8472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B50" s="60">
         <f t="shared" si="0"/>
         <v>44348</v>
@@ -8528,7 +8546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B51" s="60">
         <f t="shared" si="0"/>
         <v>44378</v>
@@ -8602,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B52" s="60">
         <f t="shared" si="0"/>
         <v>44409</v>
@@ -8676,7 +8694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B53" s="60">
         <f t="shared" si="0"/>
         <v>44440</v>
@@ -8750,7 +8768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B54" s="60">
         <f t="shared" si="0"/>
         <v>44470</v>
@@ -8824,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B55" s="60">
         <f t="shared" si="0"/>
         <v>44501</v>
@@ -8898,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B56" s="60">
         <f t="shared" si="0"/>
         <v>44531</v>
@@ -8972,7 +8990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B57" s="60">
         <f t="shared" si="0"/>
         <v>44562</v>
@@ -9046,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B58" s="60">
         <f t="shared" si="0"/>
         <v>44593</v>
@@ -9120,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B59" s="60">
         <f t="shared" si="0"/>
         <v>44621</v>
@@ -9194,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B60" s="60">
         <f t="shared" si="0"/>
         <v>44652</v>
@@ -9268,7 +9286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B61" s="60">
         <f t="shared" si="0"/>
         <v>44682</v>
@@ -9342,7 +9360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B62" s="60">
         <f t="shared" si="0"/>
         <v>44713</v>
@@ -9416,7 +9434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B63" s="60">
         <f t="shared" si="0"/>
         <v>44743</v>
@@ -9490,7 +9508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B64" s="60">
         <f t="shared" si="0"/>
         <v>44774</v>
@@ -9564,7 +9582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B65" s="60">
         <f t="shared" si="0"/>
         <v>44805</v>
@@ -9638,7 +9656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B66" s="60">
         <f t="shared" si="0"/>
         <v>44835</v>
@@ -9712,7 +9730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B67" s="60">
         <f t="shared" si="0"/>
         <v>44866</v>
@@ -9786,7 +9804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B68" s="60">
         <f t="shared" si="0"/>
         <v>44896</v>
@@ -9860,7 +9878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B69" s="60">
         <f t="shared" ref="B69:B94" si="6">EDATE(B68,1)</f>
         <v>44927</v>
@@ -9934,7 +9952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B70" s="60">
         <f t="shared" si="6"/>
         <v>44958</v>
@@ -10008,7 +10026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B71" s="60">
         <f t="shared" si="6"/>
         <v>44986</v>
@@ -10082,7 +10100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B72" s="60">
         <f t="shared" si="6"/>
         <v>45017</v>
@@ -10156,7 +10174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B73" s="60">
         <f t="shared" si="6"/>
         <v>45047</v>
@@ -10230,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B74" s="60">
         <f t="shared" si="6"/>
         <v>45078</v>
@@ -10304,7 +10322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B75" s="60">
         <f t="shared" si="6"/>
         <v>45108</v>
@@ -10378,7 +10396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B76" s="60">
         <f t="shared" si="6"/>
         <v>45139</v>
@@ -10452,7 +10470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B77" s="60">
         <f t="shared" si="6"/>
         <v>45170</v>
@@ -10526,7 +10544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B78" s="60">
         <f t="shared" si="6"/>
         <v>45200</v>
@@ -10600,7 +10618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B79" s="60">
         <f t="shared" si="6"/>
         <v>45231</v>
@@ -10674,7 +10692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B80" s="60">
         <f t="shared" si="6"/>
         <v>45261</v>
@@ -10748,7 +10766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B81" s="60">
         <f t="shared" si="6"/>
         <v>45292</v>
@@ -10822,7 +10840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B82" s="60">
         <f t="shared" si="6"/>
         <v>45323</v>
@@ -10896,7 +10914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B83" s="60">
         <f t="shared" si="6"/>
         <v>45352</v>
@@ -10970,7 +10988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B84" s="60">
         <f t="shared" si="6"/>
         <v>45383</v>
@@ -11044,7 +11062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B85" s="60">
         <f t="shared" si="6"/>
         <v>45413</v>
@@ -11118,7 +11136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B86" s="60">
         <f t="shared" si="6"/>
         <v>45444</v>
@@ -11192,7 +11210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B87" s="60">
         <f t="shared" si="6"/>
         <v>45474</v>
@@ -11266,7 +11284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B88" s="60">
         <f t="shared" si="6"/>
         <v>45505</v>
@@ -11340,7 +11358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B89" s="60">
         <f t="shared" si="6"/>
         <v>45536</v>
@@ -11414,7 +11432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B90" s="60">
         <f t="shared" si="6"/>
         <v>45566</v>
@@ -11488,7 +11506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B91" s="60">
         <f t="shared" si="6"/>
         <v>45597</v>
@@ -11562,7 +11580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B92" s="60">
         <f t="shared" si="6"/>
         <v>45627</v>
@@ -11636,7 +11654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B93" s="60">
         <f t="shared" si="6"/>
         <v>45658</v>
@@ -11710,7 +11728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B94" s="60">
         <f t="shared" si="6"/>
         <v>45689</v>
@@ -11805,16 +11823,16 @@
       <selection pane="bottomRight" activeCell="D79" sqref="D79:H79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="15" width="18" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>106</v>
       </c>
@@ -11846,12 +11864,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -11876,7 +11894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -11892,7 +11910,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>87</v>
       </c>
@@ -11926,7 +11944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>88</v>
       </c>
@@ -11961,7 +11979,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>89</v>
       </c>
@@ -11996,7 +12014,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>91</v>
       </c>
@@ -12031,7 +12049,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C10" s="78" t="s">
         <v>95</v>
       </c>
@@ -12056,7 +12074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C11" s="78" t="s">
         <v>96</v>
       </c>
@@ -12081,19 +12099,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
@@ -12118,7 +12136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C15" s="17" t="s">
         <v>21</v>
       </c>
@@ -12143,7 +12161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
@@ -12168,7 +12186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C17" s="17" t="s">
         <v>22</v>
       </c>
@@ -12193,7 +12211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C18" s="17" t="s">
         <v>9</v>
       </c>
@@ -12218,7 +12236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C19" s="17" t="s">
         <v>10</v>
       </c>
@@ -12243,7 +12261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C20" s="17" t="s">
         <v>78</v>
       </c>
@@ -12268,7 +12286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C21" s="19" t="s">
         <v>11</v>
       </c>
@@ -12293,7 +12311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C22" s="19" t="s">
         <v>12</v>
       </c>
@@ -12318,7 +12336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C23" s="19" t="s">
         <v>23</v>
       </c>
@@ -12343,12 +12361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C26" s="15" t="s">
         <v>2</v>
       </c>
@@ -12373,7 +12391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
@@ -12398,7 +12416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>8</v>
       </c>
@@ -12423,7 +12441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
         <v>22</v>
       </c>
@@ -12448,7 +12466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C30" s="17" t="s">
         <v>9</v>
       </c>
@@ -12473,7 +12491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="17" t="s">
         <v>10</v>
       </c>
@@ -12498,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C32" s="17" t="s">
         <v>78</v>
       </c>
@@ -12523,7 +12541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C33" s="19" t="s">
         <v>11</v>
       </c>
@@ -12548,7 +12566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C34" s="19" t="s">
         <v>12</v>
       </c>
@@ -12573,7 +12591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C35" s="28" t="s">
         <v>23</v>
       </c>
@@ -12593,19 +12611,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C38" s="15" t="s">
         <v>2</v>
       </c>
@@ -12630,7 +12648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C39" s="17" t="s">
         <v>21</v>
       </c>
@@ -12655,7 +12673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C40" s="17" t="s">
         <v>8</v>
       </c>
@@ -12680,7 +12698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C41" s="17" t="s">
         <v>22</v>
       </c>
@@ -12705,7 +12723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C42" s="17" t="s">
         <v>9</v>
       </c>
@@ -12730,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C43" s="17" t="s">
         <v>10</v>
       </c>
@@ -12755,7 +12773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C44" s="17" t="s">
         <v>78</v>
       </c>
@@ -12780,7 +12798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C45" s="19" t="s">
         <v>11</v>
       </c>
@@ -12805,7 +12823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C46" s="19" t="s">
         <v>12</v>
       </c>
@@ -12830,7 +12848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C47" s="19" t="s">
         <v>23</v>
       </c>
@@ -12855,12 +12873,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B49" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C50" s="15" t="s">
         <v>2</v>
       </c>
@@ -12885,7 +12903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C51" s="17" t="s">
         <v>21</v>
       </c>
@@ -12910,7 +12928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C52" s="17" t="s">
         <v>8</v>
       </c>
@@ -12935,7 +12953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C53" s="17" t="s">
         <v>22</v>
       </c>
@@ -12960,7 +12978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C54" s="17" t="s">
         <v>9</v>
       </c>
@@ -12985,7 +13003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C55" s="17" t="s">
         <v>10</v>
       </c>
@@ -13010,7 +13028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C56" s="17" t="s">
         <v>78</v>
       </c>
@@ -13035,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C57" s="19" t="s">
         <v>11</v>
       </c>
@@ -13060,7 +13078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C58" s="19" t="s">
         <v>12</v>
       </c>
@@ -13085,7 +13103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C59" s="28" t="s">
         <v>23</v>
       </c>
@@ -13105,12 +13123,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B61" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C62" s="17" t="s">
         <v>14</v>
       </c>
@@ -13135,7 +13153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C63" s="17" t="s">
         <v>15</v>
       </c>
@@ -13160,7 +13178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C64" s="19" t="s">
         <v>16</v>
       </c>
@@ -13185,7 +13203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C65" s="19" t="s">
         <v>130</v>
       </c>
@@ -13210,7 +13228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C66" s="19" t="s">
         <v>17</v>
       </c>
@@ -13235,7 +13253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C67" s="19" t="s">
         <v>100</v>
       </c>
@@ -13260,7 +13278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C68" s="19" t="s">
         <v>99</v>
       </c>
@@ -13285,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C69" s="81" t="s">
         <v>97</v>
       </c>
@@ -13310,7 +13328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B71" s="6" t="s">
         <v>46</v>
       </c>
@@ -13318,7 +13336,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C72" s="28" t="s">
         <v>14</v>
       </c>
@@ -13361,7 +13379,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C73" s="17" t="s">
         <v>15</v>
       </c>
@@ -13410,7 +13428,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C74" s="19" t="s">
         <v>16</v>
       </c>
@@ -13459,7 +13477,7 @@
         <v>1.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C75" s="19" t="s">
         <v>130</v>
       </c>
@@ -13508,7 +13526,7 @@
         <v>1.3000000000000002E-3</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C76" s="19" t="s">
         <v>17</v>
       </c>
@@ -13557,7 +13575,7 @@
         <v>1.4000000000000002E-3</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C77" s="19" t="s">
         <v>100</v>
       </c>
@@ -13606,7 +13624,7 @@
         <v>1.5000000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C78" s="19" t="s">
         <v>99</v>
       </c>
@@ -13655,7 +13673,7 @@
         <v>1.6000000000000003E-3</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C79" s="81" t="s">
         <v>97</v>
       </c>
@@ -13704,19 +13722,19 @@
         <v>1.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B81" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C82" s="17" t="s">
         <v>14</v>
       </c>
@@ -13761,7 +13779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C83" s="17" t="s">
         <v>15</v>
       </c>
@@ -13806,7 +13824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C84" s="19" t="s">
         <v>16</v>
       </c>
@@ -13851,7 +13869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C85" s="19" t="s">
         <v>130</v>
       </c>
@@ -13896,7 +13914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C86" s="19" t="s">
         <v>17</v>
       </c>
@@ -13941,7 +13959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C87" s="19" t="s">
         <v>100</v>
       </c>
@@ -13986,7 +14004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C88" s="19" t="s">
         <v>99</v>
       </c>
@@ -14031,7 +14049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C89" s="81" t="s">
         <v>97</v>
       </c>
@@ -14076,12 +14094,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B91" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C92" s="28" t="s">
         <v>14</v>
       </c>
@@ -14101,7 +14119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C93" s="17" t="s">
         <v>15</v>
       </c>
@@ -14126,7 +14144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C94" s="19" t="s">
         <v>16</v>
       </c>
@@ -14151,7 +14169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C95" s="19" t="s">
         <v>130</v>
       </c>
@@ -14176,7 +14194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C96" s="19" t="s">
         <v>17</v>
       </c>
@@ -14201,7 +14219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C97" s="19" t="s">
         <v>100</v>
       </c>
@@ -14226,7 +14244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C98" s="19" t="s">
         <v>99</v>
       </c>
@@ -14251,7 +14269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C99" s="81" t="s">
         <v>97</v>
       </c>
@@ -14276,12 +14294,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B101" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="88">
         <v>2</v>
       </c>
@@ -14309,7 +14327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="88">
         <v>3</v>
       </c>
@@ -14337,7 +14355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="88">
         <v>4</v>
       </c>
@@ -14365,7 +14383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="88">
         <v>5</v>
       </c>
@@ -14393,7 +14411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="88">
         <v>6</v>
       </c>
@@ -14421,7 +14439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="88">
         <v>7</v>
       </c>
@@ -14449,7 +14467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B109" s="6" t="s">
         <v>113</v>
       </c>
@@ -14474,10 +14492,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B111" s="6" t="s">
         <v>43</v>
       </c>
@@ -14502,14 +14520,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B113" s="6" t="s">
         <v>83</v>
       </c>
@@ -14530,7 +14548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B115" s="6" t="s">
         <v>114</v>
       </c>
@@ -14555,7 +14573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B118" s="27"/>
       <c r="C118" s="21" t="s">
         <v>115</v>
@@ -14581,7 +14599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B119" s="27"/>
       <c r="D119" s="21">
         <v>0.1</v>
@@ -14599,7 +14617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B120" s="27"/>
       <c r="D120" s="21">
         <f>SUM(D118:D119)</f>
@@ -14622,7 +14640,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="121" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B121" s="27"/>
       <c r="D121" s="21">
         <f>_xlfn.RANK.EQ(D120, $D$120:$H$120, 5)</f>
@@ -14645,16 +14663,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B122" s="27"/>
     </row>
-    <row r="123" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B123" s="27"/>
       <c r="C123" s="21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B124" s="27"/>
       <c r="D124" s="21" t="s">
         <v>117</v>
@@ -14664,7 +14682,7 @@
         <v>-22500</v>
       </c>
     </row>
-    <row r="125" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B125" s="27"/>
       <c r="D125" s="21" t="s">
         <v>118</v>
@@ -14674,7 +14692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B126" s="27"/>
       <c r="D126" s="21" t="s">
         <v>119</v>
@@ -14684,7 +14702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B127" s="27"/>
       <c r="D127" s="21" t="s">
         <v>120</v>
@@ -14694,7 +14712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F131" s="2"/>
     </row>
   </sheetData>
@@ -14707,22 +14725,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="10" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="6" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="10" width="4.1796875" customWidth="1"/>
+    <col min="11" max="11" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C2" s="48" t="s">
         <v>5</v>
       </c>
@@ -14730,7 +14750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>112</v>
       </c>
@@ -14748,7 +14768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -14777,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="E5" s="48" t="s">
         <v>84</v>
       </c>
@@ -14797,7 +14817,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -14832,14 +14852,14 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C8" s="43"/>
       <c r="D8" s="39"/>
       <c r="K8" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C9" s="46" t="s">
         <v>28</v>
       </c>
@@ -14854,7 +14874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
@@ -14885,7 +14905,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
@@ -14916,7 +14936,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
         <v>22</v>
       </c>
@@ -14941,7 +14961,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>9</v>
       </c>
@@ -14967,7 +14987,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>10</v>
       </c>
@@ -14998,7 +15018,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>78</v>
       </c>
@@ -15029,7 +15049,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>11</v>
       </c>
@@ -15056,7 +15076,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
@@ -15081,7 +15101,7 @@
         <v>1.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>23</v>
       </c>
@@ -15112,14 +15132,14 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C19" s="43"/>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
         <v>14</v>
       </c>
@@ -15150,7 +15170,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
         <v>15</v>
       </c>
@@ -15175,7 +15195,7 @@
         <v>5.6000000000000008E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
         <v>16</v>
       </c>
@@ -15200,7 +15220,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
         <v>130</v>
       </c>
@@ -15225,7 +15245,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="19" t="s">
         <v>17</v>
       </c>
@@ -15257,7 +15277,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="19" t="s">
         <v>100</v>
       </c>
@@ -15280,7 +15300,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="19" t="s">
         <v>99</v>
       </c>
@@ -15312,7 +15332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="81" t="s">
         <v>97</v>
       </c>
@@ -15337,7 +15357,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="K28" t="s">
         <v>134</v>
       </c>
@@ -15351,4 +15371,249 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="54">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>50000</v>
+      </c>
+      <c r="B3">
+        <v>99999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100000</v>
+      </c>
+      <c r="B4">
+        <v>299999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>300000</v>
+      </c>
+      <c r="B5">
+        <v>499999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>500000</v>
+      </c>
+      <c r="B6">
+        <v>999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1000000</v>
+      </c>
+      <c r="B7">
+        <v>1999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2000000</v>
+      </c>
+      <c r="B8">
+        <v>5000000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>0.17</v>
+      </c>
+      <c r="D15">
+        <f>C15*$D$14</f>
+        <v>0.20400000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="103">
+        <f>E15-D15</f>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D22" si="0">C16*$D$14</f>
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F16" s="103">
+        <f t="shared" ref="F16:F21" si="1">E16-D16</f>
+        <v>-5.1999999999999824E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>0.122</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.1464</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F17" s="103">
+        <f t="shared" si="1"/>
+        <v>-6.399999999999989E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.1164</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="F18" s="103">
+        <f t="shared" si="1"/>
+        <v>-6.4000000000000029E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F19" s="103">
+        <f t="shared" si="1"/>
+        <v>-3.1999999999999945E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="F20" s="103">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>4.3199999999999995E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F21" s="103">
+        <f t="shared" si="1"/>
+        <v>-3.1999999999999945E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update mara y/n formula in external output tab
Do this because it was deriving off CCLF Y/N instead of MARA Y/N
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1293,7 +1293,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1419,7 +1419,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F9" s="55" t="s">
         <v>3</v>
@@ -1797,10 +1797,10 @@
   <dimension ref="B2:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2759,23 +2759,23 @@
         <v>143</v>
       </c>
       <c r="D40" s="1">
-        <f>IF(Inputs!D$6 = "N", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AD$3:AD$204), 0)</f>
+        <f>IF(Inputs!D$9 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AD$3:AD$204), 0)</f>
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <f>IF(Inputs!E$6 = "N", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AE$3:AE$204), 0)</f>
-        <v>0</v>
+        <f>IF(Inputs!E$9 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AE$3:AE$204), 0)</f>
+        <v>10250</v>
       </c>
       <c r="F40" s="1">
-        <f>IF(Inputs!F$6 = "N", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AF$3:AF$204), 0)</f>
+        <f>IF(Inputs!F$9 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AF$3:AF$204), 0)</f>
         <v>40487.5</v>
       </c>
       <c r="G40" s="1">
-        <f>IF(Inputs!G$6 = "N", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AG$3:AG$204), 0)</f>
+        <f>IF(Inputs!G$9 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AG$3:AG$204), 0)</f>
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <f>IF(Inputs!H$6 = "N", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AH$3:AH$204), 0)</f>
+        <f>IF(Inputs!H$9 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AH$3:AH$204), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2784,23 +2784,23 @@
         <v>144</v>
       </c>
       <c r="D41" s="1">
-        <f>IF(Inputs!D$6 = "N", SUM(Outputs_Timeline!AD$3:AD$204), 0)</f>
+        <f>IF(Inputs!D$9 = "Y", SUM(Outputs_Timeline!AD$3:AD$204), 0)</f>
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <f>IF(Inputs!E$6 = "N", SUM(Outputs_Timeline!AE$3:AE$204), 0)</f>
-        <v>0</v>
+        <f>IF(Inputs!E$9 = "Y", SUM(Outputs_Timeline!AE$3:AE$204), 0)</f>
+        <v>32313.125</v>
       </c>
       <c r="F41" s="1">
-        <f>IF(Inputs!F$6 = "N", SUM(Outputs_Timeline!AF$3:AF$204), 0)</f>
+        <f>IF(Inputs!F$9 = "Y", SUM(Outputs_Timeline!AF$3:AF$204), 0)</f>
         <v>127636.84375</v>
       </c>
       <c r="G41" s="1">
-        <f>IF(Inputs!G$6 = "N", SUM(Outputs_Timeline!AG$3:AG$204), 0)</f>
+        <f>IF(Inputs!G$9 = "Y", SUM(Outputs_Timeline!AG$3:AG$204), 0)</f>
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f>IF(Inputs!H$6 = "N", SUM(Outputs_Timeline!AH$3:AH$204), 0)</f>
+        <f>IF(Inputs!H$9 = "Y", SUM(Outputs_Timeline!AH$3:AH$204), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="E43" s="7">
         <f>(E34/12*Inputs!$C$2+E4)*$C$37+E41</f>
-        <v>155251.6875</v>
+        <v>187564.8125</v>
       </c>
       <c r="F43" s="7">
         <f>(F34/12*Inputs!$C$2+F4)*$C$37+F41</f>
@@ -2858,13 +2858,13 @@
     <row r="47" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>847330.95625000016</v>
+        <v>879644.08125000016</v>
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C48" s="52">
         <f>SUM(D43:H43)</f>
-        <v>847330.95624999993</v>
+        <v>879644.08124999993</v>
       </c>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -2900,7 +2900,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4317,15 +4317,15 @@
         <v>0</v>
       </c>
       <c r="F47" s="49">
-        <f>IFERROR((1-G47)*F36/SUM(F36,H36),0)</f>
+        <f t="shared" ref="F47:F53" si="33">IFERROR((1-G47)*F36/SUM(F36,H36),0)</f>
         <v>0.82499999999999996</v>
       </c>
       <c r="G47" s="49">
-        <f>MIN(1,G36+$H$21)</f>
+        <f t="shared" ref="G47:G53" si="34">MIN(1,G36+$H$21)</f>
         <v>0.17499999999999999</v>
       </c>
       <c r="H47" s="49">
-        <f>IFERROR((1-G47)*H36/SUM(F36,H36),0)</f>
+        <f t="shared" ref="H47:H53" si="35">IFERROR((1-G47)*H36/SUM(F36,H36),0)</f>
         <v>0</v>
       </c>
       <c r="I47" s="49">
@@ -4336,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="29">
-        <f t="shared" ref="L47:L51" si="33">G47*$D47</f>
+        <f t="shared" ref="L47:L51" si="36">G47*$D47</f>
         <v>0</v>
       </c>
       <c r="M47" s="29">
@@ -4357,15 +4357,15 @@
         <v>910.00000000000364</v>
       </c>
       <c r="F48" s="30">
-        <f>IFERROR((1-G48)*F37/SUM(F37,H37),0)</f>
+        <f t="shared" si="33"/>
         <v>0.82499999999999996</v>
       </c>
       <c r="G48" s="30">
-        <f>MIN(1,G37+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="H48" s="30">
-        <f>IFERROR((1-G48)*H37/SUM(F37,H37),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I48" s="30">
@@ -4376,15 +4376,15 @@
         <v>750.75000000000296</v>
       </c>
       <c r="L48" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>159.25000000000063</v>
       </c>
       <c r="M48" s="18">
-        <f t="shared" ref="M48:N51" si="34">H48*$D48</f>
+        <f t="shared" ref="M48:N51" si="37">H48*$D48</f>
         <v>0</v>
       </c>
       <c r="N48" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -4397,34 +4397,34 @@
         <v>0</v>
       </c>
       <c r="F49" s="31">
-        <f>IFERROR((1-G49)*F38/SUM(F38,H38),0)</f>
+        <f t="shared" si="33"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G49" s="31">
-        <f>MIN(1,G38+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="H49" s="31">
-        <f>IFERROR((1-G49)*H38/SUM(F38,H38),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I49" s="31">
         <v>0</v>
       </c>
       <c r="K49" s="20">
-        <f t="shared" ref="K49:K51" si="35">F49*$D49</f>
+        <f t="shared" ref="K49:K51" si="38">F49*$D49</f>
         <v>0</v>
       </c>
       <c r="L49" s="20">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M49" s="20">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N49" s="20">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -4437,34 +4437,34 @@
         <v>0</v>
       </c>
       <c r="F50" s="31">
-        <f>IFERROR((1-G50)*F39/SUM(F39,H39),0)</f>
+        <f t="shared" si="33"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G50" s="31">
-        <f>MIN(1,G39+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="H50" s="31">
-        <f>IFERROR((1-G50)*H39/SUM(F39,H39),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I50" s="31">
         <v>0</v>
       </c>
       <c r="K50" s="20">
-        <f t="shared" ref="K50" si="36">F50*$D50</f>
+        <f t="shared" ref="K50" si="39">F50*$D50</f>
         <v>0</v>
       </c>
       <c r="L50" s="20">
-        <f t="shared" ref="L50" si="37">G50*$D50</f>
+        <f t="shared" ref="L50" si="40">G50*$D50</f>
         <v>0</v>
       </c>
       <c r="M50" s="20">
-        <f t="shared" ref="M50" si="38">H50*$D50</f>
+        <f t="shared" ref="M50" si="41">H50*$D50</f>
         <v>0</v>
       </c>
       <c r="N50" s="20">
-        <f t="shared" ref="N50" si="39">I50*$D50</f>
+        <f t="shared" ref="N50" si="42">I50*$D50</f>
         <v>0</v>
       </c>
     </row>
@@ -4477,34 +4477,34 @@
         <v>0</v>
       </c>
       <c r="F51" s="31">
-        <f>IFERROR((1-G51)*F40/SUM(F40,H40),0)</f>
+        <f t="shared" si="33"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G51" s="31">
-        <f>MIN(1,G40+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="H51" s="31">
-        <f>IFERROR((1-G51)*H40/SUM(F40,H40),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I51" s="31">
         <v>0</v>
       </c>
       <c r="K51" s="20">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L51" s="20">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M51" s="20">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N51" s="20">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -4517,34 +4517,34 @@
         <v>0</v>
       </c>
       <c r="F52" s="31">
-        <f>IFERROR((1-G52)*F41/SUM(F41,H41),0)</f>
+        <f t="shared" si="33"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G52" s="31">
-        <f>MIN(1,G41+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="H52" s="31">
-        <f>IFERROR((1-G52)*H41/SUM(F41,H41),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I52" s="31">
         <v>0</v>
       </c>
       <c r="K52" s="20">
-        <f t="shared" ref="K52:K54" si="40">F52*$D52</f>
+        <f t="shared" ref="K52:K54" si="43">F52*$D52</f>
         <v>0</v>
       </c>
       <c r="L52" s="20">
-        <f t="shared" ref="L52:L54" si="41">G52*$D52</f>
+        <f t="shared" ref="L52:L54" si="44">G52*$D52</f>
         <v>0</v>
       </c>
       <c r="M52" s="20">
-        <f t="shared" ref="M52:M54" si="42">H52*$D52</f>
+        <f t="shared" ref="M52:M54" si="45">H52*$D52</f>
         <v>0</v>
       </c>
       <c r="N52" s="20">
-        <f t="shared" ref="N52:N54" si="43">I52*$D52</f>
+        <f t="shared" ref="N52:N54" si="46">I52*$D52</f>
         <v>0</v>
       </c>
     </row>
@@ -4557,34 +4557,34 @@
         <v>10010</v>
       </c>
       <c r="F53" s="31">
-        <f>IFERROR((1-G53)*F42/SUM(F42,H42),0)</f>
+        <f t="shared" si="33"/>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G53" s="31">
-        <f>MIN(1,G42+$H$21)</f>
+        <f t="shared" si="34"/>
         <v>0.97499999999999998</v>
       </c>
       <c r="H53" s="31">
-        <f>IFERROR((1-G53)*H42/SUM(F42,H42),0)</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I53" s="31">
         <v>0</v>
       </c>
       <c r="K53" s="20">
-        <f t="shared" ref="K53" si="44">F53*$D53</f>
+        <f t="shared" ref="K53" si="47">F53*$D53</f>
         <v>250.25000000000023</v>
       </c>
       <c r="L53" s="20">
-        <f t="shared" ref="L53" si="45">G53*$D53</f>
+        <f t="shared" ref="L53" si="48">G53*$D53</f>
         <v>9759.75</v>
       </c>
       <c r="M53" s="20">
-        <f t="shared" ref="M53" si="46">H53*$D53</f>
+        <f t="shared" ref="M53" si="49">H53*$D53</f>
         <v>0</v>
       </c>
       <c r="N53" s="20">
-        <f t="shared" ref="N53" si="47">I53*$D53</f>
+        <f t="shared" ref="N53" si="50">I53*$D53</f>
         <v>0</v>
       </c>
     </row>
@@ -4597,34 +4597,34 @@
         <v>0</v>
       </c>
       <c r="F54" s="31">
-        <f t="shared" ref="F54" si="48">IFERROR((1-G54)*F43/SUM(F43,H43),0)</f>
+        <f t="shared" ref="F54" si="51">IFERROR((1-G54)*F43/SUM(F43,H43),0)</f>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G54" s="31">
-        <f t="shared" ref="G54" si="49">MIN(1,G43+$H$21)</f>
+        <f t="shared" ref="G54" si="52">MIN(1,G43+$H$21)</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="H54" s="31">
-        <f t="shared" ref="H54" si="50">IFERROR((1-G54)*H43/SUM(F43,H43),0)</f>
+        <f t="shared" ref="H54" si="53">IFERROR((1-G54)*H43/SUM(F43,H43),0)</f>
         <v>0</v>
       </c>
       <c r="I54" s="31">
         <v>0</v>
       </c>
       <c r="K54" s="20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="L54" s="20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="M54" s="20">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="N54" s="20">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
@@ -4637,34 +4637,34 @@
         <v>38220</v>
       </c>
       <c r="F55" s="87">
-        <f t="shared" ref="F55" si="51">IFERROR((1-G55)*F44/SUM(F44,H44),0)</f>
+        <f t="shared" ref="F55" si="54">IFERROR((1-G55)*F44/SUM(F44,H44),0)</f>
         <v>2.5000000000000022E-2</v>
       </c>
       <c r="G55" s="87">
-        <f t="shared" ref="G55" si="52">MIN(1,G44+$H$21)</f>
+        <f t="shared" ref="G55" si="55">MIN(1,G44+$H$21)</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="H55" s="87">
-        <f t="shared" ref="H55" si="53">IFERROR((1-G55)*H44/SUM(F44,H44),0)</f>
+        <f t="shared" ref="H55" si="56">IFERROR((1-G55)*H44/SUM(F44,H44),0)</f>
         <v>0</v>
       </c>
       <c r="I55" s="87">
         <v>0</v>
       </c>
       <c r="K55" s="84">
-        <f t="shared" ref="K55" si="54">F55*$D55</f>
+        <f t="shared" ref="K55" si="57">F55*$D55</f>
         <v>955.5000000000008</v>
       </c>
       <c r="L55" s="84">
-        <f t="shared" ref="L55" si="55">G55*$D55</f>
+        <f t="shared" ref="L55" si="58">G55*$D55</f>
         <v>37264.5</v>
       </c>
       <c r="M55" s="84">
-        <f t="shared" ref="M55" si="56">H55*$D55</f>
+        <f t="shared" ref="M55" si="59">H55*$D55</f>
         <v>0</v>
       </c>
       <c r="N55" s="84">
-        <f t="shared" ref="N55" si="57">I55*$D55</f>
+        <f t="shared" ref="N55" si="60">I55*$D55</f>
         <v>0</v>
       </c>
     </row>
@@ -4694,15 +4694,15 @@
         <v>0.21665259726816324</v>
       </c>
       <c r="G58" s="8">
-        <f t="shared" ref="G58:I58" si="58">IFERROR(SUM(L72:L80)/SUM($K$72:$N$80), 0)</f>
+        <f t="shared" ref="G58:I58" si="61">IFERROR(SUM(L72:L80)/SUM($K$72:$N$80), 0)</f>
         <v>0.74862611331539208</v>
       </c>
       <c r="H58" s="8">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3.1638022655986732E-2</v>
       </c>
       <c r="I58" s="8">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3.0832667604578324E-3</v>
       </c>
       <c r="K58" s="12">
@@ -4789,15 +4789,15 @@
         <v>-2047.5</v>
       </c>
       <c r="L60" s="12">
-        <f t="shared" ref="L60:N60" si="59">$D$60*G60</f>
+        <f t="shared" ref="L60:N60" si="62">$D$60*G60</f>
         <v>-1477.5</v>
       </c>
       <c r="M60" s="12">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="N60" s="12">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       <c r="C65" s="21"/>
       <c r="D65" s="1">
         <f>SUM(Outputs_Timeline!N:N)</f>
-        <v>127636.84375</v>
+        <v>159949.96875</v>
       </c>
       <c r="F65" s="3">
         <f>'MARA Prices'!$F$5</f>
@@ -4876,11 +4876,11 @@
       </c>
       <c r="K65" s="12">
         <f>$D$65*F65</f>
-        <v>12763.684375000001</v>
+        <v>15994.996875000001</v>
       </c>
       <c r="L65" s="12">
         <f>$D$65*G65</f>
-        <v>12763.684375000001</v>
+        <v>15994.996875000001</v>
       </c>
       <c r="M65" s="12">
         <f>$D$65*H65</f>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="N65" s="12">
         <f>$D$65*I65</f>
-        <v>102109.47500000001</v>
+        <v>127959.97500000001</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.35">
@@ -4902,15 +4902,15 @@
       </c>
       <c r="D67" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>847330.95625000016</v>
+        <v>879644.08125000016</v>
       </c>
       <c r="K67" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>214792.20975865333</v>
+        <v>218023.52225865333</v>
       </c>
       <c r="L67" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>513229.31116157072</v>
+        <v>516460.62366157077</v>
       </c>
       <c r="M67" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -4918,26 +4918,26 @@
       </c>
       <c r="N67" s="12">
         <f>SUM(Outputs_Timeline!AA:AA)</f>
-        <v>103636.83953217298</v>
+        <v>129487.33953217296</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D68" s="1"/>
       <c r="K68" s="53">
         <f>IFERROR(K67/$D$67, 0)</f>
-        <v>0.25349269748062897</v>
+        <v>0.24785424799179628</v>
       </c>
       <c r="L68" s="53">
         <f>IFERROR(L67/$D$67, 0)</f>
-        <v>0.60570112230166806</v>
+        <v>0.58712453669632492</v>
       </c>
       <c r="M68" s="53">
         <f>IFERROR(M67/$D$67, 0)</f>
-        <v>1.8496427732281377E-2</v>
+        <v>1.7816974082667369E-2</v>
       </c>
       <c r="N68" s="53">
         <f>IFERROR(N67/$D$67, 0)</f>
-        <v>0.12230975248542143</v>
+        <v>0.1472042412292113</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.35">
@@ -4989,19 +4989,19 @@
       </c>
       <c r="J72" s="21"/>
       <c r="K72" s="25">
-        <f t="shared" ref="K72:N74" si="60">F72*$D72</f>
+        <f t="shared" ref="K72:N74" si="63">F72*$D72</f>
         <v>7650</v>
       </c>
       <c r="L72" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>850</v>
       </c>
       <c r="M72" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="N72" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
     </row>
@@ -5033,19 +5033,19 @@
       </c>
       <c r="J73" s="21"/>
       <c r="K73" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>33676.878787878792</v>
       </c>
       <c r="L73" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>15873.5</v>
       </c>
       <c r="M73" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>8136.6666666666679</v>
       </c>
       <c r="N73" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>792.95454545454538</v>
       </c>
     </row>
@@ -5077,19 +5077,19 @@
       </c>
       <c r="J74" s="21"/>
       <c r="K74" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>3139.3950830278195</v>
       </c>
       <c r="L74" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>31860.604916972181</v>
       </c>
       <c r="M74" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="N74" s="25">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
     </row>
@@ -5108,32 +5108,32 @@
         <v>9.2801717643513637E-2</v>
       </c>
       <c r="G75" s="24">
-        <f t="shared" ref="G75:I75" si="61">IFERROR(SUM(L39,L17:L19,L50,L31:L33)/SUM($K$39:$N$39,$K$17:$M$19,$K$50:$N$50,$K$31:$N$33),0)</f>
+        <f t="shared" ref="G75:I75" si="64">IFERROR(SUM(L39,L17:L19,L50,L31:L33)/SUM($K$39:$N$39,$K$17:$M$19,$K$50:$N$50,$K$31:$N$33),0)</f>
         <v>0.90719828235648636</v>
       </c>
       <c r="H75" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I75" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="J75" s="21"/>
       <c r="K75" s="25">
-        <f t="shared" ref="K75" si="62">F75*$D75</f>
+        <f t="shared" ref="K75" si="65">F75*$D75</f>
         <v>3248.0601175229772</v>
       </c>
       <c r="L75" s="25">
-        <f t="shared" ref="L75" si="63">G75*$D75</f>
+        <f t="shared" ref="L75" si="66">G75*$D75</f>
         <v>31751.939882477021</v>
       </c>
       <c r="M75" s="25">
-        <f t="shared" ref="M75" si="64">H75*$D75</f>
+        <f t="shared" ref="M75" si="67">H75*$D75</f>
         <v>0</v>
       </c>
       <c r="N75" s="25">
-        <f t="shared" ref="N75" si="65">I75*$D75</f>
+        <f t="shared" ref="N75" si="68">I75*$D75</f>
         <v>0</v>
       </c>
     </row>
@@ -5148,36 +5148,36 @@
       </c>
       <c r="E76" s="21"/>
       <c r="F76" s="24">
-        <f>IFERROR(SUM(K40,K51)/SUM($K40:$N40,$K51:$N51),0)</f>
+        <f t="shared" ref="F76:I77" si="69">IFERROR(SUM(K40,K51)/SUM($K40:$N40,$K51:$N51),0)</f>
         <v>0</v>
       </c>
       <c r="G76" s="24">
-        <f>IFERROR(SUM(L40,L51)/SUM($K40:$N40,$K51:$N51),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="H76" s="24">
-        <f>IFERROR(SUM(M40,M51)/SUM($K40:$N40,$K51:$N51),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="I76" s="24">
-        <f>IFERROR(SUM(N40,N51)/SUM($K40:$N40,$K51:$N51),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="J76" s="21"/>
       <c r="K76" s="25">
-        <f t="shared" ref="K76:K80" si="66">F76*$D76</f>
+        <f t="shared" ref="K76:K80" si="70">F76*$D76</f>
         <v>0</v>
       </c>
       <c r="L76" s="25">
-        <f t="shared" ref="L76:L80" si="67">G76*$D76</f>
+        <f t="shared" ref="L76:L80" si="71">G76*$D76</f>
         <v>0</v>
       </c>
       <c r="M76" s="25">
-        <f t="shared" ref="M76:M80" si="68">H76*$D76</f>
+        <f t="shared" ref="M76:M80" si="72">H76*$D76</f>
         <v>0</v>
       </c>
       <c r="N76" s="25">
-        <f t="shared" ref="N76:N80" si="69">I76*$D76</f>
+        <f t="shared" ref="N76:N80" si="73">I76*$D76</f>
         <v>0</v>
       </c>
     </row>
@@ -5192,36 +5192,36 @@
       </c>
       <c r="E77" s="21"/>
       <c r="F77" s="24">
-        <f>IFERROR(SUM(K41,K52)/SUM($K41:$N41,$K52:$N52),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G77" s="24">
-        <f>IFERROR(SUM(L41,L52)/SUM($K41:$N41,$K52:$N52),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="H77" s="24">
-        <f>IFERROR(SUM(M41,M52)/SUM($K41:$N41,$K52:$N52),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="I77" s="24">
-        <f>IFERROR(SUM(N41,N52)/SUM($K41:$N41,$K52:$N52),0)</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="J77" s="21"/>
       <c r="K77" s="25">
-        <f t="shared" ref="K77:K79" si="70">F77*$D77</f>
+        <f t="shared" ref="K77:K79" si="74">F77*$D77</f>
         <v>0</v>
       </c>
       <c r="L77" s="25">
-        <f t="shared" ref="L77:L79" si="71">G77*$D77</f>
+        <f t="shared" ref="L77:L79" si="75">G77*$D77</f>
         <v>0</v>
       </c>
       <c r="M77" s="25">
-        <f t="shared" ref="M77:M79" si="72">H77*$D77</f>
+        <f t="shared" ref="M77:M79" si="76">H77*$D77</f>
         <v>0</v>
       </c>
       <c r="N77" s="25">
-        <f t="shared" ref="N77:N79" si="73">I77*$D77</f>
+        <f t="shared" ref="N77:N79" si="77">I77*$D77</f>
         <v>0</v>
       </c>
     </row>
@@ -5240,32 +5240,32 @@
         <v>8.4123804600672009E-2</v>
       </c>
       <c r="G78" s="24">
-        <f t="shared" ref="G78:I78" si="74">IFERROR(SUM(L42,L18,L53,L32)/SUM($K$42:$N$42,$K$18:$M$18,$K$53:$N$53,$K$32:$N$32),0)</f>
+        <f t="shared" ref="G78:I78" si="78">IFERROR(SUM(L42,L18,L53,L32)/SUM($K$42:$N$42,$K$18:$M$18,$K$53:$N$53,$K$32:$N$32),0)</f>
         <v>0.91587619539932796</v>
       </c>
       <c r="H78" s="24">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="I78" s="24">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="J78" s="21"/>
       <c r="K78" s="25">
-        <f t="shared" ref="K78" si="75">F78*$D78</f>
+        <f t="shared" ref="K78" si="79">F78*$D78</f>
         <v>6088.8809769966401</v>
       </c>
       <c r="L78" s="25">
-        <f t="shared" ref="L78" si="76">G78*$D78</f>
+        <f t="shared" ref="L78" si="80">G78*$D78</f>
         <v>66291.119023003354</v>
       </c>
       <c r="M78" s="25">
-        <f t="shared" ref="M78" si="77">H78*$D78</f>
+        <f t="shared" ref="M78" si="81">H78*$D78</f>
         <v>0</v>
       </c>
       <c r="N78" s="25">
-        <f t="shared" ref="N78" si="78">I78*$D78</f>
+        <f t="shared" ref="N78" si="82">I78*$D78</f>
         <v>0</v>
       </c>
     </row>
@@ -5280,36 +5280,36 @@
       </c>
       <c r="E79" s="21"/>
       <c r="F79" s="24">
-        <f t="shared" ref="F79:I79" si="79">IFERROR(SUM(K43,K54)/SUM($K43:$N43,$K54:$N54),0)</f>
+        <f t="shared" ref="F79:I79" si="83">IFERROR(SUM(K43,K54)/SUM($K43:$N43,$K54:$N54),0)</f>
         <v>0</v>
       </c>
       <c r="G79" s="24">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="H79" s="24">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="I79" s="24">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="J79" s="21"/>
       <c r="K79" s="25">
-        <f t="shared" si="70"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="L79" s="25">
-        <f t="shared" si="71"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="M79" s="25">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="N79" s="25">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
     </row>
@@ -5324,36 +5324,36 @@
       </c>
       <c r="E80" s="21"/>
       <c r="F80" s="24">
-        <f t="shared" ref="F80" si="80">IFERROR(SUM(K44,K55)/SUM($K44:$N44,$K55:$N55),0)</f>
+        <f t="shared" ref="F80" si="84">IFERROR(SUM(K44,K55)/SUM($K44:$N44,$K55:$N55),0)</f>
         <v>4.0056461731493118E-2</v>
       </c>
       <c r="G80" s="24">
-        <f t="shared" ref="G80" si="81">IFERROR(SUM(L44,L55)/SUM($K44:$N44,$K55:$N55),0)</f>
+        <f t="shared" ref="G80" si="85">IFERROR(SUM(L44,L55)/SUM($K44:$N44,$K55:$N55),0)</f>
         <v>0.95994353826850687</v>
       </c>
       <c r="H80" s="24">
-        <f t="shared" ref="H80" si="82">IFERROR(SUM(M44,M55)/SUM($K44:$N44,$K55:$N55),0)</f>
+        <f t="shared" ref="H80" si="86">IFERROR(SUM(M44,M55)/SUM($K44:$N44,$K55:$N55),0)</f>
         <v>0</v>
       </c>
       <c r="I80" s="24">
-        <f t="shared" ref="I80" si="83">IFERROR(SUM(N44,N55)/SUM($K44:$N44,$K55:$N55),0)</f>
+        <f t="shared" ref="I80" si="87">IFERROR(SUM(N44,N55)/SUM($K44:$N44,$K55:$N55),0)</f>
         <v>0</v>
       </c>
       <c r="J80" s="21"/>
       <c r="K80" s="25">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>1915.5000000000009</v>
       </c>
       <c r="L80" s="25">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>45904.5</v>
       </c>
       <c r="M80" s="25">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="N80" s="25">
-        <f t="shared" si="69"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
     </row>
@@ -8062,23 +8062,23 @@
       </c>
       <c r="N27" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!$D$62/12+N27</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q27" s="63">
         <f>$F27*Outputs_Internal!K$62/12+N27*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R27" s="63">
         <f>$F27*Outputs_Internal!L$62/12+N27*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S27" s="63">
         <f>N27*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T27" s="63">
         <f>$F27*Outputs_Internal!M$62/12</f>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="AE27" s="63">
         <f>'MARA Prices'!I$21*$G27</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF27" s="63">
         <f>'MARA Prices'!J$21*$G27</f>
@@ -8168,23 +8168,23 @@
       </c>
       <c r="N28" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!$D$62/12+N28</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q28" s="63">
         <f>$F28*Outputs_Internal!K$62/12+N28*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R28" s="63">
         <f>$F28*Outputs_Internal!L$62/12+N28*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S28" s="63">
         <f>N28*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T28" s="63">
         <f>$F28*Outputs_Internal!M$62/12</f>
@@ -8220,7 +8220,7 @@
       </c>
       <c r="AE28" s="63">
         <f>'MARA Prices'!I$21*$G28</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF28" s="63">
         <f>'MARA Prices'!J$21*$G28</f>
@@ -8274,23 +8274,23 @@
       </c>
       <c r="N29" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!$D$62/12+N29</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q29" s="63">
         <f>$F29*Outputs_Internal!K$62/12+N29*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R29" s="63">
         <f>$F29*Outputs_Internal!L$62/12+N29*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S29" s="63">
         <f>N29*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T29" s="63">
         <f>$F29*Outputs_Internal!M$62/12</f>
@@ -8302,15 +8302,15 @@
       </c>
       <c r="W29" s="63">
         <f t="shared" si="2"/>
-        <v>93052.634374999994</v>
+        <v>95552.634375000009</v>
       </c>
       <c r="X29" s="63">
         <f t="shared" si="3"/>
-        <v>21999.772948637776</v>
+        <v>22249.772948637772</v>
       </c>
       <c r="Y29" s="63">
         <f t="shared" si="4"/>
-        <v>61719.531398880899</v>
+        <v>61969.531398880907</v>
       </c>
       <c r="Z29" s="63">
         <f t="shared" si="5"/>
@@ -8318,7 +8318,7 @@
       </c>
       <c r="AA29" s="63">
         <f t="shared" si="6"/>
-        <v>8027.2803776810833</v>
+        <v>10027.280377681082</v>
       </c>
       <c r="AD29" s="63">
         <f>'MARA Prices'!H$21*$G29</f>
@@ -8326,7 +8326,7 @@
       </c>
       <c r="AE29" s="63">
         <f>'MARA Prices'!I$21*$G29</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF29" s="63">
         <f>'MARA Prices'!J$21*$G29</f>
@@ -8380,23 +8380,23 @@
       </c>
       <c r="N30" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!$D$62/12+N30</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q30" s="63">
         <f>$F30*Outputs_Internal!K$62/12+N30*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R30" s="63">
         <f>$F30*Outputs_Internal!L$62/12+N30*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S30" s="63">
         <f>N30*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T30" s="63">
         <f>$F30*Outputs_Internal!M$62/12</f>
@@ -8432,7 +8432,7 @@
       </c>
       <c r="AE30" s="63">
         <f>'MARA Prices'!I$21*$G30</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF30" s="63">
         <f>'MARA Prices'!J$21*$G30</f>
@@ -8486,23 +8486,23 @@
       </c>
       <c r="N31" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!$D$62/12+N31</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q31" s="63">
         <f>$F31*Outputs_Internal!K$62/12+N31*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R31" s="63">
         <f>$F31*Outputs_Internal!L$62/12+N31*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S31" s="63">
         <f>N31*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T31" s="63">
         <f>$F31*Outputs_Internal!M$62/12</f>
@@ -8538,7 +8538,7 @@
       </c>
       <c r="AE31" s="63">
         <f>'MARA Prices'!I$21*$G31</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF31" s="63">
         <f>'MARA Prices'!J$21*$G31</f>
@@ -8592,23 +8592,23 @@
       </c>
       <c r="N32" s="63">
         <f t="shared" si="0"/>
-        <v>3291.6666666666665</v>
+        <v>4125</v>
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!$D$62/12+N32</f>
-        <v>22580.044791666667</v>
+        <v>23413.378124999999</v>
       </c>
       <c r="Q32" s="63">
         <f>$F32*Outputs_Internal!K$62/12+N32*'MARA Prices'!$F$5</f>
-        <v>5814.5076495459252</v>
+        <v>5897.8409828792583</v>
       </c>
       <c r="R32" s="63">
         <f>$F32*Outputs_Internal!L$62/12+N32*'MARA Prices'!$F$6</f>
-        <v>13654.4271329603</v>
+        <v>13737.760466293634</v>
       </c>
       <c r="S32" s="63">
         <f>N32*'MARA Prices'!$F$4</f>
-        <v>2633.3333333333335</v>
+        <v>3300</v>
       </c>
       <c r="T32" s="63">
         <f>$F32*Outputs_Internal!M$62/12</f>
@@ -8620,15 +8620,15 @@
       </c>
       <c r="W32" s="63">
         <f t="shared" si="2"/>
-        <v>67740.134374999994</v>
+        <v>70240.134374999994</v>
       </c>
       <c r="X32" s="63">
         <f t="shared" si="3"/>
-        <v>17443.522948637776</v>
+        <v>17693.522948637776</v>
       </c>
       <c r="Y32" s="63">
         <f t="shared" si="4"/>
-        <v>40963.281398880899</v>
+        <v>41213.281398880899</v>
       </c>
       <c r="Z32" s="63">
         <f t="shared" si="5"/>
@@ -8636,7 +8636,7 @@
       </c>
       <c r="AA32" s="63">
         <f t="shared" si="6"/>
-        <v>8027.2803776810833</v>
+        <v>10027.280377681082</v>
       </c>
       <c r="AD32" s="63">
         <f>'MARA Prices'!H$21*$G32</f>
@@ -8644,7 +8644,7 @@
       </c>
       <c r="AE32" s="63">
         <f>'MARA Prices'!I$21*$G32</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="AF32" s="63">
         <f>'MARA Prices'!J$21*$G32</f>
@@ -8698,23 +8698,23 @@
       </c>
       <c r="N33" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!$D$62/12+N33</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q33" s="63">
         <f>$F33*Outputs_Internal!K$62/12+N33*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R33" s="63">
         <f>$F33*Outputs_Internal!L$62/12+N33*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S33" s="63">
         <f>N33*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T33" s="63">
         <f>$F33*Outputs_Internal!M$62/12</f>
@@ -8750,7 +8750,7 @@
       </c>
       <c r="AE33" s="63">
         <f>'MARA Prices'!I$21*$G33</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF33" s="63">
         <f>'MARA Prices'!J$21*$G33</f>
@@ -8804,23 +8804,23 @@
       </c>
       <c r="N34" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!$D$62/12+N34</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q34" s="63">
         <f>$F34*Outputs_Internal!K$62/12+N34*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R34" s="63">
         <f>$F34*Outputs_Internal!L$62/12+N34*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S34" s="63">
         <f>N34*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T34" s="63">
         <f>$F34*Outputs_Internal!M$62/12</f>
@@ -8856,7 +8856,7 @@
       </c>
       <c r="AE34" s="63">
         <f>'MARA Prices'!I$21*$G34</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF34" s="63">
         <f>'MARA Prices'!J$21*$G34</f>
@@ -8910,23 +8910,23 @@
       </c>
       <c r="N35" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!$D$62/12+N35</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q35" s="63">
         <f>$F35*Outputs_Internal!K$62/12+N35*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R35" s="63">
         <f>$F35*Outputs_Internal!L$62/12+N35*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S35" s="63">
         <f>N35*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T35" s="63">
         <f>$F35*Outputs_Internal!M$62/12</f>
@@ -8938,15 +8938,15 @@
       </c>
       <c r="W35" s="63">
         <f t="shared" si="2"/>
-        <v>68233.884374999994</v>
+        <v>70858.884374999994</v>
       </c>
       <c r="X35" s="63">
         <f t="shared" si="3"/>
-        <v>17492.897948637776</v>
+        <v>17755.397948637776</v>
       </c>
       <c r="Y35" s="63">
         <f t="shared" si="4"/>
-        <v>41012.656398880899</v>
+        <v>41275.156398880899</v>
       </c>
       <c r="Z35" s="63">
         <f t="shared" si="5"/>
@@ -8954,7 +8954,7 @@
       </c>
       <c r="AA35" s="63">
         <f t="shared" si="6"/>
-        <v>8422.2803776810815</v>
+        <v>10522.280377681082</v>
       </c>
       <c r="AD35" s="63">
         <f>'MARA Prices'!H$21*$G35</f>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="AE35" s="63">
         <f>'MARA Prices'!I$21*$G35</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF35" s="63">
         <f>'MARA Prices'!J$21*$G35</f>
@@ -9016,23 +9016,23 @@
       </c>
       <c r="N36" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!$D$62/12+N36</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q36" s="63">
         <f>$F36*Outputs_Internal!K$62/12+N36*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R36" s="63">
         <f>$F36*Outputs_Internal!L$62/12+N36*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S36" s="63">
         <f>N36*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T36" s="63">
         <f>$F36*Outputs_Internal!M$62/12</f>
@@ -9068,7 +9068,7 @@
       </c>
       <c r="AE36" s="63">
         <f>'MARA Prices'!I$21*$G36</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF36" s="63">
         <f>'MARA Prices'!J$21*$G36</f>
@@ -9122,23 +9122,23 @@
       </c>
       <c r="N37" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!$D$62/12+N37</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q37" s="63">
         <f>$F37*Outputs_Internal!K$62/12+N37*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R37" s="63">
         <f>$F37*Outputs_Internal!L$62/12+N37*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S37" s="63">
         <f>N37*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T37" s="63">
         <f>$F37*Outputs_Internal!M$62/12</f>
@@ -9174,7 +9174,7 @@
       </c>
       <c r="AE37" s="63">
         <f>'MARA Prices'!I$21*$G37</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF37" s="63">
         <f>'MARA Prices'!J$21*$G37</f>
@@ -9228,23 +9228,23 @@
       </c>
       <c r="N38" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!$D$62/12+N38</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q38" s="63">
         <f>$F38*Outputs_Internal!K$62/12+N38*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R38" s="63">
         <f>$F38*Outputs_Internal!L$62/12+N38*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S38" s="63">
         <f>N38*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T38" s="63">
         <f>$F38*Outputs_Internal!M$62/12</f>
@@ -9256,15 +9256,15 @@
       </c>
       <c r="W38" s="63">
         <f t="shared" si="7"/>
-        <v>68233.884374999994</v>
+        <v>70858.884374999994</v>
       </c>
       <c r="X38" s="63">
         <f t="shared" si="8"/>
-        <v>17492.897948637776</v>
+        <v>17755.397948637776</v>
       </c>
       <c r="Y38" s="63">
         <f t="shared" si="9"/>
-        <v>41012.656398880899</v>
+        <v>41275.156398880899</v>
       </c>
       <c r="Z38" s="63">
         <f t="shared" si="10"/>
@@ -9272,7 +9272,7 @@
       </c>
       <c r="AA38" s="63">
         <f t="shared" si="11"/>
-        <v>8422.2803776810815</v>
+        <v>10522.280377681082</v>
       </c>
       <c r="AD38" s="63">
         <f>'MARA Prices'!H$21*$G38</f>
@@ -9280,7 +9280,7 @@
       </c>
       <c r="AE38" s="63">
         <f>'MARA Prices'!I$21*$G38</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF38" s="63">
         <f>'MARA Prices'!J$21*$G38</f>
@@ -9334,23 +9334,23 @@
       </c>
       <c r="N39" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!$D$62/12+N39</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q39" s="63">
         <f>$F39*Outputs_Internal!K$62/12+N39*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R39" s="63">
         <f>$F39*Outputs_Internal!L$62/12+N39*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S39" s="63">
         <f>N39*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T39" s="63">
         <f>$F39*Outputs_Internal!M$62/12</f>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="AE39" s="63">
         <f>'MARA Prices'!I$21*$G39</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF39" s="63">
         <f>'MARA Prices'!J$21*$G39</f>
@@ -9440,23 +9440,23 @@
       </c>
       <c r="N40" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!$D$62/12+N40</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q40" s="63">
         <f>$F40*Outputs_Internal!K$62/12+N40*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R40" s="63">
         <f>$F40*Outputs_Internal!L$62/12+N40*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S40" s="63">
         <f>N40*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T40" s="63">
         <f>$F40*Outputs_Internal!M$62/12</f>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="AE40" s="63">
         <f>'MARA Prices'!I$21*$G40</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF40" s="63">
         <f>'MARA Prices'!J$21*$G40</f>
@@ -9546,23 +9546,23 @@
       </c>
       <c r="N41" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!$D$62/12+N41</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q41" s="63">
         <f>$F41*Outputs_Internal!K$62/12+N41*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R41" s="63">
         <f>$F41*Outputs_Internal!L$62/12+N41*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S41" s="63">
         <f>N41*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T41" s="63">
         <f>$F41*Outputs_Internal!M$62/12</f>
@@ -9574,15 +9574,15 @@
       </c>
       <c r="W41" s="63">
         <f t="shared" si="7"/>
-        <v>68233.884374999994</v>
+        <v>70858.884374999994</v>
       </c>
       <c r="X41" s="63">
         <f t="shared" si="8"/>
-        <v>17492.897948637776</v>
+        <v>17755.397948637776</v>
       </c>
       <c r="Y41" s="63">
         <f t="shared" si="9"/>
-        <v>41012.656398880899</v>
+        <v>41275.156398880899</v>
       </c>
       <c r="Z41" s="63">
         <f t="shared" si="10"/>
@@ -9590,7 +9590,7 @@
       </c>
       <c r="AA41" s="63">
         <f t="shared" si="11"/>
-        <v>8422.2803776810815</v>
+        <v>10522.280377681082</v>
       </c>
       <c r="AD41" s="63">
         <f>'MARA Prices'!H$21*$G41</f>
@@ -9598,7 +9598,7 @@
       </c>
       <c r="AE41" s="63">
         <f>'MARA Prices'!I$21*$G41</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF41" s="63">
         <f>'MARA Prices'!J$21*$G41</f>
@@ -9652,23 +9652,23 @@
       </c>
       <c r="N42" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!$D$62/12+N42</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q42" s="63">
         <f>$F42*Outputs_Internal!K$62/12+N42*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R42" s="63">
         <f>$F42*Outputs_Internal!L$62/12+N42*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S42" s="63">
         <f>N42*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T42" s="63">
         <f>$F42*Outputs_Internal!M$62/12</f>
@@ -9704,7 +9704,7 @@
       </c>
       <c r="AE42" s="63">
         <f>'MARA Prices'!I$21*$G42</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF42" s="63">
         <f>'MARA Prices'!J$21*$G42</f>
@@ -9758,23 +9758,23 @@
       </c>
       <c r="N43" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!$D$62/12+N43</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q43" s="63">
         <f>$F43*Outputs_Internal!K$62/12+N43*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R43" s="63">
         <f>$F43*Outputs_Internal!L$62/12+N43*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S43" s="63">
         <f>N43*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T43" s="63">
         <f>$F43*Outputs_Internal!M$62/12</f>
@@ -9810,7 +9810,7 @@
       </c>
       <c r="AE43" s="63">
         <f>'MARA Prices'!I$21*$G43</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF43" s="63">
         <f>'MARA Prices'!J$21*$G43</f>
@@ -9864,23 +9864,23 @@
       </c>
       <c r="N44" s="63">
         <f t="shared" si="0"/>
-        <v>3456.25</v>
+        <v>4331.25</v>
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!$D$62/12+N44</f>
-        <v>22744.628124999999</v>
+        <v>23619.628124999999</v>
       </c>
       <c r="Q44" s="63">
         <f>$F44*Outputs_Internal!K$62/12+N44*'MARA Prices'!$F$5</f>
-        <v>5830.9659828792583</v>
+        <v>5918.4659828792583</v>
       </c>
       <c r="R44" s="63">
         <f>$F44*Outputs_Internal!L$62/12+N44*'MARA Prices'!$F$6</f>
-        <v>13670.885466293634</v>
+        <v>13758.385466293634</v>
       </c>
       <c r="S44" s="63">
         <f>N44*'MARA Prices'!$F$4</f>
-        <v>2765</v>
+        <v>3465</v>
       </c>
       <c r="T44" s="63">
         <f>$F44*Outputs_Internal!M$62/12</f>
@@ -9892,15 +9892,15 @@
       </c>
       <c r="W44" s="63">
         <f t="shared" si="7"/>
-        <v>68233.884374999994</v>
+        <v>70858.884374999994</v>
       </c>
       <c r="X44" s="63">
         <f t="shared" si="8"/>
-        <v>17492.897948637776</v>
+        <v>17755.397948637776</v>
       </c>
       <c r="Y44" s="63">
         <f t="shared" si="9"/>
-        <v>41012.656398880899</v>
+        <v>41275.156398880899</v>
       </c>
       <c r="Z44" s="63">
         <f t="shared" si="10"/>
@@ -9908,7 +9908,7 @@
       </c>
       <c r="AA44" s="63">
         <f t="shared" si="11"/>
-        <v>8422.2803776810815</v>
+        <v>10522.280377681082</v>
       </c>
       <c r="AD44" s="63">
         <f>'MARA Prices'!H$21*$G44</f>
@@ -9916,7 +9916,7 @@
       </c>
       <c r="AE44" s="63">
         <f>'MARA Prices'!I$21*$G44</f>
-        <v>0</v>
+        <v>875.00000000000011</v>
       </c>
       <c r="AF44" s="63">
         <f>'MARA Prices'!J$21*$G44</f>
@@ -9970,23 +9970,23 @@
       </c>
       <c r="N45" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P45" s="63">
         <f>$F45*Outputs_Internal!$D$62/12+N45</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q45" s="63">
         <f>$F45*Outputs_Internal!K$62/12+N45*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R45" s="63">
         <f>$F45*Outputs_Internal!L$62/12+N45*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S45" s="63">
         <f>N45*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T45" s="63">
         <f>$F45*Outputs_Internal!M$62/12</f>
@@ -10022,7 +10022,7 @@
       </c>
       <c r="AE45" s="63">
         <f>'MARA Prices'!I$21*$G45</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF45" s="63">
         <f>'MARA Prices'!J$21*$G45</f>
@@ -10076,23 +10076,23 @@
       </c>
       <c r="N46" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P46" s="63">
         <f>$F46*Outputs_Internal!$D$62/12+N46</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q46" s="63">
         <f>$F46*Outputs_Internal!K$62/12+N46*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R46" s="63">
         <f>$F46*Outputs_Internal!L$62/12+N46*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S46" s="63">
         <f>N46*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T46" s="63">
         <f>$F46*Outputs_Internal!M$62/12</f>
@@ -10128,7 +10128,7 @@
       </c>
       <c r="AE46" s="63">
         <f>'MARA Prices'!I$21*$G46</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF46" s="63">
         <f>'MARA Prices'!J$21*$G46</f>
@@ -10182,23 +10182,23 @@
       </c>
       <c r="N47" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P47" s="63">
         <f>$F47*Outputs_Internal!$D$62/12+N47</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q47" s="63">
         <f>$F47*Outputs_Internal!K$62/12+N47*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R47" s="63">
         <f>$F47*Outputs_Internal!L$62/12+N47*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S47" s="63">
         <f>N47*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T47" s="63">
         <f>$F47*Outputs_Internal!M$62/12</f>
@@ -10210,15 +10210,15 @@
       </c>
       <c r="W47" s="63">
         <f t="shared" si="7"/>
-        <v>68752.321874999994</v>
+        <v>71508.571874999994</v>
       </c>
       <c r="X47" s="63">
         <f t="shared" si="8"/>
-        <v>17544.741698637776</v>
+        <v>17820.366698637776</v>
       </c>
       <c r="Y47" s="63">
         <f t="shared" si="9"/>
-        <v>41064.500148880899</v>
+        <v>41340.125148880899</v>
       </c>
       <c r="Z47" s="63">
         <f t="shared" si="10"/>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="AA47" s="63">
         <f t="shared" si="11"/>
-        <v>8837.0303776810815</v>
+        <v>11042.030377681082</v>
       </c>
       <c r="AD47" s="63">
         <f>'MARA Prices'!H$21*$G47</f>
@@ -10234,7 +10234,7 @@
       </c>
       <c r="AE47" s="63">
         <f>'MARA Prices'!I$21*$G47</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF47" s="63">
         <f>'MARA Prices'!J$21*$G47</f>
@@ -10288,23 +10288,23 @@
       </c>
       <c r="N48" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P48" s="63">
         <f>$F48*Outputs_Internal!$D$62/12+N48</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q48" s="63">
         <f>$F48*Outputs_Internal!K$62/12+N48*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R48" s="63">
         <f>$F48*Outputs_Internal!L$62/12+N48*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S48" s="63">
         <f>N48*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T48" s="63">
         <f>$F48*Outputs_Internal!M$62/12</f>
@@ -10340,7 +10340,7 @@
       </c>
       <c r="AE48" s="63">
         <f>'MARA Prices'!I$21*$G48</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF48" s="63">
         <f>'MARA Prices'!J$21*$G48</f>
@@ -10394,23 +10394,23 @@
       </c>
       <c r="N49" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P49" s="63">
         <f>$F49*Outputs_Internal!$D$62/12+N49</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q49" s="63">
         <f>$F49*Outputs_Internal!K$62/12+N49*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R49" s="63">
         <f>$F49*Outputs_Internal!L$62/12+N49*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S49" s="63">
         <f>N49*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T49" s="63">
         <f>$F49*Outputs_Internal!M$62/12</f>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="AE49" s="63">
         <f>'MARA Prices'!I$21*$G49</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF49" s="63">
         <f>'MARA Prices'!J$21*$G49</f>
@@ -10500,23 +10500,23 @@
       </c>
       <c r="N50" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P50" s="63">
         <f>$F50*Outputs_Internal!$D$62/12+N50</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q50" s="63">
         <f>$F50*Outputs_Internal!K$62/12+N50*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R50" s="63">
         <f>$F50*Outputs_Internal!L$62/12+N50*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S50" s="63">
         <f>N50*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T50" s="63">
         <f>$F50*Outputs_Internal!M$62/12</f>
@@ -10528,15 +10528,15 @@
       </c>
       <c r="W50" s="63">
         <f t="shared" si="7"/>
-        <v>68752.321874999994</v>
+        <v>71508.571874999994</v>
       </c>
       <c r="X50" s="63">
         <f t="shared" si="8"/>
-        <v>17544.741698637776</v>
+        <v>17820.366698637776</v>
       </c>
       <c r="Y50" s="63">
         <f t="shared" si="9"/>
-        <v>41064.500148880899</v>
+        <v>41340.125148880899</v>
       </c>
       <c r="Z50" s="63">
         <f t="shared" si="10"/>
@@ -10544,7 +10544,7 @@
       </c>
       <c r="AA50" s="63">
         <f t="shared" si="11"/>
-        <v>8837.0303776810815</v>
+        <v>11042.030377681082</v>
       </c>
       <c r="AD50" s="63">
         <f>'MARA Prices'!H$21*$G50</f>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="AE50" s="63">
         <f>'MARA Prices'!I$21*$G50</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF50" s="63">
         <f>'MARA Prices'!J$21*$G50</f>
@@ -10606,23 +10606,23 @@
       </c>
       <c r="N51" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P51" s="63">
         <f>$F51*Outputs_Internal!$D$62/12+N51</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q51" s="63">
         <f>$F51*Outputs_Internal!K$62/12+N51*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R51" s="63">
         <f>$F51*Outputs_Internal!L$62/12+N51*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S51" s="63">
         <f>N51*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T51" s="63">
         <f>$F51*Outputs_Internal!M$62/12</f>
@@ -10658,7 +10658,7 @@
       </c>
       <c r="AE51" s="63">
         <f>'MARA Prices'!I$21*$G51</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF51" s="63">
         <f>'MARA Prices'!J$21*$G51</f>
@@ -10712,23 +10712,23 @@
       </c>
       <c r="N52" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P52" s="63">
         <f>$F52*Outputs_Internal!$D$62/12+N52</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q52" s="63">
         <f>$F52*Outputs_Internal!K$62/12+N52*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R52" s="63">
         <f>$F52*Outputs_Internal!L$62/12+N52*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S52" s="63">
         <f>N52*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T52" s="63">
         <f>$F52*Outputs_Internal!M$62/12</f>
@@ -10764,7 +10764,7 @@
       </c>
       <c r="AE52" s="63">
         <f>'MARA Prices'!I$21*$G52</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF52" s="63">
         <f>'MARA Prices'!J$21*$G52</f>
@@ -10818,23 +10818,23 @@
       </c>
       <c r="N53" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P53" s="63">
         <f>$F53*Outputs_Internal!$D$62/12+N53</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q53" s="63">
         <f>$F53*Outputs_Internal!K$62/12+N53*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R53" s="63">
         <f>$F53*Outputs_Internal!L$62/12+N53*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S53" s="63">
         <f>N53*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T53" s="63">
         <f>$F53*Outputs_Internal!M$62/12</f>
@@ -10846,15 +10846,15 @@
       </c>
       <c r="W53" s="63">
         <f t="shared" si="7"/>
-        <v>68752.321874999994</v>
+        <v>71508.571874999994</v>
       </c>
       <c r="X53" s="63">
         <f t="shared" si="8"/>
-        <v>17544.741698637776</v>
+        <v>17820.366698637776</v>
       </c>
       <c r="Y53" s="63">
         <f t="shared" si="9"/>
-        <v>41064.500148880899</v>
+        <v>41340.125148880899</v>
       </c>
       <c r="Z53" s="63">
         <f t="shared" si="10"/>
@@ -10862,7 +10862,7 @@
       </c>
       <c r="AA53" s="63">
         <f t="shared" si="11"/>
-        <v>8837.0303776810815</v>
+        <v>11042.030377681082</v>
       </c>
       <c r="AD53" s="63">
         <f>'MARA Prices'!H$21*$G53</f>
@@ -10870,7 +10870,7 @@
       </c>
       <c r="AE53" s="63">
         <f>'MARA Prices'!I$21*$G53</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF53" s="63">
         <f>'MARA Prices'!J$21*$G53</f>
@@ -10924,23 +10924,23 @@
       </c>
       <c r="N54" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P54" s="63">
         <f>$F54*Outputs_Internal!$D$62/12+N54</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q54" s="63">
         <f>$F54*Outputs_Internal!K$62/12+N54*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R54" s="63">
         <f>$F54*Outputs_Internal!L$62/12+N54*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S54" s="63">
         <f>N54*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T54" s="63">
         <f>$F54*Outputs_Internal!M$62/12</f>
@@ -10976,7 +10976,7 @@
       </c>
       <c r="AE54" s="63">
         <f>'MARA Prices'!I$21*$G54</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF54" s="63">
         <f>'MARA Prices'!J$21*$G54</f>
@@ -11030,23 +11030,23 @@
       </c>
       <c r="N55" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P55" s="63">
         <f>$F55*Outputs_Internal!$D$62/12+N55</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q55" s="63">
         <f>$F55*Outputs_Internal!K$62/12+N55*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R55" s="63">
         <f>$F55*Outputs_Internal!L$62/12+N55*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S55" s="63">
         <f>N55*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T55" s="63">
         <f>$F55*Outputs_Internal!M$62/12</f>
@@ -11082,7 +11082,7 @@
       </c>
       <c r="AE55" s="63">
         <f>'MARA Prices'!I$21*$G55</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF55" s="63">
         <f>'MARA Prices'!J$21*$G55</f>
@@ -11136,23 +11136,23 @@
       </c>
       <c r="N56" s="63">
         <f t="shared" si="0"/>
-        <v>3629.0625</v>
+        <v>4547.8125</v>
       </c>
       <c r="P56" s="63">
         <f>$F56*Outputs_Internal!$D$62/12+N56</f>
-        <v>22917.440624999999</v>
+        <v>23836.190624999999</v>
       </c>
       <c r="Q56" s="63">
         <f>$F56*Outputs_Internal!K$62/12+N56*'MARA Prices'!$F$5</f>
-        <v>5848.2472328792583</v>
+        <v>5940.1222328792583</v>
       </c>
       <c r="R56" s="63">
         <f>$F56*Outputs_Internal!L$62/12+N56*'MARA Prices'!$F$6</f>
-        <v>13688.166716293634</v>
+        <v>13780.041716293634</v>
       </c>
       <c r="S56" s="63">
         <f>N56*'MARA Prices'!$F$4</f>
-        <v>2903.25</v>
+        <v>3638.25</v>
       </c>
       <c r="T56" s="63">
         <f>$F56*Outputs_Internal!M$62/12</f>
@@ -11164,15 +11164,15 @@
       </c>
       <c r="W56" s="63">
         <f t="shared" si="7"/>
-        <v>68752.321874999994</v>
+        <v>71508.571874999994</v>
       </c>
       <c r="X56" s="63">
         <f t="shared" si="8"/>
-        <v>17544.741698637776</v>
+        <v>17820.366698637776</v>
       </c>
       <c r="Y56" s="63">
         <f t="shared" si="9"/>
-        <v>41064.500148880899</v>
+        <v>41340.125148880899</v>
       </c>
       <c r="Z56" s="63">
         <f t="shared" si="10"/>
@@ -11180,7 +11180,7 @@
       </c>
       <c r="AA56" s="63">
         <f t="shared" si="11"/>
-        <v>8837.0303776810815</v>
+        <v>11042.030377681082</v>
       </c>
       <c r="AD56" s="63">
         <f>'MARA Prices'!H$21*$G56</f>
@@ -11188,7 +11188,7 @@
       </c>
       <c r="AE56" s="63">
         <f>'MARA Prices'!I$21*$G56</f>
-        <v>0</v>
+        <v>918.75000000000011</v>
       </c>
       <c r="AF56" s="63">
         <f>'MARA Prices'!J$21*$G56</f>
@@ -11242,23 +11242,23 @@
       </c>
       <c r="N57" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P57" s="63">
         <f>$F57*Outputs_Internal!$D$62/12+N57</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q57" s="63">
         <f>$F57*Outputs_Internal!K$62/12+N57*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R57" s="63">
         <f>$F57*Outputs_Internal!L$62/12+N57*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S57" s="63">
         <f>N57*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T57" s="63">
         <f>$F57*Outputs_Internal!M$62/12</f>
@@ -11294,7 +11294,7 @@
       </c>
       <c r="AE57" s="63">
         <f>'MARA Prices'!I$21*$G57</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF57" s="63">
         <f>'MARA Prices'!J$21*$G57</f>
@@ -11348,23 +11348,23 @@
       </c>
       <c r="N58" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P58" s="63">
         <f>$F58*Outputs_Internal!$D$62/12+N58</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q58" s="63">
         <f>$F58*Outputs_Internal!K$62/12+N58*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R58" s="63">
         <f>$F58*Outputs_Internal!L$62/12+N58*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S58" s="63">
         <f>N58*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T58" s="63">
         <f>$F58*Outputs_Internal!M$62/12</f>
@@ -11400,7 +11400,7 @@
       </c>
       <c r="AE58" s="63">
         <f>'MARA Prices'!I$21*$G58</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF58" s="63">
         <f>'MARA Prices'!J$21*$G58</f>
@@ -11454,23 +11454,23 @@
       </c>
       <c r="N59" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P59" s="63">
         <f>$F59*Outputs_Internal!$D$62/12+N59</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q59" s="63">
         <f>$F59*Outputs_Internal!K$62/12+N59*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R59" s="63">
         <f>$F59*Outputs_Internal!L$62/12+N59*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S59" s="63">
         <f>N59*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T59" s="63">
         <f>$F59*Outputs_Internal!M$62/12</f>
@@ -11482,15 +11482,15 @@
       </c>
       <c r="W59" s="63">
         <f t="shared" si="7"/>
-        <v>69296.681249999994</v>
+        <v>72190.743749999994</v>
       </c>
       <c r="X59" s="63">
         <f t="shared" si="8"/>
-        <v>17599.177636137774</v>
+        <v>17888.583886137774</v>
       </c>
       <c r="Y59" s="63">
         <f t="shared" si="9"/>
-        <v>41118.936086380905</v>
+        <v>41408.342336380905</v>
       </c>
       <c r="Z59" s="63">
         <f t="shared" si="10"/>
@@ -11498,7 +11498,7 @@
       </c>
       <c r="AA59" s="63">
         <f t="shared" si="11"/>
-        <v>9272.5178776810826</v>
+        <v>11587.767877681084</v>
       </c>
       <c r="AD59" s="63">
         <f>'MARA Prices'!H$21*$G59</f>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="AE59" s="63">
         <f>'MARA Prices'!I$21*$G59</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF59" s="63">
         <f>'MARA Prices'!J$21*$G59</f>
@@ -11560,23 +11560,23 @@
       </c>
       <c r="N60" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P60" s="63">
         <f>$F60*Outputs_Internal!$D$62/12+N60</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q60" s="63">
         <f>$F60*Outputs_Internal!K$62/12+N60*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R60" s="63">
         <f>$F60*Outputs_Internal!L$62/12+N60*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S60" s="63">
         <f>N60*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T60" s="63">
         <f>$F60*Outputs_Internal!M$62/12</f>
@@ -11612,7 +11612,7 @@
       </c>
       <c r="AE60" s="63">
         <f>'MARA Prices'!I$21*$G60</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF60" s="63">
         <f>'MARA Prices'!J$21*$G60</f>
@@ -11666,23 +11666,23 @@
       </c>
       <c r="N61" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P61" s="63">
         <f>$F61*Outputs_Internal!$D$62/12+N61</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q61" s="63">
         <f>$F61*Outputs_Internal!K$62/12+N61*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R61" s="63">
         <f>$F61*Outputs_Internal!L$62/12+N61*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S61" s="63">
         <f>N61*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T61" s="63">
         <f>$F61*Outputs_Internal!M$62/12</f>
@@ -11718,7 +11718,7 @@
       </c>
       <c r="AE61" s="63">
         <f>'MARA Prices'!I$21*$G61</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF61" s="63">
         <f>'MARA Prices'!J$21*$G61</f>
@@ -11772,23 +11772,23 @@
       </c>
       <c r="N62" s="63">
         <f t="shared" si="0"/>
-        <v>3810.5156250000005</v>
+        <v>4775.2031250000009</v>
       </c>
       <c r="P62" s="63">
         <f>$F62*Outputs_Internal!$D$62/12+N62</f>
-        <v>23098.893749999999</v>
+        <v>24063.581249999999</v>
       </c>
       <c r="Q62" s="63">
         <f>$F62*Outputs_Internal!K$62/12+N62*'MARA Prices'!$F$5</f>
-        <v>5866.3925453792581</v>
+        <v>5962.8612953792581</v>
       </c>
       <c r="R62" s="63">
         <f>$F62*Outputs_Internal!L$62/12+N62*'MARA Prices'!$F$6</f>
-        <v>13706.312028793634</v>
+        <v>13802.780778793634</v>
       </c>
       <c r="S62" s="63">
         <f>N62*'MARA Prices'!$F$4</f>
-        <v>3048.4125000000004</v>
+        <v>3820.1625000000008</v>
       </c>
       <c r="T62" s="63">
         <f>$F62*Outputs_Internal!M$62/12</f>
@@ -11800,15 +11800,15 @@
       </c>
       <c r="W62" s="63">
         <f t="shared" si="7"/>
-        <v>69296.681249999994</v>
+        <v>72190.743749999994</v>
       </c>
       <c r="X62" s="63">
         <f t="shared" si="8"/>
-        <v>17599.177636137774</v>
+        <v>17888.583886137774</v>
       </c>
       <c r="Y62" s="63">
         <f t="shared" si="9"/>
-        <v>41118.936086380905</v>
+        <v>41408.342336380905</v>
       </c>
       <c r="Z62" s="63">
         <f t="shared" si="10"/>
@@ -11816,7 +11816,7 @@
       </c>
       <c r="AA62" s="63">
         <f t="shared" si="11"/>
-        <v>9272.5178776810826</v>
+        <v>11587.767877681084</v>
       </c>
       <c r="AD62" s="63">
         <f>'MARA Prices'!H$21*$G62</f>
@@ -11824,7 +11824,7 @@
       </c>
       <c r="AE62" s="63">
         <f>'MARA Prices'!I$21*$G62</f>
-        <v>0</v>
+        <v>964.68750000000011</v>
       </c>
       <c r="AF62" s="63">
         <f>'MARA Prices'!J$21*$G62</f>
@@ -12557,7 +12557,7 @@
         <v>0</v>
       </c>
       <c r="AA69" s="63">
-        <f t="shared" ref="AA69:AA100" si="18">IF(MOD(MONTH($B69),3)=0,SUM(U67:U69,S67:S69),0)</f>
+        <f t="shared" ref="AA69" si="18">IF(MOD(MONTH($B69),3)=0,SUM(U67:U69,S67:S69),0)</f>
         <v>0</v>
       </c>
       <c r="AD69" s="63">
@@ -16971,23 +16971,23 @@
         <v>1.3000000000000002E-3</v>
       </c>
       <c r="K76" s="23">
-        <f>D65+D76+$J76</f>
+        <f t="shared" ref="K76:O81" si="6">D65+D76+$J76</f>
         <v>1.3000000000000002E-3</v>
       </c>
       <c r="L76" s="23">
-        <f>E65+E76+$J76</f>
+        <f t="shared" si="6"/>
         <v>35000.001300000004</v>
       </c>
       <c r="M76" s="23">
-        <f>F65+F76+$J76</f>
+        <f t="shared" si="6"/>
         <v>1.3000000000000002E-3</v>
       </c>
       <c r="N76" s="23">
-        <f>G65+G76+$J76</f>
+        <f t="shared" si="6"/>
         <v>1.3000000000000002E-3</v>
       </c>
       <c r="O76" s="23">
-        <f>H65+H76+$J76</f>
+        <f t="shared" si="6"/>
         <v>1.3000000000000002E-3</v>
       </c>
     </row>
@@ -17020,23 +17020,23 @@
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="K77" s="23">
-        <f>D66+D77+$J77</f>
+        <f t="shared" si="6"/>
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="L77" s="23">
-        <f>E66+E77+$J77</f>
+        <f t="shared" si="6"/>
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="M77" s="23">
-        <f>F66+F77+$J77</f>
+        <f t="shared" si="6"/>
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="N77" s="23">
-        <f>G66+G77+$J77</f>
+        <f t="shared" si="6"/>
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="O77" s="23">
-        <f>H66+H77+$J77</f>
+        <f t="shared" si="6"/>
         <v>1.4000000000000002E-3</v>
       </c>
     </row>
@@ -17069,23 +17069,23 @@
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="K78" s="23">
-        <f>D67+D78+$J78</f>
+        <f t="shared" si="6"/>
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="L78" s="23">
-        <f>E67+E78+$J78</f>
+        <f t="shared" si="6"/>
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="M78" s="23">
-        <f>F67+F78+$J78</f>
+        <f t="shared" si="6"/>
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="N78" s="23">
-        <f>G67+G78+$J78</f>
+        <f t="shared" si="6"/>
         <v>1.5000000000000002E-3</v>
       </c>
       <c r="O78" s="23">
-        <f>H67+H78+$J78</f>
+        <f t="shared" si="6"/>
         <v>1.5000000000000002E-3</v>
       </c>
     </row>
@@ -17118,23 +17118,23 @@
         <v>1.6000000000000003E-3</v>
       </c>
       <c r="K79" s="23">
-        <f>D68+D79+$J79</f>
+        <f t="shared" si="6"/>
         <v>1.6000000000000003E-3</v>
       </c>
       <c r="L79" s="23">
-        <f>E68+E79+$J79</f>
+        <f t="shared" si="6"/>
         <v>28000.0016</v>
       </c>
       <c r="M79" s="23">
-        <f>F68+F79+$J79</f>
+        <f t="shared" si="6"/>
         <v>44380.001600000003</v>
       </c>
       <c r="N79" s="23">
-        <f>G68+G79+$J79</f>
+        <f t="shared" si="6"/>
         <v>1.6000000000000003E-3</v>
       </c>
       <c r="O79" s="23">
-        <f>H68+H79+$J79</f>
+        <f t="shared" si="6"/>
         <v>1.6000000000000003E-3</v>
       </c>
     </row>
@@ -17167,23 +17167,23 @@
         <v>1.7000000000000003E-3</v>
       </c>
       <c r="K80" s="23">
-        <f>D69+D80+$J80</f>
+        <f t="shared" si="6"/>
         <v>1.7000000000000003E-3</v>
       </c>
       <c r="L80" s="23">
-        <f>E69+E80+$J80</f>
+        <f t="shared" si="6"/>
         <v>1.7000000000000003E-3</v>
       </c>
       <c r="M80" s="23">
-        <f>F69+F80+$J80</f>
+        <f t="shared" si="6"/>
         <v>1.7000000000000003E-3</v>
       </c>
       <c r="N80" s="23">
-        <f>G69+G80+$J80</f>
+        <f t="shared" si="6"/>
         <v>1.7000000000000003E-3</v>
       </c>
       <c r="O80" s="23">
-        <f>H69+H80+$J80</f>
+        <f t="shared" si="6"/>
         <v>1.7000000000000003E-3</v>
       </c>
     </row>
@@ -17216,23 +17216,23 @@
         <v>1.8000000000000004E-3</v>
       </c>
       <c r="K81" s="23">
-        <f>D70+D81+$J81</f>
+        <f t="shared" si="6"/>
         <v>1.8000000000000004E-3</v>
       </c>
       <c r="L81" s="23">
-        <f>E70+E81+$J81</f>
+        <f t="shared" si="6"/>
         <v>1.8000000000000004E-3</v>
       </c>
       <c r="M81" s="23">
-        <f>F70+F81+$J81</f>
+        <f t="shared" si="6"/>
         <v>47820.001799999998</v>
       </c>
       <c r="N81" s="23">
-        <f>G70+G81+$J81</f>
+        <f t="shared" si="6"/>
         <v>1.8000000000000004E-3</v>
       </c>
       <c r="O81" s="23">
-        <f>H70+H81+$J81</f>
+        <f t="shared" si="6"/>
         <v>1.8000000000000004E-3</v>
       </c>
     </row>
@@ -17257,19 +17257,19 @@
         <v>8500</v>
       </c>
       <c r="E84" s="18">
-        <f t="shared" ref="E84:H84" si="6">E62</f>
+        <f t="shared" ref="E84:H84" si="7">E62</f>
         <v>0</v>
       </c>
       <c r="F84" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G84" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H84" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K84" s="21">
@@ -17277,19 +17277,19 @@
         <v>1</v>
       </c>
       <c r="L84" s="21">
-        <f t="shared" ref="L84:O84" si="7">IF(COUNTIF(L$73:L$81,"")&gt;2,"",IFERROR(RANK(L73,L$73:L$81),8))</f>
+        <f t="shared" ref="L84:O84" si="8">IF(COUNTIF(L$73:L$81,"")&gt;2,"",IFERROR(RANK(L73,L$73:L$81),8))</f>
         <v>9</v>
       </c>
       <c r="M84" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="N84" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="O84" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -17318,23 +17318,23 @@
         <v>0</v>
       </c>
       <c r="K85" s="21">
-        <f t="shared" ref="K85:O85" si="8">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K74,K$73:K$81),8))</f>
+        <f t="shared" ref="K85:O85" si="9">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K74,K$73:K$81),8))</f>
         <v>9</v>
       </c>
       <c r="L85" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="M85" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N85" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="O85" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -17363,23 +17363,23 @@
         <v>0</v>
       </c>
       <c r="K86" s="21">
-        <f t="shared" ref="K86:O86" si="9">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K75,K$73:K$81),8))</f>
+        <f t="shared" ref="K86:O86" si="10">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K75,K$73:K$81),8))</f>
         <v>8</v>
       </c>
       <c r="L86" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="M86" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="N86" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="O86" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
     </row>
@@ -17408,23 +17408,23 @@
         <v>0</v>
       </c>
       <c r="K87" s="21">
-        <f t="shared" ref="K87:O87" si="10">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K76,K$73:K$81),8))</f>
+        <f t="shared" ref="K87:O87" si="11">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K76,K$73:K$81),8))</f>
         <v>7</v>
       </c>
       <c r="L87" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="M87" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="N87" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O87" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
     </row>
@@ -17453,23 +17453,23 @@
         <v>0</v>
       </c>
       <c r="K88" s="21">
-        <f t="shared" ref="K88:O88" si="11">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K77,K$73:K$81),8))</f>
+        <f t="shared" ref="K88:O88" si="12">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K77,K$73:K$81),8))</f>
         <v>6</v>
       </c>
       <c r="L88" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="M88" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="N88" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O88" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
     </row>
@@ -17482,39 +17482,39 @@
         <v>0</v>
       </c>
       <c r="E89" s="20">
-        <f t="shared" ref="E89:H89" si="12">E67</f>
+        <f t="shared" ref="E89:H89" si="13">E67</f>
         <v>0</v>
       </c>
       <c r="F89" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G89" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H89" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K89" s="21">
-        <f t="shared" ref="K89:O89" si="13">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K78,K$73:K$81),8))</f>
+        <f t="shared" ref="K89:O89" si="14">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K78,K$73:K$81),8))</f>
         <v>5</v>
       </c>
       <c r="L89" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="M89" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="N89" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="O89" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
     </row>
@@ -17543,23 +17543,23 @@
         <v>0</v>
       </c>
       <c r="K90" s="21">
-        <f t="shared" ref="K90:O90" si="14">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K79,K$73:K$81),8))</f>
+        <f t="shared" ref="K90:O90" si="15">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K79,K$73:K$81),8))</f>
         <v>4</v>
       </c>
       <c r="L90" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="M90" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="N90" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="O90" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
     </row>
@@ -17568,43 +17568,43 @@
         <v>98</v>
       </c>
       <c r="D91" s="20">
-        <f t="shared" ref="D91:H91" si="15">D69</f>
+        <f t="shared" ref="D91:H91" si="16">D69</f>
         <v>0</v>
       </c>
       <c r="E91" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F91" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G91" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H91" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K91" s="21">
-        <f t="shared" ref="K91:O91" si="16">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K80,K$73:K$81),8))</f>
+        <f t="shared" ref="K91:O91" si="17">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K80,K$73:K$81),8))</f>
         <v>3</v>
       </c>
       <c r="L91" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="M91" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="N91" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="O91" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
@@ -17613,43 +17613,43 @@
         <v>96</v>
       </c>
       <c r="D92" s="84">
-        <f t="shared" ref="D92:H92" si="17">D70</f>
+        <f t="shared" ref="D92:H92" si="18">D70</f>
         <v>0</v>
       </c>
       <c r="E92" s="84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F92" s="84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9600</v>
       </c>
       <c r="G92" s="84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H92" s="84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K92" s="21">
-        <f t="shared" ref="K92:O92" si="18">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K81,K$73:K$81),8))</f>
+        <f t="shared" ref="K92:O92" si="19">IF(COUNTIF(K$73:K$81,"")&gt;2,"",IFERROR(RANK(K81,K$73:K$81),8))</f>
         <v>2</v>
       </c>
       <c r="L92" s="21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="M92" s="21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="N92" s="21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="O92" s="21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -17783,23 +17783,23 @@
         <v>99</v>
       </c>
       <c r="D100" s="20">
-        <f t="shared" ref="D100:H100" si="19">D78</f>
+        <f t="shared" ref="D100:H100" si="20">D78</f>
         <v>0</v>
       </c>
       <c r="E100" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F100" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G100" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H100" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -17833,23 +17833,23 @@
         <v>98</v>
       </c>
       <c r="D102" s="20">
-        <f t="shared" ref="D102:H102" si="20">D80</f>
+        <f t="shared" ref="D102:H102" si="21">D80</f>
         <v>0</v>
       </c>
       <c r="E102" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F102" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G102" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H102" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -17858,23 +17858,23 @@
         <v>96</v>
       </c>
       <c r="D103" s="84">
-        <f t="shared" ref="D103:H103" si="21">D81</f>
+        <f t="shared" ref="D103:H103" si="22">D81</f>
         <v>0</v>
       </c>
       <c r="E103" s="84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F103" s="84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>38220</v>
       </c>
       <c r="G103" s="84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H103" s="84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -18088,19 +18088,19 @@
         <v>23500</v>
       </c>
       <c r="E114" s="7">
-        <f t="shared" ref="E114:H114" si="22">SUM(E38:E47, E50:E59, E62:E70, E73:E81, E106:E112)</f>
+        <f t="shared" ref="E114:H114" si="23">SUM(E38:E47, E50:E59, E62:E70, E73:E81, E106:E112)</f>
         <v>89900</v>
       </c>
       <c r="F114" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>170933</v>
       </c>
       <c r="G114" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H114" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -18116,19 +18116,19 @@
         <v>-11750</v>
       </c>
       <c r="E116" s="1">
-        <f t="shared" ref="E116:H116" si="23">IF(E126=1, 0, IF(E126=2, $E$129, IF(E126=3, $E$130, IF(E126=4, $E$131, IF(E126=5, $E$132, "")))))</f>
+        <f t="shared" ref="E116:H116" si="24">IF(E126=1, 0, IF(E126=2, $E$129, IF(E126=3, $E$130, IF(E126=4, $E$131, IF(E126=5, $E$132, "")))))</f>
         <v>-40455</v>
       </c>
       <c r="F116" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G116" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H116" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -18169,19 +18169,19 @@
         <v>8225</v>
       </c>
       <c r="E120" s="7">
-        <f t="shared" ref="E120:H120" si="24">SUM(E114, E116,E118)</f>
+        <f t="shared" ref="E120:H120" si="25">SUM(E114, E116,E118)</f>
         <v>49445</v>
       </c>
       <c r="F120" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>170933</v>
       </c>
       <c r="G120" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="H120" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -18195,19 +18195,19 @@
         <v>3</v>
       </c>
       <c r="E123" s="21">
-        <f t="shared" ref="E123:H123" si="25">IFERROR(_xlfn.RANK.EQ(E114,$D$114:$H$114),5)</f>
+        <f t="shared" ref="E123:H123" si="26">IFERROR(_xlfn.RANK.EQ(E114,$D$114:$H$114),5)</f>
         <v>2</v>
       </c>
       <c r="F123" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="G123" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="H123" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
     </row>
@@ -18236,19 +18236,19 @@
         <v>3.1</v>
       </c>
       <c r="E125" s="21">
-        <f t="shared" ref="E125:H125" si="26">SUM(E123:E124)</f>
+        <f t="shared" ref="E125:H125" si="27">SUM(E123:E124)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="F125" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.3</v>
       </c>
       <c r="G125" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="H125" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>4.5</v>
       </c>
     </row>
@@ -18259,19 +18259,19 @@
         <v>3</v>
       </c>
       <c r="E126" s="21">
-        <f t="shared" ref="E126:H126" si="27">_xlfn.RANK.EQ(E125, $D$125:$H$125, 5)</f>
+        <f t="shared" ref="E126:H126" si="28">_xlfn.RANK.EQ(E125, $D$125:$H$125, 5)</f>
         <v>2</v>
       </c>
       <c r="F126" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="G126" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="H126" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
     </row>
@@ -18337,7 +18337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19012,7 +19014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19498,7 +19502,7 @@
       </c>
       <c r="I20" s="106">
         <f>IF(Inputs!E$9 = "Y", SUM(I10:I16), 0)</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J20" s="106">
         <f>IF(Inputs!F$9 = "Y", SUM(J10:J16), 0)</f>
@@ -19525,7 +19529,7 @@
       </c>
       <c r="I21" s="106">
         <f>I20/12</f>
-        <v>0</v>
+        <v>833.33333333333337</v>
       </c>
       <c r="J21" s="106">
         <f>J20/12</f>

</xml_diff>

<commit_message>
Only apply knockouts for Medicare ACOs
Do this because there is not a current agreement for use of the HEDIS measures in commercial ACOI.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="157">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>Medicare ACO Quality Measures</t>
+  </si>
+  <si>
+    <t>Quality Measures</t>
+  </si>
+  <si>
+    <t>PRM Medicare ACO Assignment (CCLF Only)</t>
   </si>
 </sst>
 </file>
@@ -15347,7 +15353,7 @@
   <dimension ref="A2:O140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
@@ -15818,26 +15824,26 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D21="Y",Inputs!D$23="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!D$6="Y",0,IF(OR(Inputs!D21="Y",Inputs!D$23="Y"), Prices!$C16, 0))</f>
         <v>0</v>
       </c>
       <c r="E21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E21="Y",Inputs!E$23="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!E$6="Y",0,IF(OR(Inputs!E21="Y",Inputs!E$23="Y"), Prices!$C16, 0))</f>
         <v>0</v>
       </c>
       <c r="F21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F21="Y",Inputs!F$23="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!F$6="Y",0,IF(OR(Inputs!F21="Y",Inputs!F$23="Y"), Prices!$C16, 0))</f>
         <v>4200</v>
       </c>
       <c r="G21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G21="Y",Inputs!G$23="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!G$6="Y",0,IF(OR(Inputs!G21="Y",Inputs!G$23="Y"), Prices!$C16, 0))</f>
         <v>0</v>
       </c>
       <c r="H21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H21="Y",Inputs!H$23="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!H$6="Y",0,IF(OR(Inputs!H21="Y",Inputs!H$23="Y"), Prices!$C16, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -15893,7 +15899,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="19" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="D24" s="20">
         <f>IF(Inputs!D$6="N",0, IF(OR(Inputs!D21="Y",Inputs!D$24="Y",Inputs!D$25="Y"), Prices!$C19, 0))</f>
@@ -16098,7 +16104,7 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C34" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D34" s="18">
         <f>IF(OR(Inputs!D$6="Y", D$11 = 0), 0, IF(OR(Inputs!D21="Y",Inputs!D$23="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
@@ -16173,7 +16179,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="28" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="D37" s="29">
         <v>0</v>
@@ -16380,26 +16386,26 @@
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D47" s="18">
-        <f>IF(AND(Inputs!D21="Y",Inputs!D$23="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!D$6="Y",0,IF(AND(Inputs!D21="Y",Inputs!D$23="N"),Prices!$C16,0))</f>
         <v>0</v>
       </c>
       <c r="E47" s="18">
-        <f>IF(AND(Inputs!E21="Y",Inputs!E$23="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!E$6="Y",0,IF(AND(Inputs!E21="Y",Inputs!E$23="N"),Prices!$C16,0))</f>
         <v>0</v>
       </c>
       <c r="F47" s="18">
-        <f>IF(AND(Inputs!F21="Y",Inputs!F$23="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!F$6="Y",0,IF(AND(Inputs!F21="Y",Inputs!F$23="N"),Prices!$C16,0))</f>
         <v>0</v>
       </c>
       <c r="G47" s="18">
-        <f>IF(AND(Inputs!G21="Y",Inputs!G$23="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!G$6="Y",0,IF(AND(Inputs!G21="Y",Inputs!G$23="N"),Prices!$C16,0))</f>
         <v>0</v>
       </c>
       <c r="H47" s="18">
-        <f>IF(AND(Inputs!H21="Y",Inputs!H$23="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!H$6="Y",0,IF(AND(Inputs!H21="Y",Inputs!H$23="N"),Prices!$C16,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -16455,7 +16461,7 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C50" s="19" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="D50" s="20">
         <f>IF(Inputs!D$6="N",0,IF(AND(Inputs!D21="Y",Inputs!D$24="N",Inputs!D$25="N"),Prices!$C19,0))</f>
@@ -16660,7 +16666,7 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D60" s="18">
         <f>IF(OR(Inputs!D$6="Y", D$11 = 0), 0, IF(AND(Inputs!D21="Y",Inputs!D$23="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
@@ -16735,7 +16741,7 @@
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C63" s="28" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="D63" s="29">
         <v>0</v>
@@ -18528,7 +18534,7 @@
   <dimension ref="B2:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18853,7 +18859,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C16" s="44">
         <f>$L$28*3500</f>
@@ -18932,7 +18938,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="C19" s="45">
         <f>$L$28*1500</f>

</xml_diff>

<commit_message>
Update collaborative discount to reflect new splits
update the discount percent to 63% NY/37% PRM to reflect newly negotiated splits.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -1335,7 +1335,7 @@
         <v>58</v>
       </c>
       <c r="C1" s="70">
-        <v>43647</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
@@ -1409,7 +1409,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
@@ -1478,7 +1478,7 @@
         <v>97</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
@@ -1667,7 +1667,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="55" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E27" s="55"/>
       <c r="F27" s="55"/>
@@ -1691,7 +1691,7 @@
         <v>150</v>
       </c>
       <c r="D29" s="55" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E29" s="55"/>
       <c r="F29" s="55"/>
@@ -1742,10 +1742,10 @@
   <dimension ref="B2:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="D4" s="1">
         <f>MAX(Calcs!D4, 0)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="1">
         <f>MAX(Calcs!E4, 0)</f>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D70, Calcs!D81)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
         <f>SUM(Calcs!E70, Calcs!E81)</f>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="D25" s="1">
         <f>SUM(Calcs!D72, Calcs!D83)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <f>SUM(Calcs!E72, Calcs!E83)</f>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="D27" s="1">
         <f>SUM(Calcs!D74, Calcs!D85)</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
         <f>SUM(Calcs!E74, Calcs!E85)</f>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="D30" s="1">
         <f>SUM(Calcs!D110:D114)</f>
-        <v>-24825</v>
+        <v>-2550</v>
       </c>
       <c r="E30" s="1">
         <f>SUM(Calcs!E110:E114)</f>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="D32" s="1">
         <f>Calcs!D122</f>
-        <v>-3525</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D34" s="7">
         <f>SUM(D7:D16, D19:D27, D30:D32)</f>
-        <v>94550</v>
+        <v>55950</v>
       </c>
       <c r="E34" s="7">
         <f>SUM(E7:E16, E19:E27, E30:E31)</f>
@@ -2682,7 +2682,7 @@
     <row r="37" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C37" s="64">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.35">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D43" s="7">
         <f>(D34/12*Inputs!$C$2+D4)*$C$37+D41</f>
-        <v>287195.625</v>
+        <v>172850</v>
       </c>
       <c r="E43" s="7">
         <f>(E34/12*Inputs!$C$2+E4)*$C$37+E41</f>
@@ -2803,13 +2803,13 @@
     <row r="47" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>287195.625</v>
+        <v>172850</v>
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C48" s="52">
         <f>SUM(D43:H43)</f>
-        <v>287195.625</v>
+        <v>172850</v>
       </c>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -2845,7 +2845,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$7:$H$7, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="73">
@@ -2933,11 +2933,11 @@
       </c>
       <c r="K4" s="12">
         <f t="shared" ref="K4:N5" si="0">F4*$D4</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L4" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="M4" s="12">
         <f t="shared" si="0"/>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="D42" s="20">
         <f>SUM(Calcs!D92:H92)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F42" s="33">
         <v>0.1</v>
@@ -4147,11 +4147,11 @@
       </c>
       <c r="K42" s="20">
         <f t="shared" ref="K42" si="30">F42*$D42</f>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="L42" s="20">
         <f t="shared" ref="L42" si="31">G42*$D42</f>
-        <v>25200</v>
+        <v>0</v>
       </c>
       <c r="M42" s="20">
         <f t="shared" ref="M42" si="32">H42*$D42</f>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="D44" s="20">
         <f>SUM(Calcs!D94:H94)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F44" s="33">
         <v>0.1</v>
@@ -4223,11 +4223,11 @@
       </c>
       <c r="K44" s="20">
         <f t="shared" ref="K44" si="40">F44*$D44</f>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="L44" s="20">
         <f t="shared" ref="L44" si="41">G44*$D44</f>
-        <v>25200</v>
+        <v>0</v>
       </c>
       <c r="M44" s="20">
         <f t="shared" ref="M44" si="42">H44*$D44</f>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="D46" s="84">
         <f>SUM(Calcs!D96:H96)</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="F46" s="85">
         <v>0.1</v>
@@ -4299,11 +4299,11 @@
       </c>
       <c r="K46" s="84">
         <f t="shared" si="23"/>
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="L46" s="84">
         <f t="shared" si="23"/>
-        <v>7560</v>
+        <v>0</v>
       </c>
       <c r="M46" s="84">
         <f t="shared" si="23"/>
@@ -4710,15 +4710,15 @@
       </c>
       <c r="D60" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>-24825</v>
+        <v>-2550</v>
       </c>
       <c r="F60" s="8">
         <f>IFERROR(SUM(K74:K82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.16302131603336423</v>
+        <v>0.25632183908045975</v>
       </c>
       <c r="G60" s="8">
         <f t="shared" ref="G60:I60" si="72">IFERROR(SUM(L74:L82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.83697868396663577</v>
+        <v>0.7436781609195402</v>
       </c>
       <c r="H60" s="8">
         <f t="shared" si="72"/>
@@ -4730,11 +4730,11 @@
       </c>
       <c r="K60" s="12">
         <f>F60*$D$60</f>
-        <v>-4047.004170528267</v>
+        <v>-653.62068965517233</v>
       </c>
       <c r="L60" s="12">
         <f>G60*$D$60</f>
-        <v>-20777.995829471733</v>
+        <v>-1896.3793103448274</v>
       </c>
       <c r="M60" s="12">
         <f>H60*$D$60</f>
@@ -4755,11 +4755,11 @@
       </c>
       <c r="F61" s="3">
         <f>IFERROR(SUM(K10:K60)/SUM($K10:$N60), 0)</f>
-        <v>0.21073663858752723</v>
+        <v>0.31494869187390218</v>
       </c>
       <c r="G61" s="3">
         <f>IFERROR(SUM(L10:L60)/SUM($K10:$N60), 0)</f>
-        <v>0.78926336141247277</v>
+        <v>0.68505130812609782</v>
       </c>
       <c r="H61" s="3">
         <f>IFERROR(SUM(M10:M60)/SUM($K10:$N60), 0)</f>
@@ -4792,14 +4792,13 @@
       </c>
       <c r="D62" s="1">
         <f>Outputs_External!D32</f>
-        <v>-3525</v>
+        <v>0</v>
       </c>
       <c r="F62" s="3">
-        <v>0.58085106382978724</v>
+        <v>0.63</v>
       </c>
       <c r="G62" s="3">
-        <f>1-F62</f>
-        <v>0.41914893617021276</v>
+        <v>0.37</v>
       </c>
       <c r="H62" s="3">
         <v>0</v>
@@ -4809,11 +4808,11 @@
       </c>
       <c r="K62" s="12">
         <f>$D$62*F62</f>
-        <v>-2047.5</v>
+        <v>0</v>
       </c>
       <c r="L62" s="12">
         <f t="shared" ref="L62:N62" si="73">$D$62*G62</f>
-        <v>-1477.5</v>
+        <v>0</v>
       </c>
       <c r="M62" s="12">
         <f t="shared" si="73"/>
@@ -4835,15 +4834,15 @@
       </c>
       <c r="D64" s="1">
         <f>SUM(Outputs_External!D34:'Outputs_External'!H34)</f>
-        <v>94550</v>
+        <v>55950</v>
       </c>
       <c r="K64" s="12">
         <f>SUM(K60:K62, K38:K46, K10:K20,K25:K35,K49:K57)</f>
-        <v>18620.495829471733</v>
+        <v>17621.37931034483</v>
       </c>
       <c r="L64" s="12">
         <f>SUM(L60:L62, L38:L46, L10:L20,L25:L35,L49:L57)</f>
-        <v>75929.504170528264</v>
+        <v>38328.620689655174</v>
       </c>
       <c r="M64" s="12">
         <f>SUM(M60:M62, M38:M46, M10:M20,M25:M35,M49:M57)</f>
@@ -4860,7 +4859,7 @@
       </c>
       <c r="D65" s="23">
         <f>SUM(K64:N64)</f>
-        <v>94550</v>
+        <v>55950</v>
       </c>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
@@ -4925,15 +4924,15 @@
       </c>
       <c r="D69" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>287195.625</v>
+        <v>172850</v>
       </c>
       <c r="K69" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>56559.756082020373</v>
+        <v>55364.1379310345</v>
       </c>
       <c r="L69" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>230635.86891797962</v>
+        <v>117485.86206896555</v>
       </c>
       <c r="M69" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -4948,11 +4947,11 @@
       <c r="D70" s="1"/>
       <c r="K70" s="53">
         <f>IFERROR(K69/$D$69, 0)</f>
-        <v>0.1969380838653805</v>
+        <v>0.32030163685874746</v>
       </c>
       <c r="L70" s="53">
         <f>IFERROR(L69/$D$69, 0)</f>
-        <v>0.80306191613461941</v>
+        <v>0.67969836314125287</v>
       </c>
       <c r="M70" s="53">
         <f>IFERROR(M69/$D$69, 0)</f>
@@ -5167,16 +5166,16 @@
       </c>
       <c r="D78" s="23">
         <f>SUM(Calcs!D70:H70)+SUM(Calcs!D81:H81)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E78" s="21"/>
       <c r="F78" s="24">
         <f t="shared" ref="F78:I79" si="79">IFERROR(SUM(K42,K53)/SUM($K42:$N42,$K53:$N53),0)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="24">
         <f t="shared" si="79"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="H78" s="24">
         <f t="shared" si="79"/>
@@ -5189,11 +5188,11 @@
       <c r="J78" s="21"/>
       <c r="K78" s="25">
         <f t="shared" ref="K78:K82" si="80">F78*$D78</f>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="L78" s="25">
         <f t="shared" ref="L78:L82" si="81">G78*$D78</f>
-        <v>25200</v>
+        <v>0</v>
       </c>
       <c r="M78" s="25">
         <f t="shared" ref="M78:M82" si="82">H78*$D78</f>
@@ -5255,7 +5254,7 @@
       </c>
       <c r="D80" s="23">
         <f>SUM(Calcs!D72:H72)+SUM(Calcs!D83:H83)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E80" s="21"/>
       <c r="F80" s="24">
@@ -5277,11 +5276,11 @@
       <c r="J80" s="21"/>
       <c r="K80" s="25">
         <f t="shared" ref="K80" si="88">F80*$D80</f>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="L80" s="25">
         <f t="shared" ref="L80" si="89">G80*$D80</f>
-        <v>25200</v>
+        <v>0</v>
       </c>
       <c r="M80" s="25">
         <f t="shared" ref="M80" si="90">H80*$D80</f>
@@ -5343,16 +5342,16 @@
       </c>
       <c r="D82" s="23">
         <f>SUM(Calcs!D74:H74)+SUM(Calcs!D85:H85)</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="E82" s="21"/>
       <c r="F82" s="24">
         <f t="shared" ref="F82" si="93">IFERROR(SUM(K46,K57)/SUM($K46:$N46,$K57:$N57),0)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="24">
         <f t="shared" ref="G82" si="94">IFERROR(SUM(L46,L57)/SUM($K46:$N46,$K57:$N57),0)</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="H82" s="24">
         <f t="shared" ref="H82" si="95">IFERROR(SUM(M46,M57)/SUM($K46:$N46,$K57:$N57),0)</f>
@@ -5365,11 +5364,11 @@
       <c r="J82" s="21"/>
       <c r="K82" s="25">
         <f t="shared" si="80"/>
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="L82" s="25">
         <f t="shared" si="81"/>
-        <v>7560</v>
+        <v>0</v>
       </c>
       <c r="M82" s="25">
         <f t="shared" si="82"/>
@@ -6153,23 +6152,23 @@
       </c>
       <c r="F9" s="64">
         <f>IF(AND(B9&gt;=Inputs!$C$1,B9&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E9,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="64">
         <f>IF(AND(B9&gt;=Inputs!$C$1,B9&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B9,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D9</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="J9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!K$4, Outputs_Internal!K$5),0)*$D9</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!L$4, Outputs_Internal!L$5),0)*$D9</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!M$4, Outputs_Internal!$M$5),0)*$D9</f>
@@ -6181,15 +6180,15 @@
       </c>
       <c r="P9" s="63">
         <f>$F9*Outputs_Internal!$D$64/12+N9</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q9" s="63">
         <f>$F9*Outputs_Internal!K$64/12+N9*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R9" s="63">
         <f>$F9*Outputs_Internal!L$64/12+N9*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S9" s="63">
         <f>N9*'MARA Prices'!$F$4</f>
@@ -6259,11 +6258,11 @@
       </c>
       <c r="F10" s="64">
         <f>IF(AND(B10&gt;=Inputs!$C$1,B10&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E10,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="64">
         <f>IF(AND(B10&gt;=Inputs!$C$1,B10&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B10,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="63">
         <f>IF($B10=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D10</f>
@@ -6287,15 +6286,15 @@
       </c>
       <c r="P10" s="63">
         <f>$F10*Outputs_Internal!$D$64/12+N10</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q10" s="63">
         <f>$F10*Outputs_Internal!K$64/12+N10*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R10" s="63">
         <f>$F10*Outputs_Internal!L$64/12+N10*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S10" s="63">
         <f>N10*'MARA Prices'!$F$4</f>
@@ -6365,11 +6364,11 @@
       </c>
       <c r="F11" s="64">
         <f>IF(AND(B11&gt;=Inputs!$C$1,B11&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E11,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="64">
         <f>IF(AND(B11&gt;=Inputs!$C$1,B11&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B11,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="63">
         <f>IF($B11=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D11</f>
@@ -6393,15 +6392,15 @@
       </c>
       <c r="P11" s="63">
         <f>$F11*Outputs_Internal!$D$64/12+N11</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q11" s="63">
         <f>$F11*Outputs_Internal!K$64/12+N11*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R11" s="63">
         <f>$F11*Outputs_Internal!L$64/12+N11*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S11" s="63">
         <f>N11*'MARA Prices'!$F$4</f>
@@ -6417,15 +6416,15 @@
       </c>
       <c r="W11" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18987.5</v>
       </c>
       <c r="X11" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6905.3448275862065</v>
       </c>
       <c r="Y11" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>12082.155172413793</v>
       </c>
       <c r="Z11" s="63">
         <f t="shared" si="5"/>
@@ -6471,11 +6470,11 @@
       </c>
       <c r="F12" s="64">
         <f>IF(AND(B12&gt;=Inputs!$C$1,B12&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E12,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="64">
         <f>IF(AND(B12&gt;=Inputs!$C$1,B12&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B12,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="63">
         <f>IF($B12=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D12</f>
@@ -6499,15 +6498,15 @@
       </c>
       <c r="P12" s="63">
         <f>$F12*Outputs_Internal!$D$64/12+N12</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q12" s="63">
         <f>$F12*Outputs_Internal!K$64/12+N12*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R12" s="63">
         <f>$F12*Outputs_Internal!L$64/12+N12*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S12" s="63">
         <f>N12*'MARA Prices'!$F$4</f>
@@ -6577,11 +6576,11 @@
       </c>
       <c r="F13" s="64">
         <f>IF(AND(B13&gt;=Inputs!$C$1,B13&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E13,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="64">
         <f>IF(AND(B13&gt;=Inputs!$C$1,B13&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B13,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="63">
         <f>IF($B13=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D13</f>
@@ -6605,15 +6604,15 @@
       </c>
       <c r="P13" s="63">
         <f>$F13*Outputs_Internal!$D$64/12+N13</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q13" s="63">
         <f>$F13*Outputs_Internal!K$64/12+N13*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R13" s="63">
         <f>$F13*Outputs_Internal!L$64/12+N13*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S13" s="63">
         <f>N13*'MARA Prices'!$F$4</f>
@@ -6683,11 +6682,11 @@
       </c>
       <c r="F14" s="64">
         <f>IF(AND(B14&gt;=Inputs!$C$1,B14&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E14,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="64">
         <f>IF(AND(B14&gt;=Inputs!$C$1,B14&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B14,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="63">
         <f>IF($B14=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D14</f>
@@ -6711,15 +6710,15 @@
       </c>
       <c r="P14" s="63">
         <f>$F14*Outputs_Internal!$D$64/12+N14</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q14" s="63">
         <f>$F14*Outputs_Internal!K$64/12+N14*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R14" s="63">
         <f>$F14*Outputs_Internal!L$64/12+N14*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S14" s="63">
         <f>N14*'MARA Prices'!$F$4</f>
@@ -6735,15 +6734,15 @@
       </c>
       <c r="W14" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13987.5</v>
       </c>
       <c r="X14" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y14" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z14" s="63">
         <f t="shared" si="5"/>
@@ -6789,11 +6788,11 @@
       </c>
       <c r="F15" s="64">
         <f>IF(AND(B15&gt;=Inputs!$C$1,B15&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E15,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="64">
         <f>IF(AND(B15&gt;=Inputs!$C$1,B15&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B15,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="63">
         <f>IF($B15=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D15</f>
@@ -6817,15 +6816,15 @@
       </c>
       <c r="P15" s="63">
         <f>$F15*Outputs_Internal!$D$64/12+N15</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q15" s="63">
         <f>$F15*Outputs_Internal!K$64/12+N15*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R15" s="63">
         <f>$F15*Outputs_Internal!L$64/12+N15*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S15" s="63">
         <f>N15*'MARA Prices'!$F$4</f>
@@ -6895,11 +6894,11 @@
       </c>
       <c r="F16" s="64">
         <f>IF(AND(B16&gt;=Inputs!$C$1,B16&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E16,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="64">
         <f>IF(AND(B16&gt;=Inputs!$C$1,B16&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B16,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="63">
         <f>IF($B16=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D16</f>
@@ -6923,15 +6922,15 @@
       </c>
       <c r="P16" s="63">
         <f>$F16*Outputs_Internal!$D$64/12+N16</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q16" s="63">
         <f>$F16*Outputs_Internal!K$64/12+N16*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R16" s="63">
         <f>$F16*Outputs_Internal!L$64/12+N16*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S16" s="63">
         <f>N16*'MARA Prices'!$F$4</f>
@@ -7001,11 +7000,11 @@
       </c>
       <c r="F17" s="64">
         <f>IF(AND(B17&gt;=Inputs!$C$1,B17&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E17,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="64">
         <f>IF(AND(B17&gt;=Inputs!$C$1,B17&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B17,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="63">
         <f>IF($B17=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D17</f>
@@ -7029,15 +7028,15 @@
       </c>
       <c r="P17" s="63">
         <f>$F17*Outputs_Internal!$D$64/12+N17</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q17" s="63">
         <f>$F17*Outputs_Internal!K$64/12+N17*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R17" s="63">
         <f>$F17*Outputs_Internal!L$64/12+N17*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S17" s="63">
         <f>N17*'MARA Prices'!$F$4</f>
@@ -7053,15 +7052,15 @@
       </c>
       <c r="W17" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13987.5</v>
       </c>
       <c r="X17" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y17" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z17" s="63">
         <f t="shared" si="5"/>
@@ -7107,11 +7106,11 @@
       </c>
       <c r="F18" s="64">
         <f>IF(AND(B18&gt;=Inputs!$C$1,B18&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E18,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="64">
         <f>IF(AND(B18&gt;=Inputs!$C$1,B18&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B18,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="63">
         <f>IF($B18=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D18</f>
@@ -7135,15 +7134,15 @@
       </c>
       <c r="P18" s="63">
         <f>$F18*Outputs_Internal!$D$64/12+N18</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q18" s="63">
         <f>$F18*Outputs_Internal!K$64/12+N18*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R18" s="63">
         <f>$F18*Outputs_Internal!L$64/12+N18*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S18" s="63">
         <f>N18*'MARA Prices'!$F$4</f>
@@ -7213,11 +7212,11 @@
       </c>
       <c r="F19" s="64">
         <f>IF(AND(B19&gt;=Inputs!$C$1,B19&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E19,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="64">
         <f>IF(AND(B19&gt;=Inputs!$C$1,B19&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B19,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="63">
         <f>IF($B19=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D19</f>
@@ -7241,15 +7240,15 @@
       </c>
       <c r="P19" s="63">
         <f>$F19*Outputs_Internal!$D$64/12+N19</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q19" s="63">
         <f>$F19*Outputs_Internal!K$64/12+N19*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R19" s="63">
         <f>$F19*Outputs_Internal!L$64/12+N19*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S19" s="63">
         <f>N19*'MARA Prices'!$F$4</f>
@@ -7319,11 +7318,11 @@
       </c>
       <c r="F20" s="64">
         <f>IF(AND(B20&gt;=Inputs!$C$1,B20&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E20,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="64">
         <f>IF(AND(B20&gt;=Inputs!$C$1,B20&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B20,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="63">
         <f>IF($B20=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D20</f>
@@ -7347,15 +7346,15 @@
       </c>
       <c r="P20" s="63">
         <f>$F20*Outputs_Internal!$D$64/12+N20</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q20" s="63">
         <f>$F20*Outputs_Internal!K$64/12+N20*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R20" s="63">
         <f>$F20*Outputs_Internal!L$64/12+N20*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S20" s="63">
         <f>N20*'MARA Prices'!$F$4</f>
@@ -7371,15 +7370,15 @@
       </c>
       <c r="W20" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13987.5</v>
       </c>
       <c r="X20" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y20" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z20" s="63">
         <f t="shared" si="5"/>
@@ -7425,11 +7424,11 @@
       </c>
       <c r="F21" s="64">
         <f>IF(AND(B21&gt;=Inputs!$C$1,B21&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E21,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="64">
         <f>IF(AND(B21&gt;=Inputs!$C$1,B21&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B21,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="63">
         <f>IF($B21=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D21</f>
@@ -7453,15 +7452,15 @@
       </c>
       <c r="P21" s="63">
         <f>$F21*Outputs_Internal!$D$64/12+N21</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q21" s="63">
         <f>$F21*Outputs_Internal!K$64/12+N21*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R21" s="63">
         <f>$F21*Outputs_Internal!L$64/12+N21*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S21" s="63">
         <f>N21*'MARA Prices'!$F$4</f>
@@ -7531,11 +7530,11 @@
       </c>
       <c r="F22" s="64">
         <f>IF(AND(B22&gt;=Inputs!$C$1,B22&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E22,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="64">
         <f>IF(AND(B22&gt;=Inputs!$C$1,B22&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B22,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="63">
         <f>IF($B22=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D22</f>
@@ -7559,15 +7558,15 @@
       </c>
       <c r="P22" s="63">
         <f>$F22*Outputs_Internal!$D$64/12+N22</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q22" s="63">
         <f>$F22*Outputs_Internal!K$64/12+N22*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R22" s="63">
         <f>$F22*Outputs_Internal!L$64/12+N22*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S22" s="63">
         <f>N22*'MARA Prices'!$F$4</f>
@@ -7637,11 +7636,11 @@
       </c>
       <c r="F23" s="64">
         <f>IF(AND(B23&gt;=Inputs!$C$1,B23&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E23,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="64">
         <f>IF(AND(B23&gt;=Inputs!$C$1,B23&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B23,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="63">
         <f>IF($B23=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D23</f>
@@ -7665,15 +7664,15 @@
       </c>
       <c r="P23" s="63">
         <f>$F23*Outputs_Internal!$D$64/12+N23</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q23" s="63">
         <f>$F23*Outputs_Internal!K$64/12+N23*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R23" s="63">
         <f>$F23*Outputs_Internal!L$64/12+N23*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S23" s="63">
         <f>N23*'MARA Prices'!$F$4</f>
@@ -7689,15 +7688,15 @@
       </c>
       <c r="W23" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13987.5</v>
       </c>
       <c r="X23" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y23" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z23" s="63">
         <f t="shared" si="5"/>
@@ -7743,11 +7742,11 @@
       </c>
       <c r="F24" s="64">
         <f>IF(AND(B24&gt;=Inputs!$C$1,B24&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E24,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="64">
         <f>IF(AND(B24&gt;=Inputs!$C$1,B24&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B24,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="63">
         <f>IF($B24=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D24</f>
@@ -7771,15 +7770,15 @@
       </c>
       <c r="P24" s="63">
         <f>$F24*Outputs_Internal!$D$64/12+N24</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q24" s="63">
         <f>$F24*Outputs_Internal!K$64/12+N24*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R24" s="63">
         <f>$F24*Outputs_Internal!L$64/12+N24*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S24" s="63">
         <f>N24*'MARA Prices'!$F$4</f>
@@ -7849,11 +7848,11 @@
       </c>
       <c r="F25" s="64">
         <f>IF(AND(B25&gt;=Inputs!$C$1,B25&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E25,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="64">
         <f>IF(AND(B25&gt;=Inputs!$C$1,B25&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B25,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="63">
         <f>IF($B25=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D25</f>
@@ -7877,15 +7876,15 @@
       </c>
       <c r="P25" s="63">
         <f>$F25*Outputs_Internal!$D$64/12+N25</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q25" s="63">
         <f>$F25*Outputs_Internal!K$64/12+N25*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R25" s="63">
         <f>$F25*Outputs_Internal!L$64/12+N25*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S25" s="63">
         <f>N25*'MARA Prices'!$F$4</f>
@@ -7955,11 +7954,11 @@
       </c>
       <c r="F26" s="64">
         <f>IF(AND(B26&gt;=Inputs!$C$1,B26&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E26,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="64">
         <f>IF(AND(B26&gt;=Inputs!$C$1,B26&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B26,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="63">
         <f>IF($B26=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D26</f>
@@ -7983,15 +7982,15 @@
       </c>
       <c r="P26" s="63">
         <f>$F26*Outputs_Internal!$D$64/12+N26</f>
-        <v>0</v>
+        <v>4662.5</v>
       </c>
       <c r="Q26" s="63">
         <f>$F26*Outputs_Internal!K$64/12+N26*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R26" s="63">
         <f>$F26*Outputs_Internal!L$64/12+N26*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S26" s="63">
         <f>N26*'MARA Prices'!$F$4</f>
@@ -8007,15 +8006,15 @@
       </c>
       <c r="W26" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13987.5</v>
       </c>
       <c r="X26" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y26" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z26" s="63">
         <f t="shared" si="5"/>
@@ -8057,11 +8056,11 @@
       </c>
       <c r="E27" s="64">
         <f>IF(B27=Inputs!$C$1,D27,E26)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F27" s="64">
         <f>IF(AND(B27&gt;=Inputs!$C$1,B27&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E27,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G27" s="64">
         <f>IF(AND(B27&gt;=Inputs!$C$1,B27&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B27,"Y")+1, 0),0)</f>
@@ -8089,15 +8088,15 @@
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!$D$64/12+N27</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q27" s="63">
         <f>$F27*Outputs_Internal!K$64/12+N27*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R27" s="63">
         <f>$F27*Outputs_Internal!L$64/12+N27*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S27" s="63">
         <f>N27*'MARA Prices'!$F$4</f>
@@ -8163,11 +8162,11 @@
       </c>
       <c r="E28" s="64">
         <f>IF(B28=Inputs!$C$1,D28,E27)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F28" s="64">
         <f>IF(AND(B28&gt;=Inputs!$C$1,B28&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E28,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G28" s="64">
         <f>IF(AND(B28&gt;=Inputs!$C$1,B28&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B28,"Y")+1, 0),0)</f>
@@ -8195,15 +8194,15 @@
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!$D$64/12+N28</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q28" s="63">
         <f>$F28*Outputs_Internal!K$64/12+N28*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R28" s="63">
         <f>$F28*Outputs_Internal!L$64/12+N28*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S28" s="63">
         <f>N28*'MARA Prices'!$F$4</f>
@@ -8269,11 +8268,11 @@
       </c>
       <c r="E29" s="64">
         <f>IF(B29=Inputs!$C$1,D29,E28)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F29" s="64">
         <f>IF(AND(B29&gt;=Inputs!$C$1,B29&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E29,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G29" s="64">
         <f>IF(AND(B29&gt;=Inputs!$C$1,B29&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B29,"Y")+1, 0),0)</f>
@@ -8301,15 +8300,15 @@
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!$D$64/12+N29</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q29" s="63">
         <f>$F29*Outputs_Internal!K$64/12+N29*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R29" s="63">
         <f>$F29*Outputs_Internal!L$64/12+N29*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S29" s="63">
         <f>N29*'MARA Prices'!$F$4</f>
@@ -8325,15 +8324,15 @@
       </c>
       <c r="W29" s="63">
         <f t="shared" si="2"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X29" s="63">
         <f t="shared" si="3"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y29" s="63">
         <f t="shared" si="4"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z29" s="63">
         <f t="shared" si="5"/>
@@ -8375,11 +8374,11 @@
       </c>
       <c r="E30" s="64">
         <f>IF(B30=Inputs!$C$1,D30,E29)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F30" s="64">
         <f>IF(AND(B30&gt;=Inputs!$C$1,B30&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E30,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G30" s="64">
         <f>IF(AND(B30&gt;=Inputs!$C$1,B30&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B30,"Y")+1, 0),0)</f>
@@ -8407,15 +8406,15 @@
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!$D$64/12+N30</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q30" s="63">
         <f>$F30*Outputs_Internal!K$64/12+N30*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R30" s="63">
         <f>$F30*Outputs_Internal!L$64/12+N30*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S30" s="63">
         <f>N30*'MARA Prices'!$F$4</f>
@@ -8481,11 +8480,11 @@
       </c>
       <c r="E31" s="64">
         <f>IF(B31=Inputs!$C$1,D31,E30)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F31" s="64">
         <f>IF(AND(B31&gt;=Inputs!$C$1,B31&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E31,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G31" s="64">
         <f>IF(AND(B31&gt;=Inputs!$C$1,B31&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B31,"Y")+1, 0),0)</f>
@@ -8513,15 +8512,15 @@
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!$D$64/12+N31</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q31" s="63">
         <f>$F31*Outputs_Internal!K$64/12+N31*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R31" s="63">
         <f>$F31*Outputs_Internal!L$64/12+N31*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S31" s="63">
         <f>N31*'MARA Prices'!$F$4</f>
@@ -8587,11 +8586,11 @@
       </c>
       <c r="E32" s="64">
         <f>IF(B32=Inputs!$C$1,D32,E31)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F32" s="64">
         <f>IF(AND(B32&gt;=Inputs!$C$1,B32&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E32,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G32" s="64">
         <f>IF(AND(B32&gt;=Inputs!$C$1,B32&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B32,"Y")+1, 0),0)</f>
@@ -8619,15 +8618,15 @@
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!$D$64/12+N32</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q32" s="63">
         <f>$F32*Outputs_Internal!K$64/12+N32*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R32" s="63">
         <f>$F32*Outputs_Internal!L$64/12+N32*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S32" s="63">
         <f>N32*'MARA Prices'!$F$4</f>
@@ -8643,15 +8642,15 @@
       </c>
       <c r="W32" s="63">
         <f t="shared" si="2"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X32" s="63">
         <f t="shared" si="3"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y32" s="63">
         <f t="shared" si="4"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z32" s="63">
         <f t="shared" si="5"/>
@@ -8693,11 +8692,11 @@
       </c>
       <c r="E33" s="64">
         <f>IF(B33=Inputs!$C$1,D33,E32)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F33" s="64">
         <f>IF(AND(B33&gt;=Inputs!$C$1,B33&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E33,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G33" s="64">
         <f>IF(AND(B33&gt;=Inputs!$C$1,B33&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B33,"Y")+1, 0),0)</f>
@@ -8725,15 +8724,15 @@
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!$D$64/12+N33</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q33" s="63">
         <f>$F33*Outputs_Internal!K$64/12+N33*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R33" s="63">
         <f>$F33*Outputs_Internal!L$64/12+N33*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S33" s="63">
         <f>N33*'MARA Prices'!$F$4</f>
@@ -8799,11 +8798,11 @@
       </c>
       <c r="E34" s="64">
         <f>IF(B34=Inputs!$C$1,D34,E33)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F34" s="64">
         <f>IF(AND(B34&gt;=Inputs!$C$1,B34&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E34,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G34" s="64">
         <f>IF(AND(B34&gt;=Inputs!$C$1,B34&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B34,"Y")+1, 0),0)</f>
@@ -8831,15 +8830,15 @@
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!$D$64/12+N34</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q34" s="63">
         <f>$F34*Outputs_Internal!K$64/12+N34*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R34" s="63">
         <f>$F34*Outputs_Internal!L$64/12+N34*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S34" s="63">
         <f>N34*'MARA Prices'!$F$4</f>
@@ -8905,11 +8904,11 @@
       </c>
       <c r="E35" s="64">
         <f>IF(B35=Inputs!$C$1,D35,E34)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F35" s="64">
         <f>IF(AND(B35&gt;=Inputs!$C$1,B35&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E35,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G35" s="64">
         <f>IF(AND(B35&gt;=Inputs!$C$1,B35&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B35,"Y")+1, 0),0)</f>
@@ -8937,15 +8936,15 @@
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!$D$64/12+N35</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q35" s="63">
         <f>$F35*Outputs_Internal!K$64/12+N35*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R35" s="63">
         <f>$F35*Outputs_Internal!L$64/12+N35*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S35" s="63">
         <f>N35*'MARA Prices'!$F$4</f>
@@ -8961,15 +8960,15 @@
       </c>
       <c r="W35" s="63">
         <f t="shared" si="2"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X35" s="63">
         <f t="shared" si="3"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y35" s="63">
         <f t="shared" si="4"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z35" s="63">
         <f t="shared" si="5"/>
@@ -9011,11 +9010,11 @@
       </c>
       <c r="E36" s="64">
         <f>IF(B36=Inputs!$C$1,D36,E35)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F36" s="64">
         <f>IF(AND(B36&gt;=Inputs!$C$1,B36&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E36,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G36" s="64">
         <f>IF(AND(B36&gt;=Inputs!$C$1,B36&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B36,"Y")+1, 0),0)</f>
@@ -9043,15 +9042,15 @@
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!$D$64/12+N36</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q36" s="63">
         <f>$F36*Outputs_Internal!K$64/12+N36*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R36" s="63">
         <f>$F36*Outputs_Internal!L$64/12+N36*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S36" s="63">
         <f>N36*'MARA Prices'!$F$4</f>
@@ -9117,11 +9116,11 @@
       </c>
       <c r="E37" s="64">
         <f>IF(B37=Inputs!$C$1,D37,E36)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F37" s="64">
         <f>IF(AND(B37&gt;=Inputs!$C$1,B37&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E37,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G37" s="64">
         <f>IF(AND(B37&gt;=Inputs!$C$1,B37&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B37,"Y")+1, 0),0)</f>
@@ -9149,15 +9148,15 @@
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!$D$64/12+N37</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q37" s="63">
         <f>$F37*Outputs_Internal!K$64/12+N37*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R37" s="63">
         <f>$F37*Outputs_Internal!L$64/12+N37*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S37" s="63">
         <f>N37*'MARA Prices'!$F$4</f>
@@ -9223,11 +9222,11 @@
       </c>
       <c r="E38" s="64">
         <f>IF(B38=Inputs!$C$1,D38,E37)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F38" s="64">
         <f>IF(AND(B38&gt;=Inputs!$C$1,B38&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E38,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G38" s="64">
         <f>IF(AND(B38&gt;=Inputs!$C$1,B38&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B38,"Y")+1, 0),0)</f>
@@ -9255,15 +9254,15 @@
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!$D$64/12+N38</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q38" s="63">
         <f>$F38*Outputs_Internal!K$64/12+N38*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R38" s="63">
         <f>$F38*Outputs_Internal!L$64/12+N38*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S38" s="63">
         <f>N38*'MARA Prices'!$F$4</f>
@@ -9279,15 +9278,15 @@
       </c>
       <c r="W38" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X38" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y38" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z38" s="63">
         <f t="shared" si="10"/>
@@ -9329,11 +9328,11 @@
       </c>
       <c r="E39" s="64">
         <f>IF(B39=Inputs!$C$1,D39,E38)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F39" s="64">
         <f>IF(AND(B39&gt;=Inputs!$C$1,B39&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E39,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G39" s="64">
         <f>IF(AND(B39&gt;=Inputs!$C$1,B39&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B39,"Y")+1, 0),0)</f>
@@ -9361,15 +9360,15 @@
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!$D$64/12+N39</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q39" s="63">
         <f>$F39*Outputs_Internal!K$64/12+N39*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R39" s="63">
         <f>$F39*Outputs_Internal!L$64/12+N39*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S39" s="63">
         <f>N39*'MARA Prices'!$F$4</f>
@@ -9435,11 +9434,11 @@
       </c>
       <c r="E40" s="64">
         <f>IF(B40=Inputs!$C$1,D40,E39)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F40" s="64">
         <f>IF(AND(B40&gt;=Inputs!$C$1,B40&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E40,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G40" s="64">
         <f>IF(AND(B40&gt;=Inputs!$C$1,B40&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B40,"Y")+1, 0),0)</f>
@@ -9467,15 +9466,15 @@
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!$D$64/12+N40</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q40" s="63">
         <f>$F40*Outputs_Internal!K$64/12+N40*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R40" s="63">
         <f>$F40*Outputs_Internal!L$64/12+N40*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S40" s="63">
         <f>N40*'MARA Prices'!$F$4</f>
@@ -9541,11 +9540,11 @@
       </c>
       <c r="E41" s="64">
         <f>IF(B41=Inputs!$C$1,D41,E40)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F41" s="64">
         <f>IF(AND(B41&gt;=Inputs!$C$1,B41&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E41,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G41" s="64">
         <f>IF(AND(B41&gt;=Inputs!$C$1,B41&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B41,"Y")+1, 0),0)</f>
@@ -9573,15 +9572,15 @@
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!$D$64/12+N41</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q41" s="63">
         <f>$F41*Outputs_Internal!K$64/12+N41*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R41" s="63">
         <f>$F41*Outputs_Internal!L$64/12+N41*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S41" s="63">
         <f>N41*'MARA Prices'!$F$4</f>
@@ -9597,15 +9596,15 @@
       </c>
       <c r="W41" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X41" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y41" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z41" s="63">
         <f t="shared" si="10"/>
@@ -9647,11 +9646,11 @@
       </c>
       <c r="E42" s="64">
         <f>IF(B42=Inputs!$C$1,D42,E41)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F42" s="64">
         <f>IF(AND(B42&gt;=Inputs!$C$1,B42&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E42,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G42" s="64">
         <f>IF(AND(B42&gt;=Inputs!$C$1,B42&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B42,"Y")+1, 0),0)</f>
@@ -9679,15 +9678,15 @@
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!$D$64/12+N42</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q42" s="63">
         <f>$F42*Outputs_Internal!K$64/12+N42*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R42" s="63">
         <f>$F42*Outputs_Internal!L$64/12+N42*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S42" s="63">
         <f>N42*'MARA Prices'!$F$4</f>
@@ -9753,11 +9752,11 @@
       </c>
       <c r="E43" s="64">
         <f>IF(B43=Inputs!$C$1,D43,E42)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F43" s="64">
         <f>IF(AND(B43&gt;=Inputs!$C$1,B43&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E43,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G43" s="64">
         <f>IF(AND(B43&gt;=Inputs!$C$1,B43&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B43,"Y")+1, 0),0)</f>
@@ -9785,15 +9784,15 @@
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!$D$64/12+N43</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q43" s="63">
         <f>$F43*Outputs_Internal!K$64/12+N43*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R43" s="63">
         <f>$F43*Outputs_Internal!L$64/12+N43*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S43" s="63">
         <f>N43*'MARA Prices'!$F$4</f>
@@ -9859,11 +9858,11 @@
       </c>
       <c r="E44" s="64">
         <f>IF(B44=Inputs!$C$1,D44,E43)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F44" s="64">
         <f>IF(AND(B44&gt;=Inputs!$C$1,B44&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E44,0)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="G44" s="64">
         <f>IF(AND(B44&gt;=Inputs!$C$1,B44&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B44,"Y")+1, 0),0)</f>
@@ -9891,15 +9890,15 @@
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!$D$64/12+N44</f>
-        <v>7977.65625</v>
+        <v>4662.5</v>
       </c>
       <c r="Q44" s="63">
         <f>$F44*Outputs_Internal!K$64/12+N44*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>1468.4482758620691</v>
       </c>
       <c r="R44" s="63">
         <f>$F44*Outputs_Internal!L$64/12+N44*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>3194.0517241379312</v>
       </c>
       <c r="S44" s="63">
         <f>N44*'MARA Prices'!$F$4</f>
@@ -9915,15 +9914,15 @@
       </c>
       <c r="W44" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>13987.5</v>
       </c>
       <c r="X44" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>4405.3448275862074</v>
       </c>
       <c r="Y44" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>9582.1551724137935</v>
       </c>
       <c r="Z44" s="63">
         <f t="shared" si="10"/>
@@ -9965,15 +9964,15 @@
       </c>
       <c r="E45" s="64">
         <f>IF(B45=Inputs!$C$1,D45,E44)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F45" s="64">
         <f>IF(AND(B45&gt;=Inputs!$C$1,B45&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E45,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G45" s="64">
         <f>IF(AND(B45&gt;=Inputs!$C$1,B45&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B45,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I45" s="63">
         <f>IF($B45=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D45</f>
@@ -9997,15 +9996,15 @@
       </c>
       <c r="P45" s="63">
         <f>$F45*Outputs_Internal!$D$64/12+N45</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="63">
         <f>$F45*Outputs_Internal!K$64/12+N45*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R45" s="63">
         <f>$F45*Outputs_Internal!L$64/12+N45*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S45" s="63">
         <f>N45*'MARA Prices'!$F$4</f>
@@ -10071,15 +10070,15 @@
       </c>
       <c r="E46" s="64">
         <f>IF(B46=Inputs!$C$1,D46,E45)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F46" s="64">
         <f>IF(AND(B46&gt;=Inputs!$C$1,B46&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E46,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G46" s="64">
         <f>IF(AND(B46&gt;=Inputs!$C$1,B46&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B46,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I46" s="63">
         <f>IF($B46=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D46</f>
@@ -10103,15 +10102,15 @@
       </c>
       <c r="P46" s="63">
         <f>$F46*Outputs_Internal!$D$64/12+N46</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="63">
         <f>$F46*Outputs_Internal!K$64/12+N46*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R46" s="63">
         <f>$F46*Outputs_Internal!L$64/12+N46*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S46" s="63">
         <f>N46*'MARA Prices'!$F$4</f>
@@ -10177,15 +10176,15 @@
       </c>
       <c r="E47" s="64">
         <f>IF(B47=Inputs!$C$1,D47,E46)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F47" s="64">
         <f>IF(AND(B47&gt;=Inputs!$C$1,B47&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E47,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G47" s="64">
         <f>IF(AND(B47&gt;=Inputs!$C$1,B47&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B47,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I47" s="63">
         <f>IF($B47=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D47</f>
@@ -10209,15 +10208,15 @@
       </c>
       <c r="P47" s="63">
         <f>$F47*Outputs_Internal!$D$64/12+N47</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="63">
         <f>$F47*Outputs_Internal!K$64/12+N47*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R47" s="63">
         <f>$F47*Outputs_Internal!L$64/12+N47*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S47" s="63">
         <f>N47*'MARA Prices'!$F$4</f>
@@ -10233,15 +10232,15 @@
       </c>
       <c r="W47" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X47" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y47" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="63">
         <f t="shared" si="10"/>
@@ -10283,15 +10282,15 @@
       </c>
       <c r="E48" s="64">
         <f>IF(B48=Inputs!$C$1,D48,E47)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F48" s="64">
         <f>IF(AND(B48&gt;=Inputs!$C$1,B48&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E48,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G48" s="64">
         <f>IF(AND(B48&gt;=Inputs!$C$1,B48&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B48,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I48" s="63">
         <f>IF($B48=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D48</f>
@@ -10315,15 +10314,15 @@
       </c>
       <c r="P48" s="63">
         <f>$F48*Outputs_Internal!$D$64/12+N48</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="63">
         <f>$F48*Outputs_Internal!K$64/12+N48*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R48" s="63">
         <f>$F48*Outputs_Internal!L$64/12+N48*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S48" s="63">
         <f>N48*'MARA Prices'!$F$4</f>
@@ -10389,15 +10388,15 @@
       </c>
       <c r="E49" s="64">
         <f>IF(B49=Inputs!$C$1,D49,E48)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F49" s="64">
         <f>IF(AND(B49&gt;=Inputs!$C$1,B49&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E49,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G49" s="64">
         <f>IF(AND(B49&gt;=Inputs!$C$1,B49&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B49,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I49" s="63">
         <f>IF($B49=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D49</f>
@@ -10421,15 +10420,15 @@
       </c>
       <c r="P49" s="63">
         <f>$F49*Outputs_Internal!$D$64/12+N49</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="63">
         <f>$F49*Outputs_Internal!K$64/12+N49*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R49" s="63">
         <f>$F49*Outputs_Internal!L$64/12+N49*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S49" s="63">
         <f>N49*'MARA Prices'!$F$4</f>
@@ -10495,15 +10494,15 @@
       </c>
       <c r="E50" s="64">
         <f>IF(B50=Inputs!$C$1,D50,E49)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F50" s="64">
         <f>IF(AND(B50&gt;=Inputs!$C$1,B50&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E50,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G50" s="64">
         <f>IF(AND(B50&gt;=Inputs!$C$1,B50&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B50,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I50" s="63">
         <f>IF($B50=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D50</f>
@@ -10527,15 +10526,15 @@
       </c>
       <c r="P50" s="63">
         <f>$F50*Outputs_Internal!$D$64/12+N50</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="63">
         <f>$F50*Outputs_Internal!K$64/12+N50*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R50" s="63">
         <f>$F50*Outputs_Internal!L$64/12+N50*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S50" s="63">
         <f>N50*'MARA Prices'!$F$4</f>
@@ -10551,15 +10550,15 @@
       </c>
       <c r="W50" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X50" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y50" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="63">
         <f t="shared" si="10"/>
@@ -10601,15 +10600,15 @@
       </c>
       <c r="E51" s="64">
         <f>IF(B51=Inputs!$C$1,D51,E50)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F51" s="64">
         <f>IF(AND(B51&gt;=Inputs!$C$1,B51&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E51,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G51" s="64">
         <f>IF(AND(B51&gt;=Inputs!$C$1,B51&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B51,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I51" s="63">
         <f>IF($B51=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D51</f>
@@ -10633,15 +10632,15 @@
       </c>
       <c r="P51" s="63">
         <f>$F51*Outputs_Internal!$D$64/12+N51</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="63">
         <f>$F51*Outputs_Internal!K$64/12+N51*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R51" s="63">
         <f>$F51*Outputs_Internal!L$64/12+N51*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S51" s="63">
         <f>N51*'MARA Prices'!$F$4</f>
@@ -10707,15 +10706,15 @@
       </c>
       <c r="E52" s="64">
         <f>IF(B52=Inputs!$C$1,D52,E51)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F52" s="64">
         <f>IF(AND(B52&gt;=Inputs!$C$1,B52&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E52,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G52" s="64">
         <f>IF(AND(B52&gt;=Inputs!$C$1,B52&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B52,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I52" s="63">
         <f>IF($B52=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D52</f>
@@ -10739,15 +10738,15 @@
       </c>
       <c r="P52" s="63">
         <f>$F52*Outputs_Internal!$D$64/12+N52</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q52" s="63">
         <f>$F52*Outputs_Internal!K$64/12+N52*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R52" s="63">
         <f>$F52*Outputs_Internal!L$64/12+N52*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S52" s="63">
         <f>N52*'MARA Prices'!$F$4</f>
@@ -10813,15 +10812,15 @@
       </c>
       <c r="E53" s="64">
         <f>IF(B53=Inputs!$C$1,D53,E52)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F53" s="64">
         <f>IF(AND(B53&gt;=Inputs!$C$1,B53&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E53,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G53" s="64">
         <f>IF(AND(B53&gt;=Inputs!$C$1,B53&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B53,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I53" s="63">
         <f>IF($B53=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D53</f>
@@ -10845,15 +10844,15 @@
       </c>
       <c r="P53" s="63">
         <f>$F53*Outputs_Internal!$D$64/12+N53</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="63">
         <f>$F53*Outputs_Internal!K$64/12+N53*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R53" s="63">
         <f>$F53*Outputs_Internal!L$64/12+N53*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S53" s="63">
         <f>N53*'MARA Prices'!$F$4</f>
@@ -10869,15 +10868,15 @@
       </c>
       <c r="W53" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X53" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y53" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z53" s="63">
         <f t="shared" si="10"/>
@@ -10919,15 +10918,15 @@
       </c>
       <c r="E54" s="64">
         <f>IF(B54=Inputs!$C$1,D54,E53)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F54" s="64">
         <f>IF(AND(B54&gt;=Inputs!$C$1,B54&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E54,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G54" s="64">
         <f>IF(AND(B54&gt;=Inputs!$C$1,B54&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B54,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I54" s="63">
         <f>IF($B54=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D54</f>
@@ -10951,15 +10950,15 @@
       </c>
       <c r="P54" s="63">
         <f>$F54*Outputs_Internal!$D$64/12+N54</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q54" s="63">
         <f>$F54*Outputs_Internal!K$64/12+N54*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R54" s="63">
         <f>$F54*Outputs_Internal!L$64/12+N54*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S54" s="63">
         <f>N54*'MARA Prices'!$F$4</f>
@@ -11025,15 +11024,15 @@
       </c>
       <c r="E55" s="64">
         <f>IF(B55=Inputs!$C$1,D55,E54)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F55" s="64">
         <f>IF(AND(B55&gt;=Inputs!$C$1,B55&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E55,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G55" s="64">
         <f>IF(AND(B55&gt;=Inputs!$C$1,B55&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B55,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I55" s="63">
         <f>IF($B55=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D55</f>
@@ -11057,15 +11056,15 @@
       </c>
       <c r="P55" s="63">
         <f>$F55*Outputs_Internal!$D$64/12+N55</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q55" s="63">
         <f>$F55*Outputs_Internal!K$64/12+N55*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R55" s="63">
         <f>$F55*Outputs_Internal!L$64/12+N55*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S55" s="63">
         <f>N55*'MARA Prices'!$F$4</f>
@@ -11131,15 +11130,15 @@
       </c>
       <c r="E56" s="64">
         <f>IF(B56=Inputs!$C$1,D56,E55)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F56" s="64">
         <f>IF(AND(B56&gt;=Inputs!$C$1,B56&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E56,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G56" s="64">
         <f>IF(AND(B56&gt;=Inputs!$C$1,B56&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B56,"Y")+1, 0),0)</f>
-        <v>1.1025</v>
+        <v>0</v>
       </c>
       <c r="I56" s="63">
         <f>IF($B56=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D56</f>
@@ -11163,15 +11162,15 @@
       </c>
       <c r="P56" s="63">
         <f>$F56*Outputs_Internal!$D$64/12+N56</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="63">
         <f>$F56*Outputs_Internal!K$64/12+N56*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R56" s="63">
         <f>$F56*Outputs_Internal!L$64/12+N56*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S56" s="63">
         <f>N56*'MARA Prices'!$F$4</f>
@@ -11187,15 +11186,15 @@
       </c>
       <c r="W56" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X56" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y56" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z56" s="63">
         <f t="shared" si="10"/>
@@ -11237,15 +11236,15 @@
       </c>
       <c r="E57" s="64">
         <f>IF(B57=Inputs!$C$1,D57,E56)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F57" s="64">
         <f>IF(AND(B57&gt;=Inputs!$C$1,B57&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E57,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G57" s="64">
         <f>IF(AND(B57&gt;=Inputs!$C$1,B57&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B57,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I57" s="63">
         <f>IF($B57=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D57</f>
@@ -11269,15 +11268,15 @@
       </c>
       <c r="P57" s="63">
         <f>$F57*Outputs_Internal!$D$64/12+N57</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q57" s="63">
         <f>$F57*Outputs_Internal!K$64/12+N57*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R57" s="63">
         <f>$F57*Outputs_Internal!L$64/12+N57*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S57" s="63">
         <f>N57*'MARA Prices'!$F$4</f>
@@ -11343,15 +11342,15 @@
       </c>
       <c r="E58" s="64">
         <f>IF(B58=Inputs!$C$1,D58,E57)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F58" s="64">
         <f>IF(AND(B58&gt;=Inputs!$C$1,B58&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E58,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G58" s="64">
         <f>IF(AND(B58&gt;=Inputs!$C$1,B58&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B58,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I58" s="63">
         <f>IF($B58=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D58</f>
@@ -11375,15 +11374,15 @@
       </c>
       <c r="P58" s="63">
         <f>$F58*Outputs_Internal!$D$64/12+N58</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="63">
         <f>$F58*Outputs_Internal!K$64/12+N58*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R58" s="63">
         <f>$F58*Outputs_Internal!L$64/12+N58*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S58" s="63">
         <f>N58*'MARA Prices'!$F$4</f>
@@ -11449,15 +11448,15 @@
       </c>
       <c r="E59" s="64">
         <f>IF(B59=Inputs!$C$1,D59,E58)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F59" s="64">
         <f>IF(AND(B59&gt;=Inputs!$C$1,B59&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E59,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G59" s="64">
         <f>IF(AND(B59&gt;=Inputs!$C$1,B59&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B59,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I59" s="63">
         <f>IF($B59=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D59</f>
@@ -11481,15 +11480,15 @@
       </c>
       <c r="P59" s="63">
         <f>$F59*Outputs_Internal!$D$64/12+N59</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q59" s="63">
         <f>$F59*Outputs_Internal!K$64/12+N59*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R59" s="63">
         <f>$F59*Outputs_Internal!L$64/12+N59*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S59" s="63">
         <f>N59*'MARA Prices'!$F$4</f>
@@ -11505,15 +11504,15 @@
       </c>
       <c r="W59" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X59" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y59" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z59" s="63">
         <f t="shared" si="10"/>
@@ -11555,15 +11554,15 @@
       </c>
       <c r="E60" s="64">
         <f>IF(B60=Inputs!$C$1,D60,E59)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F60" s="64">
         <f>IF(AND(B60&gt;=Inputs!$C$1,B60&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E60,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G60" s="64">
         <f>IF(AND(B60&gt;=Inputs!$C$1,B60&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B60,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I60" s="63">
         <f>IF($B60=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D60</f>
@@ -11587,15 +11586,15 @@
       </c>
       <c r="P60" s="63">
         <f>$F60*Outputs_Internal!$D$64/12+N60</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="63">
         <f>$F60*Outputs_Internal!K$64/12+N60*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R60" s="63">
         <f>$F60*Outputs_Internal!L$64/12+N60*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S60" s="63">
         <f>N60*'MARA Prices'!$F$4</f>
@@ -11661,15 +11660,15 @@
       </c>
       <c r="E61" s="64">
         <f>IF(B61=Inputs!$C$1,D61,E60)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F61" s="64">
         <f>IF(AND(B61&gt;=Inputs!$C$1,B61&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E61,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G61" s="64">
         <f>IF(AND(B61&gt;=Inputs!$C$1,B61&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B61,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I61" s="63">
         <f>IF($B61=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D61</f>
@@ -11693,15 +11692,15 @@
       </c>
       <c r="P61" s="63">
         <f>$F61*Outputs_Internal!$D$64/12+N61</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="63">
         <f>$F61*Outputs_Internal!K$64/12+N61*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R61" s="63">
         <f>$F61*Outputs_Internal!L$64/12+N61*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S61" s="63">
         <f>N61*'MARA Prices'!$F$4</f>
@@ -11767,15 +11766,15 @@
       </c>
       <c r="E62" s="64">
         <f>IF(B62=Inputs!$C$1,D62,E61)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F62" s="64">
         <f>IF(AND(B62&gt;=Inputs!$C$1,B62&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E62,0)</f>
-        <v>1.0125</v>
+        <v>0</v>
       </c>
       <c r="G62" s="64">
         <f>IF(AND(B62&gt;=Inputs!$C$1,B62&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B62,"Y")+1, 0),0)</f>
-        <v>1.1576250000000001</v>
+        <v>0</v>
       </c>
       <c r="I62" s="63">
         <f>IF($B62=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D62</f>
@@ -11799,15 +11798,15 @@
       </c>
       <c r="P62" s="63">
         <f>$F62*Outputs_Internal!$D$64/12+N62</f>
-        <v>7977.65625</v>
+        <v>0</v>
       </c>
       <c r="Q62" s="63">
         <f>$F62*Outputs_Internal!K$64/12+N62*'MARA Prices'!$F$5</f>
-        <v>1571.1043356116772</v>
+        <v>0</v>
       </c>
       <c r="R62" s="63">
         <f>$F62*Outputs_Internal!L$64/12+N62*'MARA Prices'!$F$6</f>
-        <v>6406.5519143883221</v>
+        <v>0</v>
       </c>
       <c r="S62" s="63">
         <f>N62*'MARA Prices'!$F$4</f>
@@ -11823,15 +11822,15 @@
       </c>
       <c r="W62" s="63">
         <f t="shared" si="7"/>
-        <v>23932.96875</v>
+        <v>0</v>
       </c>
       <c r="X62" s="63">
         <f t="shared" si="8"/>
-        <v>4713.313006835032</v>
+        <v>0</v>
       </c>
       <c r="Y62" s="63">
         <f t="shared" si="9"/>
-        <v>19219.655743164967</v>
+        <v>0</v>
       </c>
       <c r="Z62" s="63">
         <f t="shared" si="10"/>
@@ -11873,7 +11872,7 @@
       </c>
       <c r="E63" s="64">
         <f>IF(B63=Inputs!$C$1,D63,E62)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F63" s="64">
         <f>IF(AND(B63&gt;=Inputs!$C$1,B63&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E63,0)</f>
@@ -11979,7 +11978,7 @@
       </c>
       <c r="E64" s="64">
         <f>IF(B64=Inputs!$C$1,D64,E63)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F64" s="64">
         <f>IF(AND(B64&gt;=Inputs!$C$1,B64&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E64,0)</f>
@@ -12085,7 +12084,7 @@
       </c>
       <c r="E65" s="64">
         <f>IF(B65=Inputs!$C$1,D65,E64)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F65" s="64">
         <f>IF(AND(B65&gt;=Inputs!$C$1,B65&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E65,0)</f>
@@ -12191,7 +12190,7 @@
       </c>
       <c r="E66" s="64">
         <f>IF(B66=Inputs!$C$1,D66,E65)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F66" s="64">
         <f>IF(AND(B66&gt;=Inputs!$C$1,B66&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E66,0)</f>
@@ -12297,7 +12296,7 @@
       </c>
       <c r="E67" s="64">
         <f>IF(B67=Inputs!$C$1,D67,E66)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F67" s="64">
         <f>IF(AND(B67&gt;=Inputs!$C$1,B67&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E67,0)</f>
@@ -12403,7 +12402,7 @@
       </c>
       <c r="E68" s="64">
         <f>IF(B68=Inputs!$C$1,D68,E67)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F68" s="64">
         <f>IF(AND(B68&gt;=Inputs!$C$1,B68&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E68,0)</f>
@@ -12509,7 +12508,7 @@
       </c>
       <c r="E69" s="64">
         <f>IF(B69=Inputs!$C$1,D69,E68)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F69" s="64">
         <f>IF(AND(B69&gt;=Inputs!$C$1,B69&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E69,0)</f>
@@ -12615,7 +12614,7 @@
       </c>
       <c r="E70" s="64">
         <f>IF(B70=Inputs!$C$1,D70,E69)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F70" s="64">
         <f>IF(AND(B70&gt;=Inputs!$C$1,B70&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E70,0)</f>
@@ -12721,7 +12720,7 @@
       </c>
       <c r="E71" s="64">
         <f>IF(B71=Inputs!$C$1,D71,E70)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F71" s="64">
         <f>IF(AND(B71&gt;=Inputs!$C$1,B71&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E71,0)</f>
@@ -12827,7 +12826,7 @@
       </c>
       <c r="E72" s="64">
         <f>IF(B72=Inputs!$C$1,D72,E71)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F72" s="64">
         <f>IF(AND(B72&gt;=Inputs!$C$1,B72&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E72,0)</f>
@@ -12933,7 +12932,7 @@
       </c>
       <c r="E73" s="64">
         <f>IF(B73=Inputs!$C$1,D73,E72)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F73" s="64">
         <f>IF(AND(B73&gt;=Inputs!$C$1,B73&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E73,0)</f>
@@ -13039,7 +13038,7 @@
       </c>
       <c r="E74" s="64">
         <f>IF(B74=Inputs!$C$1,D74,E73)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F74" s="64">
         <f>IF(AND(B74&gt;=Inputs!$C$1,B74&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E74,0)</f>
@@ -13145,7 +13144,7 @@
       </c>
       <c r="E75" s="64">
         <f>IF(B75=Inputs!$C$1,D75,E74)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F75" s="64">
         <f>IF(AND(B75&gt;=Inputs!$C$1,B75&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E75,0)</f>
@@ -13251,7 +13250,7 @@
       </c>
       <c r="E76" s="64">
         <f>IF(B76=Inputs!$C$1,D76,E75)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F76" s="64">
         <f>IF(AND(B76&gt;=Inputs!$C$1,B76&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E76,0)</f>
@@ -13357,7 +13356,7 @@
       </c>
       <c r="E77" s="64">
         <f>IF(B77=Inputs!$C$1,D77,E76)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F77" s="64">
         <f>IF(AND(B77&gt;=Inputs!$C$1,B77&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E77,0)</f>
@@ -13463,7 +13462,7 @@
       </c>
       <c r="E78" s="64">
         <f>IF(B78=Inputs!$C$1,D78,E77)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F78" s="64">
         <f>IF(AND(B78&gt;=Inputs!$C$1,B78&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E78,0)</f>
@@ -13569,7 +13568,7 @@
       </c>
       <c r="E79" s="64">
         <f>IF(B79=Inputs!$C$1,D79,E78)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F79" s="64">
         <f>IF(AND(B79&gt;=Inputs!$C$1,B79&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E79,0)</f>
@@ -13675,7 +13674,7 @@
       </c>
       <c r="E80" s="64">
         <f>IF(B80=Inputs!$C$1,D80,E79)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F80" s="64">
         <f>IF(AND(B80&gt;=Inputs!$C$1,B80&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E80,0)</f>
@@ -13781,7 +13780,7 @@
       </c>
       <c r="E81" s="64">
         <f>IF(B81=Inputs!$C$1,D81,E80)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F81" s="64">
         <f>IF(AND(B81&gt;=Inputs!$C$1,B81&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E81,0)</f>
@@ -13887,7 +13886,7 @@
       </c>
       <c r="E82" s="64">
         <f>IF(B82=Inputs!$C$1,D82,E81)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F82" s="64">
         <f>IF(AND(B82&gt;=Inputs!$C$1,B82&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E82,0)</f>
@@ -13993,7 +13992,7 @@
       </c>
       <c r="E83" s="64">
         <f>IF(B83=Inputs!$C$1,D83,E82)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F83" s="64">
         <f>IF(AND(B83&gt;=Inputs!$C$1,B83&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E83,0)</f>
@@ -14099,7 +14098,7 @@
       </c>
       <c r="E84" s="64">
         <f>IF(B84=Inputs!$C$1,D84,E83)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F84" s="64">
         <f>IF(AND(B84&gt;=Inputs!$C$1,B84&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E84,0)</f>
@@ -14205,7 +14204,7 @@
       </c>
       <c r="E85" s="64">
         <f>IF(B85=Inputs!$C$1,D85,E84)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F85" s="64">
         <f>IF(AND(B85&gt;=Inputs!$C$1,B85&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E85,0)</f>
@@ -14311,7 +14310,7 @@
       </c>
       <c r="E86" s="64">
         <f>IF(B86=Inputs!$C$1,D86,E85)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F86" s="64">
         <f>IF(AND(B86&gt;=Inputs!$C$1,B86&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E86,0)</f>
@@ -14417,7 +14416,7 @@
       </c>
       <c r="E87" s="64">
         <f>IF(B87=Inputs!$C$1,D87,E86)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F87" s="64">
         <f>IF(AND(B87&gt;=Inputs!$C$1,B87&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E87,0)</f>
@@ -14523,7 +14522,7 @@
       </c>
       <c r="E88" s="64">
         <f>IF(B88=Inputs!$C$1,D88,E87)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F88" s="64">
         <f>IF(AND(B88&gt;=Inputs!$C$1,B88&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E88,0)</f>
@@ -14629,7 +14628,7 @@
       </c>
       <c r="E89" s="64">
         <f>IF(B89=Inputs!$C$1,D89,E88)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F89" s="64">
         <f>IF(AND(B89&gt;=Inputs!$C$1,B89&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E89,0)</f>
@@ -14735,7 +14734,7 @@
       </c>
       <c r="E90" s="64">
         <f>IF(B90=Inputs!$C$1,D90,E89)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F90" s="64">
         <f>IF(AND(B90&gt;=Inputs!$C$1,B90&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E90,0)</f>
@@ -14841,7 +14840,7 @@
       </c>
       <c r="E91" s="64">
         <f>IF(B91=Inputs!$C$1,D91,E90)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F91" s="64">
         <f>IF(AND(B91&gt;=Inputs!$C$1,B91&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E91,0)</f>
@@ -14947,7 +14946,7 @@
       </c>
       <c r="E92" s="64">
         <f>IF(B92=Inputs!$C$1,D92,E91)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F92" s="64">
         <f>IF(AND(B92&gt;=Inputs!$C$1,B92&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E92,0)</f>
@@ -15053,7 +15052,7 @@
       </c>
       <c r="E93" s="64">
         <f>IF(B93=Inputs!$C$1,D93,E92)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F93" s="64">
         <f>IF(AND(B93&gt;=Inputs!$C$1,B93&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E93,0)</f>
@@ -15159,7 +15158,7 @@
       </c>
       <c r="E94" s="64">
         <f>IF(B94=Inputs!$C$1,D94,E93)</f>
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="F94" s="64">
         <f>IF(AND(B94&gt;=Inputs!$C$1,B94&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E94,0)</f>
@@ -15338,7 +15337,7 @@
       </c>
       <c r="D4" s="1">
         <f>IF(AND(Inputs!D8="Y",Inputs!D7="Y"), 0, IF(Inputs!D7="Y", SUM(Prices!$C$3, IF(Inputs!D$9 ="Y", Prices!$C$4, 0)), IF(Inputs!D7="N", Prices!$D$3, 0)))*Inputs!D12</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="1">
         <f>IF(AND(Inputs!E8="Y",Inputs!E7="Y"), 0, IF(Inputs!E7="Y", SUM(Prices!$C$3, IF(Inputs!E$9 ="Y", Prices!$C$4, 0)), IF(Inputs!E7="N", Prices!$D$3, 0)))*Inputs!E12</f>
@@ -16797,7 +16796,7 @@
       </c>
       <c r="D70" s="20">
         <f>IF(Inputs!D27="Y", Prices!$C25, 0)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E70" s="20">
         <f>IF(Inputs!E27="Y", Prices!$C25, 0)</f>
@@ -16847,7 +16846,7 @@
       </c>
       <c r="D72" s="20">
         <f>IF(Inputs!D29="Y", Prices!$C27, 0)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E72" s="20">
         <f>IF(Inputs!E29="Y", Prices!$C27, 0)</f>
@@ -16897,7 +16896,7 @@
       </c>
       <c r="D74" s="84">
         <f>IF(Inputs!D13="Y", Prices!$C29, IF(Inputs!D13="Monthly", Prices!C29 * Prices!$L$30, 0))</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="E74" s="84">
         <f>IF(Inputs!E13="Y", Prices!$C29, IF(Inputs!E13="Monthly", Prices!D29 * Prices!$L$30, 0))</f>
@@ -16947,23 +16946,23 @@
         <v>1E-3</v>
       </c>
       <c r="K77" s="23">
-        <f t="shared" ref="K77:K85" si="2">D66+D77+$J77</f>
+        <f t="shared" ref="K77:K84" si="2">D66+D77+$J77</f>
         <v>8500.0010000000002</v>
       </c>
       <c r="L77" s="23">
-        <f t="shared" ref="L77:L85" si="3">E66+E77+$J77</f>
+        <f t="shared" ref="L77:L84" si="3">E66+E77+$J77</f>
         <v>1E-3</v>
       </c>
       <c r="M77" s="23">
-        <f t="shared" ref="M77:M85" si="4">F66+F77+$J77</f>
+        <f t="shared" ref="M77:M84" si="4">F66+F77+$J77</f>
         <v>1E-3</v>
       </c>
       <c r="N77" s="23">
-        <f t="shared" ref="N77:N85" si="5">G66+G77+$J77</f>
+        <f t="shared" ref="N77:N84" si="5">G66+G77+$J77</f>
         <v>1E-3</v>
       </c>
       <c r="O77" s="23">
-        <f t="shared" ref="O77:O85" si="6">H66+H77+$J77</f>
+        <f t="shared" ref="O77:O84" si="6">H66+H77+$J77</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -17144,7 +17143,7 @@
       </c>
       <c r="K81" s="23">
         <f t="shared" si="2"/>
-        <v>28000.001400000001</v>
+        <v>1.4000000000000002E-3</v>
       </c>
       <c r="L81" s="23">
         <f t="shared" si="3"/>
@@ -17242,7 +17241,7 @@
       </c>
       <c r="K83" s="23">
         <f t="shared" si="2"/>
-        <v>28000.0016</v>
+        <v>1.6000000000000003E-3</v>
       </c>
       <c r="L83" s="23">
         <f t="shared" si="3"/>
@@ -17397,7 +17396,7 @@
       </c>
       <c r="K88" s="21">
         <f>IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K77,K$77:K$85),8))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L88" s="21">
         <f t="shared" ref="L88:O88" si="9">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L77,L$77:L$85),8))</f>
@@ -17557,7 +17556,7 @@
       </c>
       <c r="D92" s="20">
         <f>D70</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E92" s="20">
         <f>E70</f>
@@ -17577,7 +17576,7 @@
       </c>
       <c r="K92" s="21">
         <f t="shared" ref="K92:O92" si="14">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K81,K$77:K$85),8))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L92" s="21">
         <f t="shared" si="14"/>
@@ -17622,7 +17621,7 @@
       </c>
       <c r="K93" s="21">
         <f t="shared" ref="K93:O93" si="16">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K82,K$77:K$85),8))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L93" s="21">
         <f t="shared" si="16"/>
@@ -17647,7 +17646,7 @@
       </c>
       <c r="D94" s="20">
         <f>IF(D72=0,0,D72-IF(OR(Inputs!D25="Y",Inputs!D26="Y"), 0, D23))</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="E94" s="20">
         <f>IF(E72=0,0,E72-IF(OR(Inputs!E25="Y",Inputs!E26="Y"), 0, E23))</f>
@@ -17667,7 +17666,7 @@
       </c>
       <c r="K94" s="21">
         <f t="shared" ref="K94:O94" si="17">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K83,K$77:K$85),8))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L94" s="21">
         <f t="shared" si="17"/>
@@ -17712,10 +17711,10 @@
       </c>
       <c r="K95" s="21">
         <f>IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K84,K$77:K$85),8))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L95" s="21">
-        <f t="shared" ref="K95:O95" si="19">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L84,L$77:L$85),8))</f>
+        <f t="shared" ref="L95:O95" si="19">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L84,L$77:L$85),8))</f>
         <v>1</v>
       </c>
       <c r="M95" s="21">
@@ -17737,7 +17736,7 @@
       </c>
       <c r="D96" s="84">
         <f t="shared" ref="D96:H96" si="20">D74</f>
-        <v>8400</v>
+        <v>0</v>
       </c>
       <c r="E96" s="84">
         <f t="shared" si="20"/>
@@ -18015,7 +18014,7 @@
       </c>
       <c r="D110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A110, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A110, K$88:K$96, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>-8400</v>
+        <v>-2550</v>
       </c>
       <c r="E110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A110, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A110, L$88:L$96, 0)))*Prices!$L$5*-1, 0)</f>
@@ -18043,7 +18042,7 @@
       </c>
       <c r="D111" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A111, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A111, K$88:K$96, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-12600</v>
+        <v>0</v>
       </c>
       <c r="E111" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A111, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A111, L$88:L$96, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18071,7 +18070,7 @@
       </c>
       <c r="D112" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A112, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A112, K$88:K$96, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-3825</v>
+        <v>0</v>
       </c>
       <c r="E112" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A112, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A112, L$88:L$96, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18208,7 +18207,7 @@
       </c>
       <c r="D118" s="7">
         <f>SUM(D40:D50, D53:D63, D66:D74, D77:D85, D110:D116)</f>
-        <v>98075</v>
+        <v>55950</v>
       </c>
       <c r="E118" s="7">
         <f>SUM(E40:E50, E53:E63, E66:E74, E77:E85, E110:E116)</f>
@@ -18268,7 +18267,7 @@
       </c>
       <c r="D122" s="1">
         <f>IF(Inputs!$D$8 = "Y", Prices!$L$19, 0)*-1</f>
-        <v>-3525</v>
+        <v>0</v>
       </c>
       <c r="E122" s="1">
         <v>0</v>
@@ -18289,7 +18288,7 @@
       </c>
       <c r="D124" s="7">
         <f>SUM(D118, D120,D122)</f>
-        <v>94550</v>
+        <v>55950</v>
       </c>
       <c r="E124" s="7">
         <f t="shared" ref="E124:H124" si="27">SUM(E118, E120,E122)</f>

</xml_diff>

<commit_message>
Remove EBMs from ACOI Enchanced.
Do this because they are not being included.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -1317,20 +1317,20 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="66" customWidth="1"/>
-    <col min="4" max="8" width="18.7265625" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="66" customWidth="1"/>
+    <col min="4" max="8" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="91" t="s">
         <v>58</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>43101</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="67" t="s">
         <v>72</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="67" t="s">
         <v>122</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="67" t="s">
         <v>156</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="67" t="s">
         <v>131</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="68"/>
       <c r="C6" s="72"/>
       <c r="D6" s="13" t="s">
@@ -1389,7 +1389,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="69" t="s">
         <v>5</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="69" t="s">
         <v>80</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="G9" s="55"/>
       <c r="H9" s="56"/>
     </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="69" t="s">
         <v>139</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="G10" s="55"/>
       <c r="H10" s="56"/>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="69" t="s">
         <v>4</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
         <v>110</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
         <v>97</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="G13" s="55"/>
       <c r="H13" s="56"/>
     </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="69" t="s">
         <v>7</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="69" t="s">
         <v>8</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="69" t="s">
         <v>21</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="G16" s="55"/>
       <c r="H16" s="56"/>
     </row>
-    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="69" t="s">
         <v>9</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="69" t="s">
         <v>10</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
         <v>77</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="69" t="s">
         <v>11</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="G20" s="55"/>
       <c r="H20" s="56"/>
     </row>
-    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
         <v>153</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="69" t="s">
         <v>12</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="69" t="s">
         <v>13</v>
       </c>
@@ -1626,7 +1626,7 @@
       <c r="G23" s="55"/>
       <c r="H23" s="56"/>
     </row>
-    <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="G24" s="55"/>
       <c r="H24" s="56"/>
     </row>
-    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="69" t="s">
         <v>15</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="G25" s="55"/>
       <c r="H25" s="56"/>
     </row>
-    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="69" t="s">
         <v>129</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="G26" s="55"/>
       <c r="H26" s="56"/>
     </row>
-    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="69" t="s">
         <v>16</v>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="G27" s="55"/>
       <c r="H27" s="56"/>
     </row>
-    <row r="28" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="69" t="s">
         <v>99</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="G28" s="55"/>
       <c r="H28" s="56"/>
     </row>
-    <row r="29" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="69" t="s">
         <v>150</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="G29" s="55"/>
       <c r="H29" s="56"/>
     </row>
-    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="92" t="s">
         <v>98</v>
       </c>
@@ -1742,26 +1742,26 @@
   <dimension ref="B2:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="47.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.26953125" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>105</v>
       </c>
@@ -1778,12 +1778,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1829,12 +1829,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>20</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>21</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>9</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
@@ -2047,7 +2047,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>77</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C14" s="19" t="s">
         <v>11</v>
       </c>
@@ -2117,7 +2117,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C15" s="19" t="s">
         <v>149</v>
       </c>
@@ -2152,7 +2152,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C16" s="19" t="s">
         <v>22</v>
       </c>
@@ -2187,12 +2187,12 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -2227,7 +2227,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2262,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2297,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>129</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>16</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>99</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>150</v>
       </c>
@@ -2437,7 +2437,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>98</v>
       </c>
@@ -2472,7 +2472,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>97</v>
       </c>
@@ -2507,12 +2507,12 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>38</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>115</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>82</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>39</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2659,7 +2659,7 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>74</v>
       </c>
@@ -2679,16 +2679,16 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" s="64">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C38" s="64"/>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>145</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="64" t="s">
         <v>143</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="64" t="s">
         <v>144</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>73</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -2795,18 +2795,18 @@
       <c r="T45" s="8"/>
       <c r="U45" s="8"/>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
         <v>172850</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C48" s="52">
         <f>SUM(D43:H43)</f>
         <v>172850</v>
@@ -2814,17 +2814,17 @@
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D50" s="2"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2845,28 +2845,28 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="48.453125" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.26953125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.81640625" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F1" s="50" t="s">
         <v>57</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="H1" s="50"/>
       <c r="I1" s="50"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
@@ -2904,12 +2904,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>75</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>76</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
@@ -2999,7 +2999,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
         <v>132</v>
       </c>
@@ -3015,7 +3015,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="26"/>
@@ -3024,7 +3024,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>53</v>
       </c>
@@ -3036,7 +3036,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
         <v>2</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="P10" s="101"/>
       <c r="Q10" s="101"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>20</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
         <v>8</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>21</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
         <v>10</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="17" t="s">
         <v>77</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
         <v>154</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C18" s="19" t="s">
         <v>11</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C19" s="19" t="s">
         <v>149</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="19" t="s">
         <v>22</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -3465,7 +3465,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G22" s="48" t="s">
         <v>128</v>
       </c>
@@ -3477,7 +3477,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -3486,7 +3486,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>54</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C25" s="15" t="s">
         <v>2</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="17" t="s">
         <v>20</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C27" s="17" t="s">
         <v>8</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
         <v>21</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
         <v>9</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
         <v>10</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
         <v>77</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
         <v>154</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C33" s="19" t="s">
         <v>11</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C34" s="19" t="s">
         <v>149</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C35" s="28" t="s">
         <v>22</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
@@ -3961,7 +3961,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>46</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C38" s="17" t="s">
         <v>13</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C39" s="17" t="s">
         <v>14</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C40" s="19" t="s">
         <v>15</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C41" s="19" t="s">
         <v>129</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C42" s="19" t="s">
         <v>16</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C43" s="19" t="s">
         <v>99</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C44" s="19" t="s">
         <v>150</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C45" s="19" t="s">
         <v>98</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C46" s="81" t="s">
         <v>97</v>
       </c>
@@ -4314,12 +4314,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>55</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C49" s="28" t="s">
         <v>13</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C50" s="17" t="s">
         <v>14</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C51" s="19" t="s">
         <v>15</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C52" s="19" t="s">
         <v>129</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C53" s="19" t="s">
         <v>16</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C54" s="19" t="s">
         <v>99</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C55" s="19" t="s">
         <v>150</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C56" s="19" t="s">
         <v>98</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C57" s="81" t="s">
         <v>97</v>
       </c>
@@ -4691,12 +4691,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>37</v>
       </c>
@@ -4704,7 +4704,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>38</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>115</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>82</v>
       </c>
@@ -4823,12 +4823,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
         <v>39</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C65" s="21" t="s">
         <v>56</v>
       </c>
@@ -4865,14 +4865,14 @@
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C66" s="21"/>
       <c r="D66" s="23"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>147</v>
       </c>
@@ -4913,12 +4913,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
         <v>70</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D70" s="1"/>
       <c r="K70" s="53">
         <f>IFERROR(K69/$D$69, 0)</f>
@@ -4962,12 +4962,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="27" t="s">
         <v>52</v>
       </c>
@@ -4983,7 +4983,7 @@
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="27"/>
       <c r="C74" s="21" t="s">
         <v>13</v>
@@ -5027,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="27"/>
       <c r="C75" s="21" t="s">
         <v>14</v>
@@ -5071,7 +5071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" s="27"/>
       <c r="C76" s="21" t="s">
         <v>15</v>
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" s="27"/>
       <c r="C77" s="21" t="s">
         <v>152</v>
@@ -5159,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" s="27"/>
       <c r="C78" s="21" t="s">
         <v>16</v>
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" s="27"/>
       <c r="C79" s="21" t="s">
         <v>99</v>
@@ -5247,7 +5247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="27"/>
       <c r="C80" s="21" t="s">
         <v>150</v>
@@ -5291,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="27"/>
       <c r="C81" s="21" t="s">
         <v>98</v>
@@ -5335,7 +5335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="27"/>
       <c r="C82" s="21" t="s">
         <v>97</v>
@@ -5396,30 +5396,30 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="60" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="60" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" style="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.54296875" style="60" customWidth="1"/>
-    <col min="9" max="13" width="8.7265625" style="63"/>
-    <col min="14" max="14" width="10.1796875" style="63" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.453125" customWidth="1"/>
-    <col min="16" max="16" width="10.453125" style="63" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8.7265625" style="63"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="60" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" style="60" customWidth="1"/>
+    <col min="9" max="13" width="8.7109375" style="63"/>
+    <col min="14" max="14" width="10.140625" style="63" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8.7109375" style="63"/>
     <col min="19" max="19" width="14" style="63" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.81640625" style="63" customWidth="1"/>
-    <col min="21" max="21" width="14.81640625" style="63" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.54296875" customWidth="1"/>
-    <col min="26" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="63" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.5703125" customWidth="1"/>
+    <col min="26" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
       <c r="F1" s="65">
         <f>COUNTIF(F3:F94,"&gt;0")</f>
         <v>36</v>
@@ -5455,7 +5455,7 @@
       <c r="AG1" s="107"/>
       <c r="AH1" s="107"/>
     </row>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2" s="59" t="s">
         <v>61</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="60">
         <v>42917</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B4" s="60">
         <f>EDATE(B3,1)</f>
         <v>42948</v>
@@ -5713,7 +5713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5" s="60">
         <f t="shared" ref="B5:B68" si="1">EDATE(B4,1)</f>
         <v>42979</v>
@@ -5819,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" s="60">
         <f t="shared" si="1"/>
         <v>43009</v>
@@ -5925,7 +5925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="60">
         <f t="shared" si="1"/>
         <v>43040</v>
@@ -6031,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" s="60">
         <f t="shared" si="1"/>
         <v>43070</v>
@@ -6137,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="60">
         <f t="shared" si="1"/>
         <v>43101</v>
@@ -6243,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="60">
         <f t="shared" si="1"/>
         <v>43132</v>
@@ -6349,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11" s="60">
         <f t="shared" si="1"/>
         <v>43160</v>
@@ -6455,7 +6455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12" s="60">
         <f t="shared" si="1"/>
         <v>43191</v>
@@ -6561,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13" s="60">
         <f t="shared" si="1"/>
         <v>43221</v>
@@ -6667,7 +6667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14" s="60">
         <f t="shared" si="1"/>
         <v>43252</v>
@@ -6773,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15" s="60">
         <f t="shared" si="1"/>
         <v>43282</v>
@@ -6879,7 +6879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B16" s="60">
         <f t="shared" si="1"/>
         <v>43313</v>
@@ -6985,7 +6985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B17" s="60">
         <f t="shared" si="1"/>
         <v>43344</v>
@@ -7091,7 +7091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B18" s="60">
         <f t="shared" si="1"/>
         <v>43374</v>
@@ -7197,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B19" s="60">
         <f t="shared" si="1"/>
         <v>43405</v>
@@ -7303,7 +7303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B20" s="60">
         <f t="shared" si="1"/>
         <v>43435</v>
@@ -7409,7 +7409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B21" s="60">
         <f t="shared" si="1"/>
         <v>43466</v>
@@ -7515,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B22" s="60">
         <f t="shared" si="1"/>
         <v>43497</v>
@@ -7621,7 +7621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B23" s="60">
         <f t="shared" si="1"/>
         <v>43525</v>
@@ -7727,7 +7727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B24" s="60">
         <f t="shared" si="1"/>
         <v>43556</v>
@@ -7833,7 +7833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B25" s="60">
         <f t="shared" si="1"/>
         <v>43586</v>
@@ -7939,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B26" s="60">
         <f t="shared" si="1"/>
         <v>43617</v>
@@ -8045,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B27" s="60">
         <f t="shared" si="1"/>
         <v>43647</v>
@@ -8151,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B28" s="60">
         <f t="shared" si="1"/>
         <v>43678</v>
@@ -8257,7 +8257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B29" s="60">
         <f t="shared" si="1"/>
         <v>43709</v>
@@ -8363,7 +8363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B30" s="60">
         <f t="shared" si="1"/>
         <v>43739</v>
@@ -8469,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B31" s="60">
         <f t="shared" si="1"/>
         <v>43770</v>
@@ -8575,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B32" s="60">
         <f t="shared" si="1"/>
         <v>43800</v>
@@ -8681,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B33" s="60">
         <f t="shared" si="1"/>
         <v>43831</v>
@@ -8787,7 +8787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B34" s="60">
         <f t="shared" si="1"/>
         <v>43862</v>
@@ -8893,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B35" s="60">
         <f t="shared" si="1"/>
         <v>43891</v>
@@ -8999,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B36" s="60">
         <f t="shared" si="1"/>
         <v>43922</v>
@@ -9105,7 +9105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B37" s="60">
         <f t="shared" si="1"/>
         <v>43952</v>
@@ -9211,7 +9211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B38" s="60">
         <f t="shared" si="1"/>
         <v>43983</v>
@@ -9317,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B39" s="60">
         <f t="shared" si="1"/>
         <v>44013</v>
@@ -9423,7 +9423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B40" s="60">
         <f t="shared" si="1"/>
         <v>44044</v>
@@ -9529,7 +9529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B41" s="60">
         <f t="shared" si="1"/>
         <v>44075</v>
@@ -9635,7 +9635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B42" s="60">
         <f t="shared" si="1"/>
         <v>44105</v>
@@ -9741,7 +9741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B43" s="60">
         <f t="shared" si="1"/>
         <v>44136</v>
@@ -9847,7 +9847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B44" s="60">
         <f t="shared" si="1"/>
         <v>44166</v>
@@ -9953,7 +9953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B45" s="60">
         <f t="shared" si="1"/>
         <v>44197</v>
@@ -10059,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B46" s="60">
         <f t="shared" si="1"/>
         <v>44228</v>
@@ -10165,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B47" s="60">
         <f t="shared" si="1"/>
         <v>44256</v>
@@ -10271,7 +10271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B48" s="60">
         <f t="shared" si="1"/>
         <v>44287</v>
@@ -10377,7 +10377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B49" s="60">
         <f t="shared" si="1"/>
         <v>44317</v>
@@ -10483,7 +10483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B50" s="60">
         <f t="shared" si="1"/>
         <v>44348</v>
@@ -10589,7 +10589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B51" s="60">
         <f t="shared" si="1"/>
         <v>44378</v>
@@ -10695,7 +10695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B52" s="60">
         <f t="shared" si="1"/>
         <v>44409</v>
@@ -10801,7 +10801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B53" s="60">
         <f t="shared" si="1"/>
         <v>44440</v>
@@ -10907,7 +10907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B54" s="60">
         <f t="shared" si="1"/>
         <v>44470</v>
@@ -11013,7 +11013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B55" s="60">
         <f t="shared" si="1"/>
         <v>44501</v>
@@ -11119,7 +11119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B56" s="60">
         <f t="shared" si="1"/>
         <v>44531</v>
@@ -11225,7 +11225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B57" s="60">
         <f t="shared" si="1"/>
         <v>44562</v>
@@ -11331,7 +11331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B58" s="60">
         <f t="shared" si="1"/>
         <v>44593</v>
@@ -11437,7 +11437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B59" s="60">
         <f t="shared" si="1"/>
         <v>44621</v>
@@ -11543,7 +11543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B60" s="60">
         <f t="shared" si="1"/>
         <v>44652</v>
@@ -11649,7 +11649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B61" s="60">
         <f t="shared" si="1"/>
         <v>44682</v>
@@ -11755,7 +11755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B62" s="60">
         <f t="shared" si="1"/>
         <v>44713</v>
@@ -11861,7 +11861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B63" s="60">
         <f t="shared" si="1"/>
         <v>44743</v>
@@ -11967,7 +11967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B64" s="60">
         <f t="shared" si="1"/>
         <v>44774</v>
@@ -12073,7 +12073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B65" s="60">
         <f t="shared" si="1"/>
         <v>44805</v>
@@ -12179,7 +12179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B66" s="60">
         <f t="shared" si="1"/>
         <v>44835</v>
@@ -12285,7 +12285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B67" s="60">
         <f t="shared" si="1"/>
         <v>44866</v>
@@ -12391,7 +12391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B68" s="60">
         <f t="shared" si="1"/>
         <v>44896</v>
@@ -12497,7 +12497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B69" s="60">
         <f t="shared" ref="B69:B94" si="13">EDATE(B68,1)</f>
         <v>44927</v>
@@ -12603,7 +12603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B70" s="60">
         <f t="shared" si="13"/>
         <v>44958</v>
@@ -12709,7 +12709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B71" s="60">
         <f t="shared" si="13"/>
         <v>44986</v>
@@ -12815,7 +12815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B72" s="60">
         <f t="shared" si="13"/>
         <v>45017</v>
@@ -12921,7 +12921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B73" s="60">
         <f t="shared" si="13"/>
         <v>45047</v>
@@ -13027,7 +13027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B74" s="60">
         <f t="shared" si="13"/>
         <v>45078</v>
@@ -13133,7 +13133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B75" s="60">
         <f t="shared" si="13"/>
         <v>45108</v>
@@ -13239,7 +13239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B76" s="60">
         <f t="shared" si="13"/>
         <v>45139</v>
@@ -13345,7 +13345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B77" s="60">
         <f t="shared" si="13"/>
         <v>45170</v>
@@ -13451,7 +13451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B78" s="60">
         <f t="shared" si="13"/>
         <v>45200</v>
@@ -13557,7 +13557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B79" s="60">
         <f t="shared" si="13"/>
         <v>45231</v>
@@ -13663,7 +13663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B80" s="60">
         <f t="shared" si="13"/>
         <v>45261</v>
@@ -13769,7 +13769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B81" s="60">
         <f t="shared" si="13"/>
         <v>45292</v>
@@ -13875,7 +13875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B82" s="60">
         <f t="shared" si="13"/>
         <v>45323</v>
@@ -13981,7 +13981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B83" s="60">
         <f t="shared" si="13"/>
         <v>45352</v>
@@ -14087,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B84" s="60">
         <f t="shared" si="13"/>
         <v>45383</v>
@@ -14193,7 +14193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B85" s="60">
         <f t="shared" si="13"/>
         <v>45413</v>
@@ -14299,7 +14299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B86" s="60">
         <f t="shared" si="13"/>
         <v>45444</v>
@@ -14405,7 +14405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B87" s="60">
         <f t="shared" si="13"/>
         <v>45474</v>
@@ -14511,7 +14511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B88" s="60">
         <f t="shared" si="13"/>
         <v>45505</v>
@@ -14617,7 +14617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B89" s="60">
         <f t="shared" si="13"/>
         <v>45536</v>
@@ -14723,7 +14723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B90" s="60">
         <f t="shared" si="13"/>
         <v>45566</v>
@@ -14829,7 +14829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B91" s="60">
         <f t="shared" si="13"/>
         <v>45597</v>
@@ -14935,7 +14935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B92" s="60">
         <f t="shared" si="13"/>
         <v>45627</v>
@@ -15041,7 +15041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B93" s="60">
         <f t="shared" si="13"/>
         <v>45658</v>
@@ -15147,7 +15147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B94" s="60">
         <f t="shared" si="13"/>
         <v>45689</v>
@@ -15282,19 +15282,19 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" customWidth="1"/>
-    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="15" width="18" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>105</v>
       </c>
@@ -15326,12 +15326,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -15356,7 +15356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -15372,7 +15372,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>86</v>
       </c>
@@ -15406,7 +15406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
@@ -15441,7 +15441,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>88</v>
       </c>
@@ -15476,7 +15476,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>90</v>
       </c>
@@ -15511,7 +15511,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="78" t="s">
         <v>94</v>
       </c>
@@ -15536,7 +15536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="78" t="s">
         <v>95</v>
       </c>
@@ -15561,19 +15561,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
@@ -15598,7 +15598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
         <v>20</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
@@ -15648,7 +15648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
         <v>21</v>
       </c>
@@ -15673,7 +15673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" s="17" t="s">
         <v>9</v>
       </c>
@@ -15698,7 +15698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" s="17" t="s">
         <v>10</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" s="17" t="s">
         <v>77</v>
       </c>
@@ -15748,32 +15748,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D22="Y",Inputs!D$24="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!D22="Y",Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="E21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E22="Y",Inputs!E$24="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!E22="Y",Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F22="Y",Inputs!F$24="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!F22="Y",Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="G21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G22="Y",Inputs!G$24="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(Inputs!G22="Y",Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H22="Y",Inputs!H$24="Y"), Prices!$C16, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+        <f xml:space="preserve"> IF(Inputs!H22="Y",Prices!$C16, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" s="19" t="s">
         <v>11</v>
       </c>
@@ -15798,7 +15798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="19" t="s">
         <v>149</v>
       </c>
@@ -15823,7 +15823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="19" t="s">
         <v>155</v>
       </c>
@@ -15848,12 +15848,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
         <v>2</v>
       </c>
@@ -15878,7 +15878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
         <v>20</v>
       </c>
@@ -15903,7 +15903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
         <v>8</v>
       </c>
@@ -15928,7 +15928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
         <v>21</v>
       </c>
@@ -15953,7 +15953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
         <v>9</v>
       </c>
@@ -15978,7 +15978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
         <v>10</v>
       </c>
@@ -16003,7 +16003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C33" s="17" t="s">
         <v>77</v>
       </c>
@@ -16028,32 +16028,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C34" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D34" s="18">
-        <f>IF(OR(Inputs!D$7="Y", D$11 = 0), 0, IF(OR(Inputs!D22="Y",Inputs!D$24="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
+        <f>IF(OR(Inputs!D$7="Y", D$11 = 0), 0, IF(Inputs!D22="Y",PRODUCT(D$11, Prices!$E16),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E34" s="18">
-        <f>IF(OR(Inputs!E$7="Y", E$11 = 0), 0, IF(OR(Inputs!E22="Y",Inputs!E$24="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
+        <f>IF(OR(Inputs!E$7="Y", E$11 = 0), 0, IF(Inputs!E22="Y",PRODUCT(E$11, Prices!$E16),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F34" s="18">
-        <f>IF(OR(Inputs!F$7="Y", F$11 = 0), 0, IF(OR(Inputs!F22="Y",Inputs!F$24="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
+        <f>IF(OR(Inputs!F$7="Y", F$11 = 0), 0, IF(Inputs!F22="Y",PRODUCT(F$11, Prices!$E16),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G34" s="18">
-        <f>IF(OR(Inputs!G$7="Y", G$11 = 0), 0, IF(OR(Inputs!G22="Y",Inputs!G$24="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
+        <f>IF(OR(Inputs!G$7="Y", G$11 = 0), 0, IF(Inputs!G22="Y",PRODUCT(G$11, Prices!$E16),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H34" s="18">
-        <f>IF(OR(Inputs!H$7="Y", H$11 = 0), 0, IF(OR(Inputs!H22="Y",Inputs!H$24="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+        <f>IF(OR(Inputs!H$7="Y", H$11 = 0), 0, IF(Inputs!H22="Y",PRODUCT(H$11, Prices!$E16),0))*H$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" s="19" t="s">
         <v>11</v>
       </c>
@@ -16078,7 +16078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="19" t="s">
         <v>149</v>
       </c>
@@ -16103,7 +16103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="28" t="s">
         <v>155</v>
       </c>
@@ -16123,19 +16123,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="15" t="s">
         <v>2</v>
       </c>
@@ -16160,7 +16160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
         <v>20</v>
       </c>
@@ -16185,7 +16185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
         <v>8</v>
       </c>
@@ -16210,7 +16210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
         <v>21</v>
       </c>
@@ -16235,7 +16235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="17" t="s">
         <v>9</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="17" t="s">
         <v>10</v>
       </c>
@@ -16285,7 +16285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" s="17" t="s">
         <v>77</v>
       </c>
@@ -16310,32 +16310,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D47" s="18">
-        <f>IF(AND(Inputs!D22="Y",Inputs!D$24="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!D22="Y",Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="E47" s="18">
-        <f>IF(AND(Inputs!E22="Y",Inputs!E$24="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!E22="Y",Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="F47" s="18">
-        <f>IF(AND(Inputs!F22="Y",Inputs!F$24="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!F22="Y",Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="G47" s="18">
-        <f>IF(AND(Inputs!G22="Y",Inputs!G$24="N"),Prices!$C16,0)</f>
+        <f>IF(Inputs!G22="Y",Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="H47" s="18">
-        <f>IF(AND(Inputs!H22="Y",Inputs!H$24="N"),Prices!$C16,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+        <f>IF(Inputs!H22="Y",Prices!$C16,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" s="19" t="s">
         <v>11</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C49" s="19" t="s">
         <v>149</v>
       </c>
@@ -16385,7 +16385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C50" s="19" t="s">
         <v>155</v>
       </c>
@@ -16410,12 +16410,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C53" s="15" t="s">
         <v>2</v>
       </c>
@@ -16440,7 +16440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C54" s="17" t="s">
         <v>20</v>
       </c>
@@ -16465,7 +16465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
         <v>8</v>
       </c>
@@ -16490,7 +16490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" s="17" t="s">
         <v>21</v>
       </c>
@@ -16515,7 +16515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" s="17" t="s">
         <v>9</v>
       </c>
@@ -16540,7 +16540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C58" s="17" t="s">
         <v>10</v>
       </c>
@@ -16565,7 +16565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" s="17" t="s">
         <v>77</v>
       </c>
@@ -16590,32 +16590,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D60" s="18">
-        <f>IF(OR(Inputs!D$7="Y", D$11 = 0), 0, IF(AND(Inputs!D22="Y",Inputs!D$24="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$7="Y", D$11 = 0), 0, IF(Inputs!D22="Y",PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E60" s="18">
-        <f>IF(OR(Inputs!E$7="Y", E$11 = 0), 0, IF(AND(Inputs!E22="Y",Inputs!E$24="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$7="Y", E$11 = 0), 0, IF(Inputs!E22="Y",PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F60" s="18">
-        <f>IF(OR(Inputs!F$7="Y", F$11 = 0), 0, IF(AND(Inputs!F22="Y",Inputs!F$24="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$7="Y", F$11 = 0), 0, IF(Inputs!F22="Y",PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G60" s="18">
-        <f>IF(OR(Inputs!G$7="Y", G$11 = 0), 0, IF(AND(Inputs!G22="Y",Inputs!G$24="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$7="Y", G$11 = 0), 0, IF(Inputs!G22="Y",PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H60" s="18">
-        <f>IF(OR(Inputs!H$7="Y", H$11 = 0), 0, IF(AND(Inputs!H22="Y",Inputs!H$24="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+        <f>IF(OR(Inputs!H$7="Y", H$11 = 0), 0, IF(Inputs!H22="Y",PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" s="19" t="s">
         <v>11</v>
       </c>
@@ -16640,7 +16640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C62" s="19" t="s">
         <v>149</v>
       </c>
@@ -16665,7 +16665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C63" s="28" t="s">
         <v>155</v>
       </c>
@@ -16685,12 +16685,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C66" s="17" t="s">
         <v>13</v>
       </c>
@@ -16715,7 +16715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C67" s="17" t="s">
         <v>14</v>
       </c>
@@ -16740,7 +16740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C68" s="19" t="s">
         <v>15</v>
       </c>
@@ -16765,7 +16765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C69" s="19" t="s">
         <v>129</v>
       </c>
@@ -16790,7 +16790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C70" s="19" t="s">
         <v>16</v>
       </c>
@@ -16815,7 +16815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C71" s="19" t="s">
         <v>99</v>
       </c>
@@ -16840,7 +16840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C72" s="19" t="s">
         <v>150</v>
       </c>
@@ -16865,7 +16865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C73" s="19" t="s">
         <v>98</v>
       </c>
@@ -16890,7 +16890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C74" s="81" t="s">
         <v>96</v>
       </c>
@@ -16915,7 +16915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
         <v>45</v>
       </c>
@@ -16923,7 +16923,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C77" s="28" t="s">
         <v>13</v>
       </c>
@@ -16966,7 +16966,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C78" s="17" t="s">
         <v>14</v>
       </c>
@@ -17015,7 +17015,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C79" s="19" t="s">
         <v>15</v>
       </c>
@@ -17064,7 +17064,7 @@
         <v>1.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C80" s="19" t="s">
         <v>129</v>
       </c>
@@ -17113,7 +17113,7 @@
         <v>1.3000000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C81" s="19" t="s">
         <v>16</v>
       </c>
@@ -17162,7 +17162,7 @@
         <v>1.4000000000000002E-3</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C82" s="19" t="s">
         <v>99</v>
       </c>
@@ -17211,7 +17211,7 @@
         <v>1.5000000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C83" s="19" t="s">
         <v>150</v>
       </c>
@@ -17260,7 +17260,7 @@
         <v>1.6000000000000003E-3</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C84" s="19" t="s">
         <v>98</v>
       </c>
@@ -17309,7 +17309,7 @@
         <v>1.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C85" s="81" t="s">
         <v>96</v>
       </c>
@@ -17358,19 +17358,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C88" s="17" t="s">
         <v>13</v>
       </c>
@@ -17415,20 +17415,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C89" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D89" s="18">
-        <f>IF(D67=0,0,D67-SUM(D15:D21))</f>
+        <f>IF(D67=0,0,D67-SUM(D15:D20))</f>
         <v>0</v>
       </c>
       <c r="E89" s="18">
-        <f t="shared" ref="E89:H89" si="10">IF(E67=0,0,E67-SUM(E15:E21))</f>
+        <f t="shared" ref="E89:H89" si="10">IF(E67=0,0,E67-SUM(E15:E20))</f>
         <v>0</v>
       </c>
       <c r="F89" s="18">
-        <f>IF(F67=0,0,F67-SUM(F15:F21))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G89" s="18">
@@ -17460,7 +17460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C90" s="19" t="s">
         <v>15</v>
       </c>
@@ -17505,7 +17505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C91" s="19" t="s">
         <v>129</v>
       </c>
@@ -17550,7 +17550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C92" s="19" t="s">
         <v>16</v>
       </c>
@@ -17595,7 +17595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C93" s="19" t="s">
         <v>99</v>
       </c>
@@ -17640,7 +17640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C94" s="19" t="s">
         <v>150</v>
       </c>
@@ -17685,7 +17685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C95" s="19" t="s">
         <v>98</v>
       </c>
@@ -17730,7 +17730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C96" s="81" t="s">
         <v>96</v>
       </c>
@@ -17775,12 +17775,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C99" s="28" t="s">
         <v>13</v>
       </c>
@@ -17800,20 +17800,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C100" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D100" s="18">
-        <f>IF(D78=0,0,D78-SUM(D28:D34))</f>
+        <f>IF(D78=0,0,D78-SUM(D28:D33))</f>
         <v>0</v>
       </c>
       <c r="E100" s="18">
-        <f t="shared" ref="E100:H100" si="22">IF(E78=0,0,E78-SUM(E28:E34))</f>
+        <f t="shared" ref="E100:H100" si="22">IF(E78=0,0,E78-SUM(E28:E33))</f>
         <v>0</v>
       </c>
       <c r="F100" s="18">
-        <f>IF(F78=0,0,F78-SUM(F28:F34))</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G100" s="18">
@@ -17825,7 +17825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="19" t="s">
         <v>15</v>
       </c>
@@ -17850,7 +17850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="19" t="s">
         <v>129</v>
       </c>
@@ -17875,7 +17875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C103" s="19" t="s">
         <v>16</v>
       </c>
@@ -17900,7 +17900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C104" s="19" t="s">
         <v>99</v>
       </c>
@@ -17925,7 +17925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C105" s="19" t="s">
         <v>150</v>
       </c>
@@ -17950,7 +17950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" s="19" t="s">
         <v>98</v>
       </c>
@@ -17975,7 +17975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C107" s="81" t="s">
         <v>96</v>
       </c>
@@ -18000,12 +18000,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="88">
         <v>2</v>
       </c>
@@ -18033,7 +18033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="88">
         <v>3</v>
       </c>
@@ -18061,7 +18061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="88">
         <v>4</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="88">
         <v>5</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="88">
         <v>6</v>
       </c>
@@ -18145,7 +18145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="88">
         <v>7</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="88">
         <v>8</v>
       </c>
@@ -18201,7 +18201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B118" s="6" t="s">
         <v>112</v>
       </c>
@@ -18226,10 +18226,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B120" s="6" t="s">
         <v>42</v>
       </c>
@@ -18254,14 +18254,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B122" s="6" t="s">
         <v>82</v>
       </c>
@@ -18282,7 +18282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" s="6" t="s">
         <v>113</v>
       </c>
@@ -18307,7 +18307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="27"/>
       <c r="C127" s="21" t="s">
         <v>114</v>
@@ -18333,7 +18333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="27"/>
       <c r="D128" s="21">
         <v>0.1</v>
@@ -18351,7 +18351,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="129" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="27"/>
       <c r="D129" s="21">
         <f>SUM(D127:D128)</f>
@@ -18374,7 +18374,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="130" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="27"/>
       <c r="D130" s="21">
         <f>_xlfn.RANK.EQ(D129, $D$129:$H$129, 5)</f>
@@ -18397,16 +18397,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="27"/>
     </row>
-    <row r="132" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="27"/>
       <c r="C132" s="21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="133" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="27"/>
       <c r="D133" s="21" t="s">
         <v>116</v>
@@ -18416,7 +18416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="27"/>
       <c r="D134" s="21" t="s">
         <v>117</v>
@@ -18426,7 +18426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="27"/>
       <c r="D135" s="21" t="s">
         <v>118</v>
@@ -18436,7 +18436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="27"/>
       <c r="D136" s="21" t="s">
         <v>119</v>
@@ -18446,7 +18446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F140" s="2"/>
     </row>
   </sheetData>
@@ -18459,24 +18459,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
-    <col min="2" max="2" width="47.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.453125" customWidth="1"/>
-    <col min="9" max="10" width="4.1796875" customWidth="1"/>
-    <col min="11" max="11" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.54296875" customWidth="1"/>
+    <col min="6" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="10" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C2" s="48" t="s">
         <v>5</v>
       </c>
@@ -18484,7 +18482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>111</v>
       </c>
@@ -18502,7 +18500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -18531,7 +18529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E5" s="48" t="s">
         <v>83</v>
       </c>
@@ -18551,7 +18549,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
@@ -18586,14 +18584,14 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" s="43"/>
       <c r="D8" s="39"/>
       <c r="K8" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9" s="46" t="s">
         <v>27</v>
       </c>
@@ -18608,7 +18606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>20</v>
       </c>
@@ -18639,7 +18637,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
@@ -18670,7 +18668,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
@@ -18695,7 +18693,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>9</v>
       </c>
@@ -18721,7 +18719,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>10</v>
       </c>
@@ -18752,7 +18750,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>77</v>
       </c>
@@ -18783,7 +18781,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>154</v>
       </c>
@@ -18810,7 +18808,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="54"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>11</v>
       </c>
@@ -18837,7 +18835,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>149</v>
       </c>
@@ -18862,7 +18860,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>155</v>
       </c>
@@ -18893,14 +18891,14 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C20" s="43"/>
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>13</v>
       </c>
@@ -18931,7 +18929,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>14</v>
       </c>
@@ -18956,7 +18954,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>15</v>
       </c>
@@ -18981,7 +18979,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
         <v>129</v>
       </c>
@@ -19006,7 +19004,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
         <v>16</v>
       </c>
@@ -19038,7 +19036,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
         <v>99</v>
       </c>
@@ -19063,7 +19061,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
         <v>150</v>
       </c>
@@ -19088,7 +19086,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>98</v>
       </c>
@@ -19120,7 +19118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="81" t="s">
         <v>96</v>
       </c>
@@ -19145,7 +19143,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K30" t="s">
         <v>133</v>
       </c>
@@ -19165,18 +19163,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>134</v>
       </c>
@@ -19208,7 +19208,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -19245,7 +19245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>50000</v>
       </c>
@@ -19276,7 +19276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>100000</v>
       </c>
@@ -19313,7 +19313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>300000</v>
       </c>
@@ -19350,7 +19350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>500000</v>
       </c>
@@ -19387,7 +19387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1000000</v>
       </c>
@@ -19418,7 +19418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2000000</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H10" s="106">
         <f t="shared" ref="H10:H16" si="0">H2*$C2</f>
         <v>5000</v>
@@ -19471,7 +19471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H11" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -19498,7 +19498,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H12" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -19520,7 +19520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H13" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -19542,7 +19542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H14" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -19564,7 +19564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
       <c r="F15" s="103"/>
       <c r="H15" s="106">
@@ -19588,7 +19588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
       <c r="F16" s="103"/>
       <c r="H16" s="106">
@@ -19612,15 +19612,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="2"/>
       <c r="F17" s="103"/>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
       <c r="F18" s="103"/>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>
       <c r="F19" s="103"/>
       <c r="H19" s="6" t="s">
@@ -19639,7 +19639,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20" s="103"/>
       <c r="G20" t="s">
@@ -19666,7 +19666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="F21" s="103"/>
       <c r="G21" t="s">

</xml_diff>

<commit_message>
Update old datamart pricing
Do this because the monthly price was accidentally put in as the quarterly price
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1317,7 +1317,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1335,7 @@
         <v>58</v>
       </c>
       <c r="C1" s="70">
-        <v>43101</v>
+        <v>43647</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
@@ -1351,7 +1351,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
         <v>156</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="D7" s="16">
         <f>SUM(Calcs!D40, Calcs!D53)</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="E7" s="16">
         <f>SUM(Calcs!E40, Calcs!E53)</f>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="D19" s="1">
         <f>SUM(Calcs!D66, Calcs!D77)</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="E19" s="1">
         <f>SUM(Calcs!E66, Calcs!E77)</f>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="D21" s="1">
         <f>SUM(Calcs!D68, Calcs!D79)</f>
-        <v>35000</v>
+        <v>42000</v>
       </c>
       <c r="E21" s="1">
         <f>SUM(Calcs!E68, Calcs!E79)</f>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="D30" s="1">
         <f>SUM(Calcs!D110:D114)</f>
-        <v>-2550</v>
+        <v>-3060</v>
       </c>
       <c r="E30" s="1">
         <f>SUM(Calcs!E110:E114)</f>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D34" s="7">
         <f>SUM(D7:D16, D19:D27, D30:D32)</f>
-        <v>55950</v>
+        <v>67140</v>
       </c>
       <c r="E34" s="7">
         <f>SUM(E7:E16, E19:E27, E30:E31)</f>
@@ -2682,7 +2682,7 @@
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" s="64">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D43" s="7">
         <f>(D34/12*Inputs!$C$2+D4)*$C$37+D41</f>
-        <v>172850</v>
+        <v>209000.25</v>
       </c>
       <c r="E43" s="7">
         <f>(E34/12*Inputs!$C$2+E4)*$C$37+E41</f>
@@ -2803,13 +2803,13 @@
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>172850</v>
+        <v>209000.25</v>
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C48" s="52">
         <f>SUM(D43:H43)</f>
-        <v>172850</v>
+        <v>209000.25</v>
       </c>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="D10" s="16">
         <f>SUM(Calcs!D14:H14)</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="75">
@@ -3060,11 +3060,11 @@
       </c>
       <c r="K10" s="16">
         <f>(IF(Inputs!C5="New York",$H$7,-$H$7)+F10)*$D10</f>
-        <v>7125.0000000000009</v>
+        <v>8550</v>
       </c>
       <c r="L10" s="100">
         <f>(IF(Inputs!C5="New York",-$H$7,$H$7)+G10)*D10</f>
-        <v>7875</v>
+        <v>9450</v>
       </c>
       <c r="M10" s="16">
         <f t="shared" ref="M10:N20" si="2">H10*$D10</f>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="D18" s="20">
         <f>SUM(Calcs!D22:H22)</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="F18" s="33">
         <v>0.1</v>
@@ -3365,11 +3365,11 @@
       </c>
       <c r="K18" s="20">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="L18" s="20">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>10800</v>
       </c>
       <c r="M18" s="20">
         <f t="shared" si="2"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="D19" s="20">
         <f>SUM(Calcs!D23:H23)</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="F19" s="33">
         <v>0.1</v>
@@ -3403,11 +3403,11 @@
       </c>
       <c r="K19" s="20">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="L19" s="20">
         <f t="shared" si="4"/>
-        <v>9000</v>
+        <v>10800</v>
       </c>
       <c r="M19" s="20">
         <f t="shared" si="2"/>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="D20" s="20">
         <f>SUM(Calcs!D24:H24)</f>
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="F20" s="33">
         <v>0.1</v>
@@ -3441,11 +3441,11 @@
       </c>
       <c r="K20" s="20">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="L20" s="20">
         <f>G20*$D20</f>
-        <v>1350</v>
+        <v>1620</v>
       </c>
       <c r="M20" s="20">
         <f t="shared" si="2"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="D38" s="18">
         <f>SUM(Calcs!D88:H88)</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="F38" s="32">
         <v>0.9</v>
@@ -3996,11 +3996,11 @@
       </c>
       <c r="K38" s="18">
         <f t="shared" ref="K38:N46" si="23">F38*$D38</f>
-        <v>7650</v>
+        <v>9180</v>
       </c>
       <c r="L38" s="18">
         <f t="shared" si="23"/>
-        <v>850</v>
+        <v>1020</v>
       </c>
       <c r="M38" s="18">
         <f t="shared" si="23"/>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="D40" s="20">
         <f>SUM(Calcs!D90:H90)</f>
-        <v>13500</v>
+        <v>16200</v>
       </c>
       <c r="F40" s="33">
         <v>0.1</v>
@@ -4072,11 +4072,11 @@
       </c>
       <c r="K40" s="20">
         <f t="shared" si="23"/>
-        <v>1350</v>
+        <v>1620</v>
       </c>
       <c r="L40" s="20">
         <f t="shared" si="23"/>
-        <v>12150</v>
+        <v>14580</v>
       </c>
       <c r="M40" s="20">
         <f t="shared" si="23"/>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="D60" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>-2550</v>
+        <v>-3060</v>
       </c>
       <c r="F60" s="8">
         <f>IFERROR(SUM(K74:K82)/SUM($K$74:$N$82), 0)</f>
@@ -4730,11 +4730,11 @@
       </c>
       <c r="K60" s="12">
         <f>F60*$D$60</f>
-        <v>-653.62068965517233</v>
+        <v>-784.34482758620686</v>
       </c>
       <c r="L60" s="12">
         <f>G60*$D$60</f>
-        <v>-1896.3793103448274</v>
+        <v>-2275.655172413793</v>
       </c>
       <c r="M60" s="12">
         <f>H60*$D$60</f>
@@ -4834,15 +4834,15 @@
       </c>
       <c r="D64" s="1">
         <f>SUM(Outputs_External!D34:'Outputs_External'!H34)</f>
-        <v>55950</v>
+        <v>67140</v>
       </c>
       <c r="K64" s="12">
         <f>SUM(K60:K62, K38:K46, K10:K20,K25:K35,K49:K57)</f>
-        <v>17621.37931034483</v>
+        <v>21145.655172413793</v>
       </c>
       <c r="L64" s="12">
         <f>SUM(L60:L62, L38:L46, L10:L20,L25:L35,L49:L57)</f>
-        <v>38328.620689655174</v>
+        <v>45994.344827586203</v>
       </c>
       <c r="M64" s="12">
         <f>SUM(M60:M62, M38:M46, M10:M20,M25:M35,M49:M57)</f>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="D65" s="23">
         <f>SUM(K64:N64)</f>
-        <v>55950</v>
+        <v>67140</v>
       </c>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
@@ -4924,15 +4924,15 @@
       </c>
       <c r="D69" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>172850</v>
+        <v>209000.25</v>
       </c>
       <c r="K69" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>55364.1379310345</v>
+        <v>66761.17758620689</v>
       </c>
       <c r="L69" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>117485.86206896555</v>
+        <v>142239.07241379312</v>
       </c>
       <c r="M69" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -4947,11 +4947,11 @@
       <c r="D70" s="1"/>
       <c r="K70" s="53">
         <f>IFERROR(K69/$D$69, 0)</f>
-        <v>0.32030163685874746</v>
+        <v>0.31943108960973438</v>
       </c>
       <c r="L70" s="53">
         <f>IFERROR(L69/$D$69, 0)</f>
-        <v>0.67969836314125287</v>
+        <v>0.68056891039026568</v>
       </c>
       <c r="M70" s="53">
         <f>IFERROR(M69/$D$69, 0)</f>
@@ -4990,7 +4990,7 @@
       </c>
       <c r="D74" s="23">
         <f>SUM(Calcs!D66:H66)+SUM(Calcs!D77:H77)</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="E74" s="21"/>
       <c r="F74" s="24">
@@ -5012,11 +5012,11 @@
       <c r="J74" s="21"/>
       <c r="K74" s="25">
         <f t="shared" ref="K74:N76" si="74">F74*$D74</f>
-        <v>7650</v>
+        <v>9180</v>
       </c>
       <c r="L74" s="25">
         <f t="shared" si="74"/>
-        <v>850</v>
+        <v>1020</v>
       </c>
       <c r="M74" s="25">
         <f t="shared" si="74"/>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="D76" s="23">
         <f>SUM(Calcs!D68:H68)+SUM(Calcs!D79:H79)</f>
-        <v>35000</v>
+        <v>42000</v>
       </c>
       <c r="E76" s="21"/>
       <c r="F76" s="24">
@@ -5100,11 +5100,11 @@
       <c r="J76" s="21"/>
       <c r="K76" s="25">
         <f t="shared" si="74"/>
-        <v>3500</v>
+        <v>4200</v>
       </c>
       <c r="L76" s="25">
         <f t="shared" si="74"/>
-        <v>31500</v>
+        <v>37800</v>
       </c>
       <c r="M76" s="25">
         <f t="shared" si="74"/>
@@ -6152,23 +6152,23 @@
       </c>
       <c r="F9" s="64">
         <f>IF(AND(B9&gt;=Inputs!$C$1,B9&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E9,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="64">
         <f>IF(AND(B9&gt;=Inputs!$C$1,B9&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B9,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D9</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="J9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!K$4, Outputs_Internal!K$5),0)*$D9</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="K9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!L$4, Outputs_Internal!L$5),0)*$D9</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="L9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!M$4, Outputs_Internal!$M$5),0)*$D9</f>
@@ -6180,15 +6180,15 @@
       </c>
       <c r="P9" s="63">
         <f>$F9*Outputs_Internal!$D$64/12+N9</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="63">
         <f>$F9*Outputs_Internal!K$64/12+N9*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R9" s="63">
         <f>$F9*Outputs_Internal!L$64/12+N9*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S9" s="63">
         <f>N9*'MARA Prices'!$F$4</f>
@@ -6258,11 +6258,11 @@
       </c>
       <c r="F10" s="64">
         <f>IF(AND(B10&gt;=Inputs!$C$1,B10&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E10,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="64">
         <f>IF(AND(B10&gt;=Inputs!$C$1,B10&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B10,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="63">
         <f>IF($B10=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D10</f>
@@ -6286,15 +6286,15 @@
       </c>
       <c r="P10" s="63">
         <f>$F10*Outputs_Internal!$D$64/12+N10</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="63">
         <f>$F10*Outputs_Internal!K$64/12+N10*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R10" s="63">
         <f>$F10*Outputs_Internal!L$64/12+N10*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S10" s="63">
         <f>N10*'MARA Prices'!$F$4</f>
@@ -6364,11 +6364,11 @@
       </c>
       <c r="F11" s="64">
         <f>IF(AND(B11&gt;=Inputs!$C$1,B11&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E11,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="64">
         <f>IF(AND(B11&gt;=Inputs!$C$1,B11&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B11,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="63">
         <f>IF($B11=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D11</f>
@@ -6392,15 +6392,15 @@
       </c>
       <c r="P11" s="63">
         <f>$F11*Outputs_Internal!$D$64/12+N11</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="63">
         <f>$F11*Outputs_Internal!K$64/12+N11*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R11" s="63">
         <f>$F11*Outputs_Internal!L$64/12+N11*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S11" s="63">
         <f>N11*'MARA Prices'!$F$4</f>
@@ -6416,15 +6416,15 @@
       </c>
       <c r="W11" s="63">
         <f t="shared" si="2"/>
-        <v>18987.5</v>
+        <v>0</v>
       </c>
       <c r="X11" s="63">
         <f t="shared" si="3"/>
-        <v>6905.3448275862065</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="63">
         <f t="shared" si="4"/>
-        <v>12082.155172413793</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="63">
         <f t="shared" si="5"/>
@@ -6470,11 +6470,11 @@
       </c>
       <c r="F12" s="64">
         <f>IF(AND(B12&gt;=Inputs!$C$1,B12&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E12,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="64">
         <f>IF(AND(B12&gt;=Inputs!$C$1,B12&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B12,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="63">
         <f>IF($B12=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D12</f>
@@ -6498,15 +6498,15 @@
       </c>
       <c r="P12" s="63">
         <f>$F12*Outputs_Internal!$D$64/12+N12</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="63">
         <f>$F12*Outputs_Internal!K$64/12+N12*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R12" s="63">
         <f>$F12*Outputs_Internal!L$64/12+N12*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S12" s="63">
         <f>N12*'MARA Prices'!$F$4</f>
@@ -6576,11 +6576,11 @@
       </c>
       <c r="F13" s="64">
         <f>IF(AND(B13&gt;=Inputs!$C$1,B13&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E13,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="64">
         <f>IF(AND(B13&gt;=Inputs!$C$1,B13&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B13,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="63">
         <f>IF($B13=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D13</f>
@@ -6604,15 +6604,15 @@
       </c>
       <c r="P13" s="63">
         <f>$F13*Outputs_Internal!$D$64/12+N13</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="63">
         <f>$F13*Outputs_Internal!K$64/12+N13*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R13" s="63">
         <f>$F13*Outputs_Internal!L$64/12+N13*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S13" s="63">
         <f>N13*'MARA Prices'!$F$4</f>
@@ -6682,11 +6682,11 @@
       </c>
       <c r="F14" s="64">
         <f>IF(AND(B14&gt;=Inputs!$C$1,B14&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E14,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="64">
         <f>IF(AND(B14&gt;=Inputs!$C$1,B14&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B14,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="63">
         <f>IF($B14=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D14</f>
@@ -6710,15 +6710,15 @@
       </c>
       <c r="P14" s="63">
         <f>$F14*Outputs_Internal!$D$64/12+N14</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="63">
         <f>$F14*Outputs_Internal!K$64/12+N14*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R14" s="63">
         <f>$F14*Outputs_Internal!L$64/12+N14*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S14" s="63">
         <f>N14*'MARA Prices'!$F$4</f>
@@ -6734,15 +6734,15 @@
       </c>
       <c r="W14" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>0</v>
       </c>
       <c r="X14" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="63">
         <f t="shared" si="5"/>
@@ -6788,11 +6788,11 @@
       </c>
       <c r="F15" s="64">
         <f>IF(AND(B15&gt;=Inputs!$C$1,B15&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E15,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="64">
         <f>IF(AND(B15&gt;=Inputs!$C$1,B15&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B15,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="63">
         <f>IF($B15=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D15</f>
@@ -6816,15 +6816,15 @@
       </c>
       <c r="P15" s="63">
         <f>$F15*Outputs_Internal!$D$64/12+N15</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="63">
         <f>$F15*Outputs_Internal!K$64/12+N15*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R15" s="63">
         <f>$F15*Outputs_Internal!L$64/12+N15*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S15" s="63">
         <f>N15*'MARA Prices'!$F$4</f>
@@ -6894,11 +6894,11 @@
       </c>
       <c r="F16" s="64">
         <f>IF(AND(B16&gt;=Inputs!$C$1,B16&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E16,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="64">
         <f>IF(AND(B16&gt;=Inputs!$C$1,B16&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B16,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="63">
         <f>IF($B16=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D16</f>
@@ -6922,15 +6922,15 @@
       </c>
       <c r="P16" s="63">
         <f>$F16*Outputs_Internal!$D$64/12+N16</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="63">
         <f>$F16*Outputs_Internal!K$64/12+N16*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R16" s="63">
         <f>$F16*Outputs_Internal!L$64/12+N16*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S16" s="63">
         <f>N16*'MARA Prices'!$F$4</f>
@@ -7000,11 +7000,11 @@
       </c>
       <c r="F17" s="64">
         <f>IF(AND(B17&gt;=Inputs!$C$1,B17&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E17,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="64">
         <f>IF(AND(B17&gt;=Inputs!$C$1,B17&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B17,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="63">
         <f>IF($B17=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D17</f>
@@ -7028,15 +7028,15 @@
       </c>
       <c r="P17" s="63">
         <f>$F17*Outputs_Internal!$D$64/12+N17</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="63">
         <f>$F17*Outputs_Internal!K$64/12+N17*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R17" s="63">
         <f>$F17*Outputs_Internal!L$64/12+N17*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S17" s="63">
         <f>N17*'MARA Prices'!$F$4</f>
@@ -7052,15 +7052,15 @@
       </c>
       <c r="W17" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>0</v>
       </c>
       <c r="X17" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="63">
         <f t="shared" si="5"/>
@@ -7106,11 +7106,11 @@
       </c>
       <c r="F18" s="64">
         <f>IF(AND(B18&gt;=Inputs!$C$1,B18&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E18,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="64">
         <f>IF(AND(B18&gt;=Inputs!$C$1,B18&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B18,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="63">
         <f>IF($B18=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D18</f>
@@ -7134,15 +7134,15 @@
       </c>
       <c r="P18" s="63">
         <f>$F18*Outputs_Internal!$D$64/12+N18</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="63">
         <f>$F18*Outputs_Internal!K$64/12+N18*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R18" s="63">
         <f>$F18*Outputs_Internal!L$64/12+N18*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S18" s="63">
         <f>N18*'MARA Prices'!$F$4</f>
@@ -7212,11 +7212,11 @@
       </c>
       <c r="F19" s="64">
         <f>IF(AND(B19&gt;=Inputs!$C$1,B19&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E19,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="64">
         <f>IF(AND(B19&gt;=Inputs!$C$1,B19&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B19,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="63">
         <f>IF($B19=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D19</f>
@@ -7240,15 +7240,15 @@
       </c>
       <c r="P19" s="63">
         <f>$F19*Outputs_Internal!$D$64/12+N19</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="63">
         <f>$F19*Outputs_Internal!K$64/12+N19*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R19" s="63">
         <f>$F19*Outputs_Internal!L$64/12+N19*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S19" s="63">
         <f>N19*'MARA Prices'!$F$4</f>
@@ -7318,11 +7318,11 @@
       </c>
       <c r="F20" s="64">
         <f>IF(AND(B20&gt;=Inputs!$C$1,B20&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E20,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="64">
         <f>IF(AND(B20&gt;=Inputs!$C$1,B20&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B20,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="63">
         <f>IF($B20=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D20</f>
@@ -7346,15 +7346,15 @@
       </c>
       <c r="P20" s="63">
         <f>$F20*Outputs_Internal!$D$64/12+N20</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="63">
         <f>$F20*Outputs_Internal!K$64/12+N20*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R20" s="63">
         <f>$F20*Outputs_Internal!L$64/12+N20*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S20" s="63">
         <f>N20*'MARA Prices'!$F$4</f>
@@ -7370,15 +7370,15 @@
       </c>
       <c r="W20" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>0</v>
       </c>
       <c r="X20" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="63">
         <f t="shared" si="5"/>
@@ -7424,11 +7424,11 @@
       </c>
       <c r="F21" s="64">
         <f>IF(AND(B21&gt;=Inputs!$C$1,B21&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E21,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="64">
         <f>IF(AND(B21&gt;=Inputs!$C$1,B21&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B21,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="63">
         <f>IF($B21=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D21</f>
@@ -7452,15 +7452,15 @@
       </c>
       <c r="P21" s="63">
         <f>$F21*Outputs_Internal!$D$64/12+N21</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="63">
         <f>$F21*Outputs_Internal!K$64/12+N21*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R21" s="63">
         <f>$F21*Outputs_Internal!L$64/12+N21*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S21" s="63">
         <f>N21*'MARA Prices'!$F$4</f>
@@ -7530,11 +7530,11 @@
       </c>
       <c r="F22" s="64">
         <f>IF(AND(B22&gt;=Inputs!$C$1,B22&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E22,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="64">
         <f>IF(AND(B22&gt;=Inputs!$C$1,B22&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B22,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="63">
         <f>IF($B22=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D22</f>
@@ -7558,15 +7558,15 @@
       </c>
       <c r="P22" s="63">
         <f>$F22*Outputs_Internal!$D$64/12+N22</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="63">
         <f>$F22*Outputs_Internal!K$64/12+N22*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R22" s="63">
         <f>$F22*Outputs_Internal!L$64/12+N22*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S22" s="63">
         <f>N22*'MARA Prices'!$F$4</f>
@@ -7636,11 +7636,11 @@
       </c>
       <c r="F23" s="64">
         <f>IF(AND(B23&gt;=Inputs!$C$1,B23&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E23,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="64">
         <f>IF(AND(B23&gt;=Inputs!$C$1,B23&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B23,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="63">
         <f>IF($B23=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D23</f>
@@ -7664,15 +7664,15 @@
       </c>
       <c r="P23" s="63">
         <f>$F23*Outputs_Internal!$D$64/12+N23</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="63">
         <f>$F23*Outputs_Internal!K$64/12+N23*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R23" s="63">
         <f>$F23*Outputs_Internal!L$64/12+N23*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S23" s="63">
         <f>N23*'MARA Prices'!$F$4</f>
@@ -7688,15 +7688,15 @@
       </c>
       <c r="W23" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>0</v>
       </c>
       <c r="X23" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="63">
         <f t="shared" si="5"/>
@@ -7742,11 +7742,11 @@
       </c>
       <c r="F24" s="64">
         <f>IF(AND(B24&gt;=Inputs!$C$1,B24&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E24,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="64">
         <f>IF(AND(B24&gt;=Inputs!$C$1,B24&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B24,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="63">
         <f>IF($B24=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D24</f>
@@ -7770,15 +7770,15 @@
       </c>
       <c r="P24" s="63">
         <f>$F24*Outputs_Internal!$D$64/12+N24</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="63">
         <f>$F24*Outputs_Internal!K$64/12+N24*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R24" s="63">
         <f>$F24*Outputs_Internal!L$64/12+N24*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S24" s="63">
         <f>N24*'MARA Prices'!$F$4</f>
@@ -7848,11 +7848,11 @@
       </c>
       <c r="F25" s="64">
         <f>IF(AND(B25&gt;=Inputs!$C$1,B25&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E25,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="64">
         <f>IF(AND(B25&gt;=Inputs!$C$1,B25&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B25,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="63">
         <f>IF($B25=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D25</f>
@@ -7876,15 +7876,15 @@
       </c>
       <c r="P25" s="63">
         <f>$F25*Outputs_Internal!$D$64/12+N25</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="63">
         <f>$F25*Outputs_Internal!K$64/12+N25*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R25" s="63">
         <f>$F25*Outputs_Internal!L$64/12+N25*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S25" s="63">
         <f>N25*'MARA Prices'!$F$4</f>
@@ -7954,11 +7954,11 @@
       </c>
       <c r="F26" s="64">
         <f>IF(AND(B26&gt;=Inputs!$C$1,B26&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E26,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="64">
         <f>IF(AND(B26&gt;=Inputs!$C$1,B26&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B26,"Y")+1, 0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="63">
         <f>IF($B26=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D26</f>
@@ -7982,15 +7982,15 @@
       </c>
       <c r="P26" s="63">
         <f>$F26*Outputs_Internal!$D$64/12+N26</f>
-        <v>4662.5</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="63">
         <f>$F26*Outputs_Internal!K$64/12+N26*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>0</v>
       </c>
       <c r="R26" s="63">
         <f>$F26*Outputs_Internal!L$64/12+N26*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>0</v>
       </c>
       <c r="S26" s="63">
         <f>N26*'MARA Prices'!$F$4</f>
@@ -8006,15 +8006,15 @@
       </c>
       <c r="W26" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>0</v>
       </c>
       <c r="X26" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="63">
         <f t="shared" si="5"/>
@@ -8056,11 +8056,11 @@
       </c>
       <c r="E27" s="64">
         <f>IF(B27=Inputs!$C$1,D27,E26)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F27" s="64">
         <f>IF(AND(B27&gt;=Inputs!$C$1,B27&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E27,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G27" s="64">
         <f>IF(AND(B27&gt;=Inputs!$C$1,B27&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B27,"Y")+1, 0),0)</f>
@@ -8068,15 +8068,15 @@
       </c>
       <c r="I27" s="63">
         <f>IF($B27=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D27</f>
-        <v>0</v>
+        <v>5062.5</v>
       </c>
       <c r="J27" s="63">
         <f>IF($B27=Inputs!$C$1,SUM(Outputs_Internal!K$4, Outputs_Internal!K$5),0)*$D27</f>
-        <v>0</v>
+        <v>2531.25</v>
       </c>
       <c r="K27" s="63">
         <f>IF($B27=Inputs!$C$1,SUM(Outputs_Internal!L$4, Outputs_Internal!L$5),0)*$D27</f>
-        <v>0</v>
+        <v>2531.25</v>
       </c>
       <c r="L27" s="63">
         <f>IF($B27=Inputs!$C$1,SUM(Outputs_Internal!M$4, Outputs_Internal!$M$5),0)*$D27</f>
@@ -8088,15 +8088,15 @@
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!$D$64/12+N27</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q27" s="63">
         <f>$F27*Outputs_Internal!K$64/12+N27*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R27" s="63">
         <f>$F27*Outputs_Internal!L$64/12+N27*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S27" s="63">
         <f>N27*'MARA Prices'!$F$4</f>
@@ -8162,11 +8162,11 @@
       </c>
       <c r="E28" s="64">
         <f>IF(B28=Inputs!$C$1,D28,E27)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F28" s="64">
         <f>IF(AND(B28&gt;=Inputs!$C$1,B28&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E28,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G28" s="64">
         <f>IF(AND(B28&gt;=Inputs!$C$1,B28&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B28,"Y")+1, 0),0)</f>
@@ -8194,15 +8194,15 @@
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!$D$64/12+N28</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q28" s="63">
         <f>$F28*Outputs_Internal!K$64/12+N28*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R28" s="63">
         <f>$F28*Outputs_Internal!L$64/12+N28*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S28" s="63">
         <f>N28*'MARA Prices'!$F$4</f>
@@ -8268,11 +8268,11 @@
       </c>
       <c r="E29" s="64">
         <f>IF(B29=Inputs!$C$1,D29,E28)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F29" s="64">
         <f>IF(AND(B29&gt;=Inputs!$C$1,B29&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E29,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G29" s="64">
         <f>IF(AND(B29&gt;=Inputs!$C$1,B29&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B29,"Y")+1, 0),0)</f>
@@ -8300,15 +8300,15 @@
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!$D$64/12+N29</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q29" s="63">
         <f>$F29*Outputs_Internal!K$64/12+N29*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R29" s="63">
         <f>$F29*Outputs_Internal!L$64/12+N29*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S29" s="63">
         <f>N29*'MARA Prices'!$F$4</f>
@@ -8324,15 +8324,15 @@
       </c>
       <c r="W29" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>22057.3125</v>
       </c>
       <c r="X29" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>7883.7439655172402</v>
       </c>
       <c r="Y29" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>14173.56853448276</v>
       </c>
       <c r="Z29" s="63">
         <f t="shared" si="5"/>
@@ -8374,11 +8374,11 @@
       </c>
       <c r="E30" s="64">
         <f>IF(B30=Inputs!$C$1,D30,E29)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F30" s="64">
         <f>IF(AND(B30&gt;=Inputs!$C$1,B30&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E30,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G30" s="64">
         <f>IF(AND(B30&gt;=Inputs!$C$1,B30&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B30,"Y")+1, 0),0)</f>
@@ -8406,15 +8406,15 @@
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!$D$64/12+N30</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q30" s="63">
         <f>$F30*Outputs_Internal!K$64/12+N30*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R30" s="63">
         <f>$F30*Outputs_Internal!L$64/12+N30*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S30" s="63">
         <f>N30*'MARA Prices'!$F$4</f>
@@ -8480,11 +8480,11 @@
       </c>
       <c r="E31" s="64">
         <f>IF(B31=Inputs!$C$1,D31,E30)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F31" s="64">
         <f>IF(AND(B31&gt;=Inputs!$C$1,B31&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E31,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G31" s="64">
         <f>IF(AND(B31&gt;=Inputs!$C$1,B31&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B31,"Y")+1, 0),0)</f>
@@ -8512,15 +8512,15 @@
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!$D$64/12+N31</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q31" s="63">
         <f>$F31*Outputs_Internal!K$64/12+N31*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R31" s="63">
         <f>$F31*Outputs_Internal!L$64/12+N31*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S31" s="63">
         <f>N31*'MARA Prices'!$F$4</f>
@@ -8586,11 +8586,11 @@
       </c>
       <c r="E32" s="64">
         <f>IF(B32=Inputs!$C$1,D32,E31)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F32" s="64">
         <f>IF(AND(B32&gt;=Inputs!$C$1,B32&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E32,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G32" s="64">
         <f>IF(AND(B32&gt;=Inputs!$C$1,B32&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B32,"Y")+1, 0),0)</f>
@@ -8618,15 +8618,15 @@
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!$D$64/12+N32</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q32" s="63">
         <f>$F32*Outputs_Internal!K$64/12+N32*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R32" s="63">
         <f>$F32*Outputs_Internal!L$64/12+N32*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S32" s="63">
         <f>N32*'MARA Prices'!$F$4</f>
@@ -8642,15 +8642,15 @@
       </c>
       <c r="W32" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>16994.8125</v>
       </c>
       <c r="X32" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y32" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z32" s="63">
         <f t="shared" si="5"/>
@@ -8692,11 +8692,11 @@
       </c>
       <c r="E33" s="64">
         <f>IF(B33=Inputs!$C$1,D33,E32)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F33" s="64">
         <f>IF(AND(B33&gt;=Inputs!$C$1,B33&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E33,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G33" s="64">
         <f>IF(AND(B33&gt;=Inputs!$C$1,B33&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B33,"Y")+1, 0),0)</f>
@@ -8724,15 +8724,15 @@
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!$D$64/12+N33</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q33" s="63">
         <f>$F33*Outputs_Internal!K$64/12+N33*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R33" s="63">
         <f>$F33*Outputs_Internal!L$64/12+N33*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S33" s="63">
         <f>N33*'MARA Prices'!$F$4</f>
@@ -8798,11 +8798,11 @@
       </c>
       <c r="E34" s="64">
         <f>IF(B34=Inputs!$C$1,D34,E33)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F34" s="64">
         <f>IF(AND(B34&gt;=Inputs!$C$1,B34&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E34,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G34" s="64">
         <f>IF(AND(B34&gt;=Inputs!$C$1,B34&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B34,"Y")+1, 0),0)</f>
@@ -8830,15 +8830,15 @@
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!$D$64/12+N34</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q34" s="63">
         <f>$F34*Outputs_Internal!K$64/12+N34*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R34" s="63">
         <f>$F34*Outputs_Internal!L$64/12+N34*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S34" s="63">
         <f>N34*'MARA Prices'!$F$4</f>
@@ -8904,11 +8904,11 @@
       </c>
       <c r="E35" s="64">
         <f>IF(B35=Inputs!$C$1,D35,E34)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F35" s="64">
         <f>IF(AND(B35&gt;=Inputs!$C$1,B35&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E35,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G35" s="64">
         <f>IF(AND(B35&gt;=Inputs!$C$1,B35&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B35,"Y")+1, 0),0)</f>
@@ -8936,15 +8936,15 @@
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!$D$64/12+N35</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q35" s="63">
         <f>$F35*Outputs_Internal!K$64/12+N35*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R35" s="63">
         <f>$F35*Outputs_Internal!L$64/12+N35*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S35" s="63">
         <f>N35*'MARA Prices'!$F$4</f>
@@ -8960,15 +8960,15 @@
       </c>
       <c r="W35" s="63">
         <f t="shared" si="2"/>
-        <v>13987.5</v>
+        <v>16994.8125</v>
       </c>
       <c r="X35" s="63">
         <f t="shared" si="3"/>
-        <v>4405.3448275862074</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y35" s="63">
         <f t="shared" si="4"/>
-        <v>9582.1551724137935</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z35" s="63">
         <f t="shared" si="5"/>
@@ -9010,11 +9010,11 @@
       </c>
       <c r="E36" s="64">
         <f>IF(B36=Inputs!$C$1,D36,E35)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F36" s="64">
         <f>IF(AND(B36&gt;=Inputs!$C$1,B36&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E36,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G36" s="64">
         <f>IF(AND(B36&gt;=Inputs!$C$1,B36&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B36,"Y")+1, 0),0)</f>
@@ -9042,15 +9042,15 @@
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!$D$64/12+N36</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q36" s="63">
         <f>$F36*Outputs_Internal!K$64/12+N36*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R36" s="63">
         <f>$F36*Outputs_Internal!L$64/12+N36*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S36" s="63">
         <f>N36*'MARA Prices'!$F$4</f>
@@ -9116,11 +9116,11 @@
       </c>
       <c r="E37" s="64">
         <f>IF(B37=Inputs!$C$1,D37,E36)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F37" s="64">
         <f>IF(AND(B37&gt;=Inputs!$C$1,B37&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E37,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G37" s="64">
         <f>IF(AND(B37&gt;=Inputs!$C$1,B37&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B37,"Y")+1, 0),0)</f>
@@ -9148,15 +9148,15 @@
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!$D$64/12+N37</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q37" s="63">
         <f>$F37*Outputs_Internal!K$64/12+N37*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R37" s="63">
         <f>$F37*Outputs_Internal!L$64/12+N37*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S37" s="63">
         <f>N37*'MARA Prices'!$F$4</f>
@@ -9222,11 +9222,11 @@
       </c>
       <c r="E38" s="64">
         <f>IF(B38=Inputs!$C$1,D38,E37)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F38" s="64">
         <f>IF(AND(B38&gt;=Inputs!$C$1,B38&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E38,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G38" s="64">
         <f>IF(AND(B38&gt;=Inputs!$C$1,B38&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B38,"Y")+1, 0),0)</f>
@@ -9254,15 +9254,15 @@
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!$D$64/12+N38</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q38" s="63">
         <f>$F38*Outputs_Internal!K$64/12+N38*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R38" s="63">
         <f>$F38*Outputs_Internal!L$64/12+N38*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S38" s="63">
         <f>N38*'MARA Prices'!$F$4</f>
@@ -9278,15 +9278,15 @@
       </c>
       <c r="W38" s="63">
         <f t="shared" si="7"/>
-        <v>13987.5</v>
+        <v>16994.8125</v>
       </c>
       <c r="X38" s="63">
         <f t="shared" si="8"/>
-        <v>4405.3448275862074</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y38" s="63">
         <f t="shared" si="9"/>
-        <v>9582.1551724137935</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z38" s="63">
         <f t="shared" si="10"/>
@@ -9328,11 +9328,11 @@
       </c>
       <c r="E39" s="64">
         <f>IF(B39=Inputs!$C$1,D39,E38)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F39" s="64">
         <f>IF(AND(B39&gt;=Inputs!$C$1,B39&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E39,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G39" s="64">
         <f>IF(AND(B39&gt;=Inputs!$C$1,B39&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B39,"Y")+1, 0),0)</f>
@@ -9360,15 +9360,15 @@
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!$D$64/12+N39</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q39" s="63">
         <f>$F39*Outputs_Internal!K$64/12+N39*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R39" s="63">
         <f>$F39*Outputs_Internal!L$64/12+N39*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S39" s="63">
         <f>N39*'MARA Prices'!$F$4</f>
@@ -9434,11 +9434,11 @@
       </c>
       <c r="E40" s="64">
         <f>IF(B40=Inputs!$C$1,D40,E39)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F40" s="64">
         <f>IF(AND(B40&gt;=Inputs!$C$1,B40&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E40,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G40" s="64">
         <f>IF(AND(B40&gt;=Inputs!$C$1,B40&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B40,"Y")+1, 0),0)</f>
@@ -9466,15 +9466,15 @@
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!$D$64/12+N40</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q40" s="63">
         <f>$F40*Outputs_Internal!K$64/12+N40*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R40" s="63">
         <f>$F40*Outputs_Internal!L$64/12+N40*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S40" s="63">
         <f>N40*'MARA Prices'!$F$4</f>
@@ -9540,11 +9540,11 @@
       </c>
       <c r="E41" s="64">
         <f>IF(B41=Inputs!$C$1,D41,E40)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F41" s="64">
         <f>IF(AND(B41&gt;=Inputs!$C$1,B41&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E41,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G41" s="64">
         <f>IF(AND(B41&gt;=Inputs!$C$1,B41&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B41,"Y")+1, 0),0)</f>
@@ -9572,15 +9572,15 @@
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!$D$64/12+N41</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q41" s="63">
         <f>$F41*Outputs_Internal!K$64/12+N41*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R41" s="63">
         <f>$F41*Outputs_Internal!L$64/12+N41*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S41" s="63">
         <f>N41*'MARA Prices'!$F$4</f>
@@ -9596,15 +9596,15 @@
       </c>
       <c r="W41" s="63">
         <f t="shared" si="7"/>
-        <v>13987.5</v>
+        <v>16994.8125</v>
       </c>
       <c r="X41" s="63">
         <f t="shared" si="8"/>
-        <v>4405.3448275862074</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y41" s="63">
         <f t="shared" si="9"/>
-        <v>9582.1551724137935</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z41" s="63">
         <f t="shared" si="10"/>
@@ -9646,11 +9646,11 @@
       </c>
       <c r="E42" s="64">
         <f>IF(B42=Inputs!$C$1,D42,E41)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F42" s="64">
         <f>IF(AND(B42&gt;=Inputs!$C$1,B42&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E42,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G42" s="64">
         <f>IF(AND(B42&gt;=Inputs!$C$1,B42&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B42,"Y")+1, 0),0)</f>
@@ -9678,15 +9678,15 @@
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!$D$64/12+N42</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q42" s="63">
         <f>$F42*Outputs_Internal!K$64/12+N42*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R42" s="63">
         <f>$F42*Outputs_Internal!L$64/12+N42*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S42" s="63">
         <f>N42*'MARA Prices'!$F$4</f>
@@ -9752,11 +9752,11 @@
       </c>
       <c r="E43" s="64">
         <f>IF(B43=Inputs!$C$1,D43,E42)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F43" s="64">
         <f>IF(AND(B43&gt;=Inputs!$C$1,B43&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E43,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G43" s="64">
         <f>IF(AND(B43&gt;=Inputs!$C$1,B43&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B43,"Y")+1, 0),0)</f>
@@ -9784,15 +9784,15 @@
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!$D$64/12+N43</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q43" s="63">
         <f>$F43*Outputs_Internal!K$64/12+N43*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R43" s="63">
         <f>$F43*Outputs_Internal!L$64/12+N43*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S43" s="63">
         <f>N43*'MARA Prices'!$F$4</f>
@@ -9858,11 +9858,11 @@
       </c>
       <c r="E44" s="64">
         <f>IF(B44=Inputs!$C$1,D44,E43)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F44" s="64">
         <f>IF(AND(B44&gt;=Inputs!$C$1,B44&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E44,0)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="G44" s="64">
         <f>IF(AND(B44&gt;=Inputs!$C$1,B44&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B44,"Y")+1, 0),0)</f>
@@ -9890,15 +9890,15 @@
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!$D$64/12+N44</f>
-        <v>4662.5</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q44" s="63">
         <f>$F44*Outputs_Internal!K$64/12+N44*'MARA Prices'!$F$5</f>
-        <v>1468.4482758620691</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R44" s="63">
         <f>$F44*Outputs_Internal!L$64/12+N44*'MARA Prices'!$F$6</f>
-        <v>3194.0517241379312</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S44" s="63">
         <f>N44*'MARA Prices'!$F$4</f>
@@ -9914,15 +9914,15 @@
       </c>
       <c r="W44" s="63">
         <f t="shared" si="7"/>
-        <v>13987.5</v>
+        <v>16994.8125</v>
       </c>
       <c r="X44" s="63">
         <f t="shared" si="8"/>
-        <v>4405.3448275862074</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y44" s="63">
         <f t="shared" si="9"/>
-        <v>9582.1551724137935</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z44" s="63">
         <f t="shared" si="10"/>
@@ -9964,15 +9964,15 @@
       </c>
       <c r="E45" s="64">
         <f>IF(B45=Inputs!$C$1,D45,E44)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F45" s="64">
         <f>IF(AND(B45&gt;=Inputs!$C$1,B45&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E45,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G45" s="64">
         <f>IF(AND(B45&gt;=Inputs!$C$1,B45&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B45,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I45" s="63">
         <f>IF($B45=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D45</f>
@@ -9996,15 +9996,15 @@
       </c>
       <c r="P45" s="63">
         <f>$F45*Outputs_Internal!$D$64/12+N45</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q45" s="63">
         <f>$F45*Outputs_Internal!K$64/12+N45*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R45" s="63">
         <f>$F45*Outputs_Internal!L$64/12+N45*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S45" s="63">
         <f>N45*'MARA Prices'!$F$4</f>
@@ -10070,15 +10070,15 @@
       </c>
       <c r="E46" s="64">
         <f>IF(B46=Inputs!$C$1,D46,E45)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F46" s="64">
         <f>IF(AND(B46&gt;=Inputs!$C$1,B46&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E46,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G46" s="64">
         <f>IF(AND(B46&gt;=Inputs!$C$1,B46&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B46,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I46" s="63">
         <f>IF($B46=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D46</f>
@@ -10102,15 +10102,15 @@
       </c>
       <c r="P46" s="63">
         <f>$F46*Outputs_Internal!$D$64/12+N46</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q46" s="63">
         <f>$F46*Outputs_Internal!K$64/12+N46*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R46" s="63">
         <f>$F46*Outputs_Internal!L$64/12+N46*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S46" s="63">
         <f>N46*'MARA Prices'!$F$4</f>
@@ -10176,15 +10176,15 @@
       </c>
       <c r="E47" s="64">
         <f>IF(B47=Inputs!$C$1,D47,E46)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F47" s="64">
         <f>IF(AND(B47&gt;=Inputs!$C$1,B47&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E47,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G47" s="64">
         <f>IF(AND(B47&gt;=Inputs!$C$1,B47&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B47,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I47" s="63">
         <f>IF($B47=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D47</f>
@@ -10208,15 +10208,15 @@
       </c>
       <c r="P47" s="63">
         <f>$F47*Outputs_Internal!$D$64/12+N47</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q47" s="63">
         <f>$F47*Outputs_Internal!K$64/12+N47*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R47" s="63">
         <f>$F47*Outputs_Internal!L$64/12+N47*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S47" s="63">
         <f>N47*'MARA Prices'!$F$4</f>
@@ -10232,15 +10232,15 @@
       </c>
       <c r="W47" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X47" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y47" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z47" s="63">
         <f t="shared" si="10"/>
@@ -10282,15 +10282,15 @@
       </c>
       <c r="E48" s="64">
         <f>IF(B48=Inputs!$C$1,D48,E47)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F48" s="64">
         <f>IF(AND(B48&gt;=Inputs!$C$1,B48&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E48,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G48" s="64">
         <f>IF(AND(B48&gt;=Inputs!$C$1,B48&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B48,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I48" s="63">
         <f>IF($B48=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D48</f>
@@ -10314,15 +10314,15 @@
       </c>
       <c r="P48" s="63">
         <f>$F48*Outputs_Internal!$D$64/12+N48</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q48" s="63">
         <f>$F48*Outputs_Internal!K$64/12+N48*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R48" s="63">
         <f>$F48*Outputs_Internal!L$64/12+N48*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S48" s="63">
         <f>N48*'MARA Prices'!$F$4</f>
@@ -10388,15 +10388,15 @@
       </c>
       <c r="E49" s="64">
         <f>IF(B49=Inputs!$C$1,D49,E48)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F49" s="64">
         <f>IF(AND(B49&gt;=Inputs!$C$1,B49&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E49,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G49" s="64">
         <f>IF(AND(B49&gt;=Inputs!$C$1,B49&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B49,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I49" s="63">
         <f>IF($B49=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D49</f>
@@ -10420,15 +10420,15 @@
       </c>
       <c r="P49" s="63">
         <f>$F49*Outputs_Internal!$D$64/12+N49</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q49" s="63">
         <f>$F49*Outputs_Internal!K$64/12+N49*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R49" s="63">
         <f>$F49*Outputs_Internal!L$64/12+N49*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S49" s="63">
         <f>N49*'MARA Prices'!$F$4</f>
@@ -10494,15 +10494,15 @@
       </c>
       <c r="E50" s="64">
         <f>IF(B50=Inputs!$C$1,D50,E49)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F50" s="64">
         <f>IF(AND(B50&gt;=Inputs!$C$1,B50&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E50,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G50" s="64">
         <f>IF(AND(B50&gt;=Inputs!$C$1,B50&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B50,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I50" s="63">
         <f>IF($B50=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D50</f>
@@ -10526,15 +10526,15 @@
       </c>
       <c r="P50" s="63">
         <f>$F50*Outputs_Internal!$D$64/12+N50</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q50" s="63">
         <f>$F50*Outputs_Internal!K$64/12+N50*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R50" s="63">
         <f>$F50*Outputs_Internal!L$64/12+N50*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S50" s="63">
         <f>N50*'MARA Prices'!$F$4</f>
@@ -10550,15 +10550,15 @@
       </c>
       <c r="W50" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X50" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y50" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z50" s="63">
         <f t="shared" si="10"/>
@@ -10600,15 +10600,15 @@
       </c>
       <c r="E51" s="64">
         <f>IF(B51=Inputs!$C$1,D51,E50)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F51" s="64">
         <f>IF(AND(B51&gt;=Inputs!$C$1,B51&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E51,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G51" s="64">
         <f>IF(AND(B51&gt;=Inputs!$C$1,B51&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B51,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I51" s="63">
         <f>IF($B51=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D51</f>
@@ -10632,15 +10632,15 @@
       </c>
       <c r="P51" s="63">
         <f>$F51*Outputs_Internal!$D$64/12+N51</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q51" s="63">
         <f>$F51*Outputs_Internal!K$64/12+N51*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R51" s="63">
         <f>$F51*Outputs_Internal!L$64/12+N51*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S51" s="63">
         <f>N51*'MARA Prices'!$F$4</f>
@@ -10706,15 +10706,15 @@
       </c>
       <c r="E52" s="64">
         <f>IF(B52=Inputs!$C$1,D52,E51)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F52" s="64">
         <f>IF(AND(B52&gt;=Inputs!$C$1,B52&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E52,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G52" s="64">
         <f>IF(AND(B52&gt;=Inputs!$C$1,B52&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B52,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I52" s="63">
         <f>IF($B52=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D52</f>
@@ -10738,15 +10738,15 @@
       </c>
       <c r="P52" s="63">
         <f>$F52*Outputs_Internal!$D$64/12+N52</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q52" s="63">
         <f>$F52*Outputs_Internal!K$64/12+N52*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R52" s="63">
         <f>$F52*Outputs_Internal!L$64/12+N52*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S52" s="63">
         <f>N52*'MARA Prices'!$F$4</f>
@@ -10812,15 +10812,15 @@
       </c>
       <c r="E53" s="64">
         <f>IF(B53=Inputs!$C$1,D53,E52)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F53" s="64">
         <f>IF(AND(B53&gt;=Inputs!$C$1,B53&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E53,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G53" s="64">
         <f>IF(AND(B53&gt;=Inputs!$C$1,B53&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B53,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I53" s="63">
         <f>IF($B53=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D53</f>
@@ -10844,15 +10844,15 @@
       </c>
       <c r="P53" s="63">
         <f>$F53*Outputs_Internal!$D$64/12+N53</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q53" s="63">
         <f>$F53*Outputs_Internal!K$64/12+N53*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R53" s="63">
         <f>$F53*Outputs_Internal!L$64/12+N53*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S53" s="63">
         <f>N53*'MARA Prices'!$F$4</f>
@@ -10868,15 +10868,15 @@
       </c>
       <c r="W53" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X53" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y53" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z53" s="63">
         <f t="shared" si="10"/>
@@ -10918,15 +10918,15 @@
       </c>
       <c r="E54" s="64">
         <f>IF(B54=Inputs!$C$1,D54,E53)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F54" s="64">
         <f>IF(AND(B54&gt;=Inputs!$C$1,B54&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E54,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G54" s="64">
         <f>IF(AND(B54&gt;=Inputs!$C$1,B54&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B54,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I54" s="63">
         <f>IF($B54=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D54</f>
@@ -10950,15 +10950,15 @@
       </c>
       <c r="P54" s="63">
         <f>$F54*Outputs_Internal!$D$64/12+N54</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q54" s="63">
         <f>$F54*Outputs_Internal!K$64/12+N54*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R54" s="63">
         <f>$F54*Outputs_Internal!L$64/12+N54*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S54" s="63">
         <f>N54*'MARA Prices'!$F$4</f>
@@ -11024,15 +11024,15 @@
       </c>
       <c r="E55" s="64">
         <f>IF(B55=Inputs!$C$1,D55,E54)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F55" s="64">
         <f>IF(AND(B55&gt;=Inputs!$C$1,B55&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E55,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G55" s="64">
         <f>IF(AND(B55&gt;=Inputs!$C$1,B55&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B55,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I55" s="63">
         <f>IF($B55=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D55</f>
@@ -11056,15 +11056,15 @@
       </c>
       <c r="P55" s="63">
         <f>$F55*Outputs_Internal!$D$64/12+N55</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q55" s="63">
         <f>$F55*Outputs_Internal!K$64/12+N55*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R55" s="63">
         <f>$F55*Outputs_Internal!L$64/12+N55*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S55" s="63">
         <f>N55*'MARA Prices'!$F$4</f>
@@ -11130,15 +11130,15 @@
       </c>
       <c r="E56" s="64">
         <f>IF(B56=Inputs!$C$1,D56,E55)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F56" s="64">
         <f>IF(AND(B56&gt;=Inputs!$C$1,B56&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E56,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G56" s="64">
         <f>IF(AND(B56&gt;=Inputs!$C$1,B56&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B56,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1025</v>
       </c>
       <c r="I56" s="63">
         <f>IF($B56=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D56</f>
@@ -11162,15 +11162,15 @@
       </c>
       <c r="P56" s="63">
         <f>$F56*Outputs_Internal!$D$64/12+N56</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q56" s="63">
         <f>$F56*Outputs_Internal!K$64/12+N56*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R56" s="63">
         <f>$F56*Outputs_Internal!L$64/12+N56*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S56" s="63">
         <f>N56*'MARA Prices'!$F$4</f>
@@ -11186,15 +11186,15 @@
       </c>
       <c r="W56" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X56" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y56" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z56" s="63">
         <f t="shared" si="10"/>
@@ -11236,15 +11236,15 @@
       </c>
       <c r="E57" s="64">
         <f>IF(B57=Inputs!$C$1,D57,E56)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F57" s="64">
         <f>IF(AND(B57&gt;=Inputs!$C$1,B57&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E57,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G57" s="64">
         <f>IF(AND(B57&gt;=Inputs!$C$1,B57&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B57,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I57" s="63">
         <f>IF($B57=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D57</f>
@@ -11268,15 +11268,15 @@
       </c>
       <c r="P57" s="63">
         <f>$F57*Outputs_Internal!$D$64/12+N57</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q57" s="63">
         <f>$F57*Outputs_Internal!K$64/12+N57*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R57" s="63">
         <f>$F57*Outputs_Internal!L$64/12+N57*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S57" s="63">
         <f>N57*'MARA Prices'!$F$4</f>
@@ -11342,15 +11342,15 @@
       </c>
       <c r="E58" s="64">
         <f>IF(B58=Inputs!$C$1,D58,E57)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F58" s="64">
         <f>IF(AND(B58&gt;=Inputs!$C$1,B58&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E58,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G58" s="64">
         <f>IF(AND(B58&gt;=Inputs!$C$1,B58&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B58,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I58" s="63">
         <f>IF($B58=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D58</f>
@@ -11374,15 +11374,15 @@
       </c>
       <c r="P58" s="63">
         <f>$F58*Outputs_Internal!$D$64/12+N58</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q58" s="63">
         <f>$F58*Outputs_Internal!K$64/12+N58*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R58" s="63">
         <f>$F58*Outputs_Internal!L$64/12+N58*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S58" s="63">
         <f>N58*'MARA Prices'!$F$4</f>
@@ -11448,15 +11448,15 @@
       </c>
       <c r="E59" s="64">
         <f>IF(B59=Inputs!$C$1,D59,E58)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F59" s="64">
         <f>IF(AND(B59&gt;=Inputs!$C$1,B59&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E59,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G59" s="64">
         <f>IF(AND(B59&gt;=Inputs!$C$1,B59&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B59,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I59" s="63">
         <f>IF($B59=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D59</f>
@@ -11480,15 +11480,15 @@
       </c>
       <c r="P59" s="63">
         <f>$F59*Outputs_Internal!$D$64/12+N59</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q59" s="63">
         <f>$F59*Outputs_Internal!K$64/12+N59*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R59" s="63">
         <f>$F59*Outputs_Internal!L$64/12+N59*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S59" s="63">
         <f>N59*'MARA Prices'!$F$4</f>
@@ -11504,15 +11504,15 @@
       </c>
       <c r="W59" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X59" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y59" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z59" s="63">
         <f t="shared" si="10"/>
@@ -11554,15 +11554,15 @@
       </c>
       <c r="E60" s="64">
         <f>IF(B60=Inputs!$C$1,D60,E59)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F60" s="64">
         <f>IF(AND(B60&gt;=Inputs!$C$1,B60&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E60,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G60" s="64">
         <f>IF(AND(B60&gt;=Inputs!$C$1,B60&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B60,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I60" s="63">
         <f>IF($B60=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D60</f>
@@ -11586,15 +11586,15 @@
       </c>
       <c r="P60" s="63">
         <f>$F60*Outputs_Internal!$D$64/12+N60</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q60" s="63">
         <f>$F60*Outputs_Internal!K$64/12+N60*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R60" s="63">
         <f>$F60*Outputs_Internal!L$64/12+N60*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S60" s="63">
         <f>N60*'MARA Prices'!$F$4</f>
@@ -11660,15 +11660,15 @@
       </c>
       <c r="E61" s="64">
         <f>IF(B61=Inputs!$C$1,D61,E60)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F61" s="64">
         <f>IF(AND(B61&gt;=Inputs!$C$1,B61&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E61,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G61" s="64">
         <f>IF(AND(B61&gt;=Inputs!$C$1,B61&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B61,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I61" s="63">
         <f>IF($B61=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D61</f>
@@ -11692,15 +11692,15 @@
       </c>
       <c r="P61" s="63">
         <f>$F61*Outputs_Internal!$D$64/12+N61</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q61" s="63">
         <f>$F61*Outputs_Internal!K$64/12+N61*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R61" s="63">
         <f>$F61*Outputs_Internal!L$64/12+N61*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S61" s="63">
         <f>N61*'MARA Prices'!$F$4</f>
@@ -11766,15 +11766,15 @@
       </c>
       <c r="E62" s="64">
         <f>IF(B62=Inputs!$C$1,D62,E61)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F62" s="64">
         <f>IF(AND(B62&gt;=Inputs!$C$1,B62&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E62,0)</f>
-        <v>0</v>
+        <v>1.0125</v>
       </c>
       <c r="G62" s="64">
         <f>IF(AND(B62&gt;=Inputs!$C$1,B62&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),(1+'MARA Prices'!$F$1)^IFERROR(DATEDIF('MARA Prices'!$F$2,B62,"Y")+1, 0),0)</f>
-        <v>0</v>
+        <v>1.1576250000000001</v>
       </c>
       <c r="I62" s="63">
         <f>IF($B62=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D62</f>
@@ -11798,15 +11798,15 @@
       </c>
       <c r="P62" s="63">
         <f>$F62*Outputs_Internal!$D$64/12+N62</f>
-        <v>0</v>
+        <v>5664.9375</v>
       </c>
       <c r="Q62" s="63">
         <f>$F62*Outputs_Internal!K$64/12+N62*'MARA Prices'!$F$5</f>
-        <v>0</v>
+        <v>1784.1646551724136</v>
       </c>
       <c r="R62" s="63">
         <f>$F62*Outputs_Internal!L$64/12+N62*'MARA Prices'!$F$6</f>
-        <v>0</v>
+        <v>3880.7728448275861</v>
       </c>
       <c r="S62" s="63">
         <f>N62*'MARA Prices'!$F$4</f>
@@ -11822,15 +11822,15 @@
       </c>
       <c r="W62" s="63">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16994.8125</v>
       </c>
       <c r="X62" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5352.4939655172411</v>
       </c>
       <c r="Y62" s="63">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>11642.318534482758</v>
       </c>
       <c r="Z62" s="63">
         <f t="shared" si="10"/>
@@ -11872,7 +11872,7 @@
       </c>
       <c r="E63" s="64">
         <f>IF(B63=Inputs!$C$1,D63,E62)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F63" s="64">
         <f>IF(AND(B63&gt;=Inputs!$C$1,B63&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E63,0)</f>
@@ -11978,7 +11978,7 @@
       </c>
       <c r="E64" s="64">
         <f>IF(B64=Inputs!$C$1,D64,E63)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F64" s="64">
         <f>IF(AND(B64&gt;=Inputs!$C$1,B64&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E64,0)</f>
@@ -12084,7 +12084,7 @@
       </c>
       <c r="E65" s="64">
         <f>IF(B65=Inputs!$C$1,D65,E64)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F65" s="64">
         <f>IF(AND(B65&gt;=Inputs!$C$1,B65&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E65,0)</f>
@@ -12190,7 +12190,7 @@
       </c>
       <c r="E66" s="64">
         <f>IF(B66=Inputs!$C$1,D66,E65)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F66" s="64">
         <f>IF(AND(B66&gt;=Inputs!$C$1,B66&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E66,0)</f>
@@ -12296,7 +12296,7 @@
       </c>
       <c r="E67" s="64">
         <f>IF(B67=Inputs!$C$1,D67,E66)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F67" s="64">
         <f>IF(AND(B67&gt;=Inputs!$C$1,B67&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E67,0)</f>
@@ -12402,7 +12402,7 @@
       </c>
       <c r="E68" s="64">
         <f>IF(B68=Inputs!$C$1,D68,E67)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F68" s="64">
         <f>IF(AND(B68&gt;=Inputs!$C$1,B68&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E68,0)</f>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="E69" s="64">
         <f>IF(B69=Inputs!$C$1,D69,E68)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F69" s="64">
         <f>IF(AND(B69&gt;=Inputs!$C$1,B69&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E69,0)</f>
@@ -12614,7 +12614,7 @@
       </c>
       <c r="E70" s="64">
         <f>IF(B70=Inputs!$C$1,D70,E69)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F70" s="64">
         <f>IF(AND(B70&gt;=Inputs!$C$1,B70&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E70,0)</f>
@@ -12720,7 +12720,7 @@
       </c>
       <c r="E71" s="64">
         <f>IF(B71=Inputs!$C$1,D71,E70)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F71" s="64">
         <f>IF(AND(B71&gt;=Inputs!$C$1,B71&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E71,0)</f>
@@ -12826,7 +12826,7 @@
       </c>
       <c r="E72" s="64">
         <f>IF(B72=Inputs!$C$1,D72,E71)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F72" s="64">
         <f>IF(AND(B72&gt;=Inputs!$C$1,B72&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E72,0)</f>
@@ -12932,7 +12932,7 @@
       </c>
       <c r="E73" s="64">
         <f>IF(B73=Inputs!$C$1,D73,E72)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F73" s="64">
         <f>IF(AND(B73&gt;=Inputs!$C$1,B73&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E73,0)</f>
@@ -13038,7 +13038,7 @@
       </c>
       <c r="E74" s="64">
         <f>IF(B74=Inputs!$C$1,D74,E73)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F74" s="64">
         <f>IF(AND(B74&gt;=Inputs!$C$1,B74&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E74,0)</f>
@@ -13144,7 +13144,7 @@
       </c>
       <c r="E75" s="64">
         <f>IF(B75=Inputs!$C$1,D75,E74)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F75" s="64">
         <f>IF(AND(B75&gt;=Inputs!$C$1,B75&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E75,0)</f>
@@ -13250,7 +13250,7 @@
       </c>
       <c r="E76" s="64">
         <f>IF(B76=Inputs!$C$1,D76,E75)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F76" s="64">
         <f>IF(AND(B76&gt;=Inputs!$C$1,B76&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E76,0)</f>
@@ -13356,7 +13356,7 @@
       </c>
       <c r="E77" s="64">
         <f>IF(B77=Inputs!$C$1,D77,E76)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F77" s="64">
         <f>IF(AND(B77&gt;=Inputs!$C$1,B77&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E77,0)</f>
@@ -13462,7 +13462,7 @@
       </c>
       <c r="E78" s="64">
         <f>IF(B78=Inputs!$C$1,D78,E77)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F78" s="64">
         <f>IF(AND(B78&gt;=Inputs!$C$1,B78&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E78,0)</f>
@@ -13568,7 +13568,7 @@
       </c>
       <c r="E79" s="64">
         <f>IF(B79=Inputs!$C$1,D79,E78)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F79" s="64">
         <f>IF(AND(B79&gt;=Inputs!$C$1,B79&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E79,0)</f>
@@ -13674,7 +13674,7 @@
       </c>
       <c r="E80" s="64">
         <f>IF(B80=Inputs!$C$1,D80,E79)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F80" s="64">
         <f>IF(AND(B80&gt;=Inputs!$C$1,B80&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E80,0)</f>
@@ -13780,7 +13780,7 @@
       </c>
       <c r="E81" s="64">
         <f>IF(B81=Inputs!$C$1,D81,E80)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F81" s="64">
         <f>IF(AND(B81&gt;=Inputs!$C$1,B81&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E81,0)</f>
@@ -13886,7 +13886,7 @@
       </c>
       <c r="E82" s="64">
         <f>IF(B82=Inputs!$C$1,D82,E81)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F82" s="64">
         <f>IF(AND(B82&gt;=Inputs!$C$1,B82&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E82,0)</f>
@@ -13992,7 +13992,7 @@
       </c>
       <c r="E83" s="64">
         <f>IF(B83=Inputs!$C$1,D83,E82)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F83" s="64">
         <f>IF(AND(B83&gt;=Inputs!$C$1,B83&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E83,0)</f>
@@ -14098,7 +14098,7 @@
       </c>
       <c r="E84" s="64">
         <f>IF(B84=Inputs!$C$1,D84,E83)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F84" s="64">
         <f>IF(AND(B84&gt;=Inputs!$C$1,B84&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E84,0)</f>
@@ -14204,7 +14204,7 @@
       </c>
       <c r="E85" s="64">
         <f>IF(B85=Inputs!$C$1,D85,E84)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F85" s="64">
         <f>IF(AND(B85&gt;=Inputs!$C$1,B85&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E85,0)</f>
@@ -14310,7 +14310,7 @@
       </c>
       <c r="E86" s="64">
         <f>IF(B86=Inputs!$C$1,D86,E85)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F86" s="64">
         <f>IF(AND(B86&gt;=Inputs!$C$1,B86&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E86,0)</f>
@@ -14416,7 +14416,7 @@
       </c>
       <c r="E87" s="64">
         <f>IF(B87=Inputs!$C$1,D87,E86)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F87" s="64">
         <f>IF(AND(B87&gt;=Inputs!$C$1,B87&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E87,0)</f>
@@ -14522,7 +14522,7 @@
       </c>
       <c r="E88" s="64">
         <f>IF(B88=Inputs!$C$1,D88,E87)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F88" s="64">
         <f>IF(AND(B88&gt;=Inputs!$C$1,B88&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E88,0)</f>
@@ -14628,7 +14628,7 @@
       </c>
       <c r="E89" s="64">
         <f>IF(B89=Inputs!$C$1,D89,E88)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F89" s="64">
         <f>IF(AND(B89&gt;=Inputs!$C$1,B89&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E89,0)</f>
@@ -14734,7 +14734,7 @@
       </c>
       <c r="E90" s="64">
         <f>IF(B90=Inputs!$C$1,D90,E89)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F90" s="64">
         <f>IF(AND(B90&gt;=Inputs!$C$1,B90&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E90,0)</f>
@@ -14840,7 +14840,7 @@
       </c>
       <c r="E91" s="64">
         <f>IF(B91=Inputs!$C$1,D91,E90)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F91" s="64">
         <f>IF(AND(B91&gt;=Inputs!$C$1,B91&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E91,0)</f>
@@ -14946,7 +14946,7 @@
       </c>
       <c r="E92" s="64">
         <f>IF(B92=Inputs!$C$1,D92,E91)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F92" s="64">
         <f>IF(AND(B92&gt;=Inputs!$C$1,B92&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E92,0)</f>
@@ -15052,7 +15052,7 @@
       </c>
       <c r="E93" s="64">
         <f>IF(B93=Inputs!$C$1,D93,E92)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F93" s="64">
         <f>IF(AND(B93&gt;=Inputs!$C$1,B93&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E93,0)</f>
@@ -15158,7 +15158,7 @@
       </c>
       <c r="E94" s="64">
         <f>IF(B94=Inputs!$C$1,D94,E93)</f>
-        <v>1</v>
+        <v>1.0125</v>
       </c>
       <c r="F94" s="64">
         <f>IF(AND(B94&gt;=Inputs!$C$1,B94&lt;EDATE(Inputs!$C$1,Inputs!$C$2)),E94,0)</f>
@@ -15579,7 +15579,7 @@
       </c>
       <c r="D14" s="16">
         <f>IF(Inputs!D7="Y", Prices!$C$6, IF(Inputs!D7="N", Prices!$D$6, 0))</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="E14" s="16">
         <f>IF(Inputs!E7="Y", Prices!$C$6, IF(Inputs!E7="N", Prices!$D$6, 0))</f>
@@ -15779,7 +15779,7 @@
       </c>
       <c r="D22" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D20="Y",Inputs!D$25="Y",Inputs!D$26="Y"), Prices!$C17, 0)</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="E22" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!E20="Y",Inputs!E$25="Y",Inputs!E$26="Y"), Prices!$C17, 0)</f>
@@ -15804,7 +15804,7 @@
       </c>
       <c r="D23" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D21="Y",Inputs!D$25="Y",Inputs!D$26="Y",Inputs!D$29="Y"), Prices!$C18, 0)</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="E23" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!E21="Y",Inputs!E$25="Y",Inputs!E$26="Y",Inputs!E$29="Y"), Prices!$C18, 0)</f>
@@ -15829,7 +15829,7 @@
       </c>
       <c r="D24" s="20">
         <f>IF(Inputs!D$7="N",0, IF(OR(Inputs!D22="Y",Inputs!D$25="Y",Inputs!D$26="Y"), Prices!$C19, 0))</f>
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="E24" s="20">
         <f>IF(Inputs!E$7="N",0, IF(OR(Inputs!E22="Y",Inputs!E$25="Y",Inputs!E$26="Y"), Prices!$C19, 0))</f>
@@ -16141,7 +16141,7 @@
       </c>
       <c r="D40" s="16">
         <f>IF(Inputs!D7="Y", Prices!$C$6, IF(Inputs!D7="N", Prices!$D$6, 0))</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="E40" s="16">
         <f>IF(Inputs!E7="Y", Prices!$C$6, IF(Inputs!E7="N", Prices!$D$6, 0))</f>
@@ -16696,7 +16696,7 @@
       </c>
       <c r="D66" s="18">
         <f>IF(Inputs!D$24 = "Y", 0, IF(Inputs!D23="Y", Prices!$C21, 0))</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="E66" s="18">
         <f>IF(Inputs!E$24 = "Y", 0, IF(Inputs!E23="Y", Prices!$C21, 0))</f>
@@ -16746,7 +16746,7 @@
       </c>
       <c r="D68" s="20">
         <f>IF(Inputs!D25="Y", Prices!$C23, 0)</f>
-        <v>35000</v>
+        <v>42000</v>
       </c>
       <c r="E68" s="20">
         <f>IF(Inputs!E25="Y", Prices!$C23, 0)</f>
@@ -16947,7 +16947,7 @@
       </c>
       <c r="K77" s="23">
         <f t="shared" ref="K77:K84" si="2">D66+D77+$J77</f>
-        <v>8500.0010000000002</v>
+        <v>10200.001</v>
       </c>
       <c r="L77" s="23">
         <f t="shared" ref="L77:L84" si="3">E66+E77+$J77</f>
@@ -17045,7 +17045,7 @@
       </c>
       <c r="K79" s="23">
         <f t="shared" si="2"/>
-        <v>35000.001199999999</v>
+        <v>42000.001199999999</v>
       </c>
       <c r="L79" s="23">
         <f t="shared" si="3"/>
@@ -17339,23 +17339,23 @@
       </c>
       <c r="K85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, D74+D85+$J85)</f>
-        <v>0</v>
+        <v>1.8000000000000004E-3</v>
       </c>
       <c r="L85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, E74+E85+$J85)</f>
-        <v>0</v>
+        <v>1.8000000000000004E-3</v>
       </c>
       <c r="M85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, F74+F85+$J85)</f>
-        <v>0</v>
+        <v>1.8000000000000004E-3</v>
       </c>
       <c r="N85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, G74+G85+$J85)</f>
-        <v>0</v>
+        <v>1.8000000000000004E-3</v>
       </c>
       <c r="O85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, H74+H85+$J85)</f>
-        <v>0</v>
+        <v>1.8000000000000004E-3</v>
       </c>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
@@ -17376,7 +17376,7 @@
       </c>
       <c r="D88" s="18">
         <f>D66</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="E88" s="18">
         <f t="shared" ref="E88:H88" si="8">E66</f>
@@ -17400,19 +17400,19 @@
       </c>
       <c r="L88" s="21">
         <f t="shared" ref="L88:O88" si="9">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L77,L$77:L$85),8))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M88" s="21">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N88" s="21">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O88" s="21">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
@@ -17441,23 +17441,23 @@
       </c>
       <c r="K89" s="21">
         <f t="shared" ref="K89:O89" si="11">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K78,K$77:K$85),8))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L89" s="21">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M89" s="21">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N89" s="21">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O89" s="21">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
@@ -17466,7 +17466,7 @@
       </c>
       <c r="D90" s="20">
         <f>IF(D68=0,0,D68-SUM(D22:D24))</f>
-        <v>13500</v>
+        <v>16200</v>
       </c>
       <c r="E90" s="20">
         <f>IF(E68=0,0,E68-SUM(E22:E24))</f>
@@ -17490,19 +17490,19 @@
       </c>
       <c r="L90" s="21">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M90" s="21">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N90" s="21">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O90" s="21">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
@@ -17531,23 +17531,23 @@
       </c>
       <c r="K91" s="21">
         <f t="shared" ref="K91:O91" si="13">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K80,K$77:K$85),8))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L91" s="21">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M91" s="21">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N91" s="21">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O91" s="21">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
@@ -17576,23 +17576,23 @@
       </c>
       <c r="K92" s="21">
         <f t="shared" ref="K92:O92" si="14">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K81,K$77:K$85),8))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L92" s="21">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M92" s="21">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N92" s="21">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O92" s="21">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
@@ -17621,23 +17621,23 @@
       </c>
       <c r="K93" s="21">
         <f t="shared" ref="K93:O93" si="16">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K82,K$77:K$85),8))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L93" s="21">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M93" s="21">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N93" s="21">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O93" s="21">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
@@ -17666,23 +17666,23 @@
       </c>
       <c r="K94" s="21">
         <f t="shared" ref="K94:O94" si="17">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K83,K$77:K$85),8))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L94" s="21">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M94" s="21">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N94" s="21">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O94" s="21">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
@@ -17711,23 +17711,23 @@
       </c>
       <c r="K95" s="21">
         <f>IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K84,K$77:K$85),8))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L95" s="21">
         <f t="shared" ref="L95:O95" si="19">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L84,L$77:L$85),8))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M95" s="21">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N95" s="21">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O95" s="21">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
@@ -17756,23 +17756,23 @@
       </c>
       <c r="K96" s="21">
         <f t="shared" ref="K96:O96" si="21">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K85,K$77:K$85),8))</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L96" s="21">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M96" s="21">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N96" s="21">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="O96" s="21">
         <f t="shared" si="21"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -18014,7 +18014,7 @@
       </c>
       <c r="D110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A110, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A110, K$88:K$96, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>-2550</v>
+        <v>-3060</v>
       </c>
       <c r="E110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A110, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A110, L$88:L$96, 0)))*Prices!$L$5*-1, 0)</f>
@@ -18207,7 +18207,7 @@
       </c>
       <c r="D118" s="7">
         <f>SUM(D40:D50, D53:D63, D66:D74, D77:D85, D110:D116)</f>
-        <v>55950</v>
+        <v>67140</v>
       </c>
       <c r="E118" s="7">
         <f>SUM(E40:E50, E53:E63, E66:E74, E77:E85, E110:E116)</f>
@@ -18288,7 +18288,7 @@
       </c>
       <c r="D124" s="7">
         <f>SUM(D118, D120,D122)</f>
-        <v>55950</v>
+        <v>67140</v>
       </c>
       <c r="E124" s="7">
         <f t="shared" ref="E124:H124" si="27">SUM(E118, E120,E122)</f>
@@ -18459,7 +18459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18555,27 +18557,27 @@
       </c>
       <c r="C6" s="42">
         <f>$L$28*15000</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="D6" s="42">
         <f>IF(Inputs!$C$3="Monthly",33000,30000)</f>
-        <v>30000</v>
+        <v>33000</v>
       </c>
       <c r="E6" s="38">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.4,0.27), 2)</f>
-        <v>0.27</v>
+        <v>0.4</v>
       </c>
       <c r="F6" s="38">
         <f>ROUND($E6*F$4, 2)</f>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="G6" s="38">
         <f>ROUND($E6*G$4, 2)</f>
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="H6" s="38">
         <f>MAX(ROUND($E6*H$4, 2) + IF(ROUND($E6*H$4, 2) = G6, -0.01, 0), 0.01)</f>
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="K6" t="s">
         <v>26</v>
@@ -18612,15 +18614,15 @@
       </c>
       <c r="C10" s="44">
         <f>$L$28*1000</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="E10" s="40">
         <f>ROUND($L$28*0.04, 2)</f>
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F10" s="40">
         <f t="shared" ref="F10:H19" si="0">ROUND($E10*F$4, 2)</f>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G10" s="40">
         <f t="shared" si="0"/>
@@ -18643,19 +18645,19 @@
       </c>
       <c r="C11" s="44">
         <f>$L$28*4000</f>
-        <v>4000</v>
+        <v>4800</v>
       </c>
       <c r="E11" s="40">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.07,0.05), 2)</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F11" s="40">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="G11" s="40">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H11" s="40">
         <f t="shared" ref="H11:H14" si="1">MAX(ROUND($E11*H$4, 2) + IF(ROUND($E11*H$4, 2) = G11, -0.01, 0), 0.01)</f>
@@ -18674,15 +18676,15 @@
       </c>
       <c r="C12" s="44">
         <f>$L$28*2000</f>
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="E12" s="40">
         <f>ROUND($L$28*0.04, 2)</f>
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F12" s="40">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G12" s="40">
         <f t="shared" si="0"/>
@@ -18699,15 +18701,15 @@
       </c>
       <c r="C13" s="44">
         <f>$L$28*2000</f>
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="E13" s="40">
         <f>ROUND($L$28*0.04, 2)</f>
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F13" s="40">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G13" s="40">
         <f t="shared" si="0"/>
@@ -18725,19 +18727,19 @@
       </c>
       <c r="C14" s="44">
         <f>$L$28*6000</f>
-        <v>6000</v>
+        <v>7200</v>
       </c>
       <c r="E14" s="40">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.07,0.05), 2)</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F14" s="40">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H14" s="40">
         <f t="shared" si="1"/>
@@ -18756,19 +18758,19 @@
       </c>
       <c r="C15" s="44">
         <f>$L$28*4000</f>
-        <v>4000</v>
+        <v>4800</v>
       </c>
       <c r="E15" s="40">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.07,0.05), 2)</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F15" s="40">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="G15" s="40">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H15" s="40">
         <f>MAX(ROUND($E15*H$4, 2) + IF(ROUND($E15*H$4, 2) = G15, -0.01, 0), 0.01)</f>
@@ -18787,19 +18789,19 @@
       </c>
       <c r="C16" s="44">
         <f>$L$28*3500</f>
-        <v>3500</v>
+        <v>4200</v>
       </c>
       <c r="E16" s="108">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.07,0.05), 2)</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F16" s="108">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="G16" s="108">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H16" s="108">
         <f>MAX(ROUND($E16*H$4, 2) + IF(ROUND($E16*H$4, 2) = G16, -0.01, 0), 0.01)</f>
@@ -18814,23 +18816,23 @@
       </c>
       <c r="C17" s="45">
         <f>$L$28*10000</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="E17" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.25,0.18), 2)</f>
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="F17" s="41">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="G17" s="41">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H17" s="41">
         <f t="shared" ref="H17:H29" si="2">MAX(ROUND($E17*H$4, 2) + IF(ROUND($E17*H$4, 2) = G17, -0.01, 0), 0.01)</f>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="3"/>
@@ -18841,23 +18843,23 @@
       </c>
       <c r="C18" s="45">
         <f>$L$28*10000</f>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="E18" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.25,0.18), 2)</f>
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="F18" s="41">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="G18" s="41">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H18" s="109">
         <f t="shared" si="2"/>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -18866,7 +18868,7 @@
       </c>
       <c r="C19" s="45">
         <f>$L$28*1500</f>
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="E19" s="41">
         <f>ROUND($L$28*0, 2)</f>
@@ -18904,7 +18906,7 @@
       </c>
       <c r="C21" s="44">
         <f>$L$28*8500</f>
-        <v>8500</v>
+        <v>10200</v>
       </c>
       <c r="E21" s="40">
         <f>ROUND($L$28*0, 2)</f>
@@ -18935,23 +18937,23 @@
       </c>
       <c r="C22" s="44">
         <f>$L$28*33000</f>
-        <v>33000</v>
+        <v>39600</v>
       </c>
       <c r="E22" s="40">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.4,0.28), 2)</f>
-        <v>0.28000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="F22" s="40">
         <f t="shared" si="3"/>
-        <v>0.17</v>
+        <v>0.24</v>
       </c>
       <c r="G22" s="40">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H22" s="40">
         <f t="shared" si="2"/>
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
@@ -18960,23 +18962,23 @@
       </c>
       <c r="C23" s="45">
         <f>$L$28*35000</f>
-        <v>35000</v>
+        <v>42000</v>
       </c>
       <c r="E23" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.42,0.29), 2)</f>
-        <v>0.28999999999999998</v>
+        <v>0.42</v>
       </c>
       <c r="F23" s="41">
         <f t="shared" si="3"/>
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="G23" s="41">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H23" s="41">
         <f t="shared" si="2"/>
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -18985,23 +18987,23 @@
       </c>
       <c r="C24" s="45">
         <f>$L$28*35000</f>
-        <v>35000</v>
+        <v>42000</v>
       </c>
       <c r="E24" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.42,0.29), 2)</f>
-        <v>0.28999999999999998</v>
+        <v>0.42</v>
       </c>
       <c r="F24" s="41">
         <f t="shared" si="3"/>
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="G24" s="41">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H24" s="41">
         <f t="shared" si="2"/>
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
@@ -19010,23 +19012,23 @@
       </c>
       <c r="C25" s="45">
         <f>$L$28*28000</f>
-        <v>28000</v>
+        <v>33600</v>
       </c>
       <c r="E25" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.25,0.18), 2)</f>
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="F25" s="41">
         <f t="shared" si="3"/>
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="G25" s="41">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H25" s="41">
         <f t="shared" si="2"/>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>125</v>
@@ -19042,23 +19044,23 @@
       </c>
       <c r="C26" s="45">
         <f>$L$28*33600</f>
-        <v>33600</v>
+        <v>40320</v>
       </c>
       <c r="E26" s="41">
         <f>ROUND($L$28*0.25, 2)</f>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="F26" s="41">
         <f t="shared" si="3"/>
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="G26" s="41">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H26" s="41">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -19067,23 +19069,23 @@
       </c>
       <c r="C27" s="45">
         <f>$L$28*28000</f>
-        <v>28000</v>
+        <v>33600</v>
       </c>
       <c r="E27" s="41">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.25,0.18), 2)</f>
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="F27" s="41">
         <f t="shared" si="3"/>
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="G27" s="41">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="H27" s="41">
         <f t="shared" si="2"/>
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -19092,30 +19094,30 @@
       </c>
       <c r="C28" s="45">
         <f>$L$28*20000</f>
-        <v>20000</v>
+        <v>24000</v>
       </c>
       <c r="E28" s="41">
         <f>ROUND($L$28*0.14, 2)</f>
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="F28" s="41">
         <f t="shared" si="3"/>
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="G28" s="41">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H28" s="41">
         <f t="shared" si="2"/>
-        <v>1.9999999999999997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>126</v>
       </c>
       <c r="L28" s="97">
         <f>IF(Inputs!$C$3="Monthly",Prices!$L$25,1)</f>
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -19123,24 +19125,24 @@
         <v>96</v>
       </c>
       <c r="C29" s="82">
-        <f>$L$28*IF(Inputs!$C$4 = "Yes", 8400, 9600)</f>
-        <v>8400</v>
+        <f>$L$28*IF(Inputs!$C$4 = "Yes", 6750, 9600)</f>
+        <v>11520</v>
       </c>
       <c r="E29" s="83">
         <f>ROUND(IF(Inputs!$C$3="Monthly",0.6,0.42), 2)</f>
-        <v>0.42</v>
+        <v>0.6</v>
       </c>
       <c r="F29" s="83">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="G29" s="83">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H29" s="83">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -19149,7 +19151,7 @@
       </c>
       <c r="L30" s="102">
         <f>IF(Inputs!$C$3="Quarterly",$L$25,1)</f>
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Makes sure datamart isn't counted in discount splits under old pricing
Do this so we dont' get dinged on the splits when the datamart is not counted as a product.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -1317,7 +1317,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1478,7 @@
         <v>97</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="D27" s="1">
         <f>SUM(Calcs!D74, Calcs!D85)</f>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="E27" s="1">
         <f>SUM(Calcs!E74, Calcs!E85)</f>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="D30" s="1">
         <f>SUM(Calcs!D110:D114)</f>
-        <v>-3060</v>
+        <v>-8046</v>
       </c>
       <c r="E30" s="1">
         <f>SUM(Calcs!E110:E114)</f>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D34" s="7">
         <f>SUM(D7:D16, D19:D27, D30:D32)</f>
-        <v>67140</v>
+        <v>73674</v>
       </c>
       <c r="E34" s="7">
         <f>SUM(E7:E16, E19:E27, E30:E31)</f>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D43" s="7">
         <f>(D34/12*Inputs!$C$2+D4)*$C$37+D41</f>
-        <v>209000.25</v>
+        <v>228847.27499999999</v>
       </c>
       <c r="E43" s="7">
         <f>(E34/12*Inputs!$C$2+E4)*$C$37+E41</f>
@@ -2803,13 +2803,13 @@
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>209000.25</v>
+        <v>228847.27500000005</v>
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C48" s="52">
         <f>SUM(D43:H43)</f>
-        <v>209000.25</v>
+        <v>228847.27499999999</v>
       </c>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -2842,10 +2842,10 @@
   <dimension ref="B1:Q82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="D46" s="84">
         <f>SUM(Calcs!D96:H96)</f>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="F46" s="85">
         <v>0.1</v>
@@ -4299,11 +4299,11 @@
       </c>
       <c r="K46" s="84">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1152</v>
       </c>
       <c r="L46" s="84">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>10368</v>
       </c>
       <c r="M46" s="84">
         <f t="shared" si="23"/>
@@ -4710,15 +4710,15 @@
       </c>
       <c r="D60" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>-3060</v>
+        <v>-8046</v>
       </c>
       <c r="F60" s="8">
         <f>IFERROR(SUM(K74:K82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.25632183908045975</v>
+        <v>0.228060263653484</v>
       </c>
       <c r="G60" s="8">
         <f t="shared" ref="G60:I60" si="72">IFERROR(SUM(L74:L82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.7436781609195402</v>
+        <v>0.77193973634651603</v>
       </c>
       <c r="H60" s="8">
         <f t="shared" si="72"/>
@@ -4730,11 +4730,11 @@
       </c>
       <c r="K60" s="12">
         <f>F60*$D$60</f>
-        <v>-784.34482758620686</v>
+        <v>-1834.9728813559323</v>
       </c>
       <c r="L60" s="12">
         <f>G60*$D$60</f>
-        <v>-2275.655172413793</v>
+        <v>-6211.0271186440677</v>
       </c>
       <c r="M60" s="12">
         <f>H60*$D$60</f>
@@ -4755,11 +4755,11 @@
       </c>
       <c r="F61" s="3">
         <f>IFERROR(SUM(K10:K60)/SUM($K10:$N60), 0)</f>
-        <v>0.31494869187390218</v>
+        <v>0.28839247385297478</v>
       </c>
       <c r="G61" s="3">
         <f>IFERROR(SUM(L10:L60)/SUM($K10:$N60), 0)</f>
-        <v>0.68505130812609782</v>
+        <v>0.71160752614702516</v>
       </c>
       <c r="H61" s="3">
         <f>IFERROR(SUM(M10:M60)/SUM($K10:$N60), 0)</f>
@@ -4834,15 +4834,15 @@
       </c>
       <c r="D64" s="1">
         <f>SUM(Outputs_External!D34:'Outputs_External'!H34)</f>
-        <v>67140</v>
+        <v>73674</v>
       </c>
       <c r="K64" s="12">
         <f>SUM(K60:K62, K38:K46, K10:K20,K25:K35,K49:K57)</f>
-        <v>21145.655172413793</v>
+        <v>21247.027118644066</v>
       </c>
       <c r="L64" s="12">
         <f>SUM(L60:L62, L38:L46, L10:L20,L25:L35,L49:L57)</f>
-        <v>45994.344827586203</v>
+        <v>52426.972881355934</v>
       </c>
       <c r="M64" s="12">
         <f>SUM(M60:M62, M38:M46, M10:M20,M25:M35,M49:M57)</f>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="D65" s="23">
         <f>SUM(K64:N64)</f>
-        <v>67140</v>
+        <v>73674</v>
       </c>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
@@ -4924,15 +4924,15 @@
       </c>
       <c r="D69" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>209000.25</v>
+        <v>228847.27500000005</v>
       </c>
       <c r="K69" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>66761.17758620689</v>
+        <v>67069.094872881353</v>
       </c>
       <c r="L69" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>142239.07241379312</v>
+        <v>161778.18012711869</v>
       </c>
       <c r="M69" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -4947,11 +4947,11 @@
       <c r="D70" s="1"/>
       <c r="K70" s="53">
         <f>IFERROR(K69/$D$69, 0)</f>
-        <v>0.31943108960973438</v>
+        <v>0.2930736006049508</v>
       </c>
       <c r="L70" s="53">
         <f>IFERROR(L69/$D$69, 0)</f>
-        <v>0.68056891039026568</v>
+        <v>0.7069263993950492</v>
       </c>
       <c r="M70" s="53">
         <f>IFERROR(M69/$D$69, 0)</f>
@@ -5341,17 +5341,17 @@
         <v>97</v>
       </c>
       <c r="D82" s="23">
-        <f>SUM(Calcs!D74:H74)+SUM(Calcs!D85:H85)</f>
-        <v>0</v>
+        <f>IF(Inputs!$C$4 = "Yes", 0, SUM(Calcs!D74:H74)+SUM(Calcs!D85:H85))</f>
+        <v>11520</v>
       </c>
       <c r="E82" s="21"/>
       <c r="F82" s="24">
         <f t="shared" ref="F82" si="93">IFERROR(SUM(K46,K57)/SUM($K46:$N46,$K57:$N57),0)</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G82" s="24">
         <f t="shared" ref="G82" si="94">IFERROR(SUM(L46,L57)/SUM($K46:$N46,$K57:$N57),0)</f>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H82" s="24">
         <f t="shared" ref="H82" si="95">IFERROR(SUM(M46,M57)/SUM($K46:$N46,$K57:$N57),0)</f>
@@ -5363,12 +5363,12 @@
       </c>
       <c r="J82" s="21"/>
       <c r="K82" s="25">
-        <f t="shared" si="80"/>
-        <v>0</v>
+        <f>F82*$D82</f>
+        <v>1152</v>
       </c>
       <c r="L82" s="25">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>10368</v>
       </c>
       <c r="M82" s="25">
         <f t="shared" si="82"/>
@@ -5393,7 +5393,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="R27" sqref="R27:R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8088,15 +8088,15 @@
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!$D$64/12+N27</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q27" s="63">
         <f>$F27*Outputs_Internal!K$64/12+N27*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R27" s="63">
         <f>$F27*Outputs_Internal!L$64/12+N27*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S27" s="63">
         <f>N27*'MARA Prices'!$F$4</f>
@@ -8194,15 +8194,15 @@
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!$D$64/12+N28</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q28" s="63">
         <f>$F28*Outputs_Internal!K$64/12+N28*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R28" s="63">
         <f>$F28*Outputs_Internal!L$64/12+N28*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S28" s="63">
         <f>N28*'MARA Prices'!$F$4</f>
@@ -8300,15 +8300,15 @@
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!$D$64/12+N29</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q29" s="63">
         <f>$F29*Outputs_Internal!K$64/12+N29*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R29" s="63">
         <f>$F29*Outputs_Internal!L$64/12+N29*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S29" s="63">
         <f>N29*'MARA Prices'!$F$4</f>
@@ -8324,15 +8324,15 @@
       </c>
       <c r="W29" s="63">
         <f t="shared" si="2"/>
-        <v>22057.3125</v>
+        <v>23711.231250000004</v>
       </c>
       <c r="X29" s="63">
         <f t="shared" si="3"/>
-        <v>7883.7439655172402</v>
+        <v>7909.40373940678</v>
       </c>
       <c r="Y29" s="63">
         <f t="shared" si="4"/>
-        <v>14173.56853448276</v>
+        <v>15801.827510593223</v>
       </c>
       <c r="Z29" s="63">
         <f t="shared" si="5"/>
@@ -8406,15 +8406,15 @@
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!$D$64/12+N30</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q30" s="63">
         <f>$F30*Outputs_Internal!K$64/12+N30*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R30" s="63">
         <f>$F30*Outputs_Internal!L$64/12+N30*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S30" s="63">
         <f>N30*'MARA Prices'!$F$4</f>
@@ -8512,15 +8512,15 @@
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!$D$64/12+N31</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q31" s="63">
         <f>$F31*Outputs_Internal!K$64/12+N31*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R31" s="63">
         <f>$F31*Outputs_Internal!L$64/12+N31*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S31" s="63">
         <f>N31*'MARA Prices'!$F$4</f>
@@ -8618,15 +8618,15 @@
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!$D$64/12+N32</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q32" s="63">
         <f>$F32*Outputs_Internal!K$64/12+N32*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R32" s="63">
         <f>$F32*Outputs_Internal!L$64/12+N32*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S32" s="63">
         <f>N32*'MARA Prices'!$F$4</f>
@@ -8642,15 +8642,15 @@
       </c>
       <c r="W32" s="63">
         <f t="shared" si="2"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X32" s="63">
         <f t="shared" si="3"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y32" s="63">
         <f t="shared" si="4"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z32" s="63">
         <f t="shared" si="5"/>
@@ -8724,15 +8724,15 @@
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!$D$64/12+N33</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q33" s="63">
         <f>$F33*Outputs_Internal!K$64/12+N33*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R33" s="63">
         <f>$F33*Outputs_Internal!L$64/12+N33*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S33" s="63">
         <f>N33*'MARA Prices'!$F$4</f>
@@ -8830,15 +8830,15 @@
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!$D$64/12+N34</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q34" s="63">
         <f>$F34*Outputs_Internal!K$64/12+N34*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R34" s="63">
         <f>$F34*Outputs_Internal!L$64/12+N34*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S34" s="63">
         <f>N34*'MARA Prices'!$F$4</f>
@@ -8936,15 +8936,15 @@
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!$D$64/12+N35</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q35" s="63">
         <f>$F35*Outputs_Internal!K$64/12+N35*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R35" s="63">
         <f>$F35*Outputs_Internal!L$64/12+N35*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S35" s="63">
         <f>N35*'MARA Prices'!$F$4</f>
@@ -8960,15 +8960,15 @@
       </c>
       <c r="W35" s="63">
         <f t="shared" si="2"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X35" s="63">
         <f t="shared" si="3"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y35" s="63">
         <f t="shared" si="4"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z35" s="63">
         <f t="shared" si="5"/>
@@ -9042,15 +9042,15 @@
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!$D$64/12+N36</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q36" s="63">
         <f>$F36*Outputs_Internal!K$64/12+N36*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R36" s="63">
         <f>$F36*Outputs_Internal!L$64/12+N36*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S36" s="63">
         <f>N36*'MARA Prices'!$F$4</f>
@@ -9148,15 +9148,15 @@
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!$D$64/12+N37</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q37" s="63">
         <f>$F37*Outputs_Internal!K$64/12+N37*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R37" s="63">
         <f>$F37*Outputs_Internal!L$64/12+N37*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S37" s="63">
         <f>N37*'MARA Prices'!$F$4</f>
@@ -9254,15 +9254,15 @@
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!$D$64/12+N38</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q38" s="63">
         <f>$F38*Outputs_Internal!K$64/12+N38*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R38" s="63">
         <f>$F38*Outputs_Internal!L$64/12+N38*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S38" s="63">
         <f>N38*'MARA Prices'!$F$4</f>
@@ -9278,15 +9278,15 @@
       </c>
       <c r="W38" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X38" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y38" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z38" s="63">
         <f t="shared" si="10"/>
@@ -9360,15 +9360,15 @@
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!$D$64/12+N39</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q39" s="63">
         <f>$F39*Outputs_Internal!K$64/12+N39*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R39" s="63">
         <f>$F39*Outputs_Internal!L$64/12+N39*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S39" s="63">
         <f>N39*'MARA Prices'!$F$4</f>
@@ -9466,15 +9466,15 @@
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!$D$64/12+N40</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q40" s="63">
         <f>$F40*Outputs_Internal!K$64/12+N40*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R40" s="63">
         <f>$F40*Outputs_Internal!L$64/12+N40*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S40" s="63">
         <f>N40*'MARA Prices'!$F$4</f>
@@ -9572,15 +9572,15 @@
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!$D$64/12+N41</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q41" s="63">
         <f>$F41*Outputs_Internal!K$64/12+N41*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R41" s="63">
         <f>$F41*Outputs_Internal!L$64/12+N41*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S41" s="63">
         <f>N41*'MARA Prices'!$F$4</f>
@@ -9596,15 +9596,15 @@
       </c>
       <c r="W41" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X41" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y41" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z41" s="63">
         <f t="shared" si="10"/>
@@ -9678,15 +9678,15 @@
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!$D$64/12+N42</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q42" s="63">
         <f>$F42*Outputs_Internal!K$64/12+N42*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R42" s="63">
         <f>$F42*Outputs_Internal!L$64/12+N42*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S42" s="63">
         <f>N42*'MARA Prices'!$F$4</f>
@@ -9784,15 +9784,15 @@
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!$D$64/12+N43</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q43" s="63">
         <f>$F43*Outputs_Internal!K$64/12+N43*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R43" s="63">
         <f>$F43*Outputs_Internal!L$64/12+N43*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S43" s="63">
         <f>N43*'MARA Prices'!$F$4</f>
@@ -9890,15 +9890,15 @@
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!$D$64/12+N44</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q44" s="63">
         <f>$F44*Outputs_Internal!K$64/12+N44*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R44" s="63">
         <f>$F44*Outputs_Internal!L$64/12+N44*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S44" s="63">
         <f>N44*'MARA Prices'!$F$4</f>
@@ -9914,15 +9914,15 @@
       </c>
       <c r="W44" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X44" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y44" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z44" s="63">
         <f t="shared" si="10"/>
@@ -9996,15 +9996,15 @@
       </c>
       <c r="P45" s="63">
         <f>$F45*Outputs_Internal!$D$64/12+N45</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q45" s="63">
         <f>$F45*Outputs_Internal!K$64/12+N45*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R45" s="63">
         <f>$F45*Outputs_Internal!L$64/12+N45*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S45" s="63">
         <f>N45*'MARA Prices'!$F$4</f>
@@ -10102,15 +10102,15 @@
       </c>
       <c r="P46" s="63">
         <f>$F46*Outputs_Internal!$D$64/12+N46</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q46" s="63">
         <f>$F46*Outputs_Internal!K$64/12+N46*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R46" s="63">
         <f>$F46*Outputs_Internal!L$64/12+N46*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S46" s="63">
         <f>N46*'MARA Prices'!$F$4</f>
@@ -10208,15 +10208,15 @@
       </c>
       <c r="P47" s="63">
         <f>$F47*Outputs_Internal!$D$64/12+N47</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q47" s="63">
         <f>$F47*Outputs_Internal!K$64/12+N47*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R47" s="63">
         <f>$F47*Outputs_Internal!L$64/12+N47*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S47" s="63">
         <f>N47*'MARA Prices'!$F$4</f>
@@ -10232,15 +10232,15 @@
       </c>
       <c r="W47" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X47" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y47" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z47" s="63">
         <f t="shared" si="10"/>
@@ -10314,15 +10314,15 @@
       </c>
       <c r="P48" s="63">
         <f>$F48*Outputs_Internal!$D$64/12+N48</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q48" s="63">
         <f>$F48*Outputs_Internal!K$64/12+N48*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R48" s="63">
         <f>$F48*Outputs_Internal!L$64/12+N48*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S48" s="63">
         <f>N48*'MARA Prices'!$F$4</f>
@@ -10420,15 +10420,15 @@
       </c>
       <c r="P49" s="63">
         <f>$F49*Outputs_Internal!$D$64/12+N49</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q49" s="63">
         <f>$F49*Outputs_Internal!K$64/12+N49*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R49" s="63">
         <f>$F49*Outputs_Internal!L$64/12+N49*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S49" s="63">
         <f>N49*'MARA Prices'!$F$4</f>
@@ -10526,15 +10526,15 @@
       </c>
       <c r="P50" s="63">
         <f>$F50*Outputs_Internal!$D$64/12+N50</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q50" s="63">
         <f>$F50*Outputs_Internal!K$64/12+N50*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R50" s="63">
         <f>$F50*Outputs_Internal!L$64/12+N50*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S50" s="63">
         <f>N50*'MARA Prices'!$F$4</f>
@@ -10550,15 +10550,15 @@
       </c>
       <c r="W50" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X50" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y50" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z50" s="63">
         <f t="shared" si="10"/>
@@ -10632,15 +10632,15 @@
       </c>
       <c r="P51" s="63">
         <f>$F51*Outputs_Internal!$D$64/12+N51</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q51" s="63">
         <f>$F51*Outputs_Internal!K$64/12+N51*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R51" s="63">
         <f>$F51*Outputs_Internal!L$64/12+N51*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S51" s="63">
         <f>N51*'MARA Prices'!$F$4</f>
@@ -10738,15 +10738,15 @@
       </c>
       <c r="P52" s="63">
         <f>$F52*Outputs_Internal!$D$64/12+N52</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q52" s="63">
         <f>$F52*Outputs_Internal!K$64/12+N52*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R52" s="63">
         <f>$F52*Outputs_Internal!L$64/12+N52*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S52" s="63">
         <f>N52*'MARA Prices'!$F$4</f>
@@ -10844,15 +10844,15 @@
       </c>
       <c r="P53" s="63">
         <f>$F53*Outputs_Internal!$D$64/12+N53</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q53" s="63">
         <f>$F53*Outputs_Internal!K$64/12+N53*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R53" s="63">
         <f>$F53*Outputs_Internal!L$64/12+N53*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S53" s="63">
         <f>N53*'MARA Prices'!$F$4</f>
@@ -10868,15 +10868,15 @@
       </c>
       <c r="W53" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X53" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y53" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z53" s="63">
         <f t="shared" si="10"/>
@@ -10950,15 +10950,15 @@
       </c>
       <c r="P54" s="63">
         <f>$F54*Outputs_Internal!$D$64/12+N54</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q54" s="63">
         <f>$F54*Outputs_Internal!K$64/12+N54*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R54" s="63">
         <f>$F54*Outputs_Internal!L$64/12+N54*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S54" s="63">
         <f>N54*'MARA Prices'!$F$4</f>
@@ -11056,15 +11056,15 @@
       </c>
       <c r="P55" s="63">
         <f>$F55*Outputs_Internal!$D$64/12+N55</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q55" s="63">
         <f>$F55*Outputs_Internal!K$64/12+N55*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R55" s="63">
         <f>$F55*Outputs_Internal!L$64/12+N55*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S55" s="63">
         <f>N55*'MARA Prices'!$F$4</f>
@@ -11162,15 +11162,15 @@
       </c>
       <c r="P56" s="63">
         <f>$F56*Outputs_Internal!$D$64/12+N56</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q56" s="63">
         <f>$F56*Outputs_Internal!K$64/12+N56*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R56" s="63">
         <f>$F56*Outputs_Internal!L$64/12+N56*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S56" s="63">
         <f>N56*'MARA Prices'!$F$4</f>
@@ -11186,15 +11186,15 @@
       </c>
       <c r="W56" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X56" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y56" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z56" s="63">
         <f t="shared" si="10"/>
@@ -11268,15 +11268,15 @@
       </c>
       <c r="P57" s="63">
         <f>$F57*Outputs_Internal!$D$64/12+N57</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q57" s="63">
         <f>$F57*Outputs_Internal!K$64/12+N57*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R57" s="63">
         <f>$F57*Outputs_Internal!L$64/12+N57*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S57" s="63">
         <f>N57*'MARA Prices'!$F$4</f>
@@ -11374,15 +11374,15 @@
       </c>
       <c r="P58" s="63">
         <f>$F58*Outputs_Internal!$D$64/12+N58</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q58" s="63">
         <f>$F58*Outputs_Internal!K$64/12+N58*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R58" s="63">
         <f>$F58*Outputs_Internal!L$64/12+N58*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S58" s="63">
         <f>N58*'MARA Prices'!$F$4</f>
@@ -11480,15 +11480,15 @@
       </c>
       <c r="P59" s="63">
         <f>$F59*Outputs_Internal!$D$64/12+N59</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q59" s="63">
         <f>$F59*Outputs_Internal!K$64/12+N59*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R59" s="63">
         <f>$F59*Outputs_Internal!L$64/12+N59*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S59" s="63">
         <f>N59*'MARA Prices'!$F$4</f>
@@ -11504,15 +11504,15 @@
       </c>
       <c r="W59" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X59" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y59" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z59" s="63">
         <f t="shared" si="10"/>
@@ -11586,15 +11586,15 @@
       </c>
       <c r="P60" s="63">
         <f>$F60*Outputs_Internal!$D$64/12+N60</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q60" s="63">
         <f>$F60*Outputs_Internal!K$64/12+N60*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R60" s="63">
         <f>$F60*Outputs_Internal!L$64/12+N60*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S60" s="63">
         <f>N60*'MARA Prices'!$F$4</f>
@@ -11692,15 +11692,15 @@
       </c>
       <c r="P61" s="63">
         <f>$F61*Outputs_Internal!$D$64/12+N61</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q61" s="63">
         <f>$F61*Outputs_Internal!K$64/12+N61*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R61" s="63">
         <f>$F61*Outputs_Internal!L$64/12+N61*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S61" s="63">
         <f>N61*'MARA Prices'!$F$4</f>
@@ -11798,15 +11798,15 @@
       </c>
       <c r="P62" s="63">
         <f>$F62*Outputs_Internal!$D$64/12+N62</f>
-        <v>5664.9375</v>
+        <v>6216.2437500000005</v>
       </c>
       <c r="Q62" s="63">
         <f>$F62*Outputs_Internal!K$64/12+N62*'MARA Prices'!$F$5</f>
-        <v>1784.1646551724136</v>
+        <v>1792.7179131355931</v>
       </c>
       <c r="R62" s="63">
         <f>$F62*Outputs_Internal!L$64/12+N62*'MARA Prices'!$F$6</f>
-        <v>3880.7728448275861</v>
+        <v>4423.5258368644072</v>
       </c>
       <c r="S62" s="63">
         <f>N62*'MARA Prices'!$F$4</f>
@@ -11822,15 +11822,15 @@
       </c>
       <c r="W62" s="63">
         <f t="shared" si="7"/>
-        <v>16994.8125</v>
+        <v>18648.731250000001</v>
       </c>
       <c r="X62" s="63">
         <f t="shared" si="8"/>
-        <v>5352.4939655172411</v>
+        <v>5378.1537394067791</v>
       </c>
       <c r="Y62" s="63">
         <f t="shared" si="9"/>
-        <v>11642.318534482758</v>
+        <v>13270.577510593223</v>
       </c>
       <c r="Z62" s="63">
         <f t="shared" si="10"/>
@@ -16896,7 +16896,7 @@
       </c>
       <c r="D74" s="84">
         <f>IF(Inputs!D13="Y", Prices!$C29, IF(Inputs!D13="Monthly", Prices!C29 * Prices!$L$30, 0))</f>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="E74" s="84">
         <f>IF(Inputs!E13="Y", Prices!$C29, IF(Inputs!E13="Monthly", Prices!D29 * Prices!$L$30, 0))</f>
@@ -17339,7 +17339,7 @@
       </c>
       <c r="K85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, D74+D85+$J85)</f>
-        <v>1.8000000000000004E-3</v>
+        <v>11520.0018</v>
       </c>
       <c r="L85" s="23">
         <f>IF(Inputs!$C$4="Yes", 0, E74+E85+$J85)</f>
@@ -17396,7 +17396,7 @@
       </c>
       <c r="K88" s="21">
         <f>IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K77,K$77:K$85),8))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L88" s="21">
         <f t="shared" ref="L88:O88" si="9">IF(COUNTIF(L$77:L$85,"")&gt;2,"",IFERROR(RANK(L77,L$77:L$85),8))</f>
@@ -17736,7 +17736,7 @@
       </c>
       <c r="D96" s="84">
         <f t="shared" ref="D96:H96" si="20">D74</f>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="E96" s="84">
         <f t="shared" si="20"/>
@@ -17756,7 +17756,7 @@
       </c>
       <c r="K96" s="21">
         <f t="shared" ref="K96:O96" si="21">IF(COUNTIF(K$77:K$85,"")&gt;2,"",IFERROR(RANK(K85,K$77:K$85),8))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L96" s="21">
         <f t="shared" si="21"/>
@@ -18014,7 +18014,7 @@
       </c>
       <c r="D110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A110, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A110, K$88:K$96, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>-3060</v>
+        <v>-3456</v>
       </c>
       <c r="E110" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A110, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A110, L$88:L$96, 0)))*Prices!$L$5*-1, 0)</f>
@@ -18042,7 +18042,7 @@
       </c>
       <c r="D111" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$66:D$74, MATCH($A111, K$88:K$96, 0)), INDEX(D$77:D$85, MATCH($A111, K$88:K$96, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>0</v>
+        <v>-4590</v>
       </c>
       <c r="E111" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$66:E$74, MATCH($A111, L$88:L$96, 0)), INDEX(E$77:E$85, MATCH($A111, L$88:L$96, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18207,7 +18207,7 @@
       </c>
       <c r="D118" s="7">
         <f>SUM(D40:D50, D53:D63, D66:D74, D77:D85, D110:D116)</f>
-        <v>67140</v>
+        <v>73674</v>
       </c>
       <c r="E118" s="7">
         <f>SUM(E40:E50, E53:E63, E66:E74, E77:E85, E110:E116)</f>
@@ -18288,7 +18288,7 @@
       </c>
       <c r="D124" s="7">
         <f>SUM(D118, D120,D122)</f>
-        <v>67140</v>
+        <v>73674</v>
       </c>
       <c r="E124" s="7">
         <f t="shared" ref="E124:H124" si="27">SUM(E118, E120,E122)</f>

</xml_diff>

<commit_message>
Remove UNH specific hacks.
Do this so it doesn't carry that baggage forward.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\PRM\NYMilliman_Share\Q32019_Recon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="3"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="160">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>PRM</t>
-  </si>
-  <si>
-    <t>Datamart Discounts</t>
   </si>
   <si>
     <t>Totals</t>
@@ -1325,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1344,7 +1341,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="90" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="69">
         <v>43466</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="70">
         <v>36</v>
@@ -1360,23 +1357,23 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="54" t="s">
         <v>122</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="54" t="s">
         <v>41</v>
@@ -1386,24 +1383,24 @@
       <c r="B6" s="67"/>
       <c r="C6" s="71"/>
       <c r="D6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="69">
         <v>43101</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="54" t="s">
         <v>28</v>
@@ -1465,7 +1462,7 @@
     </row>
     <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="54" t="s">
         <v>28</v>
@@ -1492,12 +1489,12 @@
       <c r="G12" s="54"/>
       <c r="H12" s="55"/>
       <c r="L12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="54">
         <v>1</v>
@@ -1509,12 +1506,12 @@
       <c r="G13" s="54"/>
       <c r="H13" s="55"/>
       <c r="L13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="54" t="s">
         <v>3</v>
@@ -1610,7 +1607,7 @@
     </row>
     <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="54" t="s">
         <v>28</v>
@@ -1622,7 +1619,7 @@
       <c r="G20" s="54"/>
       <c r="H20" s="55"/>
       <c r="L20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1641,7 +1638,7 @@
     </row>
     <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="68" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D22" s="54" t="s">
         <v>28</v>
@@ -1653,7 +1650,7 @@
       <c r="G22" s="54"/>
       <c r="H22" s="55"/>
       <c r="L22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1670,7 +1667,7 @@
       <c r="G23" s="54"/>
       <c r="H23" s="55"/>
       <c r="L23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1717,7 +1714,7 @@
     </row>
     <row r="27" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="54" t="s">
         <v>28</v>
@@ -1745,7 +1742,7 @@
     </row>
     <row r="29" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="54" t="s">
         <v>3</v>
@@ -1759,7 +1756,7 @@
     </row>
     <row r="30" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" s="54" t="s">
         <v>28</v>
@@ -1773,7 +1770,7 @@
     </row>
     <row r="31" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="92"/>
       <c r="D31" s="93" t="s">
@@ -1838,19 +1835,19 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>107</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -2124,7 +2121,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D48, Calcs!D61)</f>
@@ -2194,7 +2191,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C15" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D15" s="20">
         <f>SUM(Calcs!D51, Calcs!D64)</f>
@@ -2374,7 +2371,7 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="1">
         <f>SUM(Calcs!D71, Calcs!D82)</f>
@@ -2444,15 +2441,15 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1">
         <f>SUM(Calcs!D73, Calcs!D84)</f>
-        <v>23520</v>
+        <v>28224</v>
       </c>
       <c r="E24" s="1">
         <f>SUM(Calcs!E73, Calcs!E84)</f>
-        <v>33925.707900000001</v>
+        <v>40710.849479999997</v>
       </c>
       <c r="F24" s="1">
         <f>SUM(Calcs!F73, Calcs!F84)</f>
@@ -2479,7 +2476,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="1">
         <f>SUM(Calcs!D74, Calcs!D85)</f>
@@ -2514,7 +2511,7 @@
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(Calcs!D75, Calcs!D86)</f>
@@ -2549,7 +2546,7 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" s="1">
         <f>SUM(Calcs!D76, Calcs!D87)</f>
@@ -2593,11 +2590,11 @@
       </c>
       <c r="D30" s="1">
         <f>SUM(Calcs!D112:D116)</f>
-        <v>-42768</v>
+        <v>-44884.800000000003</v>
       </c>
       <c r="E30" s="1">
         <f>SUM(Calcs!E112:E116)</f>
-        <v>-76887.915525000004</v>
+        <v>-79941.229235999999</v>
       </c>
       <c r="F30" s="1">
         <f>SUM(Calcs!F112:F116)</f>
@@ -2624,11 +2621,11 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" s="1">
         <f>Calcs!D122</f>
-        <v>-56462.400000000001</v>
+        <v>-57626.640000000007</v>
       </c>
       <c r="E31" s="1">
         <f>Calcs!E122</f>
@@ -2659,7 +2656,7 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1">
         <f>Calcs!D124</f>
@@ -2694,11 +2691,11 @@
       </c>
       <c r="D34" s="7">
         <f>SUM(D7:D16, D19:D27, D30:D32)</f>
-        <v>69009.600000000006</v>
+        <v>70432.56</v>
       </c>
       <c r="E34" s="7">
         <f>SUM(E7:E16, E19:E27, E30:E31)</f>
-        <v>238361.35153499997</v>
+        <v>242093.17940399999</v>
       </c>
       <c r="F34" s="7">
         <f>SUM(F7:F16, F19:F27, F30:F31)</f>
@@ -2736,7 +2733,7 @@
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -2765,7 +2762,7 @@
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="63"/>
       <c r="D39" s="103"/>
@@ -2776,7 +2773,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1">
         <f>IF(Inputs!D$11 = "Y", SUMIF(Outputs_Timeline!$B$3:$B$204,"&lt;" &amp; EDATE(Inputs!$C$1,12), Outputs_Timeline!AD$3:AD$204), 0)</f>
@@ -2801,7 +2798,7 @@
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="1">
         <f>IF(Inputs!D$11 = "Y", SUM(Outputs_Timeline!AD$3:AD$204), 0)</f>
@@ -2826,15 +2823,15 @@
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="7">
         <f>(D34/12*Inputs!$C$2+D4)*$C$37+D41</f>
-        <v>212028.80000000002</v>
+        <v>216297.68</v>
       </c>
       <c r="E43" s="7">
         <f>(E34/12*Inputs!$C$2+E4)*$C$37+E41</f>
-        <v>735084.05460499984</v>
+        <v>746279.53821199993</v>
       </c>
       <c r="F43" s="7">
         <f>(F34/12*Inputs!$C$2+F4)*$C$37+F41</f>
@@ -2872,19 +2869,19 @@
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C47" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>947112.854605</v>
+        <v>962577.21821199975</v>
       </c>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C48" s="51">
         <f>SUM(D43:H43)</f>
-        <v>947112.85460499988</v>
+        <v>962577.21821199986</v>
       </c>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -2943,7 +2940,7 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F1" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="49"/>
       <c r="H1" s="49"/>
@@ -2951,7 +2948,7 @@
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>40</v>
@@ -2960,10 +2957,10 @@
         <v>41</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="109"/>
       <c r="K2" s="9" t="s">
@@ -2973,10 +2970,10 @@
         <v>41</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -2986,7 +2983,7 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$8:$H$8, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -3025,7 +3022,7 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1">
         <f>SUMIF(Inputs!$D$8:$H$8, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -3076,7 +3073,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D7" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
@@ -3101,7 +3098,7 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="18">
         <f>SUM(Calcs!D22:H22)</f>
@@ -3400,7 +3397,7 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" s="18">
         <f>SUM(Calcs!D23:H23)</f>
@@ -3481,7 +3478,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C19" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="20">
         <f>SUM(Calcs!D25:H25)</f>
@@ -3575,7 +3572,7 @@
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
       <c r="G22" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="98">
         <v>7.4999999999999997E-2</v>
@@ -3599,7 +3596,7 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="11"/>
@@ -3877,7 +3874,7 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="18">
         <f>SUM(Calcs!D35:H35)</f>
@@ -3921,7 +3918,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" s="18">
         <f>SUM(Calcs!D36:H36)</f>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C34" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" s="20">
         <f>SUM(Calcs!D38:H38)</f>
@@ -4108,7 +4105,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="11"/>
@@ -4245,7 +4242,7 @@
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C41" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="20">
         <f>SUM(Calcs!D93:H93)</f>
@@ -4326,11 +4323,11 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C43" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D43" s="20">
         <f>SUM(Calcs!D95:H95)</f>
-        <v>47334</v>
+        <v>56800.800000000003</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="33">
@@ -4349,11 +4346,11 @@
       <c r="J43" s="3"/>
       <c r="K43" s="20">
         <f t="shared" ref="K43:K45" si="35">F43*$D43</f>
-        <v>4733.4000000000005</v>
+        <v>5680.0800000000008</v>
       </c>
       <c r="L43" s="20">
         <f t="shared" ref="L43:L45" si="36">G43*$D43</f>
-        <v>42600.6</v>
+        <v>51120.72</v>
       </c>
       <c r="M43" s="20">
         <f t="shared" ref="M43:M45" si="37">H43*$D43</f>
@@ -4367,7 +4364,7 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C44" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="20">
         <f>SUM(Calcs!D96:H96)</f>
@@ -4408,7 +4405,7 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C45" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" s="20">
         <f>SUM(Calcs!D97:H97)</f>
@@ -4449,7 +4446,7 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C46" s="80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" s="83">
         <f>SUM(Calcs!D98:H98)</f>
@@ -4495,7 +4492,7 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -4634,7 +4631,7 @@
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C52" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="20">
         <f>SUM(Calcs!D104:H104)</f>
@@ -4718,11 +4715,11 @@
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C54" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D54" s="20">
         <f>SUM(Calcs!D106:H106)</f>
-        <v>10111.707899999999</v>
+        <v>12134.049479999996</v>
       </c>
       <c r="F54" s="31">
         <f t="shared" si="46"/>
@@ -4742,11 +4739,11 @@
       <c r="J54" s="3"/>
       <c r="K54" s="20">
         <f t="shared" ref="K54:K56" si="54">F54*$D54</f>
-        <v>252.7926975000002</v>
+        <v>303.3512370000002</v>
       </c>
       <c r="L54" s="20">
         <f t="shared" ref="L54:L56" si="55">G54*$D54</f>
-        <v>9858.9152024999985</v>
+        <v>11830.698242999995</v>
       </c>
       <c r="M54" s="20">
         <f t="shared" ref="M54:M56" si="56">H54*$D54</f>
@@ -4760,7 +4757,7 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C55" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D55" s="20">
         <f>SUM(Calcs!D107:H107)</f>
@@ -4802,7 +4799,7 @@
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C56" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D56" s="20">
         <f>SUM(Calcs!D108:H108)</f>
@@ -4844,7 +4841,7 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C57" s="80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D57" s="83">
         <f>SUM(Calcs!D109:H109)</f>
@@ -4905,16 +4902,16 @@
       </c>
       <c r="D60" s="2">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>-119655.915525</v>
+        <v>-124826.029236</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="8">
         <f>IFERROR(SUM(K74:K82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.2333898119485166</v>
+        <v>0.22938411257884686</v>
       </c>
       <c r="G60" s="8">
         <f t="shared" ref="G60:I60" si="72">IFERROR(SUM(L74:L82)/SUM($K$74:$N$82), 0)</f>
-        <v>0.76339398171803019</v>
+        <v>0.7674875658496656</v>
       </c>
       <c r="H60" s="8">
         <f t="shared" si="72"/>
@@ -4922,16 +4919,16 @@
       </c>
       <c r="I60" s="8">
         <f t="shared" si="72"/>
-        <v>3.2162063334532707E-3</v>
+        <v>3.1283215714875668E-3</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="12">
         <f>F60*$D$60</f>
-        <v>-27926.471622907338</v>
+        <v>-28633.107943041054</v>
       </c>
       <c r="L60" s="12">
         <f>G60*$D$60</f>
-        <v>-91344.605788746019</v>
+        <v>-95802.425333016829</v>
       </c>
       <c r="M60" s="12">
         <f>H60*$D$60</f>
@@ -4939,25 +4936,25 @@
       </c>
       <c r="N60" s="12">
         <f>I60*$D$60</f>
-        <v>-384.83811334665455</v>
+        <v>-390.49595994211649</v>
       </c>
       <c r="O60" s="1"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D61" s="2">
         <f>SUM(Outputs_External!D31:'Outputs_External'!H31)</f>
-        <v>-56462.400000000001</v>
+        <v>-57626.640000000007</v>
       </c>
       <c r="F61" s="3">
         <f>IFERROR(SUM(K10:K60)/SUM($K10:$N60), 0)</f>
-        <v>0.26275266295580363</v>
+        <v>0.25905218915982015</v>
       </c>
       <c r="G61" s="3">
         <f>IFERROR(SUM(L10:L60)/SUM($K10:$N60), 0)</f>
-        <v>0.73468991500368186</v>
+        <v>0.73844933281557934</v>
       </c>
       <c r="H61" s="3">
         <f>IFERROR(SUM(M10:M60)/SUM($K10:$N60), 0)</f>
@@ -4965,16 +4962,16 @@
       </c>
       <c r="I61" s="3">
         <f>1-F61-G61-H61</f>
-        <v>2.5574220405144565E-3</v>
+        <v>2.49847802460057E-3</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="12">
         <f>F61*$D$61</f>
-        <v>-14835.645956875767</v>
+        <v>-14928.30724592486</v>
       </c>
       <c r="L61" s="12">
         <f>G61*$D$61</f>
-        <v>-41482.355856903887</v>
+        <v>-42554.353860403578</v>
       </c>
       <c r="M61" s="12">
         <f>H61*$D$61</f>
@@ -4982,13 +4979,13 @@
       </c>
       <c r="N61" s="12">
         <f>I61*$D$61</f>
-        <v>-144.39818622034346</v>
+        <v>-143.97889367156822</v>
       </c>
       <c r="O61" s="1"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D62" s="1">
         <f>Outputs_External!D32</f>
@@ -5037,15 +5034,15 @@
       </c>
       <c r="D64" s="2">
         <f>SUM(Outputs_External!D34:'Outputs_External'!H34)</f>
-        <v>307370.951535</v>
+        <v>312525.73940399999</v>
       </c>
       <c r="K64" s="12">
         <f>SUM(K60:K62, K38:K46, K10:K20,K25:K35,K49:K57)</f>
-        <v>80762.536031080555</v>
+        <v>80960.476961397741</v>
       </c>
       <c r="L64" s="12">
         <f>SUM(L60:L62, L38:L46, L10:L20,L25:L35,L49:L57)</f>
-        <v>225822.33825785012</v>
+        <v>230784.42375057965</v>
       </c>
       <c r="M64" s="12">
         <f>SUM(M60:M62, M38:M46, M10:M20,M25:M35,M49:M57)</f>
@@ -5053,17 +5050,17 @@
       </c>
       <c r="N64" s="12">
         <f>SUM(N60:N62, N38:N46, N10:N20,N25:N35,N49:N57)</f>
-        <v>786.07724606936563</v>
+        <v>780.83869202267897</v>
       </c>
       <c r="O64" s="1"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C65" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D65" s="23">
         <f>SUM(K64:N64)</f>
-        <v>307370.95153500006</v>
+        <v>312525.73940400005</v>
       </c>
       <c r="E65" s="2"/>
       <c r="K65" s="12"/>
@@ -5081,7 +5078,7 @@
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" s="21"/>
       <c r="D67" s="1">
@@ -5129,19 +5126,19 @@
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D69" s="7">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>947112.854605</v>
+        <v>962577.21821199975</v>
       </c>
       <c r="K69" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>246787.60809324161</v>
+        <v>247381.43088419328</v>
       </c>
       <c r="L69" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>697967.01477355044</v>
+        <v>712853.271251739</v>
       </c>
       <c r="M69" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -5149,7 +5146,7 @@
       </c>
       <c r="N69" s="12">
         <f>SUM(Outputs_Timeline!AA:AA)</f>
-        <v>2358.2317382080973</v>
+        <v>2342.5160760680365</v>
       </c>
       <c r="O69" s="1"/>
     </row>
@@ -5157,11 +5154,11 @@
       <c r="D70" s="1"/>
       <c r="K70" s="52">
         <f>IFERROR(K69/$D$69, 0)</f>
-        <v>0.2605683228702097</v>
+        <v>0.25699905026186642</v>
       </c>
       <c r="L70" s="52">
         <f>IFERROR(L69/$D$69, 0)</f>
-        <v>0.7369417608260026</v>
+        <v>0.74056736204070317</v>
       </c>
       <c r="M70" s="52">
         <f>IFERROR(M69/$D$69, 0)</f>
@@ -5169,7 +5166,7 @@
       </c>
       <c r="N70" s="52">
         <f>IFERROR(N69/$D$69, 0)</f>
-        <v>2.4899163037879093E-3</v>
+        <v>2.4335876974309572E-3</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
@@ -5179,7 +5176,7 @@
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="21"/>
       <c r="D73" s="21"/>
@@ -5328,7 +5325,7 @@
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="27"/>
       <c r="C77" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D77" s="23">
         <f>SUM(Calcs!D71:H71)+SUM(Calcs!D82:H82)</f>
@@ -5416,11 +5413,11 @@
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="27"/>
       <c r="C79" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D79" s="23">
         <f>SUM(Calcs!D73:H73)+SUM(Calcs!D84:H84)</f>
-        <v>57445.707900000001</v>
+        <v>68934.849480000004</v>
       </c>
       <c r="E79" s="21"/>
       <c r="F79" s="24">
@@ -5429,7 +5426,7 @@
       </c>
       <c r="G79" s="24">
         <f t="shared" si="79"/>
-        <v>0.91320164935246617</v>
+        <v>0.91320164935246606</v>
       </c>
       <c r="H79" s="24">
         <f t="shared" si="79"/>
@@ -5442,11 +5439,11 @@
       <c r="J79" s="97"/>
       <c r="K79" s="25">
         <f t="shared" ref="K79:K81" si="84">F79*$D79</f>
-        <v>4986.1926975000006</v>
+        <v>5983.4312370000007</v>
       </c>
       <c r="L79" s="25">
         <f t="shared" ref="L79:L81" si="85">G79*$D79</f>
-        <v>52459.515202499999</v>
+        <v>62951.418242999993</v>
       </c>
       <c r="M79" s="25">
         <f t="shared" ref="M79:M81" si="86">H79*$D79</f>
@@ -5460,7 +5457,7 @@
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="27"/>
       <c r="C80" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D80" s="23">
         <f>SUM(Calcs!D74:H74)+SUM(Calcs!D85:H85)</f>
@@ -5504,7 +5501,7 @@
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="27"/>
       <c r="C81" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D81" s="23">
         <f>SUM(Calcs!D75:H75)+SUM(Calcs!D86:H86)</f>
@@ -5548,7 +5545,7 @@
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="27"/>
       <c r="C82" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D82" s="23">
         <f>IF(Inputs!$C$4 = "Yes", 0, SUM(Calcs!D76:H76)+SUM(Calcs!D87:H87))</f>
@@ -5599,7 +5596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5636,7 +5633,7 @@
       </c>
       <c r="G1" s="64"/>
       <c r="I1" s="60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" s="60"/>
       <c r="K1" s="60"/>
@@ -5644,7 +5641,7 @@
       <c r="M1" s="60"/>
       <c r="N1" s="60"/>
       <c r="P1" s="60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="60"/>
       <c r="R1" s="60"/>
@@ -5652,13 +5649,13 @@
       <c r="T1" s="60"/>
       <c r="U1" s="60"/>
       <c r="W1" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X1" s="60"/>
       <c r="Y1" s="60"/>
       <c r="Z1" s="60"/>
       <c r="AD1" s="60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AE1" s="60"/>
       <c r="AF1" s="106"/>
@@ -5667,85 +5664,85 @@
     </row>
     <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="58"/>
       <c r="D2" s="58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="58"/>
       <c r="I2" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="61" t="s">
         <v>63</v>
-      </c>
-      <c r="J2" s="61" t="s">
-        <v>64</v>
       </c>
       <c r="K2" s="61" t="s">
         <v>41</v>
       </c>
       <c r="L2" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M2" s="61"/>
       <c r="N2" s="104" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P2" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="61" t="s">
         <v>63</v>
-      </c>
-      <c r="Q2" s="61" t="s">
-        <v>64</v>
       </c>
       <c r="R2" s="61" t="s">
         <v>41</v>
       </c>
       <c r="S2" s="61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T2" s="61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U2" s="61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W2" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" s="61" t="s">
         <v>63</v>
-      </c>
-      <c r="X2" s="61" t="s">
-        <v>64</v>
       </c>
       <c r="Y2" s="61" t="s">
         <v>41</v>
       </c>
       <c r="Z2" s="61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA2" s="61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD2" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE2" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="AE2" s="61" t="s">
+      <c r="AF2" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="AF2" s="61" t="s">
+      <c r="AG2" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="AG2" s="61" t="s">
+      <c r="AH2" s="61" t="s">
         <v>108</v>
-      </c>
-      <c r="AH2" s="61" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.25">
@@ -7623,15 +7620,15 @@
       </c>
       <c r="P21" s="62">
         <f>$F21*Outputs_Internal!$D$64/12+N21</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q21" s="62">
         <f>$F21*Outputs_Internal!K$64/12+N21*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R21" s="62">
         <f>$F21*Outputs_Internal!L$64/12+N21*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S21" s="62">
         <f>N21*'MARA Prices'!$F$4</f>
@@ -7643,7 +7640,7 @@
       </c>
       <c r="U21" s="62">
         <f>$F21*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W21" s="62">
         <f t="shared" si="2"/>
@@ -7727,15 +7724,15 @@
       </c>
       <c r="P22" s="62">
         <f>$F22*Outputs_Internal!$D$64/12+N22</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q22" s="62">
         <f>$F22*Outputs_Internal!K$64/12+N22*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R22" s="62">
         <f>$F22*Outputs_Internal!L$64/12+N22*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S22" s="62">
         <f>N22*'MARA Prices'!$F$4</f>
@@ -7747,7 +7744,7 @@
       </c>
       <c r="U22" s="62">
         <f>$F22*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W22" s="62">
         <f t="shared" si="2"/>
@@ -7831,15 +7828,15 @@
       </c>
       <c r="P23" s="62">
         <f>$F23*Outputs_Internal!$D$64/12+N23</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q23" s="62">
         <f>$F23*Outputs_Internal!K$64/12+N23*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R23" s="62">
         <f>$F23*Outputs_Internal!L$64/12+N23*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S23" s="62">
         <f>N23*'MARA Prices'!$F$4</f>
@@ -7851,19 +7848,19 @@
       </c>
       <c r="U23" s="62">
         <f>$F23*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W23" s="62">
         <f t="shared" si="2"/>
-        <v>101842.73788374999</v>
+        <v>103131.434851</v>
       </c>
       <c r="X23" s="62">
         <f t="shared" si="3"/>
-        <v>24690.634007770142</v>
+        <v>24740.119240349431</v>
       </c>
       <c r="Y23" s="62">
         <f t="shared" si="4"/>
-        <v>76955.584564462522</v>
+        <v>78196.105937644927</v>
       </c>
       <c r="Z23" s="62">
         <f t="shared" si="5"/>
@@ -7871,7 +7868,7 @@
       </c>
       <c r="AA23" s="62">
         <f t="shared" si="6"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD23" s="62">
         <f>'MARA Prices'!H$21*$G23</f>
@@ -7935,15 +7932,15 @@
       </c>
       <c r="P24" s="62">
         <f>$F24*Outputs_Internal!$D$64/12+N24</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q24" s="62">
         <f>$F24*Outputs_Internal!K$64/12+N24*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R24" s="62">
         <f>$F24*Outputs_Internal!L$64/12+N24*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S24" s="62">
         <f>N24*'MARA Prices'!$F$4</f>
@@ -7955,7 +7952,7 @@
       </c>
       <c r="U24" s="62">
         <f>$F24*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W24" s="62">
         <f t="shared" si="2"/>
@@ -8039,15 +8036,15 @@
       </c>
       <c r="P25" s="62">
         <f>$F25*Outputs_Internal!$D$64/12+N25</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q25" s="62">
         <f>$F25*Outputs_Internal!K$64/12+N25*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R25" s="62">
         <f>$F25*Outputs_Internal!L$64/12+N25*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S25" s="62">
         <f>N25*'MARA Prices'!$F$4</f>
@@ -8059,7 +8056,7 @@
       </c>
       <c r="U25" s="62">
         <f>$F25*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W25" s="62">
         <f t="shared" si="2"/>
@@ -8143,15 +8140,15 @@
       </c>
       <c r="P26" s="62">
         <f>$F26*Outputs_Internal!$D$64/12+N26</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q26" s="62">
         <f>$F26*Outputs_Internal!K$64/12+N26*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R26" s="62">
         <f>$F26*Outputs_Internal!L$64/12+N26*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S26" s="62">
         <f>N26*'MARA Prices'!$F$4</f>
@@ -8163,19 +8160,19 @@
       </c>
       <c r="U26" s="62">
         <f>$F26*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W26" s="62">
         <f t="shared" si="2"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X26" s="62">
         <f t="shared" si="3"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y26" s="62">
         <f t="shared" si="4"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z26" s="62">
         <f t="shared" si="5"/>
@@ -8183,7 +8180,7 @@
       </c>
       <c r="AA26" s="62">
         <f t="shared" si="6"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD26" s="62">
         <f>'MARA Prices'!H$21*$G26</f>
@@ -8247,15 +8244,15 @@
       </c>
       <c r="P27" s="62">
         <f>$F27*Outputs_Internal!$D$64/12+N27</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q27" s="62">
         <f>$F27*Outputs_Internal!K$64/12+N27*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R27" s="62">
         <f>$F27*Outputs_Internal!L$64/12+N27*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S27" s="62">
         <f>N27*'MARA Prices'!$F$4</f>
@@ -8267,7 +8264,7 @@
       </c>
       <c r="U27" s="62">
         <f>$F27*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W27" s="62">
         <f t="shared" si="2"/>
@@ -8351,15 +8348,15 @@
       </c>
       <c r="P28" s="62">
         <f>$F28*Outputs_Internal!$D$64/12+N28</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q28" s="62">
         <f>$F28*Outputs_Internal!K$64/12+N28*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R28" s="62">
         <f>$F28*Outputs_Internal!L$64/12+N28*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S28" s="62">
         <f>N28*'MARA Prices'!$F$4</f>
@@ -8371,7 +8368,7 @@
       </c>
       <c r="U28" s="62">
         <f>$F28*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W28" s="62">
         <f t="shared" si="2"/>
@@ -8455,15 +8452,15 @@
       </c>
       <c r="P29" s="62">
         <f>$F29*Outputs_Internal!$D$64/12+N29</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q29" s="62">
         <f>$F29*Outputs_Internal!K$64/12+N29*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R29" s="62">
         <f>$F29*Outputs_Internal!L$64/12+N29*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S29" s="62">
         <f>N29*'MARA Prices'!$F$4</f>
@@ -8475,19 +8472,19 @@
       </c>
       <c r="U29" s="62">
         <f>$F29*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W29" s="62">
         <f t="shared" si="2"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X29" s="62">
         <f t="shared" si="3"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y29" s="62">
         <f t="shared" si="4"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z29" s="62">
         <f t="shared" si="5"/>
@@ -8495,7 +8492,7 @@
       </c>
       <c r="AA29" s="62">
         <f t="shared" si="6"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD29" s="62">
         <f>'MARA Prices'!H$21*$G29</f>
@@ -8559,15 +8556,15 @@
       </c>
       <c r="P30" s="62">
         <f>$F30*Outputs_Internal!$D$64/12+N30</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q30" s="62">
         <f>$F30*Outputs_Internal!K$64/12+N30*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R30" s="62">
         <f>$F30*Outputs_Internal!L$64/12+N30*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S30" s="62">
         <f>N30*'MARA Prices'!$F$4</f>
@@ -8579,7 +8576,7 @@
       </c>
       <c r="U30" s="62">
         <f>$F30*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W30" s="62">
         <f t="shared" si="2"/>
@@ -8663,15 +8660,15 @@
       </c>
       <c r="P31" s="62">
         <f>$F31*Outputs_Internal!$D$64/12+N31</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q31" s="62">
         <f>$F31*Outputs_Internal!K$64/12+N31*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R31" s="62">
         <f>$F31*Outputs_Internal!L$64/12+N31*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S31" s="62">
         <f>N31*'MARA Prices'!$F$4</f>
@@ -8683,7 +8680,7 @@
       </c>
       <c r="U31" s="62">
         <f>$F31*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W31" s="62">
         <f t="shared" si="2"/>
@@ -8767,15 +8764,15 @@
       </c>
       <c r="P32" s="62">
         <f>$F32*Outputs_Internal!$D$64/12+N32</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q32" s="62">
         <f>$F32*Outputs_Internal!K$64/12+N32*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R32" s="62">
         <f>$F32*Outputs_Internal!L$64/12+N32*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S32" s="62">
         <f>N32*'MARA Prices'!$F$4</f>
@@ -8787,19 +8784,19 @@
       </c>
       <c r="U32" s="62">
         <f>$F32*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W32" s="62">
         <f t="shared" si="2"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X32" s="62">
         <f t="shared" si="3"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y32" s="62">
         <f t="shared" si="4"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z32" s="62">
         <f t="shared" si="5"/>
@@ -8807,7 +8804,7 @@
       </c>
       <c r="AA32" s="62">
         <f t="shared" si="6"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD32" s="62">
         <f>'MARA Prices'!H$21*$G32</f>
@@ -8871,15 +8868,15 @@
       </c>
       <c r="P33" s="62">
         <f>$F33*Outputs_Internal!$D$64/12+N33</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q33" s="62">
         <f>$F33*Outputs_Internal!K$64/12+N33*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R33" s="62">
         <f>$F33*Outputs_Internal!L$64/12+N33*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S33" s="62">
         <f>N33*'MARA Prices'!$F$4</f>
@@ -8891,7 +8888,7 @@
       </c>
       <c r="U33" s="62">
         <f>$F33*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W33" s="62">
         <f t="shared" si="2"/>
@@ -8975,15 +8972,15 @@
       </c>
       <c r="P34" s="62">
         <f>$F34*Outputs_Internal!$D$64/12+N34</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q34" s="62">
         <f>$F34*Outputs_Internal!K$64/12+N34*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R34" s="62">
         <f>$F34*Outputs_Internal!L$64/12+N34*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S34" s="62">
         <f>N34*'MARA Prices'!$F$4</f>
@@ -8995,7 +8992,7 @@
       </c>
       <c r="U34" s="62">
         <f>$F34*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W34" s="62">
         <f t="shared" si="2"/>
@@ -9079,15 +9076,15 @@
       </c>
       <c r="P35" s="62">
         <f>$F35*Outputs_Internal!$D$64/12+N35</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q35" s="62">
         <f>$F35*Outputs_Internal!K$64/12+N35*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R35" s="62">
         <f>$F35*Outputs_Internal!L$64/12+N35*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S35" s="62">
         <f>N35*'MARA Prices'!$F$4</f>
@@ -9099,19 +9096,19 @@
       </c>
       <c r="U35" s="62">
         <f>$F35*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W35" s="62">
         <f t="shared" si="2"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X35" s="62">
         <f t="shared" si="3"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y35" s="62">
         <f t="shared" si="4"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z35" s="62">
         <f t="shared" si="5"/>
@@ -9119,7 +9116,7 @@
       </c>
       <c r="AA35" s="62">
         <f t="shared" si="6"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD35" s="62">
         <f>'MARA Prices'!H$21*$G35</f>
@@ -9183,15 +9180,15 @@
       </c>
       <c r="P36" s="62">
         <f>$F36*Outputs_Internal!$D$64/12+N36</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q36" s="62">
         <f>$F36*Outputs_Internal!K$64/12+N36*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R36" s="62">
         <f>$F36*Outputs_Internal!L$64/12+N36*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S36" s="62">
         <f>N36*'MARA Prices'!$F$4</f>
@@ -9203,7 +9200,7 @@
       </c>
       <c r="U36" s="62">
         <f>$F36*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W36" s="62">
         <f t="shared" si="2"/>
@@ -9287,15 +9284,15 @@
       </c>
       <c r="P37" s="62">
         <f>$F37*Outputs_Internal!$D$64/12+N37</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q37" s="62">
         <f>$F37*Outputs_Internal!K$64/12+N37*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R37" s="62">
         <f>$F37*Outputs_Internal!L$64/12+N37*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S37" s="62">
         <f>N37*'MARA Prices'!$F$4</f>
@@ -9307,7 +9304,7 @@
       </c>
       <c r="U37" s="62">
         <f>$F37*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W37" s="62">
         <f t="shared" ref="W37:W68" si="7">IF(MOD(MONTH($B37),3)=0,SUM(I35:I37,P35:P37),0)</f>
@@ -9391,15 +9388,15 @@
       </c>
       <c r="P38" s="62">
         <f>$F38*Outputs_Internal!$D$64/12+N38</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q38" s="62">
         <f>$F38*Outputs_Internal!K$64/12+N38*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R38" s="62">
         <f>$F38*Outputs_Internal!L$64/12+N38*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S38" s="62">
         <f>N38*'MARA Prices'!$F$4</f>
@@ -9411,19 +9408,19 @@
       </c>
       <c r="U38" s="62">
         <f>$F38*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W38" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X38" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y38" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z38" s="62">
         <f t="shared" si="10"/>
@@ -9431,7 +9428,7 @@
       </c>
       <c r="AA38" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD38" s="62">
         <f>'MARA Prices'!H$21*$G38</f>
@@ -9495,15 +9492,15 @@
       </c>
       <c r="P39" s="62">
         <f>$F39*Outputs_Internal!$D$64/12+N39</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q39" s="62">
         <f>$F39*Outputs_Internal!K$64/12+N39*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R39" s="62">
         <f>$F39*Outputs_Internal!L$64/12+N39*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S39" s="62">
         <f>N39*'MARA Prices'!$F$4</f>
@@ -9515,7 +9512,7 @@
       </c>
       <c r="U39" s="62">
         <f>$F39*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W39" s="62">
         <f t="shared" si="7"/>
@@ -9599,15 +9596,15 @@
       </c>
       <c r="P40" s="62">
         <f>$F40*Outputs_Internal!$D$64/12+N40</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q40" s="62">
         <f>$F40*Outputs_Internal!K$64/12+N40*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R40" s="62">
         <f>$F40*Outputs_Internal!L$64/12+N40*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S40" s="62">
         <f>N40*'MARA Prices'!$F$4</f>
@@ -9619,7 +9616,7 @@
       </c>
       <c r="U40" s="62">
         <f>$F40*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W40" s="62">
         <f t="shared" si="7"/>
@@ -9703,15 +9700,15 @@
       </c>
       <c r="P41" s="62">
         <f>$F41*Outputs_Internal!$D$64/12+N41</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q41" s="62">
         <f>$F41*Outputs_Internal!K$64/12+N41*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R41" s="62">
         <f>$F41*Outputs_Internal!L$64/12+N41*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S41" s="62">
         <f>N41*'MARA Prices'!$F$4</f>
@@ -9723,19 +9720,19 @@
       </c>
       <c r="U41" s="62">
         <f>$F41*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W41" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X41" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y41" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z41" s="62">
         <f t="shared" si="10"/>
@@ -9743,7 +9740,7 @@
       </c>
       <c r="AA41" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD41" s="62">
         <f>'MARA Prices'!H$21*$G41</f>
@@ -9807,15 +9804,15 @@
       </c>
       <c r="P42" s="62">
         <f>$F42*Outputs_Internal!$D$64/12+N42</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q42" s="62">
         <f>$F42*Outputs_Internal!K$64/12+N42*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R42" s="62">
         <f>$F42*Outputs_Internal!L$64/12+N42*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S42" s="62">
         <f>N42*'MARA Prices'!$F$4</f>
@@ -9827,7 +9824,7 @@
       </c>
       <c r="U42" s="62">
         <f>$F42*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W42" s="62">
         <f t="shared" si="7"/>
@@ -9911,15 +9908,15 @@
       </c>
       <c r="P43" s="62">
         <f>$F43*Outputs_Internal!$D$64/12+N43</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q43" s="62">
         <f>$F43*Outputs_Internal!K$64/12+N43*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R43" s="62">
         <f>$F43*Outputs_Internal!L$64/12+N43*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S43" s="62">
         <f>N43*'MARA Prices'!$F$4</f>
@@ -9931,7 +9928,7 @@
       </c>
       <c r="U43" s="62">
         <f>$F43*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W43" s="62">
         <f t="shared" si="7"/>
@@ -10015,15 +10012,15 @@
       </c>
       <c r="P44" s="62">
         <f>$F44*Outputs_Internal!$D$64/12+N44</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q44" s="62">
         <f>$F44*Outputs_Internal!K$64/12+N44*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R44" s="62">
         <f>$F44*Outputs_Internal!L$64/12+N44*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S44" s="62">
         <f>N44*'MARA Prices'!$F$4</f>
@@ -10035,19 +10032,19 @@
       </c>
       <c r="U44" s="62">
         <f>$F44*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W44" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X44" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y44" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z44" s="62">
         <f t="shared" si="10"/>
@@ -10055,7 +10052,7 @@
       </c>
       <c r="AA44" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD44" s="62">
         <f>'MARA Prices'!H$21*$G44</f>
@@ -10119,15 +10116,15 @@
       </c>
       <c r="P45" s="62">
         <f>$F45*Outputs_Internal!$D$64/12+N45</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q45" s="62">
         <f>$F45*Outputs_Internal!K$64/12+N45*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R45" s="62">
         <f>$F45*Outputs_Internal!L$64/12+N45*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S45" s="62">
         <f>N45*'MARA Prices'!$F$4</f>
@@ -10139,7 +10136,7 @@
       </c>
       <c r="U45" s="62">
         <f>$F45*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W45" s="62">
         <f t="shared" si="7"/>
@@ -10223,15 +10220,15 @@
       </c>
       <c r="P46" s="62">
         <f>$F46*Outputs_Internal!$D$64/12+N46</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q46" s="62">
         <f>$F46*Outputs_Internal!K$64/12+N46*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R46" s="62">
         <f>$F46*Outputs_Internal!L$64/12+N46*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S46" s="62">
         <f>N46*'MARA Prices'!$F$4</f>
@@ -10243,7 +10240,7 @@
       </c>
       <c r="U46" s="62">
         <f>$F46*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W46" s="62">
         <f t="shared" si="7"/>
@@ -10327,15 +10324,15 @@
       </c>
       <c r="P47" s="62">
         <f>$F47*Outputs_Internal!$D$64/12+N47</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q47" s="62">
         <f>$F47*Outputs_Internal!K$64/12+N47*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R47" s="62">
         <f>$F47*Outputs_Internal!L$64/12+N47*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S47" s="62">
         <f>N47*'MARA Prices'!$F$4</f>
@@ -10347,19 +10344,19 @@
       </c>
       <c r="U47" s="62">
         <f>$F47*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W47" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X47" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y47" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z47" s="62">
         <f t="shared" si="10"/>
@@ -10367,7 +10364,7 @@
       </c>
       <c r="AA47" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD47" s="62">
         <f>'MARA Prices'!H$21*$G47</f>
@@ -10431,15 +10428,15 @@
       </c>
       <c r="P48" s="62">
         <f>$F48*Outputs_Internal!$D$64/12+N48</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q48" s="62">
         <f>$F48*Outputs_Internal!K$64/12+N48*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R48" s="62">
         <f>$F48*Outputs_Internal!L$64/12+N48*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S48" s="62">
         <f>N48*'MARA Prices'!$F$4</f>
@@ -10451,7 +10448,7 @@
       </c>
       <c r="U48" s="62">
         <f>$F48*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W48" s="62">
         <f t="shared" si="7"/>
@@ -10535,15 +10532,15 @@
       </c>
       <c r="P49" s="62">
         <f>$F49*Outputs_Internal!$D$64/12+N49</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q49" s="62">
         <f>$F49*Outputs_Internal!K$64/12+N49*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R49" s="62">
         <f>$F49*Outputs_Internal!L$64/12+N49*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S49" s="62">
         <f>N49*'MARA Prices'!$F$4</f>
@@ -10555,7 +10552,7 @@
       </c>
       <c r="U49" s="62">
         <f>$F49*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W49" s="62">
         <f t="shared" si="7"/>
@@ -10639,15 +10636,15 @@
       </c>
       <c r="P50" s="62">
         <f>$F50*Outputs_Internal!$D$64/12+N50</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q50" s="62">
         <f>$F50*Outputs_Internal!K$64/12+N50*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R50" s="62">
         <f>$F50*Outputs_Internal!L$64/12+N50*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S50" s="62">
         <f>N50*'MARA Prices'!$F$4</f>
@@ -10659,19 +10656,19 @@
       </c>
       <c r="U50" s="62">
         <f>$F50*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W50" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X50" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y50" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z50" s="62">
         <f t="shared" si="10"/>
@@ -10679,7 +10676,7 @@
       </c>
       <c r="AA50" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD50" s="62">
         <f>'MARA Prices'!H$21*$G50</f>
@@ -10743,15 +10740,15 @@
       </c>
       <c r="P51" s="62">
         <f>$F51*Outputs_Internal!$D$64/12+N51</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q51" s="62">
         <f>$F51*Outputs_Internal!K$64/12+N51*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R51" s="62">
         <f>$F51*Outputs_Internal!L$64/12+N51*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S51" s="62">
         <f>N51*'MARA Prices'!$F$4</f>
@@ -10763,7 +10760,7 @@
       </c>
       <c r="U51" s="62">
         <f>$F51*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W51" s="62">
         <f t="shared" si="7"/>
@@ -10847,15 +10844,15 @@
       </c>
       <c r="P52" s="62">
         <f>$F52*Outputs_Internal!$D$64/12+N52</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q52" s="62">
         <f>$F52*Outputs_Internal!K$64/12+N52*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R52" s="62">
         <f>$F52*Outputs_Internal!L$64/12+N52*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S52" s="62">
         <f>N52*'MARA Prices'!$F$4</f>
@@ -10867,7 +10864,7 @@
       </c>
       <c r="U52" s="62">
         <f>$F52*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W52" s="62">
         <f t="shared" si="7"/>
@@ -10951,15 +10948,15 @@
       </c>
       <c r="P53" s="62">
         <f>$F53*Outputs_Internal!$D$64/12+N53</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q53" s="62">
         <f>$F53*Outputs_Internal!K$64/12+N53*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R53" s="62">
         <f>$F53*Outputs_Internal!L$64/12+N53*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S53" s="62">
         <f>N53*'MARA Prices'!$F$4</f>
@@ -10971,19 +10968,19 @@
       </c>
       <c r="U53" s="62">
         <f>$F53*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W53" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X53" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y53" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z53" s="62">
         <f t="shared" si="10"/>
@@ -10991,7 +10988,7 @@
       </c>
       <c r="AA53" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD53" s="62">
         <f>'MARA Prices'!H$21*$G53</f>
@@ -11055,15 +11052,15 @@
       </c>
       <c r="P54" s="62">
         <f>$F54*Outputs_Internal!$D$64/12+N54</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q54" s="62">
         <f>$F54*Outputs_Internal!K$64/12+N54*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R54" s="62">
         <f>$F54*Outputs_Internal!L$64/12+N54*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S54" s="62">
         <f>N54*'MARA Prices'!$F$4</f>
@@ -11075,7 +11072,7 @@
       </c>
       <c r="U54" s="62">
         <f>$F54*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W54" s="62">
         <f t="shared" si="7"/>
@@ -11159,15 +11156,15 @@
       </c>
       <c r="P55" s="62">
         <f>$F55*Outputs_Internal!$D$64/12+N55</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q55" s="62">
         <f>$F55*Outputs_Internal!K$64/12+N55*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R55" s="62">
         <f>$F55*Outputs_Internal!L$64/12+N55*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S55" s="62">
         <f>N55*'MARA Prices'!$F$4</f>
@@ -11179,7 +11176,7 @@
       </c>
       <c r="U55" s="62">
         <f>$F55*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W55" s="62">
         <f t="shared" si="7"/>
@@ -11263,15 +11260,15 @@
       </c>
       <c r="P56" s="62">
         <f>$F56*Outputs_Internal!$D$64/12+N56</f>
-        <v>25614.245961249999</v>
+        <v>26043.811616999999</v>
       </c>
       <c r="Q56" s="62">
         <f>$F56*Outputs_Internal!K$64/12+N56*'MARA Prices'!$F$5</f>
-        <v>6730.2113359233799</v>
+        <v>6746.7064134498114</v>
       </c>
       <c r="R56" s="62">
         <f>$F56*Outputs_Internal!L$64/12+N56*'MARA Prices'!$F$6</f>
-        <v>18818.528188154178</v>
+        <v>19232.035312548305</v>
       </c>
       <c r="S56" s="62">
         <f>N56*'MARA Prices'!$F$4</f>
@@ -11283,19 +11280,19 @@
       </c>
       <c r="U56" s="62">
         <f>$F56*Outputs_Internal!N$64/12</f>
-        <v>65.506437172447136</v>
+        <v>65.069891001889914</v>
       </c>
       <c r="W56" s="62">
         <f t="shared" si="7"/>
-        <v>76842.73788375</v>
+        <v>78131.434850999998</v>
       </c>
       <c r="X56" s="62">
         <f t="shared" si="8"/>
-        <v>20190.634007770139</v>
+        <v>20240.119240349435</v>
       </c>
       <c r="Y56" s="62">
         <f t="shared" si="9"/>
-        <v>56455.584564462537</v>
+        <v>57696.105937644912</v>
       </c>
       <c r="Z56" s="62">
         <f t="shared" si="10"/>
@@ -11303,7 +11300,7 @@
       </c>
       <c r="AA56" s="62">
         <f t="shared" si="11"/>
-        <v>196.51931151734141</v>
+        <v>195.20967300566974</v>
       </c>
       <c r="AD56" s="62">
         <f>'MARA Prices'!H$21*$G56</f>
@@ -15304,10 +15301,10 @@
   <dimension ref="A2:O142"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E104" sqref="E104"/>
+      <selection pane="bottomRight" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15321,19 +15318,19 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>107</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>30</v>
@@ -15388,18 +15385,18 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="K5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="5">
         <f>IF(Inputs!D$8="N",MIN(MAX(Inputs!D$12-$K6,0),$L6-$K6),0)</f>
@@ -15433,7 +15430,7 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5">
         <f>IF(Inputs!D$8="N",MIN(MAX(Inputs!D$12-$K7,0),$L7-$K7),0)</f>
@@ -15468,7 +15465,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5">
         <f>IF(Inputs!D$8="N",MIN(MAX(Inputs!D$12-$K8,0),$L8-$K8),0)</f>
@@ -15503,7 +15500,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="5">
         <f>IF(Inputs!D$8="N",MIN(MAX(Inputs!D$12-$K9,0),$L9-$K9),0)</f>
@@ -15538,7 +15535,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="78">
         <f>IFERROR(SUMPRODUCT(D6:D9,$M$6:$M$9)/SUM(D6:D9),0)</f>
@@ -15563,7 +15560,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="79">
         <f>SUM(D6:D9)</f>
@@ -15596,7 +15593,7 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="77"/>
       <c r="D13" s="110">
@@ -15629,7 +15626,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -15784,7 +15781,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D20="Y",Inputs!D$25="Y"), Prices!$C15, 0)*D$13</f>
@@ -15809,7 +15806,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" s="18">
         <f xml:space="preserve"> IF(Inputs!D23="Y",Prices!$C16, 0)*D$13</f>
@@ -15859,7 +15856,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D22="Y",Inputs!D$26="Y",Inputs!D$27="Y",Inputs!D$30="Y"), Prices!$C18, 0)*D$13</f>
@@ -15884,7 +15881,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" s="20">
         <f>IF(Inputs!D$8="N",0, IF(OR(Inputs!D23="Y",Inputs!D$26="Y",Inputs!D$27="Y"), Prices!$C19, 0))*D$13</f>
@@ -15909,7 +15906,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -16064,7 +16061,7 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="18">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(OR(Inputs!D20="Y",Inputs!D$25="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10*D$13</f>
@@ -16089,7 +16086,7 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D36" s="18">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(Inputs!D23="Y",PRODUCT(D$11, Prices!$E16),0))*D$10*D$13</f>
@@ -16139,7 +16136,7 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D38" s="20">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(OR(Inputs!D22="Y",Inputs!D$26="Y",Inputs!D$27="Y",Inputs!D$30="Y"),PRODUCT(D$11, Prices!$E18),0))*D$10*D$13</f>
@@ -16164,7 +16161,7 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="29">
         <v>0</v>
@@ -16191,7 +16188,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -16346,7 +16343,7 @@
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="18">
         <f>IF(AND(Inputs!D20="Y",Inputs!D$25="N"),Prices!$C15,0)*D$13</f>
@@ -16371,7 +16368,7 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C49" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D49" s="18">
         <f>IF(Inputs!D23="Y",Prices!$C16,0)*D$13</f>
@@ -16421,7 +16418,7 @@
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C51" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D51" s="20">
         <f>IF(AND(Inputs!D22="Y",Inputs!D$26="N",Inputs!D$27="N",Inputs!D$30="N"),Prices!$C18,0)*D$13</f>
@@ -16446,7 +16443,7 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C52" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52" s="20">
         <f>IF(Inputs!D$8="N",0,IF(AND(Inputs!D23="Y",Inputs!D$26="N",Inputs!D$27="N"),Prices!$C19,0))*D$13</f>
@@ -16471,7 +16468,7 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
@@ -16626,7 +16623,7 @@
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D61" s="18">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(AND(Inputs!D20="Y",Inputs!D$25="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))*D$13</f>
@@ -16651,7 +16648,7 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C62" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62" s="18">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(Inputs!D23="Y",PRODUCT(D$11, Prices!$E16)*D$10,0))*D$13</f>
@@ -16701,7 +16698,7 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C64" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" s="20">
         <f>IF(OR(Inputs!D$8="Y", D$11 = 0), 0, IF(AND(Inputs!D22="Y",Inputs!D$26="N",Inputs!D$27="N",Inputs!D$30="N"),PRODUCT(D$11, Prices!$E18)*D$10,0))*D$13</f>
@@ -16726,7 +16723,7 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C65" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D65" s="29">
         <v>0</v>
@@ -16746,7 +16743,7 @@
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
@@ -16826,7 +16823,7 @@
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C71" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D71" s="20">
         <f>IF(Inputs!D27="Y", Prices!$C24, 0)*D$13</f>
@@ -16876,15 +16873,15 @@
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C73" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D73" s="20">
         <f>IF(Inputs!D29="Y", Prices!$C26 * IF(Inputs!D28="Y",1-Prices!$L$21,1), IF(Inputs!D29="Monthly", Prices!$C26 * Prices!$L$30 * IF(Inputs!D28="Y",1-Prices!$L$21,1), 0))*D$13</f>
-        <v>23520</v>
+        <v>28224</v>
       </c>
       <c r="E73" s="20">
         <f>IF(Inputs!E29="Y", Prices!$C26 * IF(Inputs!E28="Y",1-Prices!$L$21,1), IF(Inputs!E29="Monthly", Prices!$C26 * Prices!$L$30 * IF(Inputs!E28="Y",1-Prices!$L$21,1), 0))*E$13</f>
-        <v>23814</v>
+        <v>28576.799999999999</v>
       </c>
       <c r="F73" s="20">
         <f>IF(Inputs!F29="Y", Prices!$C26 * IF(Inputs!F28="Y",1-Prices!$L$21,1), IF(Inputs!F29="Monthly", Prices!$C26 * Prices!$L$30 * IF(Inputs!F28="Y",1-Prices!$L$21,1), 0))*F$13</f>
@@ -16901,7 +16898,7 @@
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C74" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D74" s="20">
         <f>IF(Inputs!D30="Y", Prices!$C27, 0)*D$13</f>
@@ -16926,7 +16923,7 @@
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D75" s="20">
         <f>IF(Inputs!D31="Y", Prices!$C28, 0)*D$13</f>
@@ -16951,7 +16948,7 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C76" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D76" s="83">
         <f>IF(Inputs!D14="Y", Prices!$C29, IF(Inputs!D14="Monthly", Prices!C29 * Prices!$L$30, 0))*D$13</f>
@@ -16976,10 +16973,10 @@
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J78" s="88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
@@ -17125,7 +17122,7 @@
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C82" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D82" s="20">
         <f>IF(Inputs!D$8="Y", 0, IF(D$11 = "", 0, IF(Inputs!D27 = "Y", D$11*Prices!$E24, 0)))*D$10*D$13</f>
@@ -17223,7 +17220,7 @@
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C84" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D84" s="20">
         <f>IF(Inputs!D$8="Y", 0, IF(D$11 = "", 0, IF(Inputs!D29 = "Y", D$11*Prices!$E26 * IF(Inputs!D28="Y",1-Prices!$L$21,1),IF(Inputs!D29="Monthly", D$11*Prices!$E26 * Prices!$L$30 * IF(Inputs!D28="Y",1-Prices!$L$21,1), 0))))*D$10*D$13</f>
@@ -17231,7 +17228,7 @@
       </c>
       <c r="E84" s="20">
         <f>IF(Inputs!E$8="Y", 0, IF(E$11 = "", 0, IF(Inputs!E29 = "Y", E$11*Prices!$E26 * IF(Inputs!E28="Y",1-Prices!$L$21,1),IF(Inputs!E29="Monthly", E$11*Prices!$E26 * Prices!$L$30 * IF(Inputs!E28="Y",1-Prices!$L$21,1), 0))))*E$10*E$13</f>
-        <v>10111.707899999999</v>
+        <v>12134.049479999996</v>
       </c>
       <c r="F84" s="20">
         <f>IF(Inputs!F$8="Y", 0, IF(F$11 = "", 0, IF(Inputs!F29 = "Y", F$11*Prices!$E26 * IF(Inputs!F28="Y",1-Prices!$L$21,1),IF(Inputs!F29="Monthly", F$11*Prices!$E26 * Prices!$L$30 * IF(Inputs!F28="Y",1-Prices!$L$21,1), 0))))*F$10*F$13</f>
@@ -17251,11 +17248,11 @@
       </c>
       <c r="K84" s="23">
         <f t="shared" si="1"/>
-        <v>23520.001499999998</v>
+        <v>28224.001499999998</v>
       </c>
       <c r="L84" s="23">
         <f t="shared" si="1"/>
-        <v>33925.7094</v>
+        <v>40710.850979999996</v>
       </c>
       <c r="M84" s="23">
         <f t="shared" si="1"/>
@@ -17272,7 +17269,7 @@
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C85" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D85" s="20">
         <f>IF(Inputs!D$8="Y", 0, IF(D$11 = "", 0, IF(Inputs!D30 = "Y", D$11*Prices!$E27, 0)))*D$10*D$13</f>
@@ -17321,7 +17318,7 @@
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C86" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D86" s="20">
         <f>IF(Inputs!D$8="Y", 0, IF(D$11 = "", 0, IF(Inputs!D31 = "Y", D$11*Prices!$E28, 0)))*D$10*D$13</f>
@@ -17370,7 +17367,7 @@
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C87" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D87" s="83">
         <f>IF(Inputs!D$8="Y", 0, IF(D$11 = "", 0, IF(Inputs!D14 = "Y", D$11*Prices!$E29, IF(Inputs!D14="Monthly", D$11*Prices!$E29*Prices!$L$30,0))))*D$10*D$13</f>
@@ -17426,7 +17423,7 @@
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
@@ -17566,7 +17563,7 @@
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C93" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D93" s="20">
         <f>IF(D71=0,0,D71-IF(Inputs!D26="Y", 0, SUM(D24:D26)))</f>
@@ -17656,15 +17653,15 @@
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C95" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D95" s="20">
         <f>D73</f>
-        <v>23520</v>
+        <v>28224</v>
       </c>
       <c r="E95" s="20">
         <f>E73</f>
-        <v>23814</v>
+        <v>28576.799999999999</v>
       </c>
       <c r="F95" s="20">
         <f t="shared" ref="F95:H95" si="12">F73</f>
@@ -17701,7 +17698,7 @@
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C96" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D96" s="20">
         <f>IF(D74=0,0,D74-IF(OR(Inputs!D26="Y",Inputs!D27="Y"), 0, D25))</f>
@@ -17746,7 +17743,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C97" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D97" s="20">
         <f>D75</f>
@@ -17791,7 +17788,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C98" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D98" s="83">
         <f>D76</f>
@@ -17836,7 +17833,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B100" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -17911,7 +17908,7 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C104" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D104" s="20">
         <f>MAX(IF(D82=0,0,D82-IF(Inputs!D26="Y", 0,SUM(D37:D38))),0)</f>
@@ -17961,7 +17958,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C106" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D106" s="20">
         <f>D84</f>
@@ -17969,7 +17966,7 @@
       </c>
       <c r="E106" s="20">
         <f>E84</f>
-        <v>10111.707899999999</v>
+        <v>12134.049479999996</v>
       </c>
       <c r="F106" s="20">
         <f t="shared" ref="F106:H106" si="22">F84</f>
@@ -17986,7 +17983,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C107" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D107" s="20">
         <f>MAX(IF(D85=0,0,D85-IF(OR(Inputs!D26="Y",Inputs!D27="Y"), 0, D38)),0)</f>
@@ -18011,7 +18008,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C108" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D108" s="20">
         <f>D86</f>
@@ -18036,7 +18033,7 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C109" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D109" s="83">
         <f>D87</f>
@@ -18125,11 +18122,11 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D114" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$68:D$76, MATCH($A114, K$90:K$98, 0)), INDEX(D$79:D$87, MATCH($A114, K$90:K$98, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-10584</v>
+        <v>-12700.800000000001</v>
       </c>
       <c r="E114" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$68:E$76, MATCH($A114, L$90:L$98, 0)), INDEX(E$79:E$87, MATCH($A114, L$90:L$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18153,7 +18150,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D115" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$68:D$76, MATCH($A115, K$90:K$98, 0)), INDEX(D$79:D$87, MATCH($A115, K$90:K$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18161,7 +18158,7 @@
       </c>
       <c r="E115" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$68:E$76, MATCH($A115, L$90:L$98, 0)), INDEX(E$79:E$87, MATCH($A115, L$90:L$98, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-15266.568555000002</v>
+        <v>-18319.882266000001</v>
       </c>
       <c r="F115" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(F$68:F$76, MATCH($A115, M$90:M$98, 0)), INDEX(F$79:F$87, MATCH($A115, M$90:M$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18181,7 +18178,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D116" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$68:D$76, MATCH($A116, K$90:K$98, 0)), INDEX(D$79:D$87, MATCH($A116, K$90:K$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18209,7 +18206,7 @@
         <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D117" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$68:D$76, MATCH($A117, K$90:K$98, 0)), INDEX(D$79:D$87, MATCH($A117, K$90:K$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18237,7 +18234,7 @@
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D118" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$68:D$76, MATCH($A118, K$90:K$98, 0)), INDEX(D$79:D$87, MATCH($A118, K$90:K$98, 0)))*Prices!$L$6*-1, 0)</f>
@@ -18262,15 +18259,15 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B120" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D120" s="7">
         <f>SUM(D42:D52, D55:D65, D68:D76, D79:D87, D112:D118)</f>
-        <v>125472</v>
+        <v>128059.20000000001</v>
       </c>
       <c r="E120" s="7">
         <f>SUM(E42:E52, E55:E65, E68:E76, E79:E87, E112:E118)</f>
-        <v>238361.35153499997</v>
+        <v>242093.17940399997</v>
       </c>
       <c r="F120" s="7">
         <f>SUM(F42:F52, F55:F65, F68:F76, F79:F87, F112:F118)</f>
@@ -18290,11 +18287,11 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B122" s="6" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="D122" s="1">
         <f>IF(D132=1, 0, IF(D132=2, $E$135, IF(D132=3, $E$136, IF(D132=4, $E$137, IF(D132=5, $E$138, "")))))</f>
-        <v>-56462.400000000001</v>
+        <v>-57626.640000000007</v>
       </c>
       <c r="E122" s="1">
         <f t="shared" ref="E122:H122" si="25">IF(E132=1, 0, IF(E132=2, $E$135, IF(E132=3, $E$136, IF(E132=4, $E$137, IF(E132=5, $E$138, "")))))</f>
@@ -18322,7 +18319,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D124" s="1">
         <f>IF(Inputs!$D$9 = "Y", Prices!$L$19, 0)*-1</f>
@@ -18343,15 +18340,15 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B126" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D126" s="7">
         <f>SUM(D120, D122,D124)</f>
-        <v>69009.600000000006</v>
+        <v>70432.56</v>
       </c>
       <c r="E126" s="7">
         <f t="shared" ref="E126:H126" si="26">SUM(E120, E122,E124)</f>
-        <v>238361.35153499997</v>
+        <v>242093.17940399997</v>
       </c>
       <c r="F126" s="7">
         <f t="shared" si="26"/>
@@ -18369,7 +18366,7 @@
     <row r="129" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="27"/>
       <c r="C129" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D129" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D120,$D$120:$H$120),5)</f>
@@ -18462,23 +18459,23 @@
     <row r="134" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="27"/>
       <c r="C134" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="27"/>
       <c r="D135" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E135" s="97">
         <f>INDEX($D$120:$H$120, 1, MATCH(2, $D$132:$H$132, 0))*Prices!$L$10*-1</f>
-        <v>-56462.400000000001</v>
+        <v>-57626.640000000007</v>
       </c>
     </row>
     <row r="136" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="27"/>
       <c r="D136" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E136" s="23">
         <f>INDEX($D$120:$H$120, 1, MATCH(3, $D$132:$H$132, 0))*Prices!$L$11*-1</f>
@@ -18488,7 +18485,7 @@
     <row r="137" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="27"/>
       <c r="D137" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E137" s="23">
         <f>INDEX($D$120:$H$120, 1, MATCH(4, $D$132:$H$132, 0))*Prices!$L$11*-1</f>
@@ -18498,7 +18495,7 @@
     <row r="138" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="27"/>
       <c r="D138" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E138" s="23">
         <f>INDEX($D$120:$H$120, 1, MATCH(5, $D$132:$H$132, 0))*Prices!$L$11*-1</f>
@@ -18518,9 +18515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18545,7 +18540,7 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1">
         <v>5000</v>
@@ -18572,7 +18567,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="75">
         <v>0.6</v>
@@ -18592,16 +18587,16 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E5" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="G5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="47" t="s">
-        <v>85</v>
-      </c>
       <c r="H5" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" t="s">
         <v>25</v>
@@ -18649,7 +18644,7 @@
       <c r="C8" s="42"/>
       <c r="D8" s="38"/>
       <c r="K8" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -18661,7 +18656,7 @@
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
       <c r="K9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -18692,7 +18687,7 @@
         <v>0.01</v>
       </c>
       <c r="K10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L10" s="3">
         <v>0.45</v>
@@ -18723,7 +18718,7 @@
         <v>0.01</v>
       </c>
       <c r="K11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L11" s="3">
         <v>0.5</v>
@@ -18805,7 +18800,7 @@
         <v>0.01</v>
       </c>
       <c r="K14" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L14" s="56">
         <v>1.2500000000000001E-2</v>
@@ -18813,7 +18808,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="43">
         <f>$L$28*4000</f>
@@ -18836,7 +18831,7 @@
         <v>0.01</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="53">
         <v>43466</v>
@@ -18846,7 +18841,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" s="43">
         <f>$L$28*3500</f>
@@ -18869,7 +18864,7 @@
         <v>0.01</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L16" s="53">
         <v>43101</v>
@@ -18904,7 +18899,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="44">
         <f>$L$28*10000</f>
@@ -18929,7 +18924,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="44">
         <f>$L$28*1500</f>
@@ -18952,7 +18947,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L19" s="1">
         <v>3525</v>
@@ -18990,7 +18985,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L21" s="3">
         <v>0.3</v>
@@ -19048,7 +19043,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24" s="44">
         <f>$L$28*35000</f>
@@ -19096,7 +19091,7 @@
         <v>0.05</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L25" s="95">
         <f>18000/15000</f>
@@ -19105,32 +19100,32 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="44">
-        <f>33600</f>
-        <v>33600</v>
+        <f>$L$28*33600</f>
+        <v>40320</v>
       </c>
       <c r="E26" s="40">
-        <f>ROUND(0.25, 2)</f>
-        <v>0.25</v>
+        <f>ROUND($L$28*0.25, 2)</f>
+        <v>0.3</v>
       </c>
       <c r="F26" s="40">
         <f t="shared" si="3"/>
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="G26" s="40">
         <f t="shared" si="3"/>
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H26" s="40">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="44">
         <f>$L$28*28000</f>
@@ -19155,7 +19150,7 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="44">
         <f>$L$28*20000</f>
@@ -19178,7 +19173,7 @@
         <v>0.03</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L28" s="96">
         <f>IF(Inputs!$C$3="Monthly",Prices!$L$25,1)</f>
@@ -19187,7 +19182,7 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="81">
         <f>$L$28*IF(Inputs!$C$4 = "Yes", 6750, 9600)</f>
@@ -19212,7 +19207,7 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L30" s="101">
         <f>IF(Inputs!$C$3="Quarterly",$L$25,1)</f>
@@ -19245,34 +19240,34 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3">
         <v>0.05</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -19286,7 +19281,7 @@
         <v>0.2</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="53">
         <v>43831</v>
@@ -19354,7 +19349,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="3">
         <v>0.8</v>
@@ -19391,7 +19386,7 @@
         <v>0.11</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="3">
         <v>0.1</v>
@@ -19691,26 +19686,26 @@
       <c r="E19" s="2"/>
       <c r="F19" s="102"/>
       <c r="H19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="J19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="K19" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="L19" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20" s="102"/>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" s="105">
         <f>IF(Inputs!D$11 = "Y", SUM(H10:H16), 0)</f>
@@ -19737,7 +19732,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="102"/>
       <c r="G21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H21" s="105">
         <f>H20/12</f>

</xml_diff>

<commit_message>
Add labeling to new composite discount sections.
Do this so it is a bit easier to remember what those sections are for in
the future.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason.altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="161">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -548,6 +548,9 @@
   </si>
   <si>
     <t>Base Year</t>
+  </si>
+  <si>
+    <t>Compoisite PMPY Scalars by line item</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1329,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,10 +1816,10 @@
   <dimension ref="B2:U51"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,7 +2919,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40:D45"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5596,10 +5599,10 @@
   <dimension ref="B1:AH94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R39" sqref="R39"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15300,10 +15303,10 @@
   <dimension ref="A2:U142"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15313,6 +15316,7 @@
     <col min="3" max="3" width="46.85546875" customWidth="1"/>
     <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="15" width="18" style="21" customWidth="1"/>
+    <col min="17" max="21" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -15910,6 +15914,9 @@
       <c r="B28" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="K28" s="21" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C29" s="15" t="s">
@@ -15935,23 +15942,23 @@
         <f>IF(Inputs!H$8="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)))*O29*H$13</f>
         <v>0</v>
       </c>
-      <c r="K29" s="21">
+      <c r="K29" s="76">
         <f>IFERROR(SUM((D$6*Prices!N6), (D$7*Prices!O6), (D$8*Prices!P6), (D$9*Prices!Q6))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L29" s="21">
+      <c r="L29" s="76">
         <f>IFERROR(SUM((E$6*Prices!O6), (E$7*Prices!P6), (E$8*Prices!Q6), (E$9*Prices!R6))/SUM(E$6:E$9),1)</f>
         <v>0.68352946804439341</v>
       </c>
-      <c r="M29" s="21">
+      <c r="M29" s="76">
         <f>IFERROR(SUM((F$6*Prices!P6), (F$7*Prices!Q6), (F$8*Prices!R6), (F$9*Prices!S6))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q6), (G$7*Prices!R6), (G$8*Prices!S6), (G$9*Prices!T6))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O29" s="21">
+      <c r="O29" s="76">
         <f>IFERROR(SUM((H$6*Prices!R6), (H$7*Prices!S6), (H$8*Prices!T6), (H$9*Prices!U6))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -15980,23 +15987,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$25="Y"),PRODUCT(H$11, Prices!$E10),0))*O30*H$13</f>
         <v>0</v>
       </c>
-      <c r="K30" s="21">
+      <c r="K30" s="76">
         <f>IFERROR(SUM((D$6*Prices!N10), (D$7*Prices!O10), (D$8*Prices!P10), (D$9*Prices!Q10))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L30" s="21">
+      <c r="L30" s="76">
         <f>IFERROR(SUM((E$6*Prices!O10), (E$7*Prices!P10), (E$8*Prices!Q10), (E$9*Prices!R10))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M30" s="21">
+      <c r="M30" s="76">
         <f>IFERROR(SUM((F$6*Prices!P10), (F$7*Prices!Q10), (F$8*Prices!R10), (F$9*Prices!S10))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N30" s="21">
+      <c r="N30" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q10), (G$7*Prices!R10), (G$8*Prices!S10), (G$9*Prices!T10))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O30" s="21">
+      <c r="O30" s="76">
         <f>IFERROR(SUM((H$6*Prices!R10), (H$7*Prices!S10), (H$8*Prices!T10), (H$9*Prices!U10))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16025,23 +16032,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$25="Y"),PRODUCT(H$11, Prices!$E11),0))*O31*H$13</f>
         <v>0</v>
       </c>
-      <c r="K31" s="21">
+      <c r="K31" s="76">
         <f>IFERROR(SUM((D$6*Prices!N11), (D$7*Prices!O11), (D$8*Prices!P11), (D$9*Prices!Q11))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L31" s="21">
+      <c r="L31" s="76">
         <f>IFERROR(SUM((E$6*Prices!O11), (E$7*Prices!P11), (E$8*Prices!Q11), (E$9*Prices!R11))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M31" s="21">
+      <c r="M31" s="76">
         <f>IFERROR(SUM((F$6*Prices!P11), (F$7*Prices!Q11), (F$8*Prices!R11), (F$9*Prices!S11))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q11), (G$7*Prices!R11), (G$8*Prices!S11), (G$9*Prices!T11))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O31" s="21">
+      <c r="O31" s="76">
         <f>IFERROR(SUM((H$6*Prices!R11), (H$7*Prices!S11), (H$8*Prices!T11), (H$9*Prices!U11))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16070,23 +16077,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$25="Y"),PRODUCT(H$11, Prices!$E12),0))*O32*H$13</f>
         <v>0</v>
       </c>
-      <c r="K32" s="21">
+      <c r="K32" s="76">
         <f>IFERROR(SUM((D$6*Prices!N12), (D$7*Prices!O12), (D$8*Prices!P12), (D$9*Prices!Q12))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L32" s="21">
+      <c r="L32" s="76">
         <f>IFERROR(SUM((E$6*Prices!O12), (E$7*Prices!P12), (E$8*Prices!Q12), (E$9*Prices!R12))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M32" s="21">
+      <c r="M32" s="76">
         <f>IFERROR(SUM((F$6*Prices!P12), (F$7*Prices!Q12), (F$8*Prices!R12), (F$9*Prices!S12))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q12), (G$7*Prices!R12), (G$8*Prices!S12), (G$9*Prices!T12))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O32" s="21">
+      <c r="O32" s="76">
         <f>IFERROR(SUM((H$6*Prices!R12), (H$7*Prices!S12), (H$8*Prices!T12), (H$9*Prices!U12))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16115,23 +16122,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H18="Y",Inputs!H$25="Y"),PRODUCT(H$11, Prices!$E13),0))*O33*H$13</f>
         <v>0</v>
       </c>
-      <c r="K33" s="21">
+      <c r="K33" s="76">
         <f>IFERROR(SUM((D$6*Prices!N13), (D$7*Prices!O13), (D$8*Prices!P13), (D$9*Prices!Q13))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L33" s="21">
+      <c r="L33" s="76">
         <f>IFERROR(SUM((E$6*Prices!O13), (E$7*Prices!P13), (E$8*Prices!Q13), (E$9*Prices!R13))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M33" s="21">
+      <c r="M33" s="76">
         <f>IFERROR(SUM((F$6*Prices!P13), (F$7*Prices!Q13), (F$8*Prices!R13), (F$9*Prices!S13))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q13), (G$7*Prices!R13), (G$8*Prices!S13), (G$9*Prices!T13))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O33" s="21">
+      <c r="O33" s="76">
         <f>IFERROR(SUM((H$6*Prices!R13), (H$7*Prices!S13), (H$8*Prices!T13), (H$9*Prices!U13))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16160,23 +16167,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(Inputs!H19="Y",PRODUCT(H$11, Prices!$E14),0))*O34*H$13</f>
         <v>0</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="76">
         <f>IFERROR(SUM((D$6*Prices!N14), (D$7*Prices!O14), (D$8*Prices!P14), (D$9*Prices!Q14))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L34" s="21">
+      <c r="L34" s="76">
         <f>IFERROR(SUM((E$6*Prices!O14), (E$7*Prices!P14), (E$8*Prices!Q14), (E$9*Prices!R14))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M34" s="21">
+      <c r="M34" s="76">
         <f>IFERROR(SUM((F$6*Prices!P14), (F$7*Prices!Q14), (F$8*Prices!R14), (F$9*Prices!S14))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q14), (G$7*Prices!R14), (G$8*Prices!S14), (G$9*Prices!T14))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O34" s="21">
+      <c r="O34" s="76">
         <f>IFERROR(SUM((H$6*Prices!R14), (H$7*Prices!S14), (H$8*Prices!T14), (H$9*Prices!U14))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16205,23 +16212,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H20="Y",Inputs!H$25="Y"),PRODUCT(H$11, Prices!$E15),0))*O35*H$13</f>
         <v>0</v>
       </c>
-      <c r="K35" s="21">
+      <c r="K35" s="76">
         <f>IFERROR(SUM((D$6*Prices!N15), (D$7*Prices!O15), (D$8*Prices!P15), (D$9*Prices!Q15))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L35" s="21">
+      <c r="L35" s="76">
         <f>IFERROR(SUM((E$6*Prices!O15), (E$7*Prices!P15), (E$8*Prices!Q15), (E$9*Prices!R15))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M35" s="21">
+      <c r="M35" s="76">
         <f>IFERROR(SUM((F$6*Prices!P15), (F$7*Prices!Q15), (F$8*Prices!R15), (F$9*Prices!S15))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q15), (G$7*Prices!R15), (G$8*Prices!S15), (G$9*Prices!T15))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O35" s="21">
+      <c r="O35" s="76">
         <f>IFERROR(SUM((H$6*Prices!R15), (H$7*Prices!S15), (H$8*Prices!T15), (H$9*Prices!U15))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16250,23 +16257,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(Inputs!H23="Y",PRODUCT(H$11, Prices!$E16),0))*O36*H$13</f>
         <v>0</v>
       </c>
-      <c r="K36" s="21">
+      <c r="K36" s="76">
         <f>IFERROR(SUM((D$6*Prices!N16), (D$7*Prices!O16), (D$8*Prices!P16), (D$9*Prices!Q16))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L36" s="21">
+      <c r="L36" s="76">
         <f>IFERROR(SUM((E$6*Prices!O16), (E$7*Prices!P16), (E$8*Prices!Q16), (E$9*Prices!R16))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M36" s="21">
+      <c r="M36" s="76">
         <f>IFERROR(SUM((F$6*Prices!P16), (F$7*Prices!Q16), (F$8*Prices!R16), (F$9*Prices!S16))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q16), (G$7*Prices!R16), (G$8*Prices!S16), (G$9*Prices!T16))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O36" s="21">
+      <c r="O36" s="76">
         <f>IFERROR(SUM((H$6*Prices!R16), (H$7*Prices!S16), (H$8*Prices!T16), (H$9*Prices!U16))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16295,23 +16302,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H21="Y",Inputs!H$26="Y",Inputs!H$27="Y"),PRODUCT(H$11, Prices!$E17),0))*O37*H$13</f>
         <v>0</v>
       </c>
-      <c r="K37" s="21">
+      <c r="K37" s="76">
         <f>IFERROR(SUM((D$6*Prices!N17), (D$7*Prices!O17), (D$8*Prices!P17), (D$9*Prices!Q17))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L37" s="21">
+      <c r="L37" s="76">
         <f>IFERROR(SUM((E$6*Prices!O17), (E$7*Prices!P17), (E$8*Prices!Q17), (E$9*Prices!R17))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="M37" s="21">
+      <c r="M37" s="76">
         <f>IFERROR(SUM((F$6*Prices!P17), (F$7*Prices!Q17), (F$8*Prices!R17), (F$9*Prices!S17))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N37" s="21">
+      <c r="N37" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q17), (G$7*Prices!R17), (G$8*Prices!S17), (G$9*Prices!T17))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O37" s="21">
+      <c r="O37" s="76">
         <f>IFERROR(SUM((H$6*Prices!R17), (H$7*Prices!S17), (H$8*Prices!T17), (H$9*Prices!U17))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16340,23 +16347,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(OR(Inputs!H22="Y",Inputs!H$26="Y",Inputs!H$27="Y"),PRODUCT(H$11, Prices!$E18),0))*O38*H$13</f>
         <v>0</v>
       </c>
-      <c r="K38" s="21">
+      <c r="K38" s="76">
         <f>IFERROR(SUM((D$6*Prices!N18), (D$7*Prices!O18), (D$8*Prices!P18), (D$9*Prices!Q18))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L38" s="21">
+      <c r="L38" s="76">
         <f>IFERROR(SUM((E$6*Prices!O18), (E$7*Prices!P18), (E$8*Prices!Q18), (E$9*Prices!R18))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="M38" s="21">
+      <c r="M38" s="76">
         <f>IFERROR(SUM((F$6*Prices!P18), (F$7*Prices!Q18), (F$8*Prices!R18), (F$9*Prices!S18))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N38" s="21">
+      <c r="N38" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q18), (G$7*Prices!R18), (G$8*Prices!S18), (G$9*Prices!T18))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O38" s="21">
+      <c r="O38" s="76">
         <f>IFERROR(SUM((H$6*Prices!R18), (H$7*Prices!S18), (H$8*Prices!T18), (H$9*Prices!U18))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16380,23 +16387,23 @@
       <c r="H39" s="29">
         <v>0</v>
       </c>
-      <c r="K39" s="21">
+      <c r="K39" s="76">
         <f>IFERROR(SUM((D$6*Prices!N19), (D$7*Prices!O19), (D$8*Prices!P19), (D$9*Prices!Q19))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L39" s="21">
+      <c r="L39" s="76">
         <f>IFERROR(SUM((E$6*Prices!O19), (E$7*Prices!P19), (E$8*Prices!Q19), (E$9*Prices!R19))/SUM(E$6:E$9),1)</f>
         <v>0</v>
       </c>
-      <c r="M39" s="21">
+      <c r="M39" s="76">
         <f>IFERROR(SUM((F$6*Prices!P19), (F$7*Prices!Q19), (F$8*Prices!R19), (F$9*Prices!S19))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N39" s="21">
+      <c r="N39" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q19), (G$7*Prices!R19), (G$8*Prices!S19), (G$9*Prices!T19))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O39" s="21">
+      <c r="O39" s="76">
         <f>IFERROR(SUM((H$6*Prices!R19), (H$7*Prices!S19), (H$8*Prices!T19), (H$9*Prices!U19))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16692,6 +16699,9 @@
       <c r="B54" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="K54" s="21" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C55" s="15" t="s">
@@ -16717,23 +16727,23 @@
         <f>IF(Inputs!H$8="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)*O55))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K55" s="21">
+      <c r="K55" s="76">
         <f>IFERROR(SUM((D$6*Prices!N6), (D$7*Prices!O6), (D$8*Prices!P6), (D$9*Prices!Q6))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L55" s="21">
+      <c r="L55" s="76">
         <f>IFERROR(SUM((E$6*Prices!O6), (E$7*Prices!P6), (E$8*Prices!Q6), (E$9*Prices!R6))/SUM(E$6:E$9),1)</f>
         <v>0.68352946804439341</v>
       </c>
-      <c r="M55" s="21">
+      <c r="M55" s="76">
         <f>IFERROR(SUM((F$6*Prices!P6), (F$7*Prices!Q6), (F$8*Prices!R6), (F$9*Prices!S6))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N55" s="21">
+      <c r="N55" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q6), (G$7*Prices!R6), (G$8*Prices!S6), (G$9*Prices!T6))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O55" s="21">
+      <c r="O55" s="76">
         <f>IFERROR(SUM((H$6*Prices!R6), (H$7*Prices!S6), (H$8*Prices!T6), (H$9*Prices!U6))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16762,23 +16772,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E10)*O56,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K56" s="21">
+      <c r="K56" s="76">
         <f>IFERROR(SUM((D$6*Prices!N10), (D$7*Prices!O10), (D$8*Prices!P10), (D$9*Prices!Q10))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L56" s="21">
+      <c r="L56" s="76">
         <f>IFERROR(SUM((E$6*Prices!O10), (E$7*Prices!P10), (E$8*Prices!Q10), (E$9*Prices!R10))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M56" s="21">
+      <c r="M56" s="76">
         <f>IFERROR(SUM((F$6*Prices!P10), (F$7*Prices!Q10), (F$8*Prices!R10), (F$9*Prices!S10))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N56" s="21">
+      <c r="N56" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q10), (G$7*Prices!R10), (G$8*Prices!S10), (G$9*Prices!T10))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O56" s="21">
+      <c r="O56" s="76">
         <f>IFERROR(SUM((H$6*Prices!R10), (H$7*Prices!S10), (H$8*Prices!T10), (H$9*Prices!U10))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16807,23 +16817,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E11)*O57,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K57" s="21">
+      <c r="K57" s="76">
         <f>IFERROR(SUM((D$6*Prices!N11), (D$7*Prices!O11), (D$8*Prices!P11), (D$9*Prices!Q11))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L57" s="21">
+      <c r="L57" s="76">
         <f>IFERROR(SUM((E$6*Prices!O11), (E$7*Prices!P11), (E$8*Prices!Q11), (E$9*Prices!R11))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M57" s="21">
+      <c r="M57" s="76">
         <f>IFERROR(SUM((F$6*Prices!P11), (F$7*Prices!Q11), (F$8*Prices!R11), (F$9*Prices!S11))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N57" s="21">
+      <c r="N57" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q11), (G$7*Prices!R11), (G$8*Prices!S11), (G$9*Prices!T11))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O57" s="21">
+      <c r="O57" s="76">
         <f>IFERROR(SUM((H$6*Prices!R11), (H$7*Prices!S11), (H$8*Prices!T11), (H$9*Prices!U11))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16852,23 +16862,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E12)*O58,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K58" s="21">
+      <c r="K58" s="76">
         <f>IFERROR(SUM((D$6*Prices!N12), (D$7*Prices!O12), (D$8*Prices!P12), (D$9*Prices!Q12))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L58" s="21">
+      <c r="L58" s="76">
         <f>IFERROR(SUM((E$6*Prices!O12), (E$7*Prices!P12), (E$8*Prices!Q12), (E$9*Prices!R12))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M58" s="21">
+      <c r="M58" s="76">
         <f>IFERROR(SUM((F$6*Prices!P12), (F$7*Prices!Q12), (F$8*Prices!R12), (F$9*Prices!S12))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N58" s="21">
+      <c r="N58" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q12), (G$7*Prices!R12), (G$8*Prices!S12), (G$9*Prices!T12))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O58" s="21">
+      <c r="O58" s="76">
         <f>IFERROR(SUM((H$6*Prices!R12), (H$7*Prices!S12), (H$8*Prices!T12), (H$9*Prices!U12))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16897,23 +16907,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H18="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E13)*O59,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K59" s="21">
+      <c r="K59" s="76">
         <f>IFERROR(SUM((D$6*Prices!N13), (D$7*Prices!O13), (D$8*Prices!P13), (D$9*Prices!Q13))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L59" s="21">
+      <c r="L59" s="76">
         <f>IFERROR(SUM((E$6*Prices!O13), (E$7*Prices!P13), (E$8*Prices!Q13), (E$9*Prices!R13))/SUM(E$6:E$9),1)</f>
         <v>0.67837734404898575</v>
       </c>
-      <c r="M59" s="21">
+      <c r="M59" s="76">
         <f>IFERROR(SUM((F$6*Prices!P13), (F$7*Prices!Q13), (F$8*Prices!R13), (F$9*Prices!S13))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N59" s="21">
+      <c r="N59" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q13), (G$7*Prices!R13), (G$8*Prices!S13), (G$9*Prices!T13))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O59" s="21">
+      <c r="O59" s="76">
         <f>IFERROR(SUM((H$6*Prices!R13), (H$7*Prices!S13), (H$8*Prices!T13), (H$9*Prices!U13))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16942,23 +16952,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H19="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E14)*O60,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K60" s="21">
+      <c r="K60" s="76">
         <f>IFERROR(SUM((D$6*Prices!N14), (D$7*Prices!O14), (D$8*Prices!P14), (D$9*Prices!Q14))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L60" s="21">
+      <c r="L60" s="76">
         <f>IFERROR(SUM((E$6*Prices!O14), (E$7*Prices!P14), (E$8*Prices!Q14), (E$9*Prices!R14))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M60" s="21">
+      <c r="M60" s="76">
         <f>IFERROR(SUM((F$6*Prices!P14), (F$7*Prices!Q14), (F$8*Prices!R14), (F$9*Prices!S14))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N60" s="21">
+      <c r="N60" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q14), (G$7*Prices!R14), (G$8*Prices!S14), (G$9*Prices!T14))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O60" s="21">
+      <c r="O60" s="76">
         <f>IFERROR(SUM((H$6*Prices!R14), (H$7*Prices!S14), (H$8*Prices!T14), (H$9*Prices!U14))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -16987,23 +16997,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H20="Y",Inputs!H$25="N"),PRODUCT(H$11, Prices!$E15)*O61,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K61" s="21">
+      <c r="K61" s="76">
         <f>IFERROR(SUM((D$6*Prices!N15), (D$7*Prices!O15), (D$8*Prices!P15), (D$9*Prices!Q15))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L61" s="21">
+      <c r="L61" s="76">
         <f>IFERROR(SUM((E$6*Prices!O15), (E$7*Prices!P15), (E$8*Prices!Q15), (E$9*Prices!R15))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M61" s="21">
+      <c r="M61" s="76">
         <f>IFERROR(SUM((F$6*Prices!P15), (F$7*Prices!Q15), (F$8*Prices!R15), (F$9*Prices!S15))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N61" s="21">
+      <c r="N61" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q15), (G$7*Prices!R15), (G$8*Prices!S15), (G$9*Prices!T15))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O61" s="21">
+      <c r="O61" s="76">
         <f>IFERROR(SUM((H$6*Prices!R15), (H$7*Prices!S15), (H$8*Prices!T15), (H$9*Prices!U15))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17032,23 +17042,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(Inputs!H23="Y",PRODUCT(H$11, Prices!$E16)*O62,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K62" s="21">
+      <c r="K62" s="76">
         <f>IFERROR(SUM((D$6*Prices!N16), (D$7*Prices!O16), (D$8*Prices!P16), (D$9*Prices!Q16))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L62" s="21">
+      <c r="L62" s="76">
         <f>IFERROR(SUM((E$6*Prices!O16), (E$7*Prices!P16), (E$8*Prices!Q16), (E$9*Prices!R16))/SUM(E$6:E$9),1)</f>
         <v>0.67012465146793498</v>
       </c>
-      <c r="M62" s="21">
+      <c r="M62" s="76">
         <f>IFERROR(SUM((F$6*Prices!P16), (F$7*Prices!Q16), (F$8*Prices!R16), (F$9*Prices!S16))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N62" s="21">
+      <c r="N62" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q16), (G$7*Prices!R16), (G$8*Prices!S16), (G$9*Prices!T16))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O62" s="21">
+      <c r="O62" s="76">
         <f>IFERROR(SUM((H$6*Prices!R16), (H$7*Prices!S16), (H$8*Prices!T16), (H$9*Prices!U16))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17077,23 +17087,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H21="Y",Inputs!H$26="N",Inputs!H$27="N"),PRODUCT(H$11, Prices!$E17)*O63,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K63" s="21">
+      <c r="K63" s="76">
         <f>IFERROR(SUM((D$6*Prices!N17), (D$7*Prices!O17), (D$8*Prices!P17), (D$9*Prices!Q17))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L63" s="21">
+      <c r="L63" s="76">
         <f>IFERROR(SUM((E$6*Prices!O17), (E$7*Prices!P17), (E$8*Prices!Q17), (E$9*Prices!R17))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="M63" s="21">
+      <c r="M63" s="76">
         <f>IFERROR(SUM((F$6*Prices!P17), (F$7*Prices!Q17), (F$8*Prices!R17), (F$9*Prices!S17))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N63" s="21">
+      <c r="N63" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q17), (G$7*Prices!R17), (G$8*Prices!S17), (G$9*Prices!T17))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O63" s="21">
+      <c r="O63" s="76">
         <f>IFERROR(SUM((H$6*Prices!R17), (H$7*Prices!S17), (H$8*Prices!T17), (H$9*Prices!U17))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17122,23 +17132,23 @@
         <f>IF(OR(Inputs!H$8="Y", H$11 = 0), 0, IF(AND(Inputs!H22="Y",Inputs!H$26="N",Inputs!H$27="N",Inputs!H$30="N"),PRODUCT(H$11, Prices!$E18)*O64,0))*H$13</f>
         <v>0</v>
       </c>
-      <c r="K64" s="21">
+      <c r="K64" s="76">
         <f>IFERROR(SUM((D$6*Prices!N18), (D$7*Prices!O18), (D$8*Prices!P18), (D$9*Prices!Q18))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L64" s="21">
+      <c r="L64" s="76">
         <f>IFERROR(SUM((E$6*Prices!O18), (E$7*Prices!P18), (E$8*Prices!Q18), (E$9*Prices!R18))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="M64" s="21">
+      <c r="M64" s="76">
         <f>IFERROR(SUM((F$6*Prices!P18), (F$7*Prices!Q18), (F$8*Prices!R18), (F$9*Prices!S18))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N64" s="21">
+      <c r="N64" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q18), (G$7*Prices!R18), (G$8*Prices!S18), (G$9*Prices!T18))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O64" s="21">
+      <c r="O64" s="76">
         <f>IFERROR(SUM((H$6*Prices!R18), (H$7*Prices!S18), (H$8*Prices!T18), (H$9*Prices!U18))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17162,23 +17172,23 @@
       <c r="H65" s="29">
         <v>0</v>
       </c>
-      <c r="K65" s="21">
+      <c r="K65" s="76">
         <f>IFERROR(SUM((D$6*Prices!N19), (D$7*Prices!O19), (D$8*Prices!P19), (D$9*Prices!Q19))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="L65" s="21">
+      <c r="L65" s="76">
         <f>IFERROR(SUM((E$6*Prices!O19), (E$7*Prices!P19), (E$8*Prices!Q19), (E$9*Prices!R19))/SUM(E$6:E$9),1)</f>
         <v>0</v>
       </c>
-      <c r="M65" s="21">
+      <c r="M65" s="76">
         <f>IFERROR(SUM((F$6*Prices!P19), (F$7*Prices!Q19), (F$8*Prices!R19), (F$9*Prices!S19))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="N65" s="21">
+      <c r="N65" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q19), (G$7*Prices!R19), (G$8*Prices!S19), (G$9*Prices!T19))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="O65" s="21">
+      <c r="O65" s="76">
         <f>IFERROR(SUM((H$6*Prices!R19), (H$7*Prices!S19), (H$8*Prices!T19), (H$9*Prices!U19))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17420,6 +17430,9 @@
       <c r="J78" s="88" t="s">
         <v>103</v>
       </c>
+      <c r="Q78" s="21" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C79" s="28" t="s">
@@ -17463,23 +17476,23 @@
         <f t="shared" si="1"/>
         <v>1E-3</v>
       </c>
-      <c r="Q79" s="21">
+      <c r="Q79" s="76">
         <f>IFERROR(SUM((D$6*Prices!N21), (D$7*Prices!O21), (D$8*Prices!P21), (D$9*Prices!Q21))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R79" s="21">
+      <c r="R79" s="76">
         <f>IFERROR(SUM((E$6*Prices!O21), (E$7*Prices!P21), (E$8*Prices!Q21), (E$9*Prices!R21))/SUM(E$6:E$9),1)</f>
         <v>0</v>
       </c>
-      <c r="S79" s="21">
+      <c r="S79" s="76">
         <f>IFERROR(SUM((F$6*Prices!P21), (F$7*Prices!Q21), (F$8*Prices!R21), (F$9*Prices!S21))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T79" s="21">
+      <c r="T79" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q21), (G$7*Prices!R21), (G$8*Prices!S21), (G$9*Prices!T21))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U79" s="21">
+      <c r="U79" s="76">
         <f>IFERROR(SUM((H$6*Prices!R21), (H$7*Prices!S21), (H$8*Prices!T21), (H$9*Prices!U21))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17532,23 +17545,23 @@
         <f t="shared" si="1"/>
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="Q80" s="21">
+      <c r="Q80" s="76">
         <f>IFERROR(SUM((D$6*Prices!N22), (D$7*Prices!O22), (D$8*Prices!P22), (D$9*Prices!Q22))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R80" s="21">
+      <c r="R80" s="76">
         <f>IFERROR(SUM((E$6*Prices!O22), (E$7*Prices!P22), (E$8*Prices!Q22), (E$9*Prices!R22))/SUM(E$6:E$9),1)</f>
         <v>0.68352946804439341</v>
       </c>
-      <c r="S80" s="21">
+      <c r="S80" s="76">
         <f>IFERROR(SUM((F$6*Prices!P22), (F$7*Prices!Q22), (F$8*Prices!R22), (F$9*Prices!S22))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T80" s="21">
+      <c r="T80" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q22), (G$7*Prices!R22), (G$8*Prices!S22), (G$9*Prices!T22))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U80" s="21">
+      <c r="U80" s="76">
         <f>IFERROR(SUM((H$6*Prices!R22), (H$7*Prices!S22), (H$8*Prices!T22), (H$9*Prices!U22))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17601,23 +17614,23 @@
         <f t="shared" si="1"/>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="Q81" s="21">
+      <c r="Q81" s="76">
         <f>IFERROR(SUM((D$6*Prices!N23), (D$7*Prices!O23), (D$8*Prices!P23), (D$9*Prices!Q23))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R81" s="21">
+      <c r="R81" s="76">
         <f>IFERROR(SUM((E$6*Prices!O23), (E$7*Prices!P23), (E$8*Prices!Q23), (E$9*Prices!R23))/SUM(E$6:E$9),1)</f>
         <v>0.6794552876642429</v>
       </c>
-      <c r="S81" s="21">
+      <c r="S81" s="76">
         <f>IFERROR(SUM((F$6*Prices!P23), (F$7*Prices!Q23), (F$8*Prices!R23), (F$9*Prices!S23))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T81" s="21">
+      <c r="T81" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q23), (G$7*Prices!R23), (G$8*Prices!S23), (G$9*Prices!T23))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U81" s="21">
+      <c r="U81" s="76">
         <f>IFERROR(SUM((H$6*Prices!R23), (H$7*Prices!S23), (H$8*Prices!T23), (H$9*Prices!U23))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17670,23 +17683,23 @@
         <f t="shared" si="1"/>
         <v>1.3000000000000002E-3</v>
       </c>
-      <c r="Q82" s="21">
+      <c r="Q82" s="76">
         <f>IFERROR(SUM((D$6*Prices!N24), (D$7*Prices!O24), (D$8*Prices!P24), (D$9*Prices!Q24))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R82" s="21">
+      <c r="R82" s="76">
         <f>IFERROR(SUM((E$6*Prices!O24), (E$7*Prices!P24), (E$8*Prices!Q24), (E$9*Prices!R24))/SUM(E$6:E$9),1)</f>
         <v>0.6794552876642429</v>
       </c>
-      <c r="S82" s="21">
+      <c r="S82" s="76">
         <f>IFERROR(SUM((F$6*Prices!P24), (F$7*Prices!Q24), (F$8*Prices!R24), (F$9*Prices!S24))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T82" s="21">
+      <c r="T82" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q24), (G$7*Prices!R24), (G$8*Prices!S24), (G$9*Prices!T24))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U82" s="21">
+      <c r="U82" s="76">
         <f>IFERROR(SUM((H$6*Prices!R24), (H$7*Prices!S24), (H$8*Prices!T24), (H$9*Prices!U24))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17739,23 +17752,23 @@
         <f t="shared" si="1"/>
         <v>1.4000000000000002E-3</v>
       </c>
-      <c r="Q83" s="21">
+      <c r="Q83" s="76">
         <f>IFERROR(SUM((D$6*Prices!N25), (D$7*Prices!O25), (D$8*Prices!P25), (D$9*Prices!Q25))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R83" s="21">
+      <c r="R83" s="76">
         <f>IFERROR(SUM((E$6*Prices!O25), (E$7*Prices!P25), (E$8*Prices!Q25), (E$9*Prices!R25))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="S83" s="21">
+      <c r="S83" s="76">
         <f>IFERROR(SUM((F$6*Prices!P25), (F$7*Prices!Q25), (F$8*Prices!R25), (F$9*Prices!S25))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T83" s="21">
+      <c r="T83" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q25), (G$7*Prices!R25), (G$8*Prices!S25), (G$9*Prices!T25))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U83" s="21">
+      <c r="U83" s="76">
         <f>IFERROR(SUM((H$6*Prices!R25), (H$7*Prices!S25), (H$8*Prices!T25), (H$9*Prices!U25))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17808,23 +17821,23 @@
         <f t="shared" si="1"/>
         <v>1.5000000000000002E-3</v>
       </c>
-      <c r="Q84" s="21">
+      <c r="Q84" s="76">
         <f>IFERROR(SUM((D$6*Prices!N26), (D$7*Prices!O26), (D$8*Prices!P26), (D$9*Prices!Q26))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R84" s="21">
+      <c r="R84" s="76">
         <f>IFERROR(SUM((E$6*Prices!O26), (E$7*Prices!P26), (E$8*Prices!Q26), (E$9*Prices!R26))/SUM(E$6:E$9),1)</f>
         <v>0.68181209337925752</v>
       </c>
-      <c r="S84" s="21">
+      <c r="S84" s="76">
         <f>IFERROR(SUM((F$6*Prices!P26), (F$7*Prices!Q26), (F$8*Prices!R26), (F$9*Prices!S26))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T84" s="21">
+      <c r="T84" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q26), (G$7*Prices!R26), (G$8*Prices!S26), (G$9*Prices!T26))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U84" s="21">
+      <c r="U84" s="76">
         <f>IFERROR(SUM((H$6*Prices!R26), (H$7*Prices!S26), (H$8*Prices!T26), (H$9*Prices!U26))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17877,23 +17890,23 @@
         <f t="shared" si="1"/>
         <v>1.6000000000000003E-3</v>
       </c>
-      <c r="Q85" s="21">
+      <c r="Q85" s="76">
         <f>IFERROR(SUM((D$6*Prices!N27), (D$7*Prices!O27), (D$8*Prices!P27), (D$9*Prices!Q27))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R85" s="21">
+      <c r="R85" s="76">
         <f>IFERROR(SUM((E$6*Prices!O27), (E$7*Prices!P27), (E$8*Prices!Q27), (E$9*Prices!R27))/SUM(E$6:E$9),1)</f>
         <v>0.68249904324531185</v>
       </c>
-      <c r="S85" s="21">
+      <c r="S85" s="76">
         <f>IFERROR(SUM((F$6*Prices!P27), (F$7*Prices!Q27), (F$8*Prices!R27), (F$9*Prices!S27))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T85" s="21">
+      <c r="T85" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q27), (G$7*Prices!R27), (G$8*Prices!S27), (G$9*Prices!T27))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U85" s="21">
+      <c r="U85" s="76">
         <f>IFERROR(SUM((H$6*Prices!R27), (H$7*Prices!S27), (H$8*Prices!T27), (H$9*Prices!U27))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -17946,23 +17959,23 @@
         <f t="shared" si="1"/>
         <v>1.7000000000000003E-3</v>
       </c>
-      <c r="Q86" s="21">
+      <c r="Q86" s="76">
         <f>IFERROR(SUM((D$6*Prices!N28), (D$7*Prices!O28), (D$8*Prices!P28), (D$9*Prices!Q28))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R86" s="21">
+      <c r="R86" s="76">
         <f>IFERROR(SUM((E$6*Prices!O28), (E$7*Prices!P28), (E$8*Prices!Q28), (E$9*Prices!R28))/SUM(E$6:E$9),1)</f>
         <v>0.6749791765156119</v>
       </c>
-      <c r="S86" s="21">
+      <c r="S86" s="76">
         <f>IFERROR(SUM((F$6*Prices!P28), (F$7*Prices!Q28), (F$8*Prices!R28), (F$9*Prices!S28))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T86" s="21">
+      <c r="T86" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q28), (G$7*Prices!R28), (G$8*Prices!S28), (G$9*Prices!T28))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U86" s="21">
+      <c r="U86" s="76">
         <f>IFERROR(SUM((H$6*Prices!R28), (H$7*Prices!S28), (H$8*Prices!T28), (H$9*Prices!U28))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -18015,23 +18028,23 @@
         <f>IF(Inputs!$C$4="Yes", 0, H76+H87+$J87)</f>
         <v>1.8000000000000004E-3</v>
       </c>
-      <c r="Q87" s="21">
+      <c r="Q87" s="76">
         <f>IFERROR(SUM((D$6*Prices!N29), (D$7*Prices!O29), (D$8*Prices!P29), (D$9*Prices!Q29))/SUM(D$6:D$9),1)</f>
         <v>1</v>
       </c>
-      <c r="R87" s="21">
+      <c r="R87" s="76">
         <f>IFERROR(SUM((E$6*Prices!O29), (E$7*Prices!P29), (E$8*Prices!Q29), (E$9*Prices!R29))/SUM(E$6:E$9),1)</f>
         <v>0.68181209337925752</v>
       </c>
-      <c r="S87" s="21">
+      <c r="S87" s="76">
         <f>IFERROR(SUM((F$6*Prices!P29), (F$7*Prices!Q29), (F$8*Prices!R29), (F$9*Prices!S29))/SUM(F$6:F$9),1)</f>
         <v>1</v>
       </c>
-      <c r="T87" s="21">
+      <c r="T87" s="76">
         <f>IFERROR(SUM((G$6*Prices!Q29), (G$7*Prices!R29), (G$8*Prices!S29), (G$9*Prices!T29))/SUM(G$6:G$9),1)</f>
         <v>1</v>
       </c>
-      <c r="U87" s="21">
+      <c r="U87" s="76">
         <f>IFERROR(SUM((H$6*Prices!R29), (H$7*Prices!S29), (H$8*Prices!T29), (H$9*Prices!U29))/SUM(H$6:H$9),1)</f>
         <v>1</v>
       </c>
@@ -19137,9 +19150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19268,7 +19279,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" ref="P6:R6" si="0">F6/$E6</f>
+        <f t="shared" ref="P6" si="0">F6/$E6</f>
         <v>0.6</v>
       </c>
       <c r="Q6" s="8">
@@ -19398,7 +19409,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" ref="P10:P29" si="5">F11/$E11</f>
+        <f t="shared" ref="P11:P29" si="5">F11/$E11</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="Q11" s="8">
@@ -19443,7 +19454,7 @@
         <v>0.6</v>
       </c>
       <c r="Q12" s="8">
-        <f t="shared" ref="Q10:Q29" si="6">G12/$E12</f>
+        <f t="shared" ref="Q12:Q29" si="6">G12/$E12</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="R12" s="8">
@@ -20186,9 +20197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
add back base fee shift
It was lost along the way during updates
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1329,7 +1329,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2919,7 +2919,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,7 +3081,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="98">
-        <v>0</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I7" s="50"/>
       <c r="K7" s="12"/>
@@ -3135,11 +3135,11 @@
       <c r="J10" s="3"/>
       <c r="K10" s="16">
         <f>(IF(Inputs!C5="New York",$H$7,-$H$7)+F10)*$D10</f>
-        <v>20565</v>
+        <v>16709.0625</v>
       </c>
       <c r="L10" s="99">
         <f>(IF(Inputs!C5="New York",-$H$7,$H$7)+G10)*D10</f>
-        <v>30847.5</v>
+        <v>34703.4375</v>
       </c>
       <c r="M10" s="16">
         <f t="shared" ref="M10:N20" si="2">H10*$D10</f>
@@ -3638,11 +3638,11 @@
       <c r="J25" s="3"/>
       <c r="K25" s="16">
         <f>(IF(Inputs!C5="New York",$H$7,-$H$7)+F25)*$D25</f>
-        <v>7522.8952500000023</v>
+        <v>5786.8425000000016</v>
       </c>
       <c r="L25" s="16">
         <f>(IF(Inputs!C5="New York",-$H$7,$H$7)+G25)*$D25</f>
-        <v>15624.474749999999</v>
+        <v>17360.5275</v>
       </c>
       <c r="M25" s="16">
         <f>H25*$D25</f>
@@ -4952,11 +4952,11 @@
       </c>
       <c r="F61" s="3">
         <f>IFERROR(SUM(K10:K60)/SUM($K10:$N60), 0)</f>
-        <v>0.25931832370956281</v>
+        <v>0.24420800408756077</v>
       </c>
       <c r="G61" s="3">
         <f>IFERROR(SUM(L10:L60)/SUM($K10:$N60), 0)</f>
-        <v>0.73819493668532088</v>
+        <v>0.75330525630732303</v>
       </c>
       <c r="H61" s="3">
         <f>IFERROR(SUM(M10:M60)/SUM($K10:$N60), 0)</f>
@@ -4969,11 +4969,11 @@
       <c r="J61" s="3"/>
       <c r="K61" s="12">
         <f>F61*$D$61</f>
-        <v>-14943.643685814443</v>
+        <v>-14072.886736672395</v>
       </c>
       <c r="L61" s="12">
         <f>G61*$D$61</f>
-        <v>-42539.693866187787</v>
+        <v>-43410.450815329837</v>
       </c>
       <c r="M61" s="12">
         <f>H61*$D$61</f>
@@ -5040,11 +5040,11 @@
       </c>
       <c r="K64" s="12">
         <f>SUM(K60:K62, K38:K46, K10:K20,K25:K35,K49:K57)</f>
-        <v>81024.249390300829</v>
+        <v>76303.016089442855</v>
       </c>
       <c r="L64" s="12">
         <f>SUM(L60:L62, L38:L46, L10:L20,L25:L35,L49:L57)</f>
-        <v>230649.68874177217</v>
+        <v>235370.92204263012</v>
       </c>
       <c r="M64" s="12">
         <f>SUM(M60:M62, M38:M46, M10:M20,M25:M35,M49:M57)</f>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="D65" s="23">
         <f>SUM(K64:N64)</f>
-        <v>312450.92221500003</v>
+        <v>312450.92221499997</v>
       </c>
       <c r="E65" s="2"/>
       <c r="K65" s="12"/>
@@ -5136,11 +5136,11 @@
       </c>
       <c r="K69" s="12">
         <f>SUM(Outputs_Timeline!X:X)</f>
-        <v>247572.74817090249</v>
+        <v>233409.04826832862</v>
       </c>
       <c r="L69" s="12">
         <f>SUM(Outputs_Timeline!Y:Y)</f>
-        <v>712449.06622531638</v>
+        <v>726612.76612789044</v>
       </c>
       <c r="M69" s="12">
         <f>SUM(Outputs_Timeline!Z:Z)</f>
@@ -5156,11 +5156,11 @@
       <c r="D70" s="1"/>
       <c r="K70" s="52">
         <f>IFERROR(K69/$D$69, 0)</f>
-        <v>0.25725779231040447</v>
+        <v>0.24254000856884364</v>
       </c>
       <c r="L70" s="52">
         <f>IFERROR(L69/$D$69, 0)</f>
-        <v>0.74032006860549737</v>
+        <v>0.75503785234705834</v>
       </c>
       <c r="M70" s="52">
         <f>IFERROR(M69/$D$69, 0)</f>
@@ -7626,11 +7626,11 @@
       </c>
       <c r="Q21" s="62">
         <f>$F21*Outputs_Internal!K$64/12+N21*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R21" s="62">
         <f>$F21*Outputs_Internal!L$64/12+N21*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S21" s="62">
         <f>N21*'MARA Prices'!$F$4</f>
@@ -7730,11 +7730,11 @@
       </c>
       <c r="Q22" s="62">
         <f>$F22*Outputs_Internal!K$64/12+N22*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R22" s="62">
         <f>$F22*Outputs_Internal!L$64/12+N22*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S22" s="62">
         <f>N22*'MARA Prices'!$F$4</f>
@@ -7834,11 +7834,11 @@
       </c>
       <c r="Q23" s="62">
         <f>$F23*Outputs_Internal!K$64/12+N23*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R23" s="62">
         <f>$F23*Outputs_Internal!L$64/12+N23*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S23" s="62">
         <f>N23*'MARA Prices'!$F$4</f>
@@ -7858,11 +7858,11 @@
       </c>
       <c r="X23" s="62">
         <f t="shared" si="3"/>
-        <v>24756.062347575207</v>
+        <v>23575.75402236071</v>
       </c>
       <c r="Y23" s="62">
         <f t="shared" si="4"/>
-        <v>78162.422185443051</v>
+        <v>79342.730510657537</v>
       </c>
       <c r="Z23" s="62">
         <f t="shared" si="5"/>
@@ -7938,11 +7938,11 @@
       </c>
       <c r="Q24" s="62">
         <f>$F24*Outputs_Internal!K$64/12+N24*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R24" s="62">
         <f>$F24*Outputs_Internal!L$64/12+N24*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S24" s="62">
         <f>N24*'MARA Prices'!$F$4</f>
@@ -8042,11 +8042,11 @@
       </c>
       <c r="Q25" s="62">
         <f>$F25*Outputs_Internal!K$64/12+N25*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R25" s="62">
         <f>$F25*Outputs_Internal!L$64/12+N25*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S25" s="62">
         <f>N25*'MARA Prices'!$F$4</f>
@@ -8146,11 +8146,11 @@
       </c>
       <c r="Q26" s="62">
         <f>$F26*Outputs_Internal!K$64/12+N26*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R26" s="62">
         <f>$F26*Outputs_Internal!L$64/12+N26*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S26" s="62">
         <f>N26*'MARA Prices'!$F$4</f>
@@ -8170,11 +8170,11 @@
       </c>
       <c r="X26" s="62">
         <f t="shared" si="3"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y26" s="62">
         <f t="shared" si="4"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z26" s="62">
         <f t="shared" si="5"/>
@@ -8250,11 +8250,11 @@
       </c>
       <c r="Q27" s="62">
         <f>$F27*Outputs_Internal!K$64/12+N27*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R27" s="62">
         <f>$F27*Outputs_Internal!L$64/12+N27*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S27" s="62">
         <f>N27*'MARA Prices'!$F$4</f>
@@ -8354,11 +8354,11 @@
       </c>
       <c r="Q28" s="62">
         <f>$F28*Outputs_Internal!K$64/12+N28*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R28" s="62">
         <f>$F28*Outputs_Internal!L$64/12+N28*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S28" s="62">
         <f>N28*'MARA Prices'!$F$4</f>
@@ -8458,11 +8458,11 @@
       </c>
       <c r="Q29" s="62">
         <f>$F29*Outputs_Internal!K$64/12+N29*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R29" s="62">
         <f>$F29*Outputs_Internal!L$64/12+N29*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S29" s="62">
         <f>N29*'MARA Prices'!$F$4</f>
@@ -8482,11 +8482,11 @@
       </c>
       <c r="X29" s="62">
         <f t="shared" si="3"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y29" s="62">
         <f t="shared" si="4"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z29" s="62">
         <f t="shared" si="5"/>
@@ -8562,11 +8562,11 @@
       </c>
       <c r="Q30" s="62">
         <f>$F30*Outputs_Internal!K$64/12+N30*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R30" s="62">
         <f>$F30*Outputs_Internal!L$64/12+N30*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S30" s="62">
         <f>N30*'MARA Prices'!$F$4</f>
@@ -8666,11 +8666,11 @@
       </c>
       <c r="Q31" s="62">
         <f>$F31*Outputs_Internal!K$64/12+N31*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R31" s="62">
         <f>$F31*Outputs_Internal!L$64/12+N31*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S31" s="62">
         <f>N31*'MARA Prices'!$F$4</f>
@@ -8770,11 +8770,11 @@
       </c>
       <c r="Q32" s="62">
         <f>$F32*Outputs_Internal!K$64/12+N32*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R32" s="62">
         <f>$F32*Outputs_Internal!L$64/12+N32*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S32" s="62">
         <f>N32*'MARA Prices'!$F$4</f>
@@ -8794,11 +8794,11 @@
       </c>
       <c r="X32" s="62">
         <f t="shared" si="3"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y32" s="62">
         <f t="shared" si="4"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z32" s="62">
         <f t="shared" si="5"/>
@@ -8874,11 +8874,11 @@
       </c>
       <c r="Q33" s="62">
         <f>$F33*Outputs_Internal!K$64/12+N33*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R33" s="62">
         <f>$F33*Outputs_Internal!L$64/12+N33*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S33" s="62">
         <f>N33*'MARA Prices'!$F$4</f>
@@ -8978,11 +8978,11 @@
       </c>
       <c r="Q34" s="62">
         <f>$F34*Outputs_Internal!K$64/12+N34*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R34" s="62">
         <f>$F34*Outputs_Internal!L$64/12+N34*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S34" s="62">
         <f>N34*'MARA Prices'!$F$4</f>
@@ -9082,11 +9082,11 @@
       </c>
       <c r="Q35" s="62">
         <f>$F35*Outputs_Internal!K$64/12+N35*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R35" s="62">
         <f>$F35*Outputs_Internal!L$64/12+N35*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S35" s="62">
         <f>N35*'MARA Prices'!$F$4</f>
@@ -9106,11 +9106,11 @@
       </c>
       <c r="X35" s="62">
         <f t="shared" si="3"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y35" s="62">
         <f t="shared" si="4"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z35" s="62">
         <f t="shared" si="5"/>
@@ -9186,11 +9186,11 @@
       </c>
       <c r="Q36" s="62">
         <f>$F36*Outputs_Internal!K$64/12+N36*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R36" s="62">
         <f>$F36*Outputs_Internal!L$64/12+N36*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S36" s="62">
         <f>N36*'MARA Prices'!$F$4</f>
@@ -9290,11 +9290,11 @@
       </c>
       <c r="Q37" s="62">
         <f>$F37*Outputs_Internal!K$64/12+N37*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R37" s="62">
         <f>$F37*Outputs_Internal!L$64/12+N37*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S37" s="62">
         <f>N37*'MARA Prices'!$F$4</f>
@@ -9394,11 +9394,11 @@
       </c>
       <c r="Q38" s="62">
         <f>$F38*Outputs_Internal!K$64/12+N38*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R38" s="62">
         <f>$F38*Outputs_Internal!L$64/12+N38*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S38" s="62">
         <f>N38*'MARA Prices'!$F$4</f>
@@ -9418,11 +9418,11 @@
       </c>
       <c r="X38" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y38" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z38" s="62">
         <f t="shared" si="10"/>
@@ -9498,11 +9498,11 @@
       </c>
       <c r="Q39" s="62">
         <f>$F39*Outputs_Internal!K$64/12+N39*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R39" s="62">
         <f>$F39*Outputs_Internal!L$64/12+N39*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S39" s="62">
         <f>N39*'MARA Prices'!$F$4</f>
@@ -9602,11 +9602,11 @@
       </c>
       <c r="Q40" s="62">
         <f>$F40*Outputs_Internal!K$64/12+N40*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R40" s="62">
         <f>$F40*Outputs_Internal!L$64/12+N40*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S40" s="62">
         <f>N40*'MARA Prices'!$F$4</f>
@@ -9706,11 +9706,11 @@
       </c>
       <c r="Q41" s="62">
         <f>$F41*Outputs_Internal!K$64/12+N41*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R41" s="62">
         <f>$F41*Outputs_Internal!L$64/12+N41*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S41" s="62">
         <f>N41*'MARA Prices'!$F$4</f>
@@ -9730,11 +9730,11 @@
       </c>
       <c r="X41" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y41" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z41" s="62">
         <f t="shared" si="10"/>
@@ -9810,11 +9810,11 @@
       </c>
       <c r="Q42" s="62">
         <f>$F42*Outputs_Internal!K$64/12+N42*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R42" s="62">
         <f>$F42*Outputs_Internal!L$64/12+N42*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S42" s="62">
         <f>N42*'MARA Prices'!$F$4</f>
@@ -9914,11 +9914,11 @@
       </c>
       <c r="Q43" s="62">
         <f>$F43*Outputs_Internal!K$64/12+N43*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R43" s="62">
         <f>$F43*Outputs_Internal!L$64/12+N43*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S43" s="62">
         <f>N43*'MARA Prices'!$F$4</f>
@@ -10018,11 +10018,11 @@
       </c>
       <c r="Q44" s="62">
         <f>$F44*Outputs_Internal!K$64/12+N44*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R44" s="62">
         <f>$F44*Outputs_Internal!L$64/12+N44*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S44" s="62">
         <f>N44*'MARA Prices'!$F$4</f>
@@ -10042,11 +10042,11 @@
       </c>
       <c r="X44" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y44" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z44" s="62">
         <f t="shared" si="10"/>
@@ -10122,11 +10122,11 @@
       </c>
       <c r="Q45" s="62">
         <f>$F45*Outputs_Internal!K$64/12+N45*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R45" s="62">
         <f>$F45*Outputs_Internal!L$64/12+N45*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S45" s="62">
         <f>N45*'MARA Prices'!$F$4</f>
@@ -10226,11 +10226,11 @@
       </c>
       <c r="Q46" s="62">
         <f>$F46*Outputs_Internal!K$64/12+N46*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R46" s="62">
         <f>$F46*Outputs_Internal!L$64/12+N46*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S46" s="62">
         <f>N46*'MARA Prices'!$F$4</f>
@@ -10330,11 +10330,11 @@
       </c>
       <c r="Q47" s="62">
         <f>$F47*Outputs_Internal!K$64/12+N47*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R47" s="62">
         <f>$F47*Outputs_Internal!L$64/12+N47*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S47" s="62">
         <f>N47*'MARA Prices'!$F$4</f>
@@ -10354,11 +10354,11 @@
       </c>
       <c r="X47" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y47" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z47" s="62">
         <f t="shared" si="10"/>
@@ -10434,11 +10434,11 @@
       </c>
       <c r="Q48" s="62">
         <f>$F48*Outputs_Internal!K$64/12+N48*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R48" s="62">
         <f>$F48*Outputs_Internal!L$64/12+N48*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S48" s="62">
         <f>N48*'MARA Prices'!$F$4</f>
@@ -10538,11 +10538,11 @@
       </c>
       <c r="Q49" s="62">
         <f>$F49*Outputs_Internal!K$64/12+N49*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R49" s="62">
         <f>$F49*Outputs_Internal!L$64/12+N49*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S49" s="62">
         <f>N49*'MARA Prices'!$F$4</f>
@@ -10642,11 +10642,11 @@
       </c>
       <c r="Q50" s="62">
         <f>$F50*Outputs_Internal!K$64/12+N50*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R50" s="62">
         <f>$F50*Outputs_Internal!L$64/12+N50*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S50" s="62">
         <f>N50*'MARA Prices'!$F$4</f>
@@ -10666,11 +10666,11 @@
       </c>
       <c r="X50" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y50" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z50" s="62">
         <f t="shared" si="10"/>
@@ -10746,11 +10746,11 @@
       </c>
       <c r="Q51" s="62">
         <f>$F51*Outputs_Internal!K$64/12+N51*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R51" s="62">
         <f>$F51*Outputs_Internal!L$64/12+N51*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S51" s="62">
         <f>N51*'MARA Prices'!$F$4</f>
@@ -10850,11 +10850,11 @@
       </c>
       <c r="Q52" s="62">
         <f>$F52*Outputs_Internal!K$64/12+N52*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R52" s="62">
         <f>$F52*Outputs_Internal!L$64/12+N52*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S52" s="62">
         <f>N52*'MARA Prices'!$F$4</f>
@@ -10954,11 +10954,11 @@
       </c>
       <c r="Q53" s="62">
         <f>$F53*Outputs_Internal!K$64/12+N53*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R53" s="62">
         <f>$F53*Outputs_Internal!L$64/12+N53*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S53" s="62">
         <f>N53*'MARA Prices'!$F$4</f>
@@ -10978,11 +10978,11 @@
       </c>
       <c r="X53" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y53" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z53" s="62">
         <f t="shared" si="10"/>
@@ -11058,11 +11058,11 @@
       </c>
       <c r="Q54" s="62">
         <f>$F54*Outputs_Internal!K$64/12+N54*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R54" s="62">
         <f>$F54*Outputs_Internal!L$64/12+N54*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S54" s="62">
         <f>N54*'MARA Prices'!$F$4</f>
@@ -11162,11 +11162,11 @@
       </c>
       <c r="Q55" s="62">
         <f>$F55*Outputs_Internal!K$64/12+N55*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R55" s="62">
         <f>$F55*Outputs_Internal!L$64/12+N55*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S55" s="62">
         <f>N55*'MARA Prices'!$F$4</f>
@@ -11266,11 +11266,11 @@
       </c>
       <c r="Q56" s="62">
         <f>$F56*Outputs_Internal!K$64/12+N56*'MARA Prices'!$F$5</f>
-        <v>6752.0207825250691</v>
+        <v>6358.5846741202377</v>
       </c>
       <c r="R56" s="62">
         <f>$F56*Outputs_Internal!L$64/12+N56*'MARA Prices'!$F$6</f>
-        <v>19220.80739514768</v>
+        <v>19614.243503552509</v>
       </c>
       <c r="S56" s="62">
         <f>N56*'MARA Prices'!$F$4</f>
@@ -11290,11 +11290,11 @@
       </c>
       <c r="X56" s="62">
         <f t="shared" si="8"/>
-        <v>20256.062347575207</v>
+        <v>19075.754022360714</v>
       </c>
       <c r="Y56" s="62">
         <f t="shared" si="9"/>
-        <v>57662.422185443036</v>
+        <v>58842.730510657522</v>
       </c>
       <c r="Z56" s="62">
         <f t="shared" si="10"/>
@@ -19150,7 +19150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>